<commit_message>
feat(docs/top): excel and visio
</commit_message>
<xml_diff>
--- a/hardware/docs/01-top/点云硬件参数分析.xlsx
+++ b/hardware/docs/01-top/点云硬件参数分析.xlsx
@@ -25,7 +25,7 @@
     <author>作者</author>
   </authors>
   <commentList>
-    <comment ref="K16" authorId="0" shapeId="0">
+    <comment ref="K17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K20" authorId="0" shapeId="0">
+    <comment ref="K21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="80">
   <si>
     <t>case</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -367,6 +367,30 @@
   </si>
   <si>
     <t>Parameters</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Top Level Module</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level 1 Module</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level 2 Module</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level 3 Module</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Area</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percentage of Area /%</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -748,7 +772,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -834,6 +858,81 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -857,75 +956,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1215,200 +1245,200 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.109375" style="37" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" style="37" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" style="37" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="37"/>
+    <col min="1" max="1" width="32.109375" style="29" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="29" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" style="29" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="39"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="58">
+      <c r="C2" s="47">
         <v>28</v>
       </c>
-      <c r="D2" s="39"/>
+      <c r="D2" s="31"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="59">
+      <c r="B3" s="48">
         <v>8</v>
       </c>
-      <c r="C3" s="58">
+      <c r="C3" s="47">
         <v>12.96</v>
       </c>
-      <c r="D3" s="39"/>
+      <c r="D3" s="31"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="59">
+      <c r="B4" s="48">
         <v>96</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="39"/>
+      <c r="D4" s="31"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="39"/>
+      <c r="D5" s="31"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="59">
+      <c r="B6" s="48">
         <v>200</v>
       </c>
-      <c r="C6" s="58">
+      <c r="C6" s="47">
         <v>250</v>
       </c>
-      <c r="D6" s="39"/>
+      <c r="D6" s="31"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="39"/>
+      <c r="D7" s="31"/>
     </row>
     <row r="8" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="56" t="s">
+      <c r="C8" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="39"/>
+      <c r="D8" s="31"/>
     </row>
     <row r="9" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="55" t="s">
+      <c r="A9" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="54"/>
+      <c r="B9" s="52"/>
       <c r="C9" s="53"/>
-      <c r="D9" s="39"/>
+      <c r="D9" s="31"/>
     </row>
     <row r="10" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="52">
+      <c r="B10" s="44">
         <v>1024</v>
       </c>
-      <c r="C10" s="51">
+      <c r="C10" s="43">
         <v>1024</v>
       </c>
-      <c r="D10" s="39"/>
+      <c r="D10" s="31"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="49">
+      <c r="B11" s="41">
         <f>B10*B6*2/1024/1024</f>
         <v>0.390625</v>
       </c>
-      <c r="C11" s="48">
+      <c r="C11" s="40">
         <f>C10*C6*2/1024/1024</f>
         <v>0.48828125</v>
       </c>
-      <c r="D11" s="39"/>
+      <c r="D11" s="31"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="44">
+      <c r="B12" s="36">
         <f>B11*24</f>
         <v>9.375</v>
       </c>
-      <c r="C12" s="43">
+      <c r="C12" s="35">
         <f>C11*24</f>
         <v>11.71875</v>
       </c>
-      <c r="D12" s="39"/>
+      <c r="D12" s="31"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="47">
+      <c r="B13" s="39">
         <v>0.1</v>
       </c>
-      <c r="C13" s="46">
+      <c r="C13" s="38">
         <v>0.60899999999999999</v>
       </c>
-      <c r="D13" s="39"/>
+      <c r="D13" s="31"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="44">
+      <c r="B14" s="36">
         <f>B11/B13</f>
         <v>3.90625</v>
       </c>
-      <c r="C14" s="43">
+      <c r="C14" s="35">
         <f>C11/C13</f>
         <v>0.80177545155993435</v>
       </c>
-      <c r="D14" s="39"/>
+      <c r="D14" s="31"/>
     </row>
     <row r="15" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="41">
+      <c r="B15" s="33">
         <f>B12/B13</f>
         <v>93.75</v>
       </c>
-      <c r="C15" s="40">
+      <c r="C15" s="32">
         <f>C12/C13</f>
         <v>19.242610837438423</v>
       </c>
-      <c r="D15" s="39"/>
+      <c r="D15" s="31"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="38"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1422,28 +1452,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O58"/>
+  <dimension ref="A1:O59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="N6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomRight" activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.88671875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="6.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" style="2" customWidth="1"/>
     <col min="3" max="3" width="18.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" style="26" customWidth="1"/>
-    <col min="6" max="6" width="16" style="10" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" style="10" customWidth="1"/>
-    <col min="9" max="9" width="22" style="11" customWidth="1"/>
-    <col min="10" max="10" width="19.77734375" style="8"/>
-    <col min="11" max="16384" width="19.77734375" style="2"/>
+    <col min="4" max="4" width="14.21875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="26" customWidth="1"/>
+    <col min="6" max="6" width="16" style="10" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" style="11" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" style="10" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="22" style="11" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="0" style="8" hidden="1" customWidth="1"/>
+    <col min="11" max="13" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="14" max="16384" width="19.77734375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -1454,14 +1485,14 @@
       <c r="C1" s="1"/>
       <c r="D1" s="6"/>
       <c r="E1" s="24"/>
-      <c r="F1" s="34">
+      <c r="F1" s="59">
         <v>0</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="34">
+      <c r="G1" s="60"/>
+      <c r="H1" s="59">
         <v>1</v>
       </c>
-      <c r="I1" s="35"/>
+      <c r="I1" s="60"/>
       <c r="J1" s="8">
         <v>2</v>
       </c>
@@ -1480,18 +1511,18 @@
       <c r="C2" s="1"/>
       <c r="D2" s="6"/>
       <c r="E2" s="25"/>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="36"/>
-      <c r="H2" s="29" t="s">
+      <c r="G2" s="61"/>
+      <c r="H2" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="36"/>
-      <c r="J2" s="29" t="s">
+      <c r="I2" s="61"/>
+      <c r="J2" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="30"/>
+      <c r="K2" s="55"/>
       <c r="L2" s="2" t="s">
         <v>41</v>
       </c>
@@ -1583,727 +1614,759 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="49"/>
+      <c r="B7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="12">
+      <c r="D8" s="6"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="12">
         <v>2207681</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H8" s="10">
         <v>2439312</v>
       </c>
-      <c r="J7" s="20">
+      <c r="J8" s="20">
         <v>806671</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L8" s="2">
         <v>806519</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N8" s="2">
         <v>1203839</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="1" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="57"/>
+      <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F9" s="10">
         <v>1673091</v>
       </c>
-      <c r="G8" s="13">
-        <f>F8/F7</f>
+      <c r="G9" s="13">
+        <f>F9/F8</f>
         <v>0.75784997923160091</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H9" s="10">
         <v>1691086</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J9" s="8">
         <v>20841</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N9" s="2">
         <v>21050</v>
       </c>
-      <c r="O8" s="2">
-        <f>N8/N7</f>
-        <v>1.7485726911987399E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="4" t="s">
+      <c r="O9" s="2">
+        <f>N9/N8*100</f>
+        <v>1.7485726911987398</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="57"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F10" s="21">
         <v>1383705</v>
       </c>
-      <c r="G9" s="11">
-        <f>F9/F8</f>
+      <c r="G10" s="11">
+        <f>F10/F9</f>
         <v>0.82703511046320854</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H10" s="10">
         <v>1401494</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J10" s="8">
         <v>19815</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="14"/>
-      <c r="J10" s="8">
-        <v>19250</v>
-      </c>
-    </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
+      <c r="A11" s="57"/>
       <c r="B11" s="1"/>
       <c r="C11" s="3"/>
-      <c r="E11" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="14">
-        <v>6429</v>
-      </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="23">
-        <v>6660</v>
+      <c r="D11" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="J11" s="8">
+        <v>19250</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
+      <c r="A12" s="57"/>
       <c r="B12" s="1"/>
       <c r="C12" s="3"/>
       <c r="E12" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="15">
-        <v>1424</v>
-      </c>
-      <c r="J12" s="8">
-        <v>1419</v>
+        <v>29</v>
+      </c>
+      <c r="H12" s="14">
+        <v>6429</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="23">
+        <v>6660</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="57"/>
       <c r="B13" s="1"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="27"/>
-      <c r="H13" s="15"/>
+      <c r="E13" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="15">
+        <v>1424</v>
+      </c>
+      <c r="J13" s="8">
+        <v>1419</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="57"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="27"/>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="57"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F15" s="10">
         <v>219671</v>
       </c>
-      <c r="G14" s="11">
-        <f>F14/F8</f>
+      <c r="G15" s="11">
+        <f>F15/F9</f>
         <v>0.13129650449377828</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H15" s="15">
         <v>219319</v>
       </c>
-      <c r="J14" s="20">
+      <c r="J15" s="20">
         <v>1006</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="25"/>
-    </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="1" t="s">
+      <c r="A16" s="57"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="25"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="57"/>
+      <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F17" s="15">
         <v>427284</v>
       </c>
-      <c r="G16" s="13">
-        <f>427284/F7</f>
+      <c r="G17" s="13">
+        <f>427284/F8</f>
         <v>0.1935442665856163</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H17" s="10">
         <v>434444</v>
       </c>
-      <c r="J16" s="28">
+      <c r="J17" s="28">
         <v>470319</v>
       </c>
-      <c r="K16" s="3">
-        <f>J16/J7</f>
+      <c r="K17" s="3">
+        <f>J17/J8</f>
         <v>0.58303695062795113</v>
       </c>
-      <c r="N16" s="2">
+      <c r="N17" s="2">
         <v>477691</v>
       </c>
-      <c r="O16" s="2">
-        <f>N16/N7</f>
-        <v>0.39680638357787046</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="15">
-        <v>9966</v>
-      </c>
-      <c r="G17" s="11">
-        <f>F17/F16</f>
-        <v>2.332406549274019E-2</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="J17" s="8">
-        <v>10227</v>
-      </c>
-      <c r="K17" s="4">
-        <v>0.75</v>
+      <c r="O17" s="50">
+        <f>N17/N8*100</f>
+        <v>39.680638357787046</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
+      <c r="A18" s="57"/>
       <c r="B18" s="1"/>
       <c r="C18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="15"/>
-      <c r="K18" s="2">
-        <v>0.193</v>
+        <v>17</v>
+      </c>
+      <c r="F18" s="15">
+        <v>9966</v>
+      </c>
+      <c r="G18" s="11">
+        <f>F18/F17</f>
+        <v>2.332406549274019E-2</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" s="8">
+        <v>10227</v>
+      </c>
+      <c r="K18" s="4">
+        <v>0.75</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
+      <c r="A19" s="57"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F19" s="15"/>
       <c r="K19" s="2">
+        <v>0.193</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="57"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="15"/>
+      <c r="K20" s="2">
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
-      <c r="B20" s="1" t="s">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="57"/>
+      <c r="B21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F21" s="16">
         <v>88906</v>
       </c>
-      <c r="G20" s="13">
-        <f>88906/F7</f>
+      <c r="G21" s="13">
+        <f>88906/F8</f>
         <v>4.0271216720169263E-2</v>
       </c>
-      <c r="J20" s="8">
+      <c r="J21" s="8">
         <v>174488</v>
       </c>
-      <c r="K20" s="3">
-        <f>J20/J7</f>
+      <c r="K21" s="3">
+        <f>J21/J8</f>
         <v>0.21630627604066591</v>
       </c>
-      <c r="N20" s="2">
+      <c r="N21" s="2">
         <v>176625</v>
       </c>
-      <c r="O20" s="2">
-        <f>N20/N7</f>
-        <v>0.14671812426744774</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="2" t="s">
+      <c r="O21" s="2">
+        <f>N21/N8*100</f>
+        <v>14.671812426744774</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="57"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F22" s="21">
         <v>52482</v>
       </c>
-      <c r="G21" s="11">
-        <f>F21/F20</f>
+      <c r="G22" s="11">
+        <f>F22/F21</f>
         <v>0.59030886554338291</v>
       </c>
-      <c r="J21" s="8">
+      <c r="J22" s="8">
         <v>58886</v>
       </c>
-      <c r="K21" s="2">
-        <f>J21/J20</f>
+      <c r="K22" s="2">
+        <f>J22/J21</f>
         <v>0.33747879510338818</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
-      <c r="B22" s="1"/>
-      <c r="D22" s="7" t="s">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="57"/>
+      <c r="B23" s="1"/>
+      <c r="D23" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="F22" s="21"/>
-      <c r="J22" s="8">
-        <v>7501</v>
-      </c>
-      <c r="K22" s="2">
-        <f>J22*6/J21</f>
-        <v>0.76429032367625582</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
-      <c r="B23" s="1"/>
-      <c r="E23" s="7" t="s">
-        <v>42</v>
       </c>
       <c r="F23" s="21"/>
       <c r="J23" s="8">
+        <v>7501</v>
+      </c>
+      <c r="K23" s="2">
+        <f>J23*6/J22</f>
+        <v>0.76429032367625582</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A24" s="57"/>
+      <c r="B24" s="1"/>
+      <c r="E24" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="21"/>
+      <c r="J24" s="8">
         <v>6756</v>
       </c>
-      <c r="K23" s="3">
-        <f>J23/J22</f>
+      <c r="K24" s="3">
+        <f>J24/J23</f>
         <v>0.90067990934542064</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" s="17">
-        <v>18793</v>
-      </c>
-      <c r="J24" s="20">
-        <v>18589</v>
-      </c>
-      <c r="K24" s="2">
-        <f>J24*6/J20</f>
-        <v>0.63920728072990696</v>
-      </c>
-    </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="32"/>
+      <c r="A25" s="57"/>
       <c r="B25" s="1"/>
       <c r="C25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" s="21">
-        <v>3249</v>
-      </c>
-      <c r="G25" s="18"/>
+        <v>19</v>
+      </c>
+      <c r="F25" s="17">
+        <v>18793</v>
+      </c>
       <c r="J25" s="20">
         <v>18589</v>
       </c>
+      <c r="K25" s="2">
+        <f>J25*6/J21</f>
+        <v>0.63920728072990696</v>
+      </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="32"/>
-      <c r="B26" s="1" t="s">
+      <c r="A26" s="57"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="21">
+        <v>3249</v>
+      </c>
+      <c r="G26" s="18"/>
+      <c r="J26" s="20">
+        <v>18589</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="57"/>
+      <c r="B27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="10">
+      <c r="F27" s="10">
         <v>10902</v>
       </c>
-      <c r="G26" s="13">
-        <f>10902/F7</f>
+      <c r="G27" s="13">
+        <f>10902/F8</f>
         <v>4.9382134465984894E-3</v>
       </c>
-      <c r="J26" s="8">
+      <c r="J27" s="8">
         <v>11312</v>
       </c>
-      <c r="K26" s="2">
-        <f>J26/J7</f>
+      <c r="K27" s="2">
+        <f>J27/J8</f>
         <v>1.4023065165352417E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="32"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F27" s="10">
-        <v>6816</v>
-      </c>
-      <c r="G27" s="11">
-        <f>F27/F26</f>
-        <v>0.62520638414969731</v>
-      </c>
-      <c r="J27" s="8">
-        <v>6819</v>
-      </c>
-      <c r="N27" s="2">
-        <v>11719</v>
+      <c r="N27" s="8">
+        <v>11312</v>
+      </c>
+      <c r="O27" s="2">
+        <f>N27/N8*100</f>
+        <v>0.93966053600190724</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="32"/>
+      <c r="A28" s="57"/>
       <c r="B28" s="1"/>
       <c r="C28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" s="10">
+        <v>6816</v>
+      </c>
+      <c r="G28" s="11">
+        <f>F28/F27</f>
+        <v>0.62520638414969731</v>
+      </c>
+      <c r="J28" s="8">
+        <v>6819</v>
+      </c>
+      <c r="N28" s="2">
+        <v>11719</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="57"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F28" s="10">
+      <c r="F29" s="10">
         <v>760</v>
       </c>
-      <c r="J28" s="8">
+      <c r="J29" s="8">
         <v>761</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
-      <c r="B29" s="1" t="s">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="57"/>
+      <c r="B30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="10">
+      <c r="F30" s="10">
         <v>2496</v>
       </c>
-      <c r="G29" s="13">
-        <f>2496/F7</f>
+      <c r="G30" s="13">
+        <f>2496/F8</f>
         <v>1.1305981253632205E-3</v>
       </c>
-      <c r="J29" s="8">
+      <c r="J30" s="8">
         <v>2797</v>
       </c>
-      <c r="K29" s="2">
-        <f>J29/J7</f>
+      <c r="K30" s="2">
+        <f>J30/J8</f>
         <v>3.4673367457116965E-3</v>
       </c>
-      <c r="N29" s="2">
+      <c r="N30" s="2">
         <v>2961</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="33"/>
-      <c r="B30" s="1" t="s">
+      <c r="O30" s="2">
+        <f>N30/N8*100</f>
+        <v>0.24596312297574677</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="58"/>
+      <c r="B31" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="F31" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="H30" s="12">
+      <c r="H31" s="12">
         <v>121931</v>
       </c>
-      <c r="I30" s="13">
-        <f>H30/F7</f>
+      <c r="I31" s="13">
+        <f>H31/F8</f>
         <v>5.5230352573582865E-2</v>
       </c>
-      <c r="J30" s="8">
+      <c r="J31" s="8">
         <v>121619</v>
       </c>
-      <c r="K30" s="2">
-        <f>J30/J7</f>
+      <c r="K31" s="2">
+        <f>J31/J8</f>
         <v>0.15076654546897061</v>
       </c>
-      <c r="N30" s="2">
+      <c r="N31" s="2">
         <v>507456</v>
       </c>
-      <c r="O30" s="2">
-        <f>N30/N7</f>
-        <v>0.42153145063417946</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H31" s="10">
-        <v>33555</v>
-      </c>
-      <c r="J31" s="9">
-        <v>33586</v>
-      </c>
-      <c r="K31" s="1"/>
-      <c r="N31" s="2">
-        <v>44581</v>
+      <c r="O31" s="50">
+        <f>N31/N8*100</f>
+        <v>42.153145063417945</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="1"/>
       <c r="C32" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H32" s="10">
-        <v>21655</v>
+        <v>33555</v>
       </c>
       <c r="J32" s="9">
-        <v>21600</v>
+        <v>33586</v>
       </c>
       <c r="K32" s="1"/>
       <c r="N32" s="2">
+        <v>44581</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H33" s="10">
+        <v>21655</v>
+      </c>
+      <c r="J33" s="9">
+        <v>21600</v>
+      </c>
+      <c r="K33" s="1"/>
+      <c r="N33" s="2">
         <v>114849</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="D33" s="7" t="s">
+    <row r="34" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="D34" s="7" t="s">
         <v>44</v>
-      </c>
-      <c r="I33" s="13"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="1"/>
-      <c r="N33" s="10">
-        <v>7094</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="E34" s="26" t="s">
-        <v>45</v>
       </c>
       <c r="I34" s="13"/>
       <c r="J34" s="9"/>
       <c r="K34" s="1"/>
       <c r="N34" s="10">
-        <v>362</v>
+        <v>7094</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
-      <c r="E35" s="25" t="s">
-        <v>46</v>
+      <c r="E35" s="26" t="s">
+        <v>45</v>
       </c>
       <c r="I35" s="13"/>
       <c r="J35" s="9"/>
       <c r="K35" s="1"/>
       <c r="N35" s="10">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="E36" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="I36" s="13"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="1"/>
+      <c r="N36" s="10">
         <v>689</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="31" t="s">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="2"/>
-      <c r="L36" s="2">
+      <c r="D37" s="6"/>
+      <c r="E37" s="2"/>
+      <c r="L37" s="2">
         <v>30.434922</v>
       </c>
-      <c r="N36" s="2">
+      <c r="N37" s="2">
         <v>74.7</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="32"/>
-      <c r="B37" s="1" t="s">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="57"/>
+      <c r="B38" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L37" s="2">
+      <c r="L38" s="2">
         <v>1.5</v>
       </c>
-      <c r="M37" s="2">
-        <f>L37/L36</f>
+      <c r="M38" s="2">
+        <f>L38/L37</f>
         <v>4.9285488558176688E-2</v>
       </c>
-      <c r="N37" s="2">
+      <c r="N38" s="2">
         <v>1.4</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="32"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="4" t="s">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="57"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="32"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="32"/>
+      <c r="A40" s="57"/>
       <c r="B40" s="1"/>
       <c r="C40" s="3"/>
-      <c r="E40" s="19" t="s">
-        <v>29</v>
+      <c r="D40" s="11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="32"/>
+      <c r="A41" s="57"/>
       <c r="B41" s="1"/>
       <c r="C41" s="3"/>
       <c r="E41" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="32"/>
+      <c r="A42" s="57"/>
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="27"/>
+      <c r="E42" s="19" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="32"/>
+      <c r="A43" s="57"/>
       <c r="B43" s="1"/>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="3"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="27"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="57"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="32"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="25"/>
-    </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="32"/>
-      <c r="B45" s="1" t="s">
+      <c r="A45" s="57"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="25"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="57"/>
+      <c r="B46" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L45" s="2">
+      <c r="L46" s="2">
         <v>7.2</v>
       </c>
-      <c r="M45" s="2">
-        <f>L45/L36</f>
+      <c r="M46" s="2">
+        <f>L46/L37</f>
         <v>0.23657034507924812</v>
       </c>
-      <c r="N45" s="2">
+      <c r="N46" s="2">
         <v>4.3</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="33"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="58"/>
       <c r="B47" s="1"/>
       <c r="C47" s="2" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="C48" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B49" s="1"/>
+      <c r="C49" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B49" s="1" t="s">
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L49" s="2">
+      <c r="L50" s="2">
         <v>12.7</v>
       </c>
-      <c r="M49" s="22">
-        <f>L49/L36</f>
+      <c r="M50" s="22">
+        <f>L50/L37</f>
         <v>0.41728380312589597</v>
       </c>
-      <c r="N49" s="2">
+      <c r="N50" s="2">
         <v>8.6</v>
-      </c>
-    </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B50" s="1"/>
-      <c r="C50" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B53" s="1"/>
+      <c r="C53" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B53" s="1" t="s">
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L53" s="2">
+      <c r="L54" s="2">
         <v>0.69</v>
       </c>
-      <c r="N53" s="2">
+      <c r="N54" s="2">
         <v>0.5</v>
-      </c>
-    </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B54" s="1"/>
-      <c r="C54" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
       <c r="C55" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B56" s="1"/>
+      <c r="C56" s="2" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B56" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L56" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="N56" s="2">
-        <v>6.7000000000000004E-2</v>
       </c>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L57" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="N57" s="2">
+        <v>6.7000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B58" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L57" s="2">
+      <c r="L58" s="2">
         <v>6.9</v>
       </c>
-      <c r="M57" s="2">
-        <f>L57/L36</f>
+      <c r="M58" s="2">
+        <f>L58/L37</f>
         <v>0.22671324736761278</v>
       </c>
-      <c r="N57" s="2">
+      <c r="N58" s="2">
         <v>59.2</v>
       </c>
-      <c r="O57" s="3">
-        <f>N57/N36</f>
+      <c r="O58" s="3">
+        <f>N58/N37</f>
         <v>0.79250334672021416</v>
       </c>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="O58" s="2" t="s">
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="O59" s="2" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A7:A30"/>
-    <mergeCell ref="A36:A46"/>
+    <mergeCell ref="A8:A31"/>
+    <mergeCell ref="A37:A47"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="F2:G2"/>

</xml_diff>

<commit_message>
feat(parameter summary): Update DSPU
</commit_message>
<xml_diff>
--- a/hardware/docs/01-top/点云硬件参数分析.xlsx
+++ b/hardware/docs/01-top/点云硬件参数分析.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="5772" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="12960" windowHeight="5775"/>
   </bookViews>
   <sheets>
     <sheet name="整体评估" sheetId="5" r:id="rId1"/>
@@ -20,6 +20,121 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>作者</author>
+  </authors>
+  <commentList>
+    <comment ref="C11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+堪称恐怖</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+4b，全跑满的真实算力</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+8b表直接给的有效算力，与真实(4b)相差8倍是因为有技术加持</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B16" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+胜在功耗低
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>作者</author>
@@ -82,7 +197,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="83">
   <si>
     <t>case</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -279,9 +394,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Energy Efficiency (TOPS/W)</t>
-  </si>
-  <si>
     <t>Power Consumption (W)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -290,10 +402,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">Performance (TOPS) </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MAC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -391,6 +499,26 @@
   </si>
   <si>
     <t>Percentage of Area /%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Real Performance (TOPS) </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Real Energy Efficiency (TOPS/W)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.78-1.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Supply Voltge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scale to 55-nm 0.9V</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -861,18 +989,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -885,9 +1007,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -923,6 +1042,15 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1236,217 +1364,234 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.109375" style="29" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" style="29" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" style="29" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="29"/>
+    <col min="1" max="1" width="32.125" style="29" customWidth="1"/>
+    <col min="2" max="2" width="25.375" style="29" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="29" customWidth="1"/>
+    <col min="4" max="16384" width="8.875" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" s="43" t="s">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="31"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="B1" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="C1" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="47">
+      <c r="D1" s="30"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="44">
         <v>28</v>
       </c>
-      <c r="D2" s="31"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" s="48">
+      <c r="D2" s="30"/>
+    </row>
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="45">
         <v>8</v>
       </c>
-      <c r="C3" s="47">
+      <c r="C3" s="44">
         <v>12.96</v>
       </c>
-      <c r="D3" s="31"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="48">
+      <c r="D3" s="30"/>
+    </row>
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="45">
         <v>96</v>
       </c>
-      <c r="C4" s="47" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" s="31"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="48" t="s">
+      <c r="C4" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="D4" s="30"/>
+    </row>
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="31"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="B5" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="48">
+      <c r="C5" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="30"/>
+    </row>
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="45">
+        <v>0.9</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="30"/>
+    </row>
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="45">
         <v>200</v>
       </c>
-      <c r="C6" s="47">
+      <c r="C7" s="44">
         <v>250</v>
       </c>
-      <c r="D6" s="31"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="48" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="47" t="s">
+      <c r="D7" s="30"/>
+    </row>
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="31"/>
-    </row>
-    <row r="8" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="34" t="s">
+      <c r="B8" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="C8" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="30"/>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="31"/>
-    </row>
-    <row r="9" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="51" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="52"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="31"/>
-    </row>
-    <row r="10" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="42" t="s">
+      <c r="B9" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="44">
+      <c r="D9" s="30"/>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="52"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="30"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="41">
         <v>1024</v>
       </c>
-      <c r="C10" s="43">
-        <v>1024</v>
-      </c>
-      <c r="D10" s="31"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="42" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="41">
-        <f>B10*B6*2/1024/1024</f>
+      <c r="C11" s="50">
+        <v>12288</v>
+      </c>
+      <c r="D11" s="30"/>
+    </row>
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="38">
+        <f>B11*B7*2/1024/1024</f>
         <v>0.390625</v>
       </c>
-      <c r="C11" s="40">
-        <f>C10*C6*2/1024/1024</f>
-        <v>0.48828125</v>
-      </c>
-      <c r="D11" s="31"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="36">
-        <f>B11*24</f>
+      <c r="C12" s="37">
+        <f>C11*C7*2/1024/1024</f>
+        <v>5.859375</v>
+      </c>
+      <c r="D12" s="30"/>
+    </row>
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="34">
+        <f>B12*24</f>
         <v>9.375</v>
       </c>
-      <c r="C12" s="35">
-        <f>C11*24</f>
-        <v>11.71875</v>
-      </c>
-      <c r="D12" s="31"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="39">
+      <c r="C13" s="49">
+        <v>11.6</v>
+      </c>
+      <c r="D13" s="30"/>
+    </row>
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="36">
         <v>0.1</v>
       </c>
-      <c r="C13" s="38">
+      <c r="C14" s="33">
         <v>0.60899999999999999</v>
       </c>
-      <c r="D13" s="31"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="36">
-        <f>B11/B13</f>
+      <c r="D14" s="30"/>
+    </row>
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="34">
+        <f>B12/B14</f>
         <v>3.90625</v>
       </c>
-      <c r="C14" s="35">
-        <f>C11/C13</f>
-        <v>0.80177545155993435</v>
-      </c>
-      <c r="D14" s="31"/>
-    </row>
-    <row r="15" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="34" t="s">
+      <c r="C15" s="49">
+        <f>C12/C14</f>
+        <v>9.6213054187192117</v>
+      </c>
+      <c r="D15" s="30"/>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="33">
-        <f>B12/B13</f>
+      <c r="B16" s="48">
+        <f>B13/B14</f>
         <v>93.75</v>
       </c>
-      <c r="C15" s="32">
-        <f>C12/C13</f>
-        <v>19.242610837438423</v>
-      </c>
-      <c r="D15" s="31"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
+      <c r="C16" s="31">
+        <f>C13/C14</f>
+        <v>19.047619047619047</v>
+      </c>
+      <c r="D16" s="30"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32">
+        <f>C16/4*(1.1/0.9)^2</f>
+        <v>7.1134626690182259</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1454,27 +1599,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="N6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="19.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.21875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" style="26" customWidth="1"/>
+    <col min="1" max="1" width="17.875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.25" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.25" style="7" customWidth="1"/>
+    <col min="5" max="5" width="13.875" style="26" customWidth="1"/>
     <col min="6" max="6" width="16" style="10" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" style="11" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" style="10" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="11" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="10.875" style="10" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="22" style="11" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="0" style="8" hidden="1" customWidth="1"/>
     <col min="11" max="13" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="14" max="16384" width="19.77734375" style="2"/>
+    <col min="14" max="16384" width="19.75" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -1503,7 +1648,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
@@ -1576,7 +1721,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1614,24 +1759,24 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="49"/>
+      <c r="A7" s="46"/>
       <c r="B7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="E7" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="N7" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="O7" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -1806,7 +1951,7 @@
       <c r="N17" s="2">
         <v>477691</v>
       </c>
-      <c r="O17" s="50">
+      <c r="O17" s="47">
         <f>N17/N8*100</f>
         <v>39.680638357787046</v>
       </c>
@@ -1919,7 +2064,7 @@
         <v>0.76429032367625582</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="57"/>
       <c r="B24" s="1"/>
       <c r="E24" s="7" t="s">
@@ -2077,7 +2222,7 @@
       <c r="N31" s="2">
         <v>507456</v>
       </c>
-      <c r="O31" s="50">
+      <c r="O31" s="47">
         <f>N31/N8*100</f>
         <v>42.153145063417945</v>
       </c>
@@ -2116,7 +2261,7 @@
         <v>114849</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="D34" s="7" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
feat(HW data analysis): Area comparison between reg and uhddpsram
</commit_message>
<xml_diff>
--- a/hardware/docs/01-top/点云硬件参数分析.xlsx
+++ b/hardware/docs/01-top/点云硬件参数分析.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="12960" windowHeight="5775"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="12960" windowHeight="4872" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="整体评估" sheetId="5" r:id="rId1"/>
     <sheet name="历次综合结果" sheetId="3" r:id="rId2"/>
+    <sheet name="T28工艺库单元特性-面积" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -196,8 +197,96 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>作者</author>
+  </authors>
+  <commentList>
+    <comment ref="D4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+reg与sram的临界点</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+宽度对面积影响较小</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+越深密度越高</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="91">
   <si>
     <t>case</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -519,6 +608,38 @@
   </si>
   <si>
     <t>Scale to 55-nm 0.9V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>面积 (um2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uhddpsram</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单位面积</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>深度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宽度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>容量</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -529,7 +650,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -608,6 +729,37 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -900,7 +1052,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1085,6 +1237,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1367,19 +1523,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="32.125" style="29" customWidth="1"/>
-    <col min="2" max="2" width="25.375" style="29" customWidth="1"/>
-    <col min="3" max="3" width="25.5" style="29" customWidth="1"/>
-    <col min="4" max="16384" width="8.875" style="29"/>
+    <col min="1" max="1" width="32.109375" style="29" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="29" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" style="29" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="39" t="s">
         <v>71</v>
       </c>
@@ -1391,7 +1547,7 @@
       </c>
       <c r="D1" s="30"/>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="35" t="s">
         <v>68</v>
       </c>
@@ -1403,7 +1559,7 @@
       </c>
       <c r="D2" s="30"/>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="35" t="s">
         <v>66</v>
       </c>
@@ -1415,7 +1571,7 @@
       </c>
       <c r="D3" s="30"/>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="35" t="s">
         <v>65</v>
       </c>
@@ -1427,7 +1583,7 @@
       </c>
       <c r="D4" s="30"/>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="35" t="s">
         <v>63</v>
       </c>
@@ -1439,7 +1595,7 @@
       </c>
       <c r="D5" s="30"/>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="35" t="s">
         <v>81</v>
       </c>
@@ -1451,7 +1607,7 @@
       </c>
       <c r="D6" s="30"/>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="35" t="s">
         <v>60</v>
       </c>
@@ -1463,7 +1619,7 @@
       </c>
       <c r="D7" s="30"/>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="35" t="s">
         <v>59</v>
       </c>
@@ -1475,7 +1631,7 @@
       </c>
       <c r="D8" s="30"/>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="14.4" thickBot="1">
       <c r="A9" s="32" t="s">
         <v>56</v>
       </c>
@@ -1487,7 +1643,7 @@
       </c>
       <c r="D9" s="30"/>
     </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="14.4" thickBot="1">
       <c r="A10" s="51" t="s">
         <v>54</v>
       </c>
@@ -1495,7 +1651,7 @@
       <c r="C10" s="53"/>
       <c r="D10" s="30"/>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="14.4" thickBot="1">
       <c r="A11" s="39" t="s">
         <v>53</v>
       </c>
@@ -1507,7 +1663,7 @@
       </c>
       <c r="D11" s="30"/>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" s="39" t="s">
         <v>78</v>
       </c>
@@ -1521,7 +1677,7 @@
       </c>
       <c r="D12" s="30"/>
     </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" s="35" t="s">
         <v>52</v>
       </c>
@@ -1534,7 +1690,7 @@
       </c>
       <c r="D13" s="30"/>
     </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" s="35" t="s">
         <v>51</v>
       </c>
@@ -1546,7 +1702,7 @@
       </c>
       <c r="D14" s="30"/>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" s="35" t="s">
         <v>79</v>
       </c>
@@ -1560,7 +1716,7 @@
       </c>
       <c r="D15" s="30"/>
     </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="14.4" thickBot="1">
       <c r="A16" s="32" t="s">
         <v>50</v>
       </c>
@@ -1574,7 +1730,7 @@
       </c>
       <c r="D16" s="30"/>
     </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="14.4" thickBot="1">
       <c r="A17" s="32" t="s">
         <v>82</v>
       </c>
@@ -1600,29 +1756,30 @@
   <dimension ref="A1:O59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="N6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O21" sqref="O21"/>
+      <selection pane="bottomRight" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="19.77734375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="17.875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.25" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.25" style="7" customWidth="1"/>
-    <col min="5" max="5" width="13.875" style="26" customWidth="1"/>
-    <col min="6" max="6" width="16" style="10" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5" style="11" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="10.875" style="10" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="22" style="11" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="0" style="8" hidden="1" customWidth="1"/>
-    <col min="11" max="13" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="14" max="16384" width="19.75" style="2"/>
+    <col min="1" max="1" width="17.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="26" customWidth="1"/>
+    <col min="6" max="6" width="16" style="10" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" style="10" customWidth="1"/>
+    <col min="9" max="9" width="22" style="11" customWidth="1"/>
+    <col min="10" max="10" width="19.77734375" style="8" customWidth="1"/>
+    <col min="11" max="12" width="19.77734375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="13.109375" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="19.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1648,7 +1805,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="13.95" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
@@ -1675,7 +1832,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1698,7 +1855,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1721,7 +1878,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="56.4" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1735,7 +1892,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1758,7 +1915,7 @@
         <v>1768</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" s="46"/>
       <c r="B7" s="1" t="s">
         <v>72</v>
@@ -1779,7 +1936,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" s="56" t="s">
         <v>14</v>
       </c>
@@ -1804,7 +1961,7 @@
         <v>1203839</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" s="57"/>
       <c r="B9" s="1" t="s">
         <v>12</v>
@@ -1830,7 +1987,7 @@
         <v>1.7485726911987398</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" s="57"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -1850,7 +2007,7 @@
         <v>19815</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" s="57"/>
       <c r="B11" s="1"/>
       <c r="C11" s="3"/>
@@ -1862,7 +2019,7 @@
         <v>19250</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" s="57"/>
       <c r="B12" s="1"/>
       <c r="C12" s="3"/>
@@ -1877,7 +2034,7 @@
         <v>6660</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" s="57"/>
       <c r="B13" s="1"/>
       <c r="C13" s="3"/>
@@ -1891,7 +2048,7 @@
         <v>1419</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" s="57"/>
       <c r="B14" s="1"/>
       <c r="C14" s="3"/>
@@ -1899,7 +2056,7 @@
       <c r="E14" s="27"/>
       <c r="H14" s="15"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15" s="57"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
@@ -1919,14 +2076,14 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="A16" s="57"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="6"/>
       <c r="E16" s="25"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15">
       <c r="A17" s="57"/>
       <c r="B17" s="1" t="s">
         <v>10</v>
@@ -1956,7 +2113,7 @@
         <v>39.680638357787046</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15">
       <c r="A18" s="57"/>
       <c r="B18" s="1"/>
       <c r="C18" s="2" t="s">
@@ -1979,7 +2136,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15">
       <c r="A19" s="57"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
@@ -1990,7 +2147,7 @@
         <v>0.193</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15">
       <c r="A20" s="57"/>
       <c r="B20" s="1"/>
       <c r="C20" s="2" t="s">
@@ -2001,7 +2158,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15">
       <c r="A21" s="57"/>
       <c r="B21" s="1" t="s">
         <v>13</v>
@@ -2028,7 +2185,7 @@
         <v>14.671812426744774</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15">
       <c r="A22" s="57"/>
       <c r="B22" s="1"/>
       <c r="C22" s="2" t="s">
@@ -2049,7 +2206,7 @@
         <v>0.33747879510338818</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15">
       <c r="A23" s="57"/>
       <c r="B23" s="1"/>
       <c r="D23" s="7" t="s">
@@ -2064,7 +2221,7 @@
         <v>0.76429032367625582</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="27.6">
       <c r="A24" s="57"/>
       <c r="B24" s="1"/>
       <c r="E24" s="7" t="s">
@@ -2079,7 +2236,7 @@
         <v>0.90067990934542064</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15">
       <c r="A25" s="57"/>
       <c r="B25" s="1"/>
       <c r="C25" s="2" t="s">
@@ -2096,7 +2253,7 @@
         <v>0.63920728072990696</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15">
       <c r="A26" s="57"/>
       <c r="B26" s="1"/>
       <c r="C26" s="2" t="s">
@@ -2110,7 +2267,7 @@
         <v>18589</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15">
       <c r="A27" s="57"/>
       <c r="B27" s="1" t="s">
         <v>9</v>
@@ -2137,7 +2294,7 @@
         <v>0.93966053600190724</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15">
       <c r="A28" s="57"/>
       <c r="B28" s="1"/>
       <c r="C28" s="2" t="s">
@@ -2157,7 +2314,7 @@
         <v>11719</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15">
       <c r="A29" s="57"/>
       <c r="B29" s="1"/>
       <c r="C29" s="2" t="s">
@@ -2170,7 +2327,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15">
       <c r="A30" s="57"/>
       <c r="B30" s="1" t="s">
         <v>8</v>
@@ -2197,7 +2354,7 @@
         <v>0.24596312297574677</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15">
       <c r="A31" s="58"/>
       <c r="B31" s="1" t="s">
         <v>11</v>
@@ -2227,7 +2384,7 @@
         <v>42.153145063417945</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15">
       <c r="A32" s="5"/>
       <c r="B32" s="1"/>
       <c r="C32" s="2" t="s">
@@ -2244,7 +2401,7 @@
         <v>44581</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14">
       <c r="A33" s="5"/>
       <c r="B33" s="1"/>
       <c r="C33" s="2" t="s">
@@ -2261,7 +2418,7 @@
         <v>114849</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="13.95" customHeight="1">
       <c r="A34" s="5"/>
       <c r="D34" s="7" t="s">
         <v>44</v>
@@ -2273,7 +2430,7 @@
         <v>7094</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14">
       <c r="A35" s="5"/>
       <c r="E35" s="26" t="s">
         <v>45</v>
@@ -2285,7 +2442,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14">
       <c r="A36" s="5"/>
       <c r="E36" s="25" t="s">
         <v>46</v>
@@ -2297,7 +2454,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14">
       <c r="A37" s="56" t="s">
         <v>24</v>
       </c>
@@ -2313,7 +2470,7 @@
         <v>74.7</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14">
       <c r="A38" s="57"/>
       <c r="B38" s="1" t="s">
         <v>12</v>
@@ -2329,14 +2486,14 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14">
       <c r="A39" s="57"/>
       <c r="B39" s="1"/>
       <c r="C39" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14">
       <c r="A40" s="57"/>
       <c r="B40" s="1"/>
       <c r="C40" s="3"/>
@@ -2344,7 +2501,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14">
       <c r="A41" s="57"/>
       <c r="B41" s="1"/>
       <c r="C41" s="3"/>
@@ -2352,7 +2509,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14">
       <c r="A42" s="57"/>
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
@@ -2360,28 +2517,28 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14">
       <c r="A43" s="57"/>
       <c r="B43" s="1"/>
       <c r="C43" s="3"/>
       <c r="D43" s="19"/>
       <c r="E43" s="27"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14">
       <c r="A44" s="57"/>
       <c r="B44" s="1"/>
       <c r="C44" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14">
       <c r="A45" s="57"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="6"/>
       <c r="E45" s="25"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14">
       <c r="A46" s="57"/>
       <c r="B46" s="1" t="s">
         <v>10</v>
@@ -2397,26 +2554,26 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14">
       <c r="A47" s="58"/>
       <c r="B47" s="1"/>
       <c r="C47" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14">
       <c r="B48" s="1"/>
       <c r="C48" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:15">
       <c r="B49" s="1"/>
       <c r="C49" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:15">
       <c r="B50" s="1" t="s">
         <v>13</v>
       </c>
@@ -2431,25 +2588,25 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:15">
       <c r="B51" s="1"/>
       <c r="C51" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:15">
       <c r="B52" s="1"/>
       <c r="C52" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:15">
       <c r="B53" s="1"/>
       <c r="C53" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:15">
       <c r="B54" s="1" t="s">
         <v>9</v>
       </c>
@@ -2460,19 +2617,19 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:15">
       <c r="B55" s="1"/>
       <c r="C55" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:15">
       <c r="B56" s="1"/>
       <c r="C56" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:15">
       <c r="B57" s="1" t="s">
         <v>8</v>
       </c>
@@ -2483,7 +2640,7 @@
         <v>6.7000000000000004E-2</v>
       </c>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:15">
       <c r="B58" s="1" t="s">
         <v>11</v>
       </c>
@@ -2502,7 +2659,7 @@
         <v>0.79250334672021416</v>
       </c>
     </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:15">
       <c r="O59" s="2" t="s">
         <v>49</v>
       </c>
@@ -2522,4 +2679,200 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="2" max="4" width="11.21875" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2">
+        <v>2048</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f>B2*C2</f>
+        <v>2048</v>
+      </c>
+      <c r="E2">
+        <v>6750</v>
+      </c>
+      <c r="F2">
+        <f>E2/(B2*C2)</f>
+        <v>3.2958984375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3">
+        <v>32</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D8" si="0">B3*C3</f>
+        <v>512</v>
+      </c>
+      <c r="E3">
+        <v>2762</v>
+      </c>
+      <c r="F3">
+        <f>E3/(B3*C3)</f>
+        <v>5.39453125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4">
+        <v>32</v>
+      </c>
+      <c r="C4">
+        <v>128</v>
+      </c>
+      <c r="D4" s="62">
+        <f t="shared" si="0"/>
+        <v>4096</v>
+      </c>
+      <c r="E4">
+        <v>15180</v>
+      </c>
+      <c r="F4">
+        <f>E4/(B4*C4)</f>
+        <v>3.7060546875</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5">
+        <v>64</v>
+      </c>
+      <c r="C5">
+        <v>128</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>8192</v>
+      </c>
+      <c r="E5">
+        <v>15867</v>
+      </c>
+      <c r="F5" s="65">
+        <f>E5/(B5*C5)</f>
+        <v>1.9368896484375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6">
+        <v>64</v>
+      </c>
+      <c r="C6">
+        <v>64</v>
+      </c>
+      <c r="D6">
+        <f>B6*C6</f>
+        <v>4096</v>
+      </c>
+      <c r="E6">
+        <v>8451</v>
+      </c>
+      <c r="F6">
+        <f>E6/(B6*C6)</f>
+        <v>2.063232421875</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7">
+        <v>128</v>
+      </c>
+      <c r="C7">
+        <v>64</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>8192</v>
+      </c>
+      <c r="E7">
+        <v>9182</v>
+      </c>
+      <c r="F7" s="64">
+        <f>E7/(B7*C7)</f>
+        <v>1.120849609375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8">
+        <v>4096</v>
+      </c>
+      <c r="C8">
+        <v>128</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>524288</v>
+      </c>
+      <c r="E8">
+        <v>118814</v>
+      </c>
+      <c r="F8" s="63">
+        <f>E8/(B8*C8)</f>
+        <v>0.22661972045898438</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat(HW Parameter.excel): Add PAD number of interlace and double ring
</commit_message>
<xml_diff>
--- a/hardware/docs/01-top/点云硬件参数分析.xlsx
+++ b/hardware/docs/01-top/点云硬件参数分析.xlsx
@@ -286,7 +286,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="103">
   <si>
     <t>case</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -640,6 +640,54 @@
   </si>
   <si>
     <t>容量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>长</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chip Size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Core Size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plan A: 单圈PAD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plan B: 双圈PAD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plan B: 交错圈PAD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plan C: 双圈交错PAD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Core利用率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAD个数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAD/Core</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -769,7 +817,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -1048,11 +1096,83 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1203,44 +1323,74 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1644,11 +1794,11 @@
       <c r="D9" s="30"/>
     </row>
     <row r="10" spans="1:4" ht="14.4" thickBot="1">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="53"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="57"/>
       <c r="D10" s="30"/>
     </row>
     <row r="11" spans="1:4" ht="14.4" thickBot="1">
@@ -1787,14 +1937,14 @@
       <c r="C1" s="1"/>
       <c r="D1" s="6"/>
       <c r="E1" s="24"/>
-      <c r="F1" s="59">
+      <c r="F1" s="63">
         <v>0</v>
       </c>
-      <c r="G1" s="60"/>
-      <c r="H1" s="59">
+      <c r="G1" s="64"/>
+      <c r="H1" s="63">
         <v>1</v>
       </c>
-      <c r="I1" s="60"/>
+      <c r="I1" s="64"/>
       <c r="J1" s="8">
         <v>2</v>
       </c>
@@ -1813,18 +1963,18 @@
       <c r="C2" s="1"/>
       <c r="D2" s="6"/>
       <c r="E2" s="25"/>
-      <c r="F2" s="54" t="s">
+      <c r="F2" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="61"/>
-      <c r="H2" s="54" t="s">
+      <c r="G2" s="65"/>
+      <c r="H2" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="61"/>
-      <c r="J2" s="54" t="s">
+      <c r="I2" s="65"/>
+      <c r="J2" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="55"/>
+      <c r="K2" s="59"/>
       <c r="L2" s="2" t="s">
         <v>41</v>
       </c>
@@ -1937,7 +2087,7 @@
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="60" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1962,7 +2112,7 @@
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="57"/>
+      <c r="A9" s="61"/>
       <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1988,7 +2138,7 @@
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="57"/>
+      <c r="A10" s="61"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
         <v>15</v>
@@ -2008,7 +2158,7 @@
       </c>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="57"/>
+      <c r="A11" s="61"/>
       <c r="B11" s="1"/>
       <c r="C11" s="3"/>
       <c r="D11" s="11" t="s">
@@ -2020,7 +2170,7 @@
       </c>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="57"/>
+      <c r="A12" s="61"/>
       <c r="B12" s="1"/>
       <c r="C12" s="3"/>
       <c r="E12" s="19" t="s">
@@ -2035,7 +2185,7 @@
       </c>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="57"/>
+      <c r="A13" s="61"/>
       <c r="B13" s="1"/>
       <c r="C13" s="3"/>
       <c r="E13" s="19" t="s">
@@ -2049,7 +2199,7 @@
       </c>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="57"/>
+      <c r="A14" s="61"/>
       <c r="B14" s="1"/>
       <c r="C14" s="3"/>
       <c r="D14" s="19"/>
@@ -2057,7 +2207,7 @@
       <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="57"/>
+      <c r="A15" s="61"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
         <v>16</v>
@@ -2077,14 +2227,14 @@
       </c>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="57"/>
+      <c r="A16" s="61"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="6"/>
       <c r="E16" s="25"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="57"/>
+      <c r="A17" s="61"/>
       <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
@@ -2114,7 +2264,7 @@
       </c>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="57"/>
+      <c r="A18" s="61"/>
       <c r="B18" s="1"/>
       <c r="C18" s="2" t="s">
         <v>17</v>
@@ -2137,7 +2287,7 @@
       </c>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="57"/>
+      <c r="A19" s="61"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
         <v>39</v>
@@ -2148,7 +2298,7 @@
       </c>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="57"/>
+      <c r="A20" s="61"/>
       <c r="B20" s="1"/>
       <c r="C20" s="2" t="s">
         <v>40</v>
@@ -2159,7 +2309,7 @@
       </c>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="57"/>
+      <c r="A21" s="61"/>
       <c r="B21" s="1" t="s">
         <v>13</v>
       </c>
@@ -2186,7 +2336,7 @@
       </c>
     </row>
     <row r="22" spans="1:15">
-      <c r="A22" s="57"/>
+      <c r="A22" s="61"/>
       <c r="B22" s="1"/>
       <c r="C22" s="2" t="s">
         <v>18</v>
@@ -2207,7 +2357,7 @@
       </c>
     </row>
     <row r="23" spans="1:15">
-      <c r="A23" s="57"/>
+      <c r="A23" s="61"/>
       <c r="B23" s="1"/>
       <c r="D23" s="7" t="s">
         <v>43</v>
@@ -2222,7 +2372,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" ht="27.6">
-      <c r="A24" s="57"/>
+      <c r="A24" s="61"/>
       <c r="B24" s="1"/>
       <c r="E24" s="7" t="s">
         <v>42</v>
@@ -2237,7 +2387,7 @@
       </c>
     </row>
     <row r="25" spans="1:15">
-      <c r="A25" s="57"/>
+      <c r="A25" s="61"/>
       <c r="B25" s="1"/>
       <c r="C25" s="2" t="s">
         <v>19</v>
@@ -2254,7 +2404,7 @@
       </c>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="57"/>
+      <c r="A26" s="61"/>
       <c r="B26" s="1"/>
       <c r="C26" s="2" t="s">
         <v>20</v>
@@ -2268,7 +2418,7 @@
       </c>
     </row>
     <row r="27" spans="1:15">
-      <c r="A27" s="57"/>
+      <c r="A27" s="61"/>
       <c r="B27" s="1" t="s">
         <v>9</v>
       </c>
@@ -2295,7 +2445,7 @@
       </c>
     </row>
     <row r="28" spans="1:15">
-      <c r="A28" s="57"/>
+      <c r="A28" s="61"/>
       <c r="B28" s="1"/>
       <c r="C28" s="2" t="s">
         <v>21</v>
@@ -2315,7 +2465,7 @@
       </c>
     </row>
     <row r="29" spans="1:15">
-      <c r="A29" s="57"/>
+      <c r="A29" s="61"/>
       <c r="B29" s="1"/>
       <c r="C29" s="2" t="s">
         <v>22</v>
@@ -2328,7 +2478,7 @@
       </c>
     </row>
     <row r="30" spans="1:15">
-      <c r="A30" s="57"/>
+      <c r="A30" s="61"/>
       <c r="B30" s="1" t="s">
         <v>8</v>
       </c>
@@ -2355,7 +2505,7 @@
       </c>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="58"/>
+      <c r="A31" s="62"/>
       <c r="B31" s="1" t="s">
         <v>11</v>
       </c>
@@ -2455,7 +2605,7 @@
       </c>
     </row>
     <row r="37" spans="1:14">
-      <c r="A37" s="56" t="s">
+      <c r="A37" s="60" t="s">
         <v>24</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -2471,7 +2621,7 @@
       </c>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="57"/>
+      <c r="A38" s="61"/>
       <c r="B38" s="1" t="s">
         <v>12</v>
       </c>
@@ -2487,14 +2637,14 @@
       </c>
     </row>
     <row r="39" spans="1:14">
-      <c r="A39" s="57"/>
+      <c r="A39" s="61"/>
       <c r="B39" s="1"/>
       <c r="C39" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:14">
-      <c r="A40" s="57"/>
+      <c r="A40" s="61"/>
       <c r="B40" s="1"/>
       <c r="C40" s="3"/>
       <c r="D40" s="11" t="s">
@@ -2502,7 +2652,7 @@
       </c>
     </row>
     <row r="41" spans="1:14">
-      <c r="A41" s="57"/>
+      <c r="A41" s="61"/>
       <c r="B41" s="1"/>
       <c r="C41" s="3"/>
       <c r="E41" s="19" t="s">
@@ -2510,7 +2660,7 @@
       </c>
     </row>
     <row r="42" spans="1:14">
-      <c r="A42" s="57"/>
+      <c r="A42" s="61"/>
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
       <c r="E42" s="19" t="s">
@@ -2518,28 +2668,28 @@
       </c>
     </row>
     <row r="43" spans="1:14">
-      <c r="A43" s="57"/>
+      <c r="A43" s="61"/>
       <c r="B43" s="1"/>
       <c r="C43" s="3"/>
       <c r="D43" s="19"/>
       <c r="E43" s="27"/>
     </row>
     <row r="44" spans="1:14">
-      <c r="A44" s="57"/>
+      <c r="A44" s="61"/>
       <c r="B44" s="1"/>
       <c r="C44" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:14">
-      <c r="A45" s="57"/>
+      <c r="A45" s="61"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="6"/>
       <c r="E45" s="25"/>
     </row>
     <row r="46" spans="1:14">
-      <c r="A46" s="57"/>
+      <c r="A46" s="61"/>
       <c r="B46" s="1" t="s">
         <v>10</v>
       </c>
@@ -2555,7 +2705,7 @@
       </c>
     </row>
     <row r="47" spans="1:14">
-      <c r="A47" s="58"/>
+      <c r="A47" s="62"/>
       <c r="B47" s="1"/>
       <c r="C47" s="2" t="s">
         <v>17</v>
@@ -2683,19 +2833,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="2" max="4" width="11.21875" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -2715,7 +2866,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>84</v>
       </c>
@@ -2737,7 +2888,7 @@
         <v>3.2958984375</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -2759,7 +2910,7 @@
         <v>5.39453125</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -2769,7 +2920,7 @@
       <c r="C4">
         <v>128</v>
       </c>
-      <c r="D4" s="62">
+      <c r="D4" s="51">
         <f t="shared" si="0"/>
         <v>4096</v>
       </c>
@@ -2781,7 +2932,7 @@
         <v>3.7060546875</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:20">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -2798,12 +2949,12 @@
       <c r="E5">
         <v>15867</v>
       </c>
-      <c r="F5" s="65">
+      <c r="F5" s="54">
         <f>E5/(B5*C5)</f>
         <v>1.9368896484375</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:20">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -2825,7 +2976,7 @@
         <v>2.063232421875</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:20">
       <c r="A7" t="s">
         <v>86</v>
       </c>
@@ -2842,12 +2993,12 @@
       <c r="E7">
         <v>9182</v>
       </c>
-      <c r="F7" s="64">
+      <c r="F7" s="53">
         <f>E7/(B7*C7)</f>
         <v>1.120849609375</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:20">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -2864,12 +3015,248 @@
       <c r="E8">
         <v>118814</v>
       </c>
-      <c r="F8" s="63">
+      <c r="F8" s="52">
         <f>E8/(B8*C8)</f>
         <v>0.22661972045898438</v>
       </c>
     </row>
+    <row r="9" spans="1:20" ht="14.4" thickBot="1"/>
+    <row r="10" spans="1:20" ht="14.4" thickBot="1">
+      <c r="H10" s="67"/>
+      <c r="I10" s="77" t="s">
+        <v>96</v>
+      </c>
+      <c r="J10" s="78"/>
+      <c r="K10" s="79"/>
+      <c r="L10" s="80" t="s">
+        <v>98</v>
+      </c>
+      <c r="M10" s="81"/>
+      <c r="N10" s="82"/>
+      <c r="O10" s="80" t="s">
+        <v>97</v>
+      </c>
+      <c r="P10" s="81"/>
+      <c r="Q10" s="82"/>
+      <c r="R10" s="69" t="s">
+        <v>99</v>
+      </c>
+      <c r="S10" s="70"/>
+      <c r="T10" s="71"/>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="H11" s="67"/>
+      <c r="I11" s="69" t="s">
+        <v>91</v>
+      </c>
+      <c r="J11" s="70" t="s">
+        <v>92</v>
+      </c>
+      <c r="K11" s="71" t="s">
+        <v>101</v>
+      </c>
+      <c r="L11" s="72" t="s">
+        <v>91</v>
+      </c>
+      <c r="M11" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="N11" s="73" t="s">
+        <v>101</v>
+      </c>
+      <c r="O11" s="72" t="s">
+        <v>91</v>
+      </c>
+      <c r="P11" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q11" s="73" t="s">
+        <v>101</v>
+      </c>
+      <c r="R11" s="72" t="s">
+        <v>91</v>
+      </c>
+      <c r="S11" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="T11" s="73" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="H12" s="67" t="s">
+        <v>93</v>
+      </c>
+      <c r="I12" s="72">
+        <v>1.5</v>
+      </c>
+      <c r="J12" s="66">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K12" s="73"/>
+      <c r="L12" s="72">
+        <v>1.5</v>
+      </c>
+      <c r="M12" s="66">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N12" s="73"/>
+      <c r="O12" s="72">
+        <v>1.5</v>
+      </c>
+      <c r="P12" s="66">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Q12" s="73"/>
+      <c r="R12" s="72">
+        <v>1.5</v>
+      </c>
+      <c r="S12" s="66">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="T12" s="73"/>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="H13" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="I13" s="72">
+        <v>0.25</v>
+      </c>
+      <c r="J13" s="66"/>
+      <c r="K13" s="73">
+        <v>83</v>
+      </c>
+      <c r="L13" s="72">
+        <v>0.35</v>
+      </c>
+      <c r="M13" s="66"/>
+      <c r="N13" s="73">
+        <f>K13*1.5</f>
+        <v>124.5</v>
+      </c>
+      <c r="O13" s="72">
+        <v>0.5</v>
+      </c>
+      <c r="P13" s="66"/>
+      <c r="Q13" s="73">
+        <f>K13*1.8</f>
+        <v>149.4</v>
+      </c>
+      <c r="R13" s="72">
+        <v>0.7</v>
+      </c>
+      <c r="S13" s="66"/>
+      <c r="T13" s="73">
+        <f>K13*1.5*1.8</f>
+        <v>224.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="H14" s="67" t="s">
+        <v>94</v>
+      </c>
+      <c r="I14" s="72">
+        <f>I12-I13*2</f>
+        <v>1</v>
+      </c>
+      <c r="J14" s="66">
+        <f>J12-I13*2</f>
+        <v>1.7000000000000002</v>
+      </c>
+      <c r="K14" s="73"/>
+      <c r="L14" s="72">
+        <f>L12-L13*2</f>
+        <v>0.8</v>
+      </c>
+      <c r="M14" s="66">
+        <f>M12-L13*2</f>
+        <v>1.5000000000000002</v>
+      </c>
+      <c r="N14" s="73"/>
+      <c r="O14" s="72">
+        <f>O12-O13*2</f>
+        <v>0.5</v>
+      </c>
+      <c r="P14" s="66">
+        <f>P12-O13*2</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="Q14" s="73"/>
+      <c r="R14" s="72">
+        <f>R12-R13*2</f>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="S14" s="66">
+        <f>S12-R13*2</f>
+        <v>0.80000000000000027</v>
+      </c>
+      <c r="T14" s="73"/>
+    </row>
+    <row r="15" spans="1:20" ht="14.4" thickBot="1">
+      <c r="H15" s="67" t="s">
+        <v>100</v>
+      </c>
+      <c r="I15" s="74">
+        <f>I14*J14/I12/J12</f>
+        <v>0.51515151515151525</v>
+      </c>
+      <c r="J15" s="75"/>
+      <c r="K15" s="76"/>
+      <c r="L15" s="83">
+        <f>L14*M14/L12/M12</f>
+        <v>0.3636363636363637</v>
+      </c>
+      <c r="M15" s="75"/>
+      <c r="N15" s="76"/>
+      <c r="O15" s="74">
+        <f>O14*P14/O12/P12</f>
+        <v>0.18181818181818185</v>
+      </c>
+      <c r="P15" s="75"/>
+      <c r="Q15" s="76"/>
+      <c r="R15" s="74">
+        <f>R14*S14/R12/S12</f>
+        <v>2.424242424242427E-2</v>
+      </c>
+      <c r="S15" s="75"/>
+      <c r="T15" s="76"/>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="H16" s="66" t="s">
+        <v>102</v>
+      </c>
+      <c r="I16" s="68">
+        <f>K13/I14/J14</f>
+        <v>48.823529411764703</v>
+      </c>
+      <c r="J16" s="68"/>
+      <c r="K16" s="68"/>
+      <c r="L16" s="68">
+        <f>N13/L14/M14</f>
+        <v>103.74999999999999</v>
+      </c>
+      <c r="M16" s="68"/>
+      <c r="N16" s="68"/>
+      <c r="O16" s="68">
+        <f>Q13/O14/P14</f>
+        <v>248.99999999999997</v>
+      </c>
+      <c r="P16" s="68"/>
+      <c r="Q16" s="68"/>
+      <c r="R16" s="68">
+        <f>T13/R14/S14</f>
+        <v>2801.2499999999964</v>
+      </c>
+      <c r="S16" s="68"/>
+      <c r="T16" s="68"/>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="O10:Q10"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
style(HW Para & NN Arch)
</commit_message>
<xml_diff>
--- a/hardware/docs/01-top/点云硬件参数分析.xlsx
+++ b/hardware/docs/01-top/点云硬件参数分析.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="12960" windowHeight="4872" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="12960" windowHeight="4872"/>
   </bookViews>
   <sheets>
     <sheet name="整体评估" sheetId="5" r:id="rId1"/>
@@ -1804,8 +1804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
@@ -2036,7 +2036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="5" ySplit="3" topLeftCell="P7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>

</xml_diff>

<commit_message>
feat(HW Parameter and Network excel): Update
</commit_message>
<xml_diff>
--- a/hardware/docs/01-top/点云硬件参数分析.xlsx
+++ b/hardware/docs/01-top/点云硬件参数分析.xlsx
@@ -26,7 +26,7 @@
     <author>作者</author>
   </authors>
   <commentList>
-    <comment ref="C11" authorId="0" shapeId="0">
+    <comment ref="C12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0" shapeId="0">
+    <comment ref="C13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C13" authorId="0" shapeId="0">
+    <comment ref="C16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -104,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B16" authorId="0" shapeId="0">
+    <comment ref="B19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -126,7 +126,33 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-胜在功耗低
+师姐100MHz综合前后90-50mW，我100MHz综合功耗63mW，后仿保守估计不变，200MHz120mW</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B21" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+胜在卷积后聚合和剪枝
 </t>
         </r>
       </text>
@@ -364,7 +390,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="117">
   <si>
     <t>case</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -561,14 +587,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Power Consumption (W)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Effective Performance (TOPS) (K=24)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MAC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -721,10 +739,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>长</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>宽</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -782,6 +796,213 @@
   </si>
   <si>
     <t>Date230214_Period1000_group_Track3vt_Notev2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAD/EDGE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAD单个长</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAD SIZE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plan B: 交错单圈PAD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAD总长度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power Consumption (W)@ 200MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>总时间计算的有效算力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>总计算量为</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>PointNeXt-S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>论文的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>TOPS</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>PointNeXt-S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>总周期为</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>FPS 3k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>倍</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>9k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技术加持的有效算力-剪枝理论加持4x4倍，实际只4倍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术加持的有效算力</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-K=30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，但可能深层没有</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，因此倍数是</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>等效与真实加速比</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -792,7 +1013,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -902,6 +1123,44 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -911,7 +1170,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -1284,11 +1543,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1465,6 +1757,40 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1503,6 +1829,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1802,10 +2131,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
@@ -1818,22 +2147,22 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="39" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D1" s="30"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C2" s="44">
         <v>28</v>
@@ -1842,7 +2171,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3" s="45">
         <v>8</v>
@@ -1854,43 +2183,43 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="35" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B4" s="45">
         <v>96</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D4" s="30"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B5" s="45" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D5" s="30"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="35" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B6" s="45">
         <v>0.9</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D6" s="30"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="35" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B7" s="45">
         <v>200</v>
@@ -1902,123 +2231,182 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="35" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D8" s="30"/>
     </row>
     <row r="9" spans="1:4" ht="14.4" thickBot="1">
       <c r="A9" s="32" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B9" s="43" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D9" s="30"/>
     </row>
-    <row r="10" spans="1:4" ht="14.4" thickBot="1">
-      <c r="A10" s="70" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="71"/>
-      <c r="C10" s="72"/>
+    <row r="10" spans="1:4">
+      <c r="A10" s="90" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="91"/>
+      <c r="C10" s="92"/>
       <c r="D10" s="30"/>
     </row>
-    <row r="11" spans="1:4" ht="14.4" thickBot="1">
-      <c r="A11" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="41">
+    <row r="11" spans="1:4" ht="15" thickBot="1">
+      <c r="A11" s="85" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="83">
+        <f>3.6/1024</f>
+        <v>3.5156250000000001E-3</v>
+      </c>
+      <c r="C11" s="84"/>
+      <c r="D11" s="30"/>
+    </row>
+    <row r="12" spans="1:4" ht="14.4" thickBot="1">
+      <c r="A12" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="41">
         <v>1024</v>
       </c>
-      <c r="C11" s="50">
+      <c r="C12" s="50">
         <v>12288</v>
       </c>
-      <c r="D11" s="30"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="38">
-        <f>B11*B7*2/1024/1024</f>
+      <c r="D12" s="30"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="38">
+        <f>B12*B7*2/1024/1024</f>
         <v>0.390625</v>
       </c>
-      <c r="C12" s="37">
-        <f>C11*C7*2/1024/1024</f>
+      <c r="C13" s="37">
+        <f>C12*C7*2/1024/1024</f>
         <v>5.859375</v>
       </c>
-      <c r="D12" s="30"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="34">
-        <f>B12*24</f>
-        <v>9.375</v>
-      </c>
-      <c r="C13" s="49">
+      <c r="D13" s="30"/>
+    </row>
+    <row r="14" spans="1:4" ht="14.4">
+      <c r="A14" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14" s="86">
+        <f>9*1024</f>
+        <v>9216</v>
+      </c>
+      <c r="C14" s="87"/>
+      <c r="D14" s="30"/>
+    </row>
+    <row r="15" spans="1:4" ht="14.4">
+      <c r="A15" s="88" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="89">
+        <f>B11/(B14*5*10^(-9))</f>
+        <v>76.293945312499986</v>
+      </c>
+      <c r="C15" s="87"/>
+      <c r="D15" s="30"/>
+    </row>
+    <row r="16" spans="1:4" ht="14.4">
+      <c r="A16" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" s="34">
+        <f>B13*10</f>
+        <v>3.90625</v>
+      </c>
+      <c r="C16" s="49">
         <v>11.6</v>
       </c>
-      <c r="D13" s="30"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="36">
-        <v>0.1</v>
-      </c>
-      <c r="C14" s="33">
+      <c r="D16" s="30"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17" s="34">
+        <f>B16*4</f>
+        <v>15.625</v>
+      </c>
+      <c r="C17" s="49"/>
+      <c r="D17" s="30"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="30"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="30"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" s="36">
+        <v>0.15</v>
+      </c>
+      <c r="C19" s="33">
         <v>0.60899999999999999</v>
       </c>
-      <c r="D14" s="30"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="35" t="s">
-        <v>79</v>
-      </c>
-      <c r="B15" s="34">
-        <f>B12/B14</f>
-        <v>3.90625</v>
-      </c>
-      <c r="C15" s="49">
-        <f>C12/C14</f>
+      <c r="D19" s="30"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="34">
+        <f>B13/B19</f>
+        <v>2.604166666666667</v>
+      </c>
+      <c r="C20" s="49">
+        <f>C13/C19</f>
         <v>9.6213054187192117</v>
       </c>
-      <c r="D15" s="30"/>
-    </row>
-    <row r="16" spans="1:4" ht="14.4" thickBot="1">
-      <c r="A16" s="32" t="s">
+      <c r="D20" s="30"/>
+    </row>
+    <row r="21" spans="1:4" ht="14.4" thickBot="1">
+      <c r="A21" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="48">
-        <f>B13/B14</f>
-        <v>93.75</v>
-      </c>
-      <c r="C16" s="31">
-        <f>C13/C14</f>
+      <c r="B21" s="48">
+        <f>B17/B19</f>
+        <v>104.16666666666667</v>
+      </c>
+      <c r="C21" s="31">
+        <f>C16/C19</f>
         <v>19.047619047619047</v>
       </c>
-      <c r="D16" s="30"/>
-    </row>
-    <row r="17" spans="1:3" ht="14.4" thickBot="1">
-      <c r="A17" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32">
-        <f>C16/4*(1.1/0.9)^2</f>
+      <c r="D21" s="30"/>
+    </row>
+    <row r="22" spans="1:4" ht="14.4" thickBot="1">
+      <c r="A22" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32">
+        <f>C21/4*(1.1/0.9)^2</f>
         <v>7.1134626690182259</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="29">
+        <f>B17/B13</f>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2037,7 +2425,7 @@
   <dimension ref="A1:T60"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="P7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="P16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
@@ -2066,21 +2454,21 @@
       <c r="G1" s="69"/>
       <c r="H1" s="68"/>
       <c r="I1" s="69"/>
-      <c r="J1" s="73" t="s">
-        <v>103</v>
-      </c>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="75"/>
-      <c r="P1" s="76" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="74"/>
-      <c r="T1" s="75"/>
+      <c r="J1" s="93" t="s">
+        <v>100</v>
+      </c>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
+      <c r="O1" s="95"/>
+      <c r="P1" s="96" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q1" s="94"/>
+      <c r="R1" s="94"/>
+      <c r="S1" s="94"/>
+      <c r="T1" s="95"/>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="1" t="s">
@@ -2090,14 +2478,14 @@
       <c r="C2" s="1"/>
       <c r="D2" s="6"/>
       <c r="E2" s="24"/>
-      <c r="F2" s="80">
+      <c r="F2" s="100">
         <v>0</v>
       </c>
-      <c r="G2" s="81"/>
-      <c r="H2" s="80">
+      <c r="G2" s="101"/>
+      <c r="H2" s="100">
         <v>1</v>
       </c>
-      <c r="I2" s="81"/>
+      <c r="I2" s="101"/>
       <c r="J2" s="8">
         <v>2</v>
       </c>
@@ -2119,18 +2507,18 @@
       <c r="C3" s="1"/>
       <c r="D3" s="6"/>
       <c r="E3" s="25"/>
-      <c r="F3" s="73" t="s">
+      <c r="F3" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="82"/>
-      <c r="H3" s="73" t="s">
+      <c r="G3" s="102"/>
+      <c r="H3" s="93" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="82"/>
-      <c r="J3" s="73" t="s">
+      <c r="I3" s="102"/>
+      <c r="J3" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="75"/>
+      <c r="K3" s="95"/>
       <c r="L3" s="2" t="s">
         <v>41</v>
       </c>
@@ -2138,7 +2526,7 @@
         <v>48</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -2164,7 +2552,7 @@
         <v>47</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -2236,26 +2624,26 @@
     <row r="8" spans="1:20">
       <c r="A8" s="46"/>
       <c r="B8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="E8" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="N8" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="O8" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="N8" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="77" t="s">
+      <c r="A9" s="97" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2283,7 +2671,7 @@
       </c>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="78"/>
+      <c r="A10" s="98"/>
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
@@ -2309,7 +2697,7 @@
       </c>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11" s="78"/>
+      <c r="A11" s="98"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
         <v>15</v>
@@ -2332,7 +2720,7 @@
       </c>
     </row>
     <row r="12" spans="1:20">
-      <c r="A12" s="78"/>
+      <c r="A12" s="98"/>
       <c r="B12" s="1"/>
       <c r="C12" s="3"/>
       <c r="D12" s="11" t="s">
@@ -2344,7 +2732,7 @@
       </c>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="78"/>
+      <c r="A13" s="98"/>
       <c r="B13" s="1"/>
       <c r="C13" s="3"/>
       <c r="E13" s="19" t="s">
@@ -2359,7 +2747,7 @@
       </c>
     </row>
     <row r="14" spans="1:20">
-      <c r="A14" s="78"/>
+      <c r="A14" s="98"/>
       <c r="B14" s="1"/>
       <c r="C14" s="3"/>
       <c r="E14" s="19" t="s">
@@ -2373,7 +2761,7 @@
       </c>
     </row>
     <row r="15" spans="1:20">
-      <c r="A15" s="78"/>
+      <c r="A15" s="98"/>
       <c r="B15" s="1"/>
       <c r="C15" s="3"/>
       <c r="D15" s="19"/>
@@ -2381,7 +2769,7 @@
       <c r="H15" s="15"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="78"/>
+      <c r="A16" s="98"/>
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
         <v>16</v>
@@ -2404,14 +2792,14 @@
       </c>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="78"/>
+      <c r="A17" s="98"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="6"/>
       <c r="E17" s="25"/>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" s="78"/>
+      <c r="A18" s="98"/>
       <c r="B18" s="1" t="s">
         <v>10</v>
       </c>
@@ -2444,7 +2832,7 @@
       </c>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" s="78"/>
+      <c r="A19" s="98"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
         <v>17</v>
@@ -2470,7 +2858,7 @@
       </c>
     </row>
     <row r="20" spans="1:16">
-      <c r="A20" s="78"/>
+      <c r="A20" s="98"/>
       <c r="B20" s="1"/>
       <c r="C20" s="2" t="s">
         <v>39</v>
@@ -2481,7 +2869,7 @@
       </c>
     </row>
     <row r="21" spans="1:16">
-      <c r="A21" s="78"/>
+      <c r="A21" s="98"/>
       <c r="B21" s="1"/>
       <c r="C21" s="2" t="s">
         <v>40</v>
@@ -2492,7 +2880,7 @@
       </c>
     </row>
     <row r="22" spans="1:16">
-      <c r="A22" s="78"/>
+      <c r="A22" s="98"/>
       <c r="B22" s="1" t="s">
         <v>13</v>
       </c>
@@ -2522,7 +2910,7 @@
       </c>
     </row>
     <row r="23" spans="1:16">
-      <c r="A23" s="78"/>
+      <c r="A23" s="98"/>
       <c r="B23" s="1"/>
       <c r="C23" s="2" t="s">
         <v>18</v>
@@ -2543,7 +2931,7 @@
       </c>
     </row>
     <row r="24" spans="1:16">
-      <c r="A24" s="78"/>
+      <c r="A24" s="98"/>
       <c r="B24" s="1"/>
       <c r="D24" s="7" t="s">
         <v>43</v>
@@ -2558,7 +2946,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" ht="27.6">
-      <c r="A25" s="78"/>
+      <c r="A25" s="98"/>
       <c r="B25" s="1"/>
       <c r="E25" s="7" t="s">
         <v>42</v>
@@ -2573,7 +2961,7 @@
       </c>
     </row>
     <row r="26" spans="1:16">
-      <c r="A26" s="78"/>
+      <c r="A26" s="98"/>
       <c r="B26" s="1"/>
       <c r="C26" s="2" t="s">
         <v>19</v>
@@ -2590,7 +2978,7 @@
       </c>
     </row>
     <row r="27" spans="1:16">
-      <c r="A27" s="78"/>
+      <c r="A27" s="98"/>
       <c r="B27" s="1"/>
       <c r="C27" s="2" t="s">
         <v>20</v>
@@ -2604,7 +2992,7 @@
       </c>
     </row>
     <row r="28" spans="1:16">
-      <c r="A28" s="78"/>
+      <c r="A28" s="98"/>
       <c r="B28" s="1" t="s">
         <v>9</v>
       </c>
@@ -2634,7 +3022,7 @@
       </c>
     </row>
     <row r="29" spans="1:16">
-      <c r="A29" s="78"/>
+      <c r="A29" s="98"/>
       <c r="B29" s="1"/>
       <c r="C29" s="2" t="s">
         <v>21</v>
@@ -2654,7 +3042,7 @@
       </c>
     </row>
     <row r="30" spans="1:16">
-      <c r="A30" s="78"/>
+      <c r="A30" s="98"/>
       <c r="B30" s="1"/>
       <c r="C30" s="2" t="s">
         <v>22</v>
@@ -2667,7 +3055,7 @@
       </c>
     </row>
     <row r="31" spans="1:16">
-      <c r="A31" s="78"/>
+      <c r="A31" s="98"/>
       <c r="B31" s="1" t="s">
         <v>8</v>
       </c>
@@ -2694,7 +3082,7 @@
       </c>
     </row>
     <row r="32" spans="1:16">
-      <c r="A32" s="79"/>
+      <c r="A32" s="99"/>
       <c r="B32" s="1" t="s">
         <v>11</v>
       </c>
@@ -2797,7 +3185,7 @@
       </c>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="77" t="s">
+      <c r="A38" s="97" t="s">
         <v>24</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -2813,7 +3201,7 @@
       </c>
     </row>
     <row r="39" spans="1:14">
-      <c r="A39" s="78"/>
+      <c r="A39" s="98"/>
       <c r="B39" s="1" t="s">
         <v>12</v>
       </c>
@@ -2829,14 +3217,14 @@
       </c>
     </row>
     <row r="40" spans="1:14">
-      <c r="A40" s="78"/>
+      <c r="A40" s="98"/>
       <c r="B40" s="1"/>
       <c r="C40" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:14">
-      <c r="A41" s="78"/>
+      <c r="A41" s="98"/>
       <c r="B41" s="1"/>
       <c r="C41" s="3"/>
       <c r="D41" s="11" t="s">
@@ -2844,7 +3232,7 @@
       </c>
     </row>
     <row r="42" spans="1:14">
-      <c r="A42" s="78"/>
+      <c r="A42" s="98"/>
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
       <c r="E42" s="19" t="s">
@@ -2852,7 +3240,7 @@
       </c>
     </row>
     <row r="43" spans="1:14">
-      <c r="A43" s="78"/>
+      <c r="A43" s="98"/>
       <c r="B43" s="1"/>
       <c r="C43" s="3"/>
       <c r="E43" s="19" t="s">
@@ -2860,28 +3248,28 @@
       </c>
     </row>
     <row r="44" spans="1:14">
-      <c r="A44" s="78"/>
+      <c r="A44" s="98"/>
       <c r="B44" s="1"/>
       <c r="C44" s="3"/>
       <c r="D44" s="19"/>
       <c r="E44" s="27"/>
     </row>
     <row r="45" spans="1:14">
-      <c r="A45" s="78"/>
+      <c r="A45" s="98"/>
       <c r="B45" s="1"/>
       <c r="C45" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:14">
-      <c r="A46" s="78"/>
+      <c r="A46" s="98"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="6"/>
       <c r="E46" s="25"/>
     </row>
     <row r="47" spans="1:14">
-      <c r="A47" s="78"/>
+      <c r="A47" s="98"/>
       <c r="B47" s="1" t="s">
         <v>10</v>
       </c>
@@ -2897,7 +3285,7 @@
       </c>
     </row>
     <row r="48" spans="1:14">
-      <c r="A48" s="79"/>
+      <c r="A48" s="99"/>
       <c r="B48" s="1"/>
       <c r="C48" s="2" t="s">
         <v>17</v>
@@ -3027,10 +3415,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3038,31 +3426,32 @@
     <col min="2" max="4" width="11.21875" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" customWidth="1"/>
     <col min="8" max="8" width="12.21875" customWidth="1"/>
+    <col min="11" max="11" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" t="s">
         <v>83</v>
       </c>
-      <c r="B1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>85</v>
-      </c>
-      <c r="F1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B2">
         <v>2048</v>
@@ -3084,7 +3473,7 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B3">
         <v>32</v>
@@ -3106,7 +3495,7 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B4">
         <v>32</v>
@@ -3128,7 +3517,7 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B5">
         <v>64</v>
@@ -3150,7 +3539,7 @@
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B6">
         <v>64</v>
@@ -3172,7 +3561,7 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B7">
         <v>128</v>
@@ -3194,7 +3583,7 @@
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B8">
         <v>4096</v>
@@ -3217,23 +3606,23 @@
     <row r="9" spans="1:20" ht="14.4" thickBot="1"/>
     <row r="10" spans="1:20" ht="14.4" thickBot="1">
       <c r="H10" s="56"/>
-      <c r="I10" s="83" t="s">
+      <c r="I10" s="104" t="s">
+        <v>93</v>
+      </c>
+      <c r="J10" s="105"/>
+      <c r="K10" s="106"/>
+      <c r="L10" s="107" t="s">
+        <v>95</v>
+      </c>
+      <c r="M10" s="108"/>
+      <c r="N10" s="109"/>
+      <c r="O10" s="107" t="s">
+        <v>94</v>
+      </c>
+      <c r="P10" s="108"/>
+      <c r="Q10" s="109"/>
+      <c r="R10" s="58" t="s">
         <v>96</v>
-      </c>
-      <c r="J10" s="84"/>
-      <c r="K10" s="85"/>
-      <c r="L10" s="86" t="s">
-        <v>98</v>
-      </c>
-      <c r="M10" s="87"/>
-      <c r="N10" s="88"/>
-      <c r="O10" s="86" t="s">
-        <v>97</v>
-      </c>
-      <c r="P10" s="87"/>
-      <c r="Q10" s="88"/>
-      <c r="R10" s="58" t="s">
-        <v>99</v>
       </c>
       <c r="S10" s="59"/>
       <c r="T10" s="60"/>
@@ -3241,45 +3630,45 @@
     <row r="11" spans="1:20">
       <c r="H11" s="56"/>
       <c r="I11" s="58" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J11" s="59" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="K11" s="60" t="s">
-        <v>101</v>
-      </c>
-      <c r="L11" s="61" t="s">
-        <v>91</v>
-      </c>
-      <c r="M11" s="55" t="s">
-        <v>92</v>
+        <v>98</v>
+      </c>
+      <c r="L11" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="M11" s="59" t="s">
+        <v>107</v>
       </c>
       <c r="N11" s="62" t="s">
-        <v>101</v>
-      </c>
-      <c r="O11" s="61" t="s">
-        <v>91</v>
-      </c>
-      <c r="P11" s="55" t="s">
-        <v>92</v>
+        <v>98</v>
+      </c>
+      <c r="O11" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="P11" s="59" t="s">
+        <v>107</v>
       </c>
       <c r="Q11" s="62" t="s">
-        <v>101</v>
-      </c>
-      <c r="R11" s="61" t="s">
-        <v>91</v>
-      </c>
-      <c r="S11" s="55" t="s">
-        <v>92</v>
+        <v>98</v>
+      </c>
+      <c r="R11" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="S11" s="59" t="s">
+        <v>107</v>
       </c>
       <c r="T11" s="62" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="H12" s="56" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I12" s="61">
         <v>1.5</v>
@@ -3312,25 +3701,25 @@
     </row>
     <row r="13" spans="1:20">
       <c r="H13" s="56" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="I13" s="61">
-        <v>0.25</v>
+        <v>0.11</v>
       </c>
       <c r="J13" s="55"/>
       <c r="K13" s="62">
         <v>83</v>
       </c>
       <c r="L13" s="61">
-        <v>0.35</v>
+        <v>0.17</v>
       </c>
       <c r="M13" s="55"/>
       <c r="N13" s="62">
-        <f>K13*1.5</f>
-        <v>124.5</v>
+        <f>K13*1.8</f>
+        <v>149.4</v>
       </c>
       <c r="O13" s="61">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="P13" s="55"/>
       <c r="Q13" s="62">
@@ -3338,7 +3727,7 @@
         <v>149.4</v>
       </c>
       <c r="R13" s="61">
-        <v>0.7</v>
+        <v>0.35</v>
       </c>
       <c r="S13" s="55"/>
       <c r="T13" s="62">
@@ -3348,105 +3737,619 @@
     </row>
     <row r="14" spans="1:20">
       <c r="H14" s="56" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I14" s="61">
         <f>I12-I13*2</f>
-        <v>1</v>
+        <v>1.28</v>
       </c>
       <c r="J14" s="55">
         <f>J12-I13*2</f>
-        <v>1.7000000000000002</v>
+        <v>1.9800000000000002</v>
       </c>
       <c r="K14" s="62"/>
       <c r="L14" s="61">
         <f>L12-L13*2</f>
-        <v>0.8</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="M14" s="55">
         <f>M12-L13*2</f>
-        <v>1.5000000000000002</v>
+        <v>1.86</v>
       </c>
       <c r="N14" s="62"/>
       <c r="O14" s="61">
         <f>O12-O13*2</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P14" s="55">
         <f>P12-O13*2</f>
-        <v>1.2000000000000002</v>
+        <v>1.7000000000000002</v>
       </c>
       <c r="Q14" s="62"/>
       <c r="R14" s="61">
         <f>R12-R13*2</f>
-        <v>0.10000000000000009</v>
+        <v>0.8</v>
       </c>
       <c r="S14" s="55">
         <f>S12-R13*2</f>
-        <v>0.80000000000000027</v>
+        <v>1.5000000000000002</v>
       </c>
       <c r="T14" s="62"/>
     </row>
     <row r="15" spans="1:20" ht="14.4" thickBot="1">
       <c r="H15" s="56" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I15" s="63">
         <f>I14*J14/I12/J12</f>
-        <v>0.51515151515151525</v>
+        <v>0.76800000000000002</v>
       </c>
       <c r="J15" s="64"/>
       <c r="K15" s="65"/>
       <c r="L15" s="66">
         <f>L14*M14/L12/M12</f>
-        <v>0.3636363636363637</v>
+        <v>0.65381818181818174</v>
       </c>
       <c r="M15" s="64"/>
       <c r="N15" s="65"/>
       <c r="O15" s="63">
         <f>O14*P14/O12/P12</f>
-        <v>0.18181818181818185</v>
+        <v>0.51515151515151525</v>
       </c>
       <c r="P15" s="64"/>
       <c r="Q15" s="65"/>
       <c r="R15" s="63">
         <f>R14*S14/R12/S12</f>
-        <v>2.424242424242427E-2</v>
+        <v>0.3636363636363637</v>
       </c>
       <c r="S15" s="64"/>
       <c r="T15" s="65"/>
     </row>
     <row r="16" spans="1:20">
       <c r="H16" s="55" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I16" s="57">
         <f>K13/I14/J14</f>
-        <v>48.823529411764703</v>
+        <v>32.749368686868685</v>
       </c>
       <c r="J16" s="57"/>
       <c r="K16" s="57"/>
       <c r="L16" s="57">
         <f>N13/L14/M14</f>
-        <v>103.74999999999999</v>
+        <v>69.243604004449395</v>
       </c>
       <c r="M16" s="57"/>
       <c r="N16" s="57"/>
       <c r="O16" s="57">
         <f>Q13/O14/P14</f>
-        <v>248.99999999999997</v>
+        <v>87.882352941176464</v>
       </c>
       <c r="P16" s="57"/>
       <c r="Q16" s="57"/>
       <c r="R16" s="57">
         <f>T13/R14/S14</f>
-        <v>2801.2499999999964</v>
+        <v>186.74999999999997</v>
       </c>
       <c r="S16" s="57"/>
       <c r="T16" s="57"/>
     </row>
+    <row r="17" spans="8:20">
+      <c r="H17" s="70" t="s">
+        <v>104</v>
+      </c>
+      <c r="I17" s="53"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="53">
+        <f>K13/(I14+J14)/2</f>
+        <v>12.730061349693251</v>
+      </c>
+      <c r="L17" s="53"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="53">
+        <f>N13/(L14+M14)/2</f>
+        <v>24.735099337748345</v>
+      </c>
+    </row>
+    <row r="18" spans="8:20">
+      <c r="H18" s="73" t="s">
+        <v>90</v>
+      </c>
+      <c r="I18" s="72">
+        <f>I20+I19*2</f>
+        <v>1.52</v>
+      </c>
+      <c r="J18" s="72">
+        <f>J20+I19*2</f>
+        <v>1.52</v>
+      </c>
+      <c r="K18" s="72">
+        <f>I18*J18</f>
+        <v>2.3104</v>
+      </c>
+      <c r="L18" s="72">
+        <f>L20+L19*2</f>
+        <v>1.6400000000000001</v>
+      </c>
+      <c r="M18" s="72">
+        <f>M20+L19*2</f>
+        <v>1.6400000000000001</v>
+      </c>
+      <c r="N18" s="72">
+        <f>L18*M18</f>
+        <v>2.6896000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="8:20">
+      <c r="H19" s="73" t="s">
+        <v>92</v>
+      </c>
+      <c r="I19" s="72">
+        <v>0.11</v>
+      </c>
+      <c r="J19" s="72"/>
+      <c r="K19" s="72">
+        <f>K17*(I18+J18)*2</f>
+        <v>77.398773006134974</v>
+      </c>
+      <c r="L19" s="72">
+        <v>0.17</v>
+      </c>
+      <c r="M19" s="72"/>
+      <c r="N19" s="72">
+        <f>N17*(L18+M18)*2</f>
+        <v>162.26225165562914</v>
+      </c>
+    </row>
+    <row r="20" spans="8:20">
+      <c r="H20" s="73" t="s">
+        <v>91</v>
+      </c>
+      <c r="I20" s="72">
+        <v>1.3</v>
+      </c>
+      <c r="J20" s="72">
+        <v>1.3</v>
+      </c>
+      <c r="K20" s="72">
+        <f>I20*J20</f>
+        <v>1.6900000000000002</v>
+      </c>
+      <c r="L20" s="72">
+        <v>1.3</v>
+      </c>
+      <c r="M20" s="72">
+        <v>1.3</v>
+      </c>
+      <c r="N20" s="72"/>
+    </row>
+    <row r="21" spans="8:20">
+      <c r="H21" s="73" t="s">
+        <v>106</v>
+      </c>
+      <c r="I21" s="72"/>
+      <c r="J21" s="72"/>
+      <c r="K21" s="72">
+        <f>I19*(I20+J20)*2</f>
+        <v>0.57200000000000006</v>
+      </c>
+      <c r="L21" s="72"/>
+      <c r="M21" s="72"/>
+      <c r="N21" s="72">
+        <f>L19*(L20+M20)*2</f>
+        <v>0.88400000000000012</v>
+      </c>
+    </row>
+    <row r="22" spans="8:20" ht="14.4" thickBot="1">
+      <c r="H22" s="73" t="s">
+        <v>97</v>
+      </c>
+      <c r="I22" s="72"/>
+      <c r="J22" s="72"/>
+      <c r="K22" s="72"/>
+      <c r="L22" s="74">
+        <f>L20*M20/L18/M18</f>
+        <v>0.62834622248661509</v>
+      </c>
+      <c r="M22" s="72"/>
+      <c r="N22" s="72"/>
+    </row>
+    <row r="23" spans="8:20">
+      <c r="H23" s="75" t="s">
+        <v>99</v>
+      </c>
+      <c r="I23" s="72"/>
+      <c r="J23" s="72"/>
+      <c r="K23" s="72"/>
+      <c r="L23" s="76">
+        <f>N19/L20/M20</f>
+        <v>96.013166660135582</v>
+      </c>
+      <c r="M23" s="72"/>
+      <c r="N23" s="72"/>
+    </row>
+    <row r="24" spans="8:20" ht="14.4" thickBot="1">
+      <c r="H24" s="78"/>
+      <c r="I24" s="72"/>
+      <c r="J24" s="72"/>
+      <c r="K24" s="72"/>
+      <c r="L24" s="77"/>
+      <c r="M24" s="72"/>
+      <c r="N24" s="72"/>
+    </row>
+    <row r="25" spans="8:20">
+      <c r="H25" s="58"/>
+      <c r="I25" s="82" t="s">
+        <v>93</v>
+      </c>
+      <c r="J25" s="82"/>
+      <c r="K25" s="82"/>
+      <c r="L25" s="103" t="s">
+        <v>108</v>
+      </c>
+      <c r="M25" s="103"/>
+      <c r="N25" s="103"/>
+      <c r="O25" s="103" t="s">
+        <v>94</v>
+      </c>
+      <c r="P25" s="103"/>
+      <c r="Q25" s="103"/>
+      <c r="R25" s="59" t="s">
+        <v>96</v>
+      </c>
+      <c r="S25" s="59"/>
+      <c r="T25" s="60"/>
+    </row>
+    <row r="26" spans="8:20">
+      <c r="H26" s="61"/>
+      <c r="I26" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="J26" s="55" t="s">
+        <v>107</v>
+      </c>
+      <c r="K26" s="55" t="s">
+        <v>109</v>
+      </c>
+      <c r="L26" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="M26" s="55" t="s">
+        <v>107</v>
+      </c>
+      <c r="N26" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="O26" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="P26" s="55" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q26" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="R26" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="S26" s="55" t="s">
+        <v>107</v>
+      </c>
+      <c r="T26" s="62" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="8:20">
+      <c r="H27" s="81" t="s">
+        <v>91</v>
+      </c>
+      <c r="I27" s="71">
+        <v>1.7</v>
+      </c>
+      <c r="J27" s="71">
+        <v>1</v>
+      </c>
+      <c r="K27" s="71">
+        <v>0.11</v>
+      </c>
+      <c r="L27" s="71">
+        <v>1.7</v>
+      </c>
+      <c r="M27" s="71">
+        <v>1</v>
+      </c>
+      <c r="N27" s="71">
+        <v>1.7</v>
+      </c>
+      <c r="O27" s="55"/>
+      <c r="P27" s="55"/>
+      <c r="Q27" s="55"/>
+      <c r="R27" s="55"/>
+      <c r="S27" s="55"/>
+      <c r="T27" s="62"/>
+    </row>
+    <row r="28" spans="8:20">
+      <c r="H28" s="81" t="s">
+        <v>90</v>
+      </c>
+      <c r="I28" s="71">
+        <f>I27+K27*2</f>
+        <v>1.92</v>
+      </c>
+      <c r="J28" s="71">
+        <f>J27+K27*2</f>
+        <v>1.22</v>
+      </c>
+      <c r="K28" s="71">
+        <f>I28*J28</f>
+        <v>2.3424</v>
+      </c>
+      <c r="L28" s="71">
+        <f>L27+L29*2</f>
+        <v>2.04</v>
+      </c>
+      <c r="M28" s="71">
+        <f>M27+L29*2</f>
+        <v>1.34</v>
+      </c>
+      <c r="N28" s="71">
+        <f>L28*M28</f>
+        <v>2.7336</v>
+      </c>
+      <c r="O28" s="55"/>
+      <c r="P28" s="55"/>
+      <c r="Q28" s="55"/>
+      <c r="R28" s="55"/>
+      <c r="S28" s="55"/>
+      <c r="T28" s="62"/>
+    </row>
+    <row r="29" spans="8:20">
+      <c r="H29" s="81" t="s">
+        <v>98</v>
+      </c>
+      <c r="J29" s="71"/>
+      <c r="K29" s="71">
+        <f>K23*(I28+J28)*2</f>
+        <v>0</v>
+      </c>
+      <c r="L29" s="71">
+        <v>0.17</v>
+      </c>
+      <c r="M29" s="71"/>
+      <c r="N29" s="71">
+        <f>N23*(L28+M28)*2</f>
+        <v>0</v>
+      </c>
+      <c r="O29" s="55"/>
+      <c r="P29" s="55"/>
+      <c r="Q29" s="55"/>
+      <c r="R29" s="55"/>
+      <c r="S29" s="55"/>
+      <c r="T29" s="62"/>
+    </row>
+    <row r="30" spans="8:20">
+      <c r="H30" s="81" t="s">
+        <v>106</v>
+      </c>
+      <c r="I30" s="71"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="71" t="e">
+        <f>K28-#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L30" s="71"/>
+      <c r="M30" s="71"/>
+      <c r="N30" s="71">
+        <f>N28-N27</f>
+        <v>1.0336000000000001</v>
+      </c>
+      <c r="O30" s="55"/>
+      <c r="P30" s="55"/>
+      <c r="Q30" s="55"/>
+      <c r="R30" s="55"/>
+      <c r="S30" s="55"/>
+      <c r="T30" s="62"/>
+    </row>
+    <row r="31" spans="8:20">
+      <c r="H31" s="81" t="s">
+        <v>97</v>
+      </c>
+      <c r="I31" s="71"/>
+      <c r="J31" s="71"/>
+      <c r="K31" s="71"/>
+      <c r="L31" s="79">
+        <f>L27*M27/L28/M28</f>
+        <v>0.62189054726368154</v>
+      </c>
+      <c r="M31" s="71"/>
+      <c r="N31" s="71"/>
+      <c r="O31" s="55"/>
+      <c r="P31" s="55"/>
+      <c r="Q31" s="55"/>
+      <c r="R31" s="55"/>
+      <c r="S31" s="55"/>
+      <c r="T31" s="62"/>
+    </row>
+    <row r="32" spans="8:20">
+      <c r="H32" s="81" t="s">
+        <v>99</v>
+      </c>
+      <c r="I32" s="71"/>
+      <c r="J32" s="71"/>
+      <c r="K32" s="71"/>
+      <c r="L32" s="71">
+        <f>N29/L27/M27</f>
+        <v>0</v>
+      </c>
+      <c r="M32" s="71"/>
+      <c r="N32" s="71"/>
+      <c r="O32" s="55"/>
+      <c r="P32" s="55"/>
+      <c r="Q32" s="55"/>
+      <c r="R32" s="55"/>
+      <c r="S32" s="55"/>
+      <c r="T32" s="62"/>
+    </row>
+    <row r="33" spans="8:20">
+      <c r="H33" s="61" t="s">
+        <v>90</v>
+      </c>
+      <c r="I33" s="55">
+        <f>I35+I34*2</f>
+        <v>1.07</v>
+      </c>
+      <c r="J33" s="55">
+        <f>J35+I34*2</f>
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="K33" s="55">
+        <f>I33*J33</f>
+        <v>2.3754000000000004</v>
+      </c>
+      <c r="L33" s="55">
+        <f>L35+L34*2</f>
+        <v>1.19</v>
+      </c>
+      <c r="M33" s="55">
+        <f>M35+L34*2</f>
+        <v>2.34</v>
+      </c>
+      <c r="N33" s="55">
+        <f>L33*M33</f>
+        <v>2.7845999999999997</v>
+      </c>
+      <c r="O33" s="55"/>
+      <c r="P33" s="55"/>
+      <c r="Q33" s="55"/>
+      <c r="R33" s="55"/>
+      <c r="S33" s="55"/>
+      <c r="T33" s="62"/>
+    </row>
+    <row r="34" spans="8:20">
+      <c r="H34" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="I34" s="55">
+        <v>0.11</v>
+      </c>
+      <c r="J34" s="55"/>
+      <c r="K34" s="55">
+        <f>K17*(I35+J35)*2</f>
+        <v>72.561349693251529</v>
+      </c>
+      <c r="L34" s="55">
+        <v>0.17</v>
+      </c>
+      <c r="M34" s="55"/>
+      <c r="N34" s="55">
+        <f>N17*(L35+M35)*2</f>
+        <v>140.99006622516558</v>
+      </c>
+      <c r="O34" s="55"/>
+      <c r="P34" s="55"/>
+      <c r="Q34" s="55"/>
+      <c r="R34" s="55"/>
+      <c r="S34" s="55"/>
+      <c r="T34" s="62"/>
+    </row>
+    <row r="35" spans="8:20">
+      <c r="H35" s="61" t="s">
+        <v>91</v>
+      </c>
+      <c r="I35" s="55">
+        <f>K35/J35</f>
+        <v>0.85</v>
+      </c>
+      <c r="J35" s="55">
+        <v>2</v>
+      </c>
+      <c r="K35" s="55">
+        <v>1.7</v>
+      </c>
+      <c r="L35" s="55">
+        <f>N35/M35</f>
+        <v>0.85</v>
+      </c>
+      <c r="M35" s="55">
+        <v>2</v>
+      </c>
+      <c r="N35" s="55">
+        <v>1.7</v>
+      </c>
+      <c r="O35" s="55"/>
+      <c r="P35" s="55"/>
+      <c r="Q35" s="55"/>
+      <c r="R35" s="55"/>
+      <c r="S35" s="55"/>
+      <c r="T35" s="62"/>
+    </row>
+    <row r="36" spans="8:20">
+      <c r="H36" s="61" t="s">
+        <v>106</v>
+      </c>
+      <c r="I36" s="55"/>
+      <c r="J36" s="55"/>
+      <c r="K36" s="55">
+        <f>K33-K35</f>
+        <v>0.67540000000000044</v>
+      </c>
+      <c r="L36" s="55"/>
+      <c r="M36" s="55"/>
+      <c r="N36" s="55">
+        <f>N33-N35</f>
+        <v>1.0845999999999998</v>
+      </c>
+      <c r="O36" s="55"/>
+      <c r="P36" s="55"/>
+      <c r="Q36" s="55"/>
+      <c r="R36" s="55"/>
+      <c r="S36" s="55"/>
+      <c r="T36" s="62"/>
+    </row>
+    <row r="37" spans="8:20">
+      <c r="H37" s="61" t="s">
+        <v>97</v>
+      </c>
+      <c r="I37" s="55"/>
+      <c r="J37" s="55"/>
+      <c r="K37" s="55"/>
+      <c r="L37" s="80">
+        <f>L35*M35/L33/M33</f>
+        <v>0.61050061050061055</v>
+      </c>
+      <c r="M37" s="55"/>
+      <c r="N37" s="55"/>
+      <c r="O37" s="55"/>
+      <c r="P37" s="55"/>
+      <c r="Q37" s="55"/>
+      <c r="R37" s="55"/>
+      <c r="S37" s="55"/>
+      <c r="T37" s="62"/>
+    </row>
+    <row r="38" spans="8:20" ht="14.4" thickBot="1">
+      <c r="H38" s="63" t="s">
+        <v>99</v>
+      </c>
+      <c r="I38" s="64"/>
+      <c r="J38" s="64"/>
+      <c r="K38" s="64"/>
+      <c r="L38" s="64">
+        <f>N34/L35/M35</f>
+        <v>82.935333073626808</v>
+      </c>
+      <c r="M38" s="64"/>
+      <c r="N38" s="64"/>
+      <c r="O38" s="64"/>
+      <c r="P38" s="64"/>
+      <c r="Q38" s="64"/>
+      <c r="R38" s="64"/>
+      <c r="S38" s="64"/>
+      <c r="T38" s="65"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
+    <mergeCell ref="O25:Q25"/>
+    <mergeCell ref="L25:N25"/>
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="L10:N10"/>
     <mergeCell ref="O10:Q10"/>

</xml_diff>

<commit_message>
feat(HW Parameter): Add SP SRAM area comparison
</commit_message>
<xml_diff>
--- a/hardware/docs/01-top/点云硬件参数分析.xlsx
+++ b/hardware/docs/01-top/点云硬件参数分析.xlsx
@@ -390,7 +390,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="165">
   <si>
     <t>case</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -643,10 +643,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UMC 55-nm LP CMOS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Technology</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -723,19 +719,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>单位面积</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>深度</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>宽度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>容量</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1005,6 +993,163 @@
     <t>等效与真实加速比</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>uhdspsram</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>密度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>容量(KB)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TSMC 28-nm HPC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>    CCUFPS_CfgMaskBaseAddr ,</t>
+  </si>
+  <si>
+    <t>    CCUFPS_CfgDistBaseAddr ,</t>
+  </si>
+  <si>
+    <t>    CCUITF_DRAMBaseAddr     [GLBWRIDX_ITFCRD                 ]  ,</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortBankFlag  [GLBWRIDX_ITFCRD                 ]  ,</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortBankFlag  [GLB_NUM_WRPORT + GLBRDIDX_FPSCRD]  ,</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortBankFlag  [GLBWRIDX_FPSMSK                 ]  ,</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortBankFlag  [GLB_NUM_WRPORT + GLBRDIDX_FPSMSK]  ,</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortBankFlag  [GLBWRIDX_FPSDST                 ]  ,</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortBankFlag  [GLB_NUM_WRPORT + GLBRDIDX_FPSDST]  ,</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortBankFlag  [GLBWRIDX_FPSIDX                 ]  ,</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortBankFlag  [GLB_NUM_WRPORT + GLBRDIDX_ITFIDX]  ,</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortBankFlag  [GLBWRIDX_FPSCRD                 ]  ,</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortParBank     [GLBWRIDX_ITFCRD                 ],</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortParBank     [GLB_NUM_WRPORT + GLBRDIDX_FPSCRD],</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortParBank     [GLBWRIDX_FPSMSK                 ],</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortParBank     [GLB_NUM_WRPORT + GLBRDIDX_FPSMSK],</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortParBank     [GLBWRIDX_FPSDST                 ],</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortParBank     [GLB_NUM_WRPORT + GLBRDIDX_FPSDST],</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortParBank     [GLBWRIDX_FPSIDX                 ],</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortParBank     [GLB_NUM_WRPORT + GLBRDIDX_ITFIDX],</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortParBank     [GLBWRIDX_FPSCRD                 ],</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortOffEmptyFull[GLBWRIDX_ITFCRD                 ],</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortOffEmptyFull[GLB_NUM_WRPORT + GLBRDIDX_FPSCRD],</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortOffEmptyFull[GLBWRIDX_FPSMSK                 ],</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortOffEmptyFull[GLB_NUM_WRPORT + GLBRDIDX_FPSMSK],</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortOffEmptyFull[GLBWRIDX_FPSDST                 ],</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortOffEmptyFull[GLB_NUM_WRPORT + GLBRDIDX_FPSDST],</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortOffEmptyFull[GLBWRIDX_FPSIDX                 ],</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortOffEmptyFull[GLB_NUM_WRPORT + GLBRDIDX_ITFIDX],</t>
+  </si>
+  <si>
+    <t>    CCUTOP_CfgPortOffEmptyFull[GLBWRIDX_FPSCRD                 ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    CCUPOL_CfgNip                                                                   ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    CCUPOL_CfgChn                                                                   ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    CCUPOL_CfgK                                                                     ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    CCUITF_DRAMBaseAddr   [GLBWRIDX_ITFMAP                 ]                        ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    CCUTOP_CfgPortBankFlag[GLBWRIDX_ITFMAP                 ]                        ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    CCUTOP_CfgPortBankFlag[GLB_NUM_WRPORT + GLBRDIDX_POLMAP]                        ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    CCUTOP_CfgPortBankFlag[GLBWRIDX_POLOFM                 ]                        ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    CCUTOP_CfgPortBankFlag[GLB_NUM_WRPORT + GLBRDIDX_POLOFM]                        ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    CCUTOP_CfgPortBankFlag[GLB_NUM_WRPORT + GLBRDIDX_POLOFM +: NUM_BANK*POOL_CORE]  ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    CCUTOP_CfgPortParBank [GLBWRIDX_ITFMAP                 ]                        ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    CCUTOP_CfgPortParBank [GLB_NUM_WRPORT + GLBRDIDX_POLMAP]                        ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    CCUTOP_CfgPortParBank [GLBWRIDX_POLOFM                 ]                        ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    CCUTOP_CfgPortParBank [GLB_NUM_WRPORT + GLBRDIDX_POLOFM +: MAXPAR_WIDTH*POOL_CORE],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    CCUTOP_CfgPortOffEmptyFull [GLBWRIDX_ITFMAP                 ]                   ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    CCUTOP_CfgPortOffEmptyFull [GLB_NUM_WRPORT + GLBRDIDX_POLMAP]                   ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    CCUTOP_CfgPortOffEmptyFull [GLBWRIDX_POLOFM                 ]                   ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    CCUTOP_CfgPortOffEmptyFull [GLB_NUM_WRPORT + GLBRDIDX_POLOFM +: POOL_CORE]</t>
+  </si>
 </sst>
 </file>
 
@@ -1013,7 +1158,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1093,13 +1238,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF00B050"/>
@@ -1110,14 +1248,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -1161,6 +1291,12 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1170,7 +1306,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -1576,11 +1712,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1734,8 +1883,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1747,7 +1894,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1757,18 +1904,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1776,7 +1923,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1785,11 +1932,34 @@
     <xf numFmtId="176" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2131,10 +2301,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
@@ -2145,31 +2315,31 @@
     <col min="4" max="16384" width="8.88671875" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D1" s="30"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:7">
       <c r="A2" s="35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>65</v>
+        <v>117</v>
       </c>
       <c r="C2" s="44">
         <v>28</v>
       </c>
       <c r="D2" s="30"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:7">
       <c r="A3" s="35" t="s">
         <v>64</v>
       </c>
@@ -2181,7 +2351,7 @@
       </c>
       <c r="D3" s="30"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:7">
       <c r="A4" s="35" t="s">
         <v>63</v>
       </c>
@@ -2193,7 +2363,7 @@
       </c>
       <c r="D4" s="30"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:7">
       <c r="A5" s="35" t="s">
         <v>61</v>
       </c>
@@ -2204,20 +2374,26 @@
         <v>59</v>
       </c>
       <c r="D5" s="30"/>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="G5" s="96" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="45">
         <v>0.9</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D6" s="30"/>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="G6" s="96" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="35" t="s">
         <v>58</v>
       </c>
@@ -2228,8 +2404,11 @@
         <v>250</v>
       </c>
       <c r="D7" s="30"/>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="G7" s="96" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="35" t="s">
         <v>57</v>
       </c>
@@ -2240,8 +2419,11 @@
         <v>55</v>
       </c>
       <c r="D8" s="30"/>
-    </row>
-    <row r="9" spans="1:4" ht="14.4" thickBot="1">
+      <c r="G8" s="96" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="14.4" thickBot="1">
       <c r="A9" s="32" t="s">
         <v>54</v>
       </c>
@@ -2252,27 +2434,36 @@
         <v>53</v>
       </c>
       <c r="D9" s="30"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="90" t="s">
+      <c r="G9" s="96" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="97" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="91"/>
-      <c r="C10" s="92"/>
+      <c r="B10" s="98"/>
+      <c r="C10" s="99"/>
       <c r="D10" s="30"/>
-    </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1">
-      <c r="A11" s="85" t="s">
-        <v>112</v>
-      </c>
-      <c r="B11" s="83">
+      <c r="G10" s="96" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" thickBot="1">
+      <c r="A11" s="83" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="81">
         <f>3.6/1024</f>
         <v>3.5156250000000001E-3</v>
       </c>
-      <c r="C11" s="84"/>
+      <c r="C11" s="82"/>
       <c r="D11" s="30"/>
-    </row>
-    <row r="12" spans="1:4" ht="14.4" thickBot="1">
+      <c r="G11" s="96" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="14.4" thickBot="1">
       <c r="A12" s="39" t="s">
         <v>51</v>
       </c>
@@ -2283,10 +2474,13 @@
         <v>12288</v>
       </c>
       <c r="D12" s="30"/>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="G12" s="96" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B13" s="38">
         <f>B12*B7*2/1024/1024</f>
@@ -2297,32 +2491,41 @@
         <v>5.859375</v>
       </c>
       <c r="D13" s="30"/>
-    </row>
-    <row r="14" spans="1:4" ht="14.4">
+      <c r="G13" s="96" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="14.4">
       <c r="A14" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="B14" s="86">
+        <v>110</v>
+      </c>
+      <c r="B14" s="84">
         <f>9*1024</f>
         <v>9216</v>
       </c>
-      <c r="C14" s="87"/>
+      <c r="C14" s="85"/>
       <c r="D14" s="30"/>
-    </row>
-    <row r="15" spans="1:4" ht="14.4">
-      <c r="A15" s="88" t="s">
-        <v>111</v>
-      </c>
-      <c r="B15" s="89">
+      <c r="G14" s="96" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="14.4">
+      <c r="A15" s="86" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" s="87">
         <f>B11/(B14*5*10^(-9))</f>
         <v>76.293945312499986</v>
       </c>
-      <c r="C15" s="87"/>
+      <c r="C15" s="85"/>
       <c r="D15" s="30"/>
-    </row>
-    <row r="16" spans="1:4" ht="14.4">
+      <c r="G15" s="96" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="14.4">
       <c r="A16" s="35" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B16" s="34">
         <f>B13*10</f>
@@ -2332,10 +2535,13 @@
         <v>11.6</v>
       </c>
       <c r="D16" s="30"/>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="G16" s="96" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="29" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B17" s="34">
         <f>B16*4</f>
@@ -2343,16 +2549,22 @@
       </c>
       <c r="C17" s="49"/>
       <c r="D17" s="30"/>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="G17" s="96" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="30"/>
       <c r="B18" s="34"/>
       <c r="C18" s="49"/>
       <c r="D18" s="30"/>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="G18" s="96" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="35" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B19" s="36">
         <v>0.15</v>
@@ -2361,10 +2573,13 @@
         <v>0.60899999999999999</v>
       </c>
       <c r="D19" s="30"/>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="G19" s="96" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B20" s="34">
         <f>B13/B19</f>
@@ -2375,8 +2590,11 @@
         <v>9.6213054187192117</v>
       </c>
       <c r="D20" s="30"/>
-    </row>
-    <row r="21" spans="1:4" ht="14.4" thickBot="1">
+      <c r="G20" s="96" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="14.4" thickBot="1">
       <c r="A21" s="32" t="s">
         <v>50</v>
       </c>
@@ -2389,27 +2607,310 @@
         <v>19.047619047619047</v>
       </c>
       <c r="D21" s="30"/>
-    </row>
-    <row r="22" spans="1:4" ht="14.4" thickBot="1">
+      <c r="G21" s="96" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="14.4" thickBot="1">
       <c r="A22" s="32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B22" s="32"/>
       <c r="C22" s="32">
         <f>C21/4*(1.1/0.9)^2</f>
         <v>7.1134626690182259</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="G22" s="96" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="29" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B23" s="29">
         <f>B17/B13</f>
         <v>40</v>
       </c>
+      <c r="G23" s="96" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="G24" s="96" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="G25" s="96" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="G26" s="96" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="G27" s="96" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="G28" s="96" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="G29" s="96" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="G30" s="96" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="G31" s="96" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="G32" s="96" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="G33" s="96" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="G34" s="96" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="29">
+        <v>33</v>
+      </c>
+      <c r="B40" s="29" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="29">
+        <v>32</v>
+      </c>
+      <c r="B41" s="29" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="29">
+        <v>31</v>
+      </c>
+      <c r="B42" s="29" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="29">
+        <v>30</v>
+      </c>
+      <c r="B43" s="29" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="29">
+        <v>29</v>
+      </c>
+      <c r="B44" s="29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="29">
+        <v>28</v>
+      </c>
+      <c r="B45" s="29" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="29">
+        <v>27</v>
+      </c>
+      <c r="B46" s="29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="29">
+        <v>26</v>
+      </c>
+      <c r="B47" s="29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="29">
+        <v>25</v>
+      </c>
+      <c r="B48" s="29" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="29">
+        <v>24</v>
+      </c>
+      <c r="B49" s="29" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="29">
+        <v>23</v>
+      </c>
+      <c r="B50" s="29" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="29">
+        <v>22</v>
+      </c>
+      <c r="B51" s="29" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="29">
+        <v>21</v>
+      </c>
+      <c r="B52" s="29" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="29">
+        <v>20</v>
+      </c>
+      <c r="B53" s="29" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="29">
+        <v>19</v>
+      </c>
+      <c r="B54" s="29" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="29">
+        <v>18</v>
+      </c>
+      <c r="B55" s="29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="29">
+        <v>17</v>
+      </c>
+      <c r="B56" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="29">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="29">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="29">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="29">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="29">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="A40:G72">
+    <sortCondition descending="1" ref="A40:A72"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="A10:C10"/>
   </mergeCells>
@@ -2428,7 +2929,7 @@
       <pane xSplit="5" ySplit="3" topLeftCell="P16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomRight" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.77734375" defaultRowHeight="13.8"/>
@@ -2449,26 +2950,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="E1" s="67"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="93" t="s">
-        <v>100</v>
-      </c>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
-      <c r="M1" s="94"/>
-      <c r="N1" s="94"/>
-      <c r="O1" s="95"/>
-      <c r="P1" s="96" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q1" s="94"/>
-      <c r="R1" s="94"/>
-      <c r="S1" s="94"/>
-      <c r="T1" s="95"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="100" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" s="101"/>
+      <c r="L1" s="101"/>
+      <c r="M1" s="101"/>
+      <c r="N1" s="101"/>
+      <c r="O1" s="102"/>
+      <c r="P1" s="103" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q1" s="101"/>
+      <c r="R1" s="101"/>
+      <c r="S1" s="101"/>
+      <c r="T1" s="102"/>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="1" t="s">
@@ -2478,14 +2979,14 @@
       <c r="C2" s="1"/>
       <c r="D2" s="6"/>
       <c r="E2" s="24"/>
-      <c r="F2" s="100">
+      <c r="F2" s="107">
         <v>0</v>
       </c>
-      <c r="G2" s="101"/>
-      <c r="H2" s="100">
+      <c r="G2" s="108"/>
+      <c r="H2" s="107">
         <v>1</v>
       </c>
-      <c r="I2" s="101"/>
+      <c r="I2" s="108"/>
       <c r="J2" s="8">
         <v>2</v>
       </c>
@@ -2507,18 +3008,18 @@
       <c r="C3" s="1"/>
       <c r="D3" s="6"/>
       <c r="E3" s="25"/>
-      <c r="F3" s="93" t="s">
+      <c r="F3" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="102"/>
-      <c r="H3" s="93" t="s">
+      <c r="G3" s="109"/>
+      <c r="H3" s="100" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="102"/>
-      <c r="J3" s="93" t="s">
+      <c r="I3" s="109"/>
+      <c r="J3" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="95"/>
+      <c r="K3" s="102"/>
       <c r="L3" s="2" t="s">
         <v>41</v>
       </c>
@@ -2526,7 +3027,7 @@
         <v>48</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -2552,7 +3053,7 @@
         <v>47</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -2624,26 +3125,26 @@
     <row r="8" spans="1:20">
       <c r="A8" s="46"/>
       <c r="B8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="N8" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="O8" s="2" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="97" t="s">
+      <c r="A9" s="104" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2671,7 +3172,7 @@
       </c>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="98"/>
+      <c r="A10" s="105"/>
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
@@ -2697,7 +3198,7 @@
       </c>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11" s="98"/>
+      <c r="A11" s="105"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
         <v>15</v>
@@ -2720,7 +3221,7 @@
       </c>
     </row>
     <row r="12" spans="1:20">
-      <c r="A12" s="98"/>
+      <c r="A12" s="105"/>
       <c r="B12" s="1"/>
       <c r="C12" s="3"/>
       <c r="D12" s="11" t="s">
@@ -2732,7 +3233,7 @@
       </c>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="98"/>
+      <c r="A13" s="105"/>
       <c r="B13" s="1"/>
       <c r="C13" s="3"/>
       <c r="E13" s="19" t="s">
@@ -2747,7 +3248,7 @@
       </c>
     </row>
     <row r="14" spans="1:20">
-      <c r="A14" s="98"/>
+      <c r="A14" s="105"/>
       <c r="B14" s="1"/>
       <c r="C14" s="3"/>
       <c r="E14" s="19" t="s">
@@ -2761,7 +3262,7 @@
       </c>
     </row>
     <row r="15" spans="1:20">
-      <c r="A15" s="98"/>
+      <c r="A15" s="105"/>
       <c r="B15" s="1"/>
       <c r="C15" s="3"/>
       <c r="D15" s="19"/>
@@ -2769,7 +3270,7 @@
       <c r="H15" s="15"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="98"/>
+      <c r="A16" s="105"/>
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
         <v>16</v>
@@ -2792,14 +3293,14 @@
       </c>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="98"/>
+      <c r="A17" s="105"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="6"/>
       <c r="E17" s="25"/>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" s="98"/>
+      <c r="A18" s="105"/>
       <c r="B18" s="1" t="s">
         <v>10</v>
       </c>
@@ -2832,7 +3333,7 @@
       </c>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" s="98"/>
+      <c r="A19" s="105"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
         <v>17</v>
@@ -2858,7 +3359,7 @@
       </c>
     </row>
     <row r="20" spans="1:16">
-      <c r="A20" s="98"/>
+      <c r="A20" s="105"/>
       <c r="B20" s="1"/>
       <c r="C20" s="2" t="s">
         <v>39</v>
@@ -2869,7 +3370,7 @@
       </c>
     </row>
     <row r="21" spans="1:16">
-      <c r="A21" s="98"/>
+      <c r="A21" s="105"/>
       <c r="B21" s="1"/>
       <c r="C21" s="2" t="s">
         <v>40</v>
@@ -2880,7 +3381,7 @@
       </c>
     </row>
     <row r="22" spans="1:16">
-      <c r="A22" s="98"/>
+      <c r="A22" s="105"/>
       <c r="B22" s="1" t="s">
         <v>13</v>
       </c>
@@ -2910,7 +3411,7 @@
       </c>
     </row>
     <row r="23" spans="1:16">
-      <c r="A23" s="98"/>
+      <c r="A23" s="105"/>
       <c r="B23" s="1"/>
       <c r="C23" s="2" t="s">
         <v>18</v>
@@ -2931,7 +3432,7 @@
       </c>
     </row>
     <row r="24" spans="1:16">
-      <c r="A24" s="98"/>
+      <c r="A24" s="105"/>
       <c r="B24" s="1"/>
       <c r="D24" s="7" t="s">
         <v>43</v>
@@ -2946,7 +3447,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" ht="27.6">
-      <c r="A25" s="98"/>
+      <c r="A25" s="105"/>
       <c r="B25" s="1"/>
       <c r="E25" s="7" t="s">
         <v>42</v>
@@ -2961,7 +3462,7 @@
       </c>
     </row>
     <row r="26" spans="1:16">
-      <c r="A26" s="98"/>
+      <c r="A26" s="105"/>
       <c r="B26" s="1"/>
       <c r="C26" s="2" t="s">
         <v>19</v>
@@ -2978,7 +3479,7 @@
       </c>
     </row>
     <row r="27" spans="1:16">
-      <c r="A27" s="98"/>
+      <c r="A27" s="105"/>
       <c r="B27" s="1"/>
       <c r="C27" s="2" t="s">
         <v>20</v>
@@ -2992,7 +3493,7 @@
       </c>
     </row>
     <row r="28" spans="1:16">
-      <c r="A28" s="98"/>
+      <c r="A28" s="105"/>
       <c r="B28" s="1" t="s">
         <v>9</v>
       </c>
@@ -3022,7 +3523,7 @@
       </c>
     </row>
     <row r="29" spans="1:16">
-      <c r="A29" s="98"/>
+      <c r="A29" s="105"/>
       <c r="B29" s="1"/>
       <c r="C29" s="2" t="s">
         <v>21</v>
@@ -3042,7 +3543,7 @@
       </c>
     </row>
     <row r="30" spans="1:16">
-      <c r="A30" s="98"/>
+      <c r="A30" s="105"/>
       <c r="B30" s="1"/>
       <c r="C30" s="2" t="s">
         <v>22</v>
@@ -3055,7 +3556,7 @@
       </c>
     </row>
     <row r="31" spans="1:16">
-      <c r="A31" s="98"/>
+      <c r="A31" s="105"/>
       <c r="B31" s="1" t="s">
         <v>8</v>
       </c>
@@ -3082,7 +3583,7 @@
       </c>
     </row>
     <row r="32" spans="1:16">
-      <c r="A32" s="99"/>
+      <c r="A32" s="106"/>
       <c r="B32" s="1" t="s">
         <v>11</v>
       </c>
@@ -3185,7 +3686,7 @@
       </c>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="97" t="s">
+      <c r="A38" s="104" t="s">
         <v>24</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -3201,7 +3702,7 @@
       </c>
     </row>
     <row r="39" spans="1:14">
-      <c r="A39" s="98"/>
+      <c r="A39" s="105"/>
       <c r="B39" s="1" t="s">
         <v>12</v>
       </c>
@@ -3217,14 +3718,14 @@
       </c>
     </row>
     <row r="40" spans="1:14">
-      <c r="A40" s="98"/>
+      <c r="A40" s="105"/>
       <c r="B40" s="1"/>
       <c r="C40" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:14">
-      <c r="A41" s="98"/>
+      <c r="A41" s="105"/>
       <c r="B41" s="1"/>
       <c r="C41" s="3"/>
       <c r="D41" s="11" t="s">
@@ -3232,7 +3733,7 @@
       </c>
     </row>
     <row r="42" spans="1:14">
-      <c r="A42" s="98"/>
+      <c r="A42" s="105"/>
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
       <c r="E42" s="19" t="s">
@@ -3240,7 +3741,7 @@
       </c>
     </row>
     <row r="43" spans="1:14">
-      <c r="A43" s="98"/>
+      <c r="A43" s="105"/>
       <c r="B43" s="1"/>
       <c r="C43" s="3"/>
       <c r="E43" s="19" t="s">
@@ -3248,28 +3749,28 @@
       </c>
     </row>
     <row r="44" spans="1:14">
-      <c r="A44" s="98"/>
+      <c r="A44" s="105"/>
       <c r="B44" s="1"/>
       <c r="C44" s="3"/>
       <c r="D44" s="19"/>
       <c r="E44" s="27"/>
     </row>
     <row r="45" spans="1:14">
-      <c r="A45" s="98"/>
+      <c r="A45" s="105"/>
       <c r="B45" s="1"/>
       <c r="C45" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:14">
-      <c r="A46" s="98"/>
+      <c r="A46" s="105"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="6"/>
       <c r="E46" s="25"/>
     </row>
     <row r="47" spans="1:14">
-      <c r="A47" s="98"/>
+      <c r="A47" s="105"/>
       <c r="B47" s="1" t="s">
         <v>10</v>
       </c>
@@ -3285,7 +3786,7 @@
       </c>
     </row>
     <row r="48" spans="1:14">
-      <c r="A48" s="99"/>
+      <c r="A48" s="106"/>
       <c r="B48" s="1"/>
       <c r="C48" s="2" t="s">
         <v>17</v>
@@ -3415,14 +3916,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T38"/>
+  <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
     <col min="2" max="4" width="11.21875" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" customWidth="1"/>
     <col min="8" max="8" width="12.21875" customWidth="1"/>
@@ -3431,27 +3933,27 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D1" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="E1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F1" t="s">
-        <v>85</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2">
         <v>2048</v>
@@ -3460,20 +3962,20 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <f>B2*C2</f>
-        <v>2048</v>
+        <f>B2*C2/8192</f>
+        <v>0.25</v>
       </c>
       <c r="E2">
         <v>6750</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F8" si="0">E2/(B2*C2)</f>
-        <v>3.2958984375</v>
+        <f>(B2*C2)/E2</f>
+        <v>0.3034074074074074</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3">
         <v>32</v>
@@ -3482,20 +3984,20 @@
         <v>16</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D8" si="1">B3*C3</f>
-        <v>512</v>
+        <f t="shared" ref="D3:D17" si="0">B3*C3/8192</f>
+        <v>6.25E-2</v>
       </c>
       <c r="E3">
         <v>2762</v>
       </c>
       <c r="F3">
-        <f t="shared" si="0"/>
-        <v>5.39453125</v>
+        <f t="shared" ref="F3:F17" si="1">(B3*C3)/E3</f>
+        <v>0.18537291817523532</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4">
         <v>32</v>
@@ -3503,21 +4005,21 @@
       <c r="C4">
         <v>128</v>
       </c>
-      <c r="D4" s="51">
-        <f t="shared" si="1"/>
-        <v>4096</v>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
       </c>
       <c r="E4">
         <v>15180</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
-        <v>3.7060546875</v>
+        <f t="shared" si="1"/>
+        <v>0.26982872200263502</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5">
         <v>64</v>
@@ -3526,20 +4028,20 @@
         <v>128</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
-        <v>8192</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>15867</v>
       </c>
-      <c r="F5" s="54">
-        <f t="shared" si="0"/>
-        <v>1.9368896484375</v>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>0.51629167454465241</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6">
         <v>64</v>
@@ -3548,20 +4050,20 @@
         <v>64</v>
       </c>
       <c r="D6">
-        <f>B6*C6</f>
-        <v>4096</v>
+        <f t="shared" si="0"/>
+        <v>0.5</v>
       </c>
       <c r="E6">
         <v>8451</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
-        <v>2.063232421875</v>
+        <f t="shared" si="1"/>
+        <v>0.48467636966039523</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7">
         <v>128</v>
@@ -3570,20 +4072,20 @@
         <v>64</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
-        <v>8192</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>9182</v>
       </c>
-      <c r="F7" s="53">
-        <f t="shared" si="0"/>
-        <v>1.120849609375</v>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0.89218035286429975</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B8">
         <v>4096</v>
@@ -3592,764 +4094,1035 @@
         <v>128</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
-        <v>524288</v>
+        <f t="shared" si="0"/>
+        <v>64</v>
       </c>
       <c r="E8">
         <v>118814</v>
       </c>
-      <c r="F8" s="52">
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>4.4126786405642431</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="14.4" thickBot="1">
+      <c r="A9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9">
+        <v>1024</v>
+      </c>
+      <c r="C9">
+        <v>32</v>
+      </c>
+      <c r="D9">
         <f t="shared" si="0"/>
-        <v>0.22661972045898438</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" ht="14.4" thickBot="1"/>
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>8301</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>3.947476207685821</v>
+      </c>
+    </row>
     <row r="10" spans="1:20" ht="14.4" thickBot="1">
-      <c r="H10" s="56"/>
-      <c r="I10" s="104" t="s">
+      <c r="A10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10">
+        <v>512</v>
+      </c>
+      <c r="C10">
+        <v>64</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>8726</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>3.7552143020857209</v>
+      </c>
+      <c r="H10" s="54"/>
+      <c r="I10" s="111" t="s">
+        <v>90</v>
+      </c>
+      <c r="J10" s="112"/>
+      <c r="K10" s="113"/>
+      <c r="L10" s="114" t="s">
+        <v>92</v>
+      </c>
+      <c r="M10" s="115"/>
+      <c r="N10" s="116"/>
+      <c r="O10" s="114" t="s">
+        <v>91</v>
+      </c>
+      <c r="P10" s="115"/>
+      <c r="Q10" s="116"/>
+      <c r="R10" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="J10" s="105"/>
-      <c r="K10" s="106"/>
-      <c r="L10" s="107" t="s">
+      <c r="S10" s="57"/>
+      <c r="T10" s="58"/>
+    </row>
+    <row r="11" spans="1:20" ht="14.4" thickBot="1">
+      <c r="A11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11">
+        <v>1024</v>
+      </c>
+      <c r="C11">
+        <v>64</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>14726</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>4.45035990764634</v>
+      </c>
+      <c r="H11" s="54"/>
+      <c r="I11" s="88"/>
+      <c r="J11" s="89"/>
+      <c r="K11" s="90"/>
+      <c r="L11" s="91"/>
+      <c r="M11" s="92"/>
+      <c r="N11" s="95"/>
+      <c r="O11" s="91"/>
+      <c r="P11" s="92"/>
+      <c r="Q11" s="95"/>
+      <c r="R11" s="56"/>
+      <c r="S11" s="57"/>
+      <c r="T11" s="94"/>
+    </row>
+    <row r="12" spans="1:20" ht="14.4" thickBot="1">
+      <c r="A12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12">
+        <v>2048</v>
+      </c>
+      <c r="C12">
+        <v>64</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E12">
+        <v>27288</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>4.8032834945763705</v>
+      </c>
+      <c r="H12" s="54"/>
+      <c r="I12" s="88"/>
+      <c r="J12" s="89"/>
+      <c r="K12" s="90"/>
+      <c r="L12" s="91"/>
+      <c r="M12" s="92"/>
+      <c r="N12" s="95"/>
+      <c r="O12" s="91"/>
+      <c r="P12" s="92"/>
+      <c r="Q12" s="95"/>
+      <c r="R12" s="56"/>
+      <c r="S12" s="57"/>
+      <c r="T12" s="94"/>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13">
+        <v>256</v>
+      </c>
+      <c r="C13">
+        <v>128</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>10836</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>3.0239940937615355</v>
+      </c>
+      <c r="H13" s="54"/>
+      <c r="I13" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="J13" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="K13" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="M10" s="108"/>
-      <c r="N10" s="109"/>
-      <c r="O10" s="107" t="s">
+      <c r="L13" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="M13" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="N13" s="60" t="s">
+        <v>95</v>
+      </c>
+      <c r="O13" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="P13" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q13" s="60" t="s">
+        <v>95</v>
+      </c>
+      <c r="R13" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="S13" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="T13" s="60" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14">
+        <v>512</v>
+      </c>
+      <c r="C14">
+        <v>128</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>16342</v>
+      </c>
+      <c r="F14" s="51">
+        <f t="shared" si="1"/>
+        <v>4.0102802594541673</v>
+      </c>
+      <c r="H14" s="54"/>
+      <c r="I14" s="93"/>
+      <c r="J14" s="55"/>
+      <c r="K14" s="94"/>
+      <c r="L14" s="93"/>
+      <c r="M14" s="55"/>
+      <c r="N14" s="60"/>
+      <c r="O14" s="93"/>
+      <c r="P14" s="55"/>
+      <c r="Q14" s="60"/>
+      <c r="R14" s="93"/>
+      <c r="S14" s="55"/>
+      <c r="T14" s="60"/>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B15">
+        <v>1024</v>
+      </c>
+      <c r="C15">
+        <v>128</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E15">
+        <v>27577</v>
+      </c>
+      <c r="F15" s="52">
+        <f t="shared" si="1"/>
+        <v>4.7529462958262316</v>
+      </c>
+      <c r="H15" s="54"/>
+      <c r="I15" s="93"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="94"/>
+      <c r="L15" s="93"/>
+      <c r="M15" s="55"/>
+      <c r="N15" s="60"/>
+      <c r="O15" s="93"/>
+      <c r="P15" s="55"/>
+      <c r="Q15" s="60"/>
+      <c r="R15" s="93"/>
+      <c r="S15" s="55"/>
+      <c r="T15" s="60"/>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16">
+        <v>2048</v>
+      </c>
+      <c r="C16">
+        <v>128</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="E16">
+        <v>51313</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>5.1087248845321849</v>
+      </c>
+      <c r="H16" s="54"/>
+      <c r="I16" s="93"/>
+      <c r="J16" s="55"/>
+      <c r="K16" s="94"/>
+      <c r="L16" s="93"/>
+      <c r="M16" s="55"/>
+      <c r="N16" s="60"/>
+      <c r="O16" s="93"/>
+      <c r="P16" s="55"/>
+      <c r="Q16" s="60"/>
+      <c r="R16" s="93"/>
+      <c r="S16" s="55"/>
+      <c r="T16" s="60"/>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17">
+        <v>128</v>
+      </c>
+      <c r="C17">
+        <v>256</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>9919</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>3.3035588264946063</v>
+      </c>
+      <c r="H17" s="54" t="s">
+        <v>87</v>
+      </c>
+      <c r="I17" s="59">
+        <v>1.5</v>
+      </c>
+      <c r="J17" s="53">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K17" s="60"/>
+      <c r="L17" s="59">
+        <v>1.5</v>
+      </c>
+      <c r="M17" s="53">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N17" s="60"/>
+      <c r="O17" s="59">
+        <v>1.5</v>
+      </c>
+      <c r="P17" s="53">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Q17" s="60"/>
+      <c r="R17" s="59">
+        <v>1.5</v>
+      </c>
+      <c r="S17" s="53">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="T17" s="60"/>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" t="s">
+        <v>114</v>
+      </c>
+      <c r="H18" s="54" t="s">
+        <v>102</v>
+      </c>
+      <c r="I18" s="59">
+        <v>0.11</v>
+      </c>
+      <c r="J18" s="53"/>
+      <c r="K18" s="60">
+        <v>83</v>
+      </c>
+      <c r="L18" s="59">
+        <v>0.17</v>
+      </c>
+      <c r="M18" s="53"/>
+      <c r="N18" s="60">
+        <f>K18*1.8</f>
+        <v>149.4</v>
+      </c>
+      <c r="O18" s="59">
+        <v>0.25</v>
+      </c>
+      <c r="P18" s="53"/>
+      <c r="Q18" s="60">
+        <f>K18*1.8</f>
+        <v>149.4</v>
+      </c>
+      <c r="R18" s="59">
+        <v>0.35</v>
+      </c>
+      <c r="S18" s="53"/>
+      <c r="T18" s="60">
+        <f>K18*1.5*1.8</f>
+        <v>224.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19" t="s">
+        <v>114</v>
+      </c>
+      <c r="H19" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="I19" s="59">
+        <f>I17-I18*2</f>
+        <v>1.28</v>
+      </c>
+      <c r="J19" s="53">
+        <f>J17-I18*2</f>
+        <v>1.9800000000000002</v>
+      </c>
+      <c r="K19" s="60"/>
+      <c r="L19" s="59">
+        <f>L17-L18*2</f>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="M19" s="53">
+        <f>M17-L18*2</f>
+        <v>1.86</v>
+      </c>
+      <c r="N19" s="60"/>
+      <c r="O19" s="59">
+        <f>O17-O18*2</f>
+        <v>1</v>
+      </c>
+      <c r="P19" s="53">
+        <f>P17-O18*2</f>
+        <v>1.7000000000000002</v>
+      </c>
+      <c r="Q19" s="60"/>
+      <c r="R19" s="59">
+        <f>R17-R18*2</f>
+        <v>0.8</v>
+      </c>
+      <c r="S19" s="53">
+        <f>S17-R18*2</f>
+        <v>1.5000000000000002</v>
+      </c>
+      <c r="T19" s="60"/>
+    </row>
+    <row r="20" spans="1:20" ht="14.4" thickBot="1">
+      <c r="A20" t="s">
+        <v>114</v>
+      </c>
+      <c r="H20" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="P10" s="108"/>
-      <c r="Q10" s="109"/>
-      <c r="R10" s="58" t="s">
+      <c r="I20" s="61">
+        <f>I19*J19/I17/J17</f>
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="J20" s="62"/>
+      <c r="K20" s="63"/>
+      <c r="L20" s="64">
+        <f>L19*M19/L17/M17</f>
+        <v>0.65381818181818174</v>
+      </c>
+      <c r="M20" s="62"/>
+      <c r="N20" s="63"/>
+      <c r="O20" s="61">
+        <f>O19*P19/O17/P17</f>
+        <v>0.51515151515151525</v>
+      </c>
+      <c r="P20" s="62"/>
+      <c r="Q20" s="63"/>
+      <c r="R20" s="61">
+        <f>R19*S19/R17/S17</f>
+        <v>0.3636363636363637</v>
+      </c>
+      <c r="S20" s="62"/>
+      <c r="T20" s="63"/>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" t="s">
+        <v>114</v>
+      </c>
+      <c r="H21" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="S10" s="59"/>
-      <c r="T10" s="60"/>
-    </row>
-    <row r="11" spans="1:20">
-      <c r="H11" s="56"/>
-      <c r="I11" s="58" t="s">
+      <c r="I21" s="55">
+        <f>K18/I19/J19</f>
+        <v>32.749368686868685</v>
+      </c>
+      <c r="J21" s="55"/>
+      <c r="K21" s="55"/>
+      <c r="L21" s="55">
+        <f>N18/L19/M19</f>
+        <v>69.243604004449395</v>
+      </c>
+      <c r="M21" s="55"/>
+      <c r="N21" s="55"/>
+      <c r="O21" s="55">
+        <f>Q18/O19/P19</f>
+        <v>87.882352941176464</v>
+      </c>
+      <c r="P21" s="55"/>
+      <c r="Q21" s="55"/>
+      <c r="R21" s="55">
+        <f>T18/R19/S19</f>
+        <v>186.74999999999997</v>
+      </c>
+      <c r="S21" s="55"/>
+      <c r="T21" s="55"/>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" t="s">
+        <v>114</v>
+      </c>
+      <c r="H22" s="68" t="s">
+        <v>101</v>
+      </c>
+      <c r="I22" s="52"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="52">
+        <f>K18/(I19+J19)/2</f>
+        <v>12.730061349693251</v>
+      </c>
+      <c r="L22" s="52"/>
+      <c r="M22" s="52"/>
+      <c r="N22" s="52">
+        <f>N18/(L19+M19)/2</f>
+        <v>24.735099337748345</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="H23" s="71" t="s">
+        <v>87</v>
+      </c>
+      <c r="I23" s="70">
+        <f>I25+I24*2</f>
+        <v>1.52</v>
+      </c>
+      <c r="J23" s="70">
+        <f>J25+I24*2</f>
+        <v>1.52</v>
+      </c>
+      <c r="K23" s="70">
+        <f>I23*J23</f>
+        <v>2.3104</v>
+      </c>
+      <c r="L23" s="70">
+        <f>L25+L24*2</f>
+        <v>1.6400000000000001</v>
+      </c>
+      <c r="M23" s="70">
+        <f>M25+L24*2</f>
+        <v>1.6400000000000001</v>
+      </c>
+      <c r="N23" s="70">
+        <f>L23*M23</f>
+        <v>2.6896000000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="H24" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="J11" s="59" t="s">
-        <v>107</v>
-      </c>
-      <c r="K11" s="60" t="s">
-        <v>98</v>
-      </c>
-      <c r="L11" s="58" t="s">
+      <c r="I24" s="70">
+        <v>0.11</v>
+      </c>
+      <c r="J24" s="70"/>
+      <c r="K24" s="70">
+        <f>K22*(I23+J23)*2</f>
+        <v>77.398773006134974</v>
+      </c>
+      <c r="L24" s="70">
+        <v>0.17</v>
+      </c>
+      <c r="M24" s="70"/>
+      <c r="N24" s="70">
+        <f>N22*(L23+M23)*2</f>
+        <v>162.26225165562914</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="H25" s="71" t="s">
+        <v>88</v>
+      </c>
+      <c r="I25" s="70">
+        <v>1.3</v>
+      </c>
+      <c r="J25" s="70">
+        <v>1.3</v>
+      </c>
+      <c r="K25" s="70">
+        <f>I25*J25</f>
+        <v>1.6900000000000002</v>
+      </c>
+      <c r="L25" s="70">
+        <v>1.3</v>
+      </c>
+      <c r="M25" s="70">
+        <v>1.3</v>
+      </c>
+      <c r="N25" s="70"/>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="H26" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="I26" s="70"/>
+      <c r="J26" s="70"/>
+      <c r="K26" s="70">
+        <f>I24*(I25+J25)*2</f>
+        <v>0.57200000000000006</v>
+      </c>
+      <c r="L26" s="70"/>
+      <c r="M26" s="70"/>
+      <c r="N26" s="70">
+        <f>L24*(L25+M25)*2</f>
+        <v>0.88400000000000012</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="14.4" thickBot="1">
+      <c r="H27" s="71" t="s">
+        <v>94</v>
+      </c>
+      <c r="I27" s="70"/>
+      <c r="J27" s="70"/>
+      <c r="K27" s="70"/>
+      <c r="L27" s="72">
+        <f>L25*M25/L23/M23</f>
+        <v>0.62834622248661509</v>
+      </c>
+      <c r="M27" s="70"/>
+      <c r="N27" s="70"/>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="H28" s="73" t="s">
+        <v>96</v>
+      </c>
+      <c r="I28" s="70"/>
+      <c r="J28" s="70"/>
+      <c r="K28" s="70"/>
+      <c r="L28" s="74">
+        <f>N24/L25/M25</f>
+        <v>96.013166660135582</v>
+      </c>
+      <c r="M28" s="70"/>
+      <c r="N28" s="70"/>
+    </row>
+    <row r="29" spans="1:20" ht="14.4" thickBot="1">
+      <c r="H29" s="76"/>
+      <c r="I29" s="70"/>
+      <c r="J29" s="70"/>
+      <c r="K29" s="70"/>
+      <c r="L29" s="75"/>
+      <c r="M29" s="70"/>
+      <c r="N29" s="70"/>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="H30" s="56"/>
+      <c r="I30" s="80" t="s">
+        <v>90</v>
+      </c>
+      <c r="J30" s="80"/>
+      <c r="K30" s="80"/>
+      <c r="L30" s="110" t="s">
+        <v>105</v>
+      </c>
+      <c r="M30" s="110"/>
+      <c r="N30" s="110"/>
+      <c r="O30" s="110" t="s">
+        <v>91</v>
+      </c>
+      <c r="P30" s="110"/>
+      <c r="Q30" s="110"/>
+      <c r="R30" s="57" t="s">
+        <v>93</v>
+      </c>
+      <c r="S30" s="57"/>
+      <c r="T30" s="58"/>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="H31" s="59"/>
+      <c r="I31" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="J31" s="53" t="s">
+        <v>104</v>
+      </c>
+      <c r="K31" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="L31" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="M31" s="53" t="s">
+        <v>104</v>
+      </c>
+      <c r="N31" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="O31" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="P31" s="53" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q31" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="R31" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="S31" s="53" t="s">
+        <v>104</v>
+      </c>
+      <c r="T31" s="60" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="H32" s="79" t="s">
+        <v>88</v>
+      </c>
+      <c r="I32" s="69">
+        <v>1.7</v>
+      </c>
+      <c r="J32" s="69">
+        <v>1</v>
+      </c>
+      <c r="K32" s="69">
+        <v>0.11</v>
+      </c>
+      <c r="L32" s="69">
+        <v>1.7</v>
+      </c>
+      <c r="M32" s="69">
+        <v>1</v>
+      </c>
+      <c r="N32" s="69">
+        <v>1.7</v>
+      </c>
+      <c r="O32" s="53"/>
+      <c r="P32" s="53"/>
+      <c r="Q32" s="53"/>
+      <c r="R32" s="53"/>
+      <c r="S32" s="53"/>
+      <c r="T32" s="60"/>
+    </row>
+    <row r="33" spans="8:20">
+      <c r="H33" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="I33" s="69">
+        <f>I32+K32*2</f>
+        <v>1.92</v>
+      </c>
+      <c r="J33" s="69">
+        <f>J32+K32*2</f>
+        <v>1.22</v>
+      </c>
+      <c r="K33" s="69">
+        <f>I33*J33</f>
+        <v>2.3424</v>
+      </c>
+      <c r="L33" s="69">
+        <f>L32+L34*2</f>
+        <v>2.04</v>
+      </c>
+      <c r="M33" s="69">
+        <f>M32+L34*2</f>
+        <v>1.34</v>
+      </c>
+      <c r="N33" s="69">
+        <f>L33*M33</f>
+        <v>2.7336</v>
+      </c>
+      <c r="O33" s="53"/>
+      <c r="P33" s="53"/>
+      <c r="Q33" s="53"/>
+      <c r="R33" s="53"/>
+      <c r="S33" s="53"/>
+      <c r="T33" s="60"/>
+    </row>
+    <row r="34" spans="8:20">
+      <c r="H34" s="79" t="s">
+        <v>95</v>
+      </c>
+      <c r="J34" s="69"/>
+      <c r="K34" s="69">
+        <f>K28*(I33+J33)*2</f>
+        <v>0</v>
+      </c>
+      <c r="L34" s="69">
+        <v>0.17</v>
+      </c>
+      <c r="M34" s="69"/>
+      <c r="N34" s="69">
+        <f>N28*(L33+M33)*2</f>
+        <v>0</v>
+      </c>
+      <c r="O34" s="53"/>
+      <c r="P34" s="53"/>
+      <c r="Q34" s="53"/>
+      <c r="R34" s="53"/>
+      <c r="S34" s="53"/>
+      <c r="T34" s="60"/>
+    </row>
+    <row r="35" spans="8:20">
+      <c r="H35" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="I35" s="69"/>
+      <c r="J35" s="69"/>
+      <c r="K35" s="69" t="e">
+        <f>K33-#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L35" s="69"/>
+      <c r="M35" s="69"/>
+      <c r="N35" s="69">
+        <f>N33-N32</f>
+        <v>1.0336000000000001</v>
+      </c>
+      <c r="O35" s="53"/>
+      <c r="P35" s="53"/>
+      <c r="Q35" s="53"/>
+      <c r="R35" s="53"/>
+      <c r="S35" s="53"/>
+      <c r="T35" s="60"/>
+    </row>
+    <row r="36" spans="8:20">
+      <c r="H36" s="79" t="s">
+        <v>94</v>
+      </c>
+      <c r="I36" s="69"/>
+      <c r="J36" s="69"/>
+      <c r="K36" s="69"/>
+      <c r="L36" s="77">
+        <f>L32*M32/L33/M33</f>
+        <v>0.62189054726368154</v>
+      </c>
+      <c r="M36" s="69"/>
+      <c r="N36" s="69"/>
+      <c r="O36" s="53"/>
+      <c r="P36" s="53"/>
+      <c r="Q36" s="53"/>
+      <c r="R36" s="53"/>
+      <c r="S36" s="53"/>
+      <c r="T36" s="60"/>
+    </row>
+    <row r="37" spans="8:20">
+      <c r="H37" s="79" t="s">
+        <v>96</v>
+      </c>
+      <c r="I37" s="69"/>
+      <c r="J37" s="69"/>
+      <c r="K37" s="69"/>
+      <c r="L37" s="69">
+        <f>N34/L32/M32</f>
+        <v>0</v>
+      </c>
+      <c r="M37" s="69"/>
+      <c r="N37" s="69"/>
+      <c r="O37" s="53"/>
+      <c r="P37" s="53"/>
+      <c r="Q37" s="53"/>
+      <c r="R37" s="53"/>
+      <c r="S37" s="53"/>
+      <c r="T37" s="60"/>
+    </row>
+    <row r="38" spans="8:20">
+      <c r="H38" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="I38" s="53">
+        <f>I40+I39*2</f>
+        <v>1.07</v>
+      </c>
+      <c r="J38" s="53">
+        <f>J40+I39*2</f>
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="K38" s="53">
+        <f>I38*J38</f>
+        <v>2.3754000000000004</v>
+      </c>
+      <c r="L38" s="53">
+        <f>L40+L39*2</f>
+        <v>1.19</v>
+      </c>
+      <c r="M38" s="53">
+        <f>M40+L39*2</f>
+        <v>2.34</v>
+      </c>
+      <c r="N38" s="53">
+        <f>L38*M38</f>
+        <v>2.7845999999999997</v>
+      </c>
+      <c r="O38" s="53"/>
+      <c r="P38" s="53"/>
+      <c r="Q38" s="53"/>
+      <c r="R38" s="53"/>
+      <c r="S38" s="53"/>
+      <c r="T38" s="60"/>
+    </row>
+    <row r="39" spans="8:20">
+      <c r="H39" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="M11" s="59" t="s">
-        <v>107</v>
-      </c>
-      <c r="N11" s="62" t="s">
-        <v>98</v>
-      </c>
-      <c r="O11" s="58" t="s">
-        <v>89</v>
-      </c>
-      <c r="P11" s="59" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q11" s="62" t="s">
-        <v>98</v>
-      </c>
-      <c r="R11" s="58" t="s">
-        <v>89</v>
-      </c>
-      <c r="S11" s="59" t="s">
-        <v>107</v>
-      </c>
-      <c r="T11" s="62" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20">
-      <c r="H12" s="56" t="s">
-        <v>90</v>
-      </c>
-      <c r="I12" s="61">
-        <v>1.5</v>
-      </c>
-      <c r="J12" s="55">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="K12" s="62"/>
-      <c r="L12" s="61">
-        <v>1.5</v>
-      </c>
-      <c r="M12" s="55">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="N12" s="62"/>
-      <c r="O12" s="61">
-        <v>1.5</v>
-      </c>
-      <c r="P12" s="55">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="Q12" s="62"/>
-      <c r="R12" s="61">
-        <v>1.5</v>
-      </c>
-      <c r="S12" s="55">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="T12" s="62"/>
-    </row>
-    <row r="13" spans="1:20">
-      <c r="H13" s="56" t="s">
-        <v>105</v>
-      </c>
-      <c r="I13" s="61">
+      <c r="I39" s="53">
         <v>0.11</v>
       </c>
-      <c r="J13" s="55"/>
-      <c r="K13" s="62">
-        <v>83</v>
-      </c>
-      <c r="L13" s="61">
+      <c r="J39" s="53"/>
+      <c r="K39" s="53">
+        <f>K22*(I40+J40)*2</f>
+        <v>72.561349693251529</v>
+      </c>
+      <c r="L39" s="53">
         <v>0.17</v>
       </c>
-      <c r="M13" s="55"/>
-      <c r="N13" s="62">
-        <f>K13*1.8</f>
-        <v>149.4</v>
-      </c>
-      <c r="O13" s="61">
-        <v>0.25</v>
-      </c>
-      <c r="P13" s="55"/>
-      <c r="Q13" s="62">
-        <f>K13*1.8</f>
-        <v>149.4</v>
-      </c>
-      <c r="R13" s="61">
-        <v>0.35</v>
-      </c>
-      <c r="S13" s="55"/>
-      <c r="T13" s="62">
-        <f>K13*1.5*1.8</f>
-        <v>224.1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20">
-      <c r="H14" s="56" t="s">
-        <v>91</v>
-      </c>
-      <c r="I14" s="61">
-        <f>I12-I13*2</f>
-        <v>1.28</v>
-      </c>
-      <c r="J14" s="55">
-        <f>J12-I13*2</f>
-        <v>1.9800000000000002</v>
-      </c>
-      <c r="K14" s="62"/>
-      <c r="L14" s="61">
-        <f>L12-L13*2</f>
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="M14" s="55">
-        <f>M12-L13*2</f>
-        <v>1.86</v>
-      </c>
-      <c r="N14" s="62"/>
-      <c r="O14" s="61">
-        <f>O12-O13*2</f>
-        <v>1</v>
-      </c>
-      <c r="P14" s="55">
-        <f>P12-O13*2</f>
-        <v>1.7000000000000002</v>
-      </c>
-      <c r="Q14" s="62"/>
-      <c r="R14" s="61">
-        <f>R12-R13*2</f>
-        <v>0.8</v>
-      </c>
-      <c r="S14" s="55">
-        <f>S12-R13*2</f>
-        <v>1.5000000000000002</v>
-      </c>
-      <c r="T14" s="62"/>
-    </row>
-    <row r="15" spans="1:20" ht="14.4" thickBot="1">
-      <c r="H15" s="56" t="s">
-        <v>97</v>
-      </c>
-      <c r="I15" s="63">
-        <f>I14*J14/I12/J12</f>
-        <v>0.76800000000000002</v>
-      </c>
-      <c r="J15" s="64"/>
-      <c r="K15" s="65"/>
-      <c r="L15" s="66">
-        <f>L14*M14/L12/M12</f>
-        <v>0.65381818181818174</v>
-      </c>
-      <c r="M15" s="64"/>
-      <c r="N15" s="65"/>
-      <c r="O15" s="63">
-        <f>O14*P14/O12/P12</f>
-        <v>0.51515151515151525</v>
-      </c>
-      <c r="P15" s="64"/>
-      <c r="Q15" s="65"/>
-      <c r="R15" s="63">
-        <f>R14*S14/R12/S12</f>
-        <v>0.3636363636363637</v>
-      </c>
-      <c r="S15" s="64"/>
-      <c r="T15" s="65"/>
-    </row>
-    <row r="16" spans="1:20">
-      <c r="H16" s="55" t="s">
-        <v>99</v>
-      </c>
-      <c r="I16" s="57">
-        <f>K13/I14/J14</f>
-        <v>32.749368686868685</v>
-      </c>
-      <c r="J16" s="57"/>
-      <c r="K16" s="57"/>
-      <c r="L16" s="57">
-        <f>N13/L14/M14</f>
-        <v>69.243604004449395</v>
-      </c>
-      <c r="M16" s="57"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="57">
-        <f>Q13/O14/P14</f>
-        <v>87.882352941176464</v>
-      </c>
-      <c r="P16" s="57"/>
-      <c r="Q16" s="57"/>
-      <c r="R16" s="57">
-        <f>T13/R14/S14</f>
-        <v>186.74999999999997</v>
-      </c>
-      <c r="S16" s="57"/>
-      <c r="T16" s="57"/>
-    </row>
-    <row r="17" spans="8:20">
-      <c r="H17" s="70" t="s">
-        <v>104</v>
-      </c>
-      <c r="I17" s="53"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="53">
-        <f>K13/(I14+J14)/2</f>
-        <v>12.730061349693251</v>
-      </c>
-      <c r="L17" s="53"/>
-      <c r="M17" s="53"/>
-      <c r="N17" s="53">
-        <f>N13/(L14+M14)/2</f>
-        <v>24.735099337748345</v>
-      </c>
-    </row>
-    <row r="18" spans="8:20">
-      <c r="H18" s="73" t="s">
-        <v>90</v>
-      </c>
-      <c r="I18" s="72">
-        <f>I20+I19*2</f>
-        <v>1.52</v>
-      </c>
-      <c r="J18" s="72">
-        <f>J20+I19*2</f>
-        <v>1.52</v>
-      </c>
-      <c r="K18" s="72">
-        <f>I18*J18</f>
-        <v>2.3104</v>
-      </c>
-      <c r="L18" s="72">
-        <f>L20+L19*2</f>
-        <v>1.6400000000000001</v>
-      </c>
-      <c r="M18" s="72">
-        <f>M20+L19*2</f>
-        <v>1.6400000000000001</v>
-      </c>
-      <c r="N18" s="72">
-        <f>L18*M18</f>
-        <v>2.6896000000000004</v>
-      </c>
-    </row>
-    <row r="19" spans="8:20">
-      <c r="H19" s="73" t="s">
-        <v>92</v>
-      </c>
-      <c r="I19" s="72">
-        <v>0.11</v>
-      </c>
-      <c r="J19" s="72"/>
-      <c r="K19" s="72">
-        <f>K17*(I18+J18)*2</f>
-        <v>77.398773006134974</v>
-      </c>
-      <c r="L19" s="72">
-        <v>0.17</v>
-      </c>
-      <c r="M19" s="72"/>
-      <c r="N19" s="72">
-        <f>N17*(L18+M18)*2</f>
-        <v>162.26225165562914</v>
-      </c>
-    </row>
-    <row r="20" spans="8:20">
-      <c r="H20" s="73" t="s">
-        <v>91</v>
-      </c>
-      <c r="I20" s="72">
-        <v>1.3</v>
-      </c>
-      <c r="J20" s="72">
-        <v>1.3</v>
-      </c>
-      <c r="K20" s="72">
-        <f>I20*J20</f>
-        <v>1.6900000000000002</v>
-      </c>
-      <c r="L20" s="72">
-        <v>1.3</v>
-      </c>
-      <c r="M20" s="72">
-        <v>1.3</v>
-      </c>
-      <c r="N20" s="72"/>
-    </row>
-    <row r="21" spans="8:20">
-      <c r="H21" s="73" t="s">
-        <v>106</v>
-      </c>
-      <c r="I21" s="72"/>
-      <c r="J21" s="72"/>
-      <c r="K21" s="72">
-        <f>I19*(I20+J20)*2</f>
-        <v>0.57200000000000006</v>
-      </c>
-      <c r="L21" s="72"/>
-      <c r="M21" s="72"/>
-      <c r="N21" s="72">
-        <f>L19*(L20+M20)*2</f>
-        <v>0.88400000000000012</v>
-      </c>
-    </row>
-    <row r="22" spans="8:20" ht="14.4" thickBot="1">
-      <c r="H22" s="73" t="s">
-        <v>97</v>
-      </c>
-      <c r="I22" s="72"/>
-      <c r="J22" s="72"/>
-      <c r="K22" s="72"/>
-      <c r="L22" s="74">
-        <f>L20*M20/L18/M18</f>
-        <v>0.62834622248661509</v>
-      </c>
-      <c r="M22" s="72"/>
-      <c r="N22" s="72"/>
-    </row>
-    <row r="23" spans="8:20">
-      <c r="H23" s="75" t="s">
-        <v>99</v>
-      </c>
-      <c r="I23" s="72"/>
-      <c r="J23" s="72"/>
-      <c r="K23" s="72"/>
-      <c r="L23" s="76">
-        <f>N19/L20/M20</f>
-        <v>96.013166660135582</v>
-      </c>
-      <c r="M23" s="72"/>
-      <c r="N23" s="72"/>
-    </row>
-    <row r="24" spans="8:20" ht="14.4" thickBot="1">
-      <c r="H24" s="78"/>
-      <c r="I24" s="72"/>
-      <c r="J24" s="72"/>
-      <c r="K24" s="72"/>
-      <c r="L24" s="77"/>
-      <c r="M24" s="72"/>
-      <c r="N24" s="72"/>
-    </row>
-    <row r="25" spans="8:20">
-      <c r="H25" s="58"/>
-      <c r="I25" s="82" t="s">
-        <v>93</v>
-      </c>
-      <c r="J25" s="82"/>
-      <c r="K25" s="82"/>
-      <c r="L25" s="103" t="s">
-        <v>108</v>
-      </c>
-      <c r="M25" s="103"/>
-      <c r="N25" s="103"/>
-      <c r="O25" s="103" t="s">
+      <c r="M39" s="53"/>
+      <c r="N39" s="53">
+        <f>N22*(L40+M40)*2</f>
+        <v>140.99006622516558</v>
+      </c>
+      <c r="O39" s="53"/>
+      <c r="P39" s="53"/>
+      <c r="Q39" s="53"/>
+      <c r="R39" s="53"/>
+      <c r="S39" s="53"/>
+      <c r="T39" s="60"/>
+    </row>
+    <row r="40" spans="8:20">
+      <c r="H40" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="I40" s="53">
+        <f>K40/J40</f>
+        <v>0.85</v>
+      </c>
+      <c r="J40" s="53">
+        <v>2</v>
+      </c>
+      <c r="K40" s="53">
+        <v>1.7</v>
+      </c>
+      <c r="L40" s="53">
+        <f>N40/M40</f>
+        <v>0.85</v>
+      </c>
+      <c r="M40" s="53">
+        <v>2</v>
+      </c>
+      <c r="N40" s="53">
+        <v>1.7</v>
+      </c>
+      <c r="O40" s="53"/>
+      <c r="P40" s="53"/>
+      <c r="Q40" s="53"/>
+      <c r="R40" s="53"/>
+      <c r="S40" s="53"/>
+      <c r="T40" s="60"/>
+    </row>
+    <row r="41" spans="8:20">
+      <c r="H41" s="59" t="s">
+        <v>103</v>
+      </c>
+      <c r="I41" s="53"/>
+      <c r="J41" s="53"/>
+      <c r="K41" s="53">
+        <f>K38-K40</f>
+        <v>0.67540000000000044</v>
+      </c>
+      <c r="L41" s="53"/>
+      <c r="M41" s="53"/>
+      <c r="N41" s="53">
+        <f>N38-N40</f>
+        <v>1.0845999999999998</v>
+      </c>
+      <c r="O41" s="53"/>
+      <c r="P41" s="53"/>
+      <c r="Q41" s="53"/>
+      <c r="R41" s="53"/>
+      <c r="S41" s="53"/>
+      <c r="T41" s="60"/>
+    </row>
+    <row r="42" spans="8:20">
+      <c r="H42" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="P25" s="103"/>
-      <c r="Q25" s="103"/>
-      <c r="R25" s="59" t="s">
+      <c r="I42" s="53"/>
+      <c r="J42" s="53"/>
+      <c r="K42" s="53"/>
+      <c r="L42" s="78">
+        <f>L40*M40/L38/M38</f>
+        <v>0.61050061050061055</v>
+      </c>
+      <c r="M42" s="53"/>
+      <c r="N42" s="53"/>
+      <c r="O42" s="53"/>
+      <c r="P42" s="53"/>
+      <c r="Q42" s="53"/>
+      <c r="R42" s="53"/>
+      <c r="S42" s="53"/>
+      <c r="T42" s="60"/>
+    </row>
+    <row r="43" spans="8:20" ht="14.4" thickBot="1">
+      <c r="H43" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="S25" s="59"/>
-      <c r="T25" s="60"/>
-    </row>
-    <row r="26" spans="8:20">
-      <c r="H26" s="61"/>
-      <c r="I26" s="55" t="s">
-        <v>89</v>
-      </c>
-      <c r="J26" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="K26" s="55" t="s">
-        <v>109</v>
-      </c>
-      <c r="L26" s="55" t="s">
-        <v>89</v>
-      </c>
-      <c r="M26" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="N26" s="55" t="s">
-        <v>98</v>
-      </c>
-      <c r="O26" s="55" t="s">
-        <v>89</v>
-      </c>
-      <c r="P26" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q26" s="55" t="s">
-        <v>98</v>
-      </c>
-      <c r="R26" s="55" t="s">
-        <v>89</v>
-      </c>
-      <c r="S26" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="T26" s="62" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="27" spans="8:20">
-      <c r="H27" s="81" t="s">
-        <v>91</v>
-      </c>
-      <c r="I27" s="71">
-        <v>1.7</v>
-      </c>
-      <c r="J27" s="71">
-        <v>1</v>
-      </c>
-      <c r="K27" s="71">
-        <v>0.11</v>
-      </c>
-      <c r="L27" s="71">
-        <v>1.7</v>
-      </c>
-      <c r="M27" s="71">
-        <v>1</v>
-      </c>
-      <c r="N27" s="71">
-        <v>1.7</v>
-      </c>
-      <c r="O27" s="55"/>
-      <c r="P27" s="55"/>
-      <c r="Q27" s="55"/>
-      <c r="R27" s="55"/>
-      <c r="S27" s="55"/>
-      <c r="T27" s="62"/>
-    </row>
-    <row r="28" spans="8:20">
-      <c r="H28" s="81" t="s">
-        <v>90</v>
-      </c>
-      <c r="I28" s="71">
-        <f>I27+K27*2</f>
-        <v>1.92</v>
-      </c>
-      <c r="J28" s="71">
-        <f>J27+K27*2</f>
-        <v>1.22</v>
-      </c>
-      <c r="K28" s="71">
-        <f>I28*J28</f>
-        <v>2.3424</v>
-      </c>
-      <c r="L28" s="71">
-        <f>L27+L29*2</f>
-        <v>2.04</v>
-      </c>
-      <c r="M28" s="71">
-        <f>M27+L29*2</f>
-        <v>1.34</v>
-      </c>
-      <c r="N28" s="71">
-        <f>L28*M28</f>
-        <v>2.7336</v>
-      </c>
-      <c r="O28" s="55"/>
-      <c r="P28" s="55"/>
-      <c r="Q28" s="55"/>
-      <c r="R28" s="55"/>
-      <c r="S28" s="55"/>
-      <c r="T28" s="62"/>
-    </row>
-    <row r="29" spans="8:20">
-      <c r="H29" s="81" t="s">
-        <v>98</v>
-      </c>
-      <c r="J29" s="71"/>
-      <c r="K29" s="71">
-        <f>K23*(I28+J28)*2</f>
-        <v>0</v>
-      </c>
-      <c r="L29" s="71">
-        <v>0.17</v>
-      </c>
-      <c r="M29" s="71"/>
-      <c r="N29" s="71">
-        <f>N23*(L28+M28)*2</f>
-        <v>0</v>
-      </c>
-      <c r="O29" s="55"/>
-      <c r="P29" s="55"/>
-      <c r="Q29" s="55"/>
-      <c r="R29" s="55"/>
-      <c r="S29" s="55"/>
-      <c r="T29" s="62"/>
-    </row>
-    <row r="30" spans="8:20">
-      <c r="H30" s="81" t="s">
-        <v>106</v>
-      </c>
-      <c r="I30" s="71"/>
-      <c r="J30" s="71"/>
-      <c r="K30" s="71" t="e">
-        <f>K28-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L30" s="71"/>
-      <c r="M30" s="71"/>
-      <c r="N30" s="71">
-        <f>N28-N27</f>
-        <v>1.0336000000000001</v>
-      </c>
-      <c r="O30" s="55"/>
-      <c r="P30" s="55"/>
-      <c r="Q30" s="55"/>
-      <c r="R30" s="55"/>
-      <c r="S30" s="55"/>
-      <c r="T30" s="62"/>
-    </row>
-    <row r="31" spans="8:20">
-      <c r="H31" s="81" t="s">
-        <v>97</v>
-      </c>
-      <c r="I31" s="71"/>
-      <c r="J31" s="71"/>
-      <c r="K31" s="71"/>
-      <c r="L31" s="79">
-        <f>L27*M27/L28/M28</f>
-        <v>0.62189054726368154</v>
-      </c>
-      <c r="M31" s="71"/>
-      <c r="N31" s="71"/>
-      <c r="O31" s="55"/>
-      <c r="P31" s="55"/>
-      <c r="Q31" s="55"/>
-      <c r="R31" s="55"/>
-      <c r="S31" s="55"/>
-      <c r="T31" s="62"/>
-    </row>
-    <row r="32" spans="8:20">
-      <c r="H32" s="81" t="s">
-        <v>99</v>
-      </c>
-      <c r="I32" s="71"/>
-      <c r="J32" s="71"/>
-      <c r="K32" s="71"/>
-      <c r="L32" s="71">
-        <f>N29/L27/M27</f>
-        <v>0</v>
-      </c>
-      <c r="M32" s="71"/>
-      <c r="N32" s="71"/>
-      <c r="O32" s="55"/>
-      <c r="P32" s="55"/>
-      <c r="Q32" s="55"/>
-      <c r="R32" s="55"/>
-      <c r="S32" s="55"/>
-      <c r="T32" s="62"/>
-    </row>
-    <row r="33" spans="8:20">
-      <c r="H33" s="61" t="s">
-        <v>90</v>
-      </c>
-      <c r="I33" s="55">
-        <f>I35+I34*2</f>
-        <v>1.07</v>
-      </c>
-      <c r="J33" s="55">
-        <f>J35+I34*2</f>
-        <v>2.2200000000000002</v>
-      </c>
-      <c r="K33" s="55">
-        <f>I33*J33</f>
-        <v>2.3754000000000004</v>
-      </c>
-      <c r="L33" s="55">
-        <f>L35+L34*2</f>
-        <v>1.19</v>
-      </c>
-      <c r="M33" s="55">
-        <f>M35+L34*2</f>
-        <v>2.34</v>
-      </c>
-      <c r="N33" s="55">
-        <f>L33*M33</f>
-        <v>2.7845999999999997</v>
-      </c>
-      <c r="O33" s="55"/>
-      <c r="P33" s="55"/>
-      <c r="Q33" s="55"/>
-      <c r="R33" s="55"/>
-      <c r="S33" s="55"/>
-      <c r="T33" s="62"/>
-    </row>
-    <row r="34" spans="8:20">
-      <c r="H34" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="I34" s="55">
-        <v>0.11</v>
-      </c>
-      <c r="J34" s="55"/>
-      <c r="K34" s="55">
-        <f>K17*(I35+J35)*2</f>
-        <v>72.561349693251529</v>
-      </c>
-      <c r="L34" s="55">
-        <v>0.17</v>
-      </c>
-      <c r="M34" s="55"/>
-      <c r="N34" s="55">
-        <f>N17*(L35+M35)*2</f>
-        <v>140.99006622516558</v>
-      </c>
-      <c r="O34" s="55"/>
-      <c r="P34" s="55"/>
-      <c r="Q34" s="55"/>
-      <c r="R34" s="55"/>
-      <c r="S34" s="55"/>
-      <c r="T34" s="62"/>
-    </row>
-    <row r="35" spans="8:20">
-      <c r="H35" s="61" t="s">
-        <v>91</v>
-      </c>
-      <c r="I35" s="55">
-        <f>K35/J35</f>
-        <v>0.85</v>
-      </c>
-      <c r="J35" s="55">
-        <v>2</v>
-      </c>
-      <c r="K35" s="55">
-        <v>1.7</v>
-      </c>
-      <c r="L35" s="55">
-        <f>N35/M35</f>
-        <v>0.85</v>
-      </c>
-      <c r="M35" s="55">
-        <v>2</v>
-      </c>
-      <c r="N35" s="55">
-        <v>1.7</v>
-      </c>
-      <c r="O35" s="55"/>
-      <c r="P35" s="55"/>
-      <c r="Q35" s="55"/>
-      <c r="R35" s="55"/>
-      <c r="S35" s="55"/>
-      <c r="T35" s="62"/>
-    </row>
-    <row r="36" spans="8:20">
-      <c r="H36" s="61" t="s">
-        <v>106</v>
-      </c>
-      <c r="I36" s="55"/>
-      <c r="J36" s="55"/>
-      <c r="K36" s="55">
-        <f>K33-K35</f>
-        <v>0.67540000000000044</v>
-      </c>
-      <c r="L36" s="55"/>
-      <c r="M36" s="55"/>
-      <c r="N36" s="55">
-        <f>N33-N35</f>
-        <v>1.0845999999999998</v>
-      </c>
-      <c r="O36" s="55"/>
-      <c r="P36" s="55"/>
-      <c r="Q36" s="55"/>
-      <c r="R36" s="55"/>
-      <c r="S36" s="55"/>
-      <c r="T36" s="62"/>
-    </row>
-    <row r="37" spans="8:20">
-      <c r="H37" s="61" t="s">
-        <v>97</v>
-      </c>
-      <c r="I37" s="55"/>
-      <c r="J37" s="55"/>
-      <c r="K37" s="55"/>
-      <c r="L37" s="80">
-        <f>L35*M35/L33/M33</f>
-        <v>0.61050061050061055</v>
-      </c>
-      <c r="M37" s="55"/>
-      <c r="N37" s="55"/>
-      <c r="O37" s="55"/>
-      <c r="P37" s="55"/>
-      <c r="Q37" s="55"/>
-      <c r="R37" s="55"/>
-      <c r="S37" s="55"/>
-      <c r="T37" s="62"/>
-    </row>
-    <row r="38" spans="8:20" ht="14.4" thickBot="1">
-      <c r="H38" s="63" t="s">
-        <v>99</v>
-      </c>
-      <c r="I38" s="64"/>
-      <c r="J38" s="64"/>
-      <c r="K38" s="64"/>
-      <c r="L38" s="64">
-        <f>N34/L35/M35</f>
+      <c r="I43" s="62"/>
+      <c r="J43" s="62"/>
+      <c r="K43" s="62"/>
+      <c r="L43" s="62">
+        <f>N39/L40/M40</f>
         <v>82.935333073626808</v>
       </c>
-      <c r="M38" s="64"/>
-      <c r="N38" s="64"/>
-      <c r="O38" s="64"/>
-      <c r="P38" s="64"/>
-      <c r="Q38" s="64"/>
-      <c r="R38" s="64"/>
-      <c r="S38" s="64"/>
-      <c r="T38" s="65"/>
+      <c r="M43" s="62"/>
+      <c r="N43" s="62"/>
+      <c r="O43" s="62"/>
+      <c r="P43" s="62"/>
+      <c r="Q43" s="62"/>
+      <c r="R43" s="62"/>
+      <c r="S43" s="62"/>
+      <c r="T43" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="O25:Q25"/>
-    <mergeCell ref="L25:N25"/>
+    <mergeCell ref="O30:Q30"/>
+    <mergeCell ref="L30:N30"/>
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="L10:N10"/>
     <mergeCell ref="O10:Q10"/>

</xml_diff>

<commit_message>
style(HW and Parameter): Update Style for PPT
</commit_message>
<xml_diff>
--- a/hardware/docs/01-top/点云硬件参数分析.xlsx
+++ b/hardware/docs/01-top/点云硬件参数分析.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="12960" windowHeight="4872"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="12960" windowHeight="4872" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="整体评估" sheetId="5" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <author>作者</author>
   </authors>
   <commentList>
-    <comment ref="C12" authorId="0" shapeId="0">
+    <comment ref="C9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -49,6 +49,58 @@
           </rPr>
           <t xml:space="preserve">
 堪称恐怖</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+师姐100MHz综合前后90-50mW，我100MHz综合功耗63mW，后仿保守估计不变，200MHz120mW</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+总计算量为PointNeXt-S论文的TOPS</t>
         </r>
       </text>
     </comment>
@@ -78,7 +130,59 @@
         </r>
       </text>
     </comment>
-    <comment ref="C16" authorId="0" shapeId="0">
+    <comment ref="A15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+PointNeXt-S总周期为FPS 3k的3倍9k</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A16" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+总时间计算的有效算力</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -104,33 +208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B19" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">
-师姐100MHz综合前后90-50mW，我100MHz综合功耗63mW，后仿保守估计不变，200MHz120mW</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B21" authorId="0" shapeId="0">
+    <comment ref="B25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -390,7 +468,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="120">
   <si>
     <t>case</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -623,10 +701,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>130KB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>On-Chip SRAM</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -651,14 +725,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PCNA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Parameters</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Top Level Module</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -703,30 +769,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>面积 (um2)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>uhddpsram</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>深度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>宽度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>宽</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -812,117 +858,6 @@
   </si>
   <si>
     <t>Power Consumption (W)@ 200MHz</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>总时间计算的有效算力</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>总计算量为</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>PointNeXt-S</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>论文的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>TOPS</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>PointNeXt-S</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>总周期为</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>FPS 3k</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>倍</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>9k</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t/>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -998,165 +933,80 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>密度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>容量(KB)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TSMC 28-nm HPC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>    CCUFPS_CfgMaskBaseAddr ,</t>
-  </si>
-  <si>
-    <t>    CCUFPS_CfgDistBaseAddr ,</t>
-  </si>
-  <si>
-    <t>    CCUITF_DRAMBaseAddr     [GLBWRIDX_ITFCRD                 ]  ,</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortBankFlag  [GLBWRIDX_ITFCRD                 ]  ,</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortBankFlag  [GLB_NUM_WRPORT + GLBRDIDX_FPSCRD]  ,</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortBankFlag  [GLBWRIDX_FPSMSK                 ]  ,</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortBankFlag  [GLB_NUM_WRPORT + GLBRDIDX_FPSMSK]  ,</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortBankFlag  [GLBWRIDX_FPSDST                 ]  ,</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortBankFlag  [GLB_NUM_WRPORT + GLBRDIDX_FPSDST]  ,</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortBankFlag  [GLBWRIDX_FPSIDX                 ]  ,</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortBankFlag  [GLB_NUM_WRPORT + GLBRDIDX_ITFIDX]  ,</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortBankFlag  [GLBWRIDX_FPSCRD                 ]  ,</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortParBank     [GLBWRIDX_ITFCRD                 ],</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortParBank     [GLB_NUM_WRPORT + GLBRDIDX_FPSCRD],</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortParBank     [GLBWRIDX_FPSMSK                 ],</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortParBank     [GLB_NUM_WRPORT + GLBRDIDX_FPSMSK],</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortParBank     [GLBWRIDX_FPSDST                 ],</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortParBank     [GLB_NUM_WRPORT + GLBRDIDX_FPSDST],</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortParBank     [GLBWRIDX_FPSIDX                 ],</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortParBank     [GLB_NUM_WRPORT + GLBRDIDX_ITFIDX],</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortParBank     [GLBWRIDX_FPSCRD                 ],</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortOffEmptyFull[GLBWRIDX_ITFCRD                 ],</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortOffEmptyFull[GLB_NUM_WRPORT + GLBRDIDX_FPSCRD],</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortOffEmptyFull[GLBWRIDX_FPSMSK                 ],</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortOffEmptyFull[GLB_NUM_WRPORT + GLBRDIDX_FPSMSK],</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortOffEmptyFull[GLBWRIDX_FPSDST                 ],</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortOffEmptyFull[GLB_NUM_WRPORT + GLBRDIDX_FPSDST],</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortOffEmptyFull[GLBWRIDX_FPSIDX                 ],</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortOffEmptyFull[GLB_NUM_WRPORT + GLBRDIDX_ITFIDX],</t>
-  </si>
-  <si>
-    <t>    CCUTOP_CfgPortOffEmptyFull[GLBWRIDX_FPSCRD                 ]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    CCUPOL_CfgNip                                                                   ,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    CCUPOL_CfgChn                                                                   ,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    CCUPOL_CfgK                                                                     ,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    CCUITF_DRAMBaseAddr   [GLBWRIDX_ITFMAP                 ]                        ,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    CCUTOP_CfgPortBankFlag[GLBWRIDX_ITFMAP                 ]                        ,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    CCUTOP_CfgPortBankFlag[GLB_NUM_WRPORT + GLBRDIDX_POLMAP]                        ,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    CCUTOP_CfgPortBankFlag[GLBWRIDX_POLOFM                 ]                        ,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    CCUTOP_CfgPortBankFlag[GLB_NUM_WRPORT + GLBRDIDX_POLOFM]                        ,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    CCUTOP_CfgPortBankFlag[GLB_NUM_WRPORT + GLBRDIDX_POLOFM +: NUM_BANK*POOL_CORE]  ,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    CCUTOP_CfgPortParBank [GLBWRIDX_ITFMAP                 ]                        ,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    CCUTOP_CfgPortParBank [GLB_NUM_WRPORT + GLBRDIDX_POLMAP]                        ,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    CCUTOP_CfgPortParBank [GLBWRIDX_POLOFM                 ]                        ,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    CCUTOP_CfgPortParBank [GLB_NUM_WRPORT + GLBRDIDX_POLOFM +: MAXPAR_WIDTH*POOL_CORE],</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    CCUTOP_CfgPortOffEmptyFull [GLBWRIDX_ITFMAP                 ]                   ,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    CCUTOP_CfgPortOffEmptyFull [GLB_NUM_WRPORT + GLBRDIDX_POLMAP]                   ,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    CCUTOP_CfgPortOffEmptyFull [GLBWRIDX_POLOFM                 ]                   ,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    CCUTOP_CfgPortOffEmptyFull [GLB_NUM_WRPORT + GLBRDIDX_POLOFM +: POOL_CORE]</t>
+    <t>28 nm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Proposed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>128KB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TOP (PointNeXt-S)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inference Time (Cycles)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Effective Energy Efficiency (TOPS/W)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Speedup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Word</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IO bit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Size (KB)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Area (um2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Density (bit/um2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="5">
     <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="177" formatCode="0.0000_ "/>
+    <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="179" formatCode="0.0_ "/>
+    <numFmt numFmtId="180" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -1306,7 +1156,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -1577,7 +1427,101 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
@@ -1589,109 +1533,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -1729,7 +1570,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1881,30 +1722,29 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1912,31 +1752,78 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1944,83 +1831,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="180" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2301,50 +2135,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="32.109375" style="29" customWidth="1"/>
+    <col min="1" max="1" width="56.44140625" style="29" customWidth="1"/>
     <col min="2" max="2" width="25.33203125" style="29" customWidth="1"/>
     <col min="3" max="3" width="25.44140625" style="29" customWidth="1"/>
     <col min="4" max="16384" width="8.88671875" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="39" t="s">
-        <v>68</v>
-      </c>
+      <c r="A1" s="39"/>
       <c r="B1" s="41" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D1" s="30"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" s="44">
-        <v>28</v>
+        <v>104</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>105</v>
       </c>
       <c r="D2" s="30"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" s="45">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C3" s="44">
         <v>12.96</v>
@@ -2353,45 +2185,41 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="45">
-        <v>96</v>
+        <v>140</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4" s="30"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="45" t="s">
-        <v>60</v>
+        <v>107</v>
       </c>
       <c r="C5" s="44" t="s">
         <v>59</v>
       </c>
       <c r="D5" s="30"/>
-      <c r="G5" s="96" t="s">
-        <v>118</v>
-      </c>
+      <c r="G5" s="90"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="35" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B6" s="45">
         <v>0.9</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D6" s="30"/>
-      <c r="G6" s="96" t="s">
-        <v>119</v>
-      </c>
+      <c r="G6" s="90"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="35" t="s">
@@ -2404,11 +2232,9 @@
         <v>250</v>
       </c>
       <c r="D7" s="30"/>
-      <c r="G7" s="96" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="G7" s="90"/>
+    </row>
+    <row r="8" spans="1:7" ht="14.4" thickBot="1">
       <c r="A8" s="35" t="s">
         <v>57</v>
       </c>
@@ -2419,501 +2245,226 @@
         <v>55</v>
       </c>
       <c r="D8" s="30"/>
-      <c r="G8" s="96" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="14.4" thickBot="1">
-      <c r="A9" s="32" t="s">
+      <c r="G8" s="90"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="41">
+        <v>1024</v>
+      </c>
+      <c r="C9" s="50">
+        <v>12288</v>
+      </c>
+      <c r="D9" s="30"/>
+      <c r="G9" s="90"/>
+    </row>
+    <row r="10" spans="1:7" ht="14.4" thickBot="1">
+      <c r="A10" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B10" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C10" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="30"/>
-      <c r="G9" s="96" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="97" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="98"/>
-      <c r="C10" s="99"/>
       <c r="D10" s="30"/>
-      <c r="G10" s="96" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1">
-      <c r="A11" s="83" t="s">
-        <v>109</v>
-      </c>
-      <c r="B11" s="81">
+      <c r="G10" s="90"/>
+    </row>
+    <row r="11" spans="1:7" ht="14.4" thickBot="1">
+      <c r="A11" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="36">
+        <v>0.15</v>
+      </c>
+      <c r="C11" s="33">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="D11" s="30"/>
+      <c r="G11" s="90"/>
+    </row>
+    <row r="12" spans="1:7" ht="14.4" thickBot="1">
+      <c r="A12" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="110">
         <f>3.6/1024</f>
         <v>3.5156250000000001E-3</v>
       </c>
-      <c r="C11" s="82"/>
-      <c r="D11" s="30"/>
-      <c r="G11" s="96" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="14.4" thickBot="1">
-      <c r="A12" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="41">
-        <v>1024</v>
-      </c>
-      <c r="C12" s="50">
-        <v>12288</v>
+      <c r="C12" s="91" t="s">
+        <v>112</v>
       </c>
       <c r="D12" s="30"/>
-      <c r="G12" s="96" t="s">
-        <v>125</v>
-      </c>
+      <c r="G12" s="90"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="39" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B13" s="38">
-        <f>B12*B7*2/1024/1024</f>
+        <f>B9*B7*2/1024/1024</f>
         <v>0.390625</v>
       </c>
       <c r="C13" s="37">
-        <f>C12*C7*2/1024/1024</f>
+        <f>C9*C7*2/1024/1024</f>
         <v>5.859375</v>
       </c>
       <c r="D13" s="30"/>
-      <c r="G13" s="96" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="14.4">
+      <c r="G13" s="90"/>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="B14" s="84">
+        <v>73</v>
+      </c>
+      <c r="B14" s="34">
+        <f>B13/B11</f>
+        <v>2.604166666666667</v>
+      </c>
+      <c r="C14" s="49">
+        <f>C13/C11</f>
+        <v>9.6213054187192117</v>
+      </c>
+      <c r="D14" s="30"/>
+      <c r="G14" s="90"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="111">
         <f>9*1024</f>
         <v>9216</v>
       </c>
-      <c r="C14" s="85"/>
-      <c r="D14" s="30"/>
-      <c r="G14" s="96" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="14.4">
-      <c r="A15" s="86" t="s">
-        <v>108</v>
-      </c>
-      <c r="B15" s="87">
-        <f>B11/(B14*5*10^(-9))</f>
+      <c r="C15" s="80" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" s="30"/>
+      <c r="G15" s="90"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="81">
+        <f>B12/(B15*5*10^(-9))</f>
         <v>76.293945312499986</v>
       </c>
-      <c r="C15" s="85"/>
-      <c r="D15" s="30"/>
-      <c r="G15" s="96" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="14.4">
-      <c r="A16" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="B16" s="34">
+      <c r="C16" s="80">
+        <f>C23/C11</f>
+        <v>19.047619047619047</v>
+      </c>
+      <c r="D16" s="30"/>
+      <c r="G16" s="90"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" s="112">
+        <f>B16/B14</f>
+        <v>29.296874999999993</v>
+      </c>
+      <c r="C17" s="109">
+        <f>C16/C14</f>
+        <v>1.9797333333333333</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="35"/>
+    </row>
+    <row r="21" spans="1:7" ht="14.4" thickBot="1">
+      <c r="A21" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32">
+        <f>C25/4*(1.1/0.9)^2</f>
+        <v>7.1134626690182259</v>
+      </c>
+      <c r="G21" s="90"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="29">
+        <f>B24/B13</f>
+        <v>40</v>
+      </c>
+      <c r="G22" s="90"/>
+    </row>
+    <row r="23" spans="1:7" ht="14.4">
+      <c r="A23" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" s="34">
         <f>B13*10</f>
         <v>3.90625</v>
       </c>
-      <c r="C16" s="49">
+      <c r="C23" s="49">
         <v>11.6</v>
       </c>
-      <c r="D16" s="30"/>
-      <c r="G16" s="96" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="B17" s="34">
-        <f>B16*4</f>
+      <c r="D23" s="30"/>
+      <c r="G23" s="90"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="34">
+        <f>B23*4</f>
         <v>15.625</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="30"/>
-      <c r="G17" s="96" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="30"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="30"/>
-      <c r="G18" s="96" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="35" t="s">
-        <v>107</v>
-      </c>
-      <c r="B19" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="C19" s="33">
-        <v>0.60899999999999999</v>
-      </c>
-      <c r="D19" s="30"/>
-      <c r="G19" s="96" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="34">
-        <f>B13/B19</f>
-        <v>2.604166666666667</v>
-      </c>
-      <c r="C20" s="49">
-        <f>C13/C19</f>
-        <v>9.6213054187192117</v>
-      </c>
-      <c r="D20" s="30"/>
-      <c r="G20" s="96" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="14.4" thickBot="1">
-      <c r="A21" s="32" t="s">
+      <c r="C24" s="49"/>
+      <c r="D24" s="30"/>
+      <c r="G24" s="90"/>
+    </row>
+    <row r="25" spans="1:7" ht="14.4" thickBot="1">
+      <c r="A25" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="48">
-        <f>B17/B19</f>
+      <c r="B25" s="48">
+        <f>B24/B11</f>
         <v>104.16666666666667</v>
       </c>
-      <c r="C21" s="31">
-        <f>C16/C19</f>
+      <c r="C25" s="31">
+        <f>C23/C11</f>
         <v>19.047619047619047</v>
       </c>
-      <c r="D21" s="30"/>
-      <c r="G21" s="96" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="14.4" thickBot="1">
-      <c r="A22" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32">
-        <f>C21/4*(1.1/0.9)^2</f>
-        <v>7.1134626690182259</v>
-      </c>
-      <c r="G22" s="96" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="B23" s="29">
-        <f>B17/B13</f>
-        <v>40</v>
-      </c>
-      <c r="G23" s="96" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="G24" s="96" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="G25" s="96" t="s">
-        <v>138</v>
-      </c>
+      <c r="D25" s="30"/>
+      <c r="G25" s="90"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="G26" s="96" t="s">
-        <v>139</v>
-      </c>
+      <c r="G26" s="90"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="G27" s="96" t="s">
-        <v>140</v>
-      </c>
+      <c r="G27" s="90"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="G28" s="96" t="s">
-        <v>141</v>
-      </c>
+      <c r="G28" s="90"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="G29" s="96" t="s">
-        <v>142</v>
-      </c>
+      <c r="G29" s="90"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="G30" s="96" t="s">
-        <v>143</v>
-      </c>
+      <c r="G30" s="90"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="G31" s="96" t="s">
-        <v>144</v>
-      </c>
+      <c r="G31" s="90"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="G32" s="96" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="G33" s="96" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="G34" s="96" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="29">
-        <v>33</v>
-      </c>
-      <c r="B40" s="29" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="29">
-        <v>32</v>
-      </c>
-      <c r="B41" s="29" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="29">
-        <v>31</v>
-      </c>
-      <c r="B42" s="29" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="29">
-        <v>30</v>
-      </c>
-      <c r="B43" s="29" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="29">
-        <v>29</v>
-      </c>
-      <c r="B44" s="29" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="29">
-        <v>28</v>
-      </c>
-      <c r="B45" s="29" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="29">
-        <v>27</v>
-      </c>
-      <c r="B46" s="29" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="29">
-        <v>26</v>
-      </c>
-      <c r="B47" s="29" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="29">
-        <v>25</v>
-      </c>
-      <c r="B48" s="29" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="29">
-        <v>24</v>
-      </c>
-      <c r="B49" s="29" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="29">
-        <v>23</v>
-      </c>
-      <c r="B50" s="29" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="29">
-        <v>22</v>
-      </c>
-      <c r="B51" s="29" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="29">
-        <v>21</v>
-      </c>
-      <c r="B52" s="29" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="29">
-        <v>20</v>
-      </c>
-      <c r="B53" s="29" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="29">
-        <v>19</v>
-      </c>
-      <c r="B54" s="29" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="29">
-        <v>18</v>
-      </c>
-      <c r="B55" s="29" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="29">
-        <v>17</v>
-      </c>
-      <c r="B56" s="29" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="29">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="29">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="29">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="29">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="29">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="29">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="29">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="29">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1">
-      <c r="A65" s="29">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" s="29">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1">
-      <c r="A67" s="29">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1">
-      <c r="A68" s="29">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1">
-      <c r="A69" s="29">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1">
-      <c r="A70" s="29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1">
-      <c r="A71" s="29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72" s="29">
-        <v>1</v>
-      </c>
+      <c r="G32" s="90"/>
+    </row>
+    <row r="33" spans="7:7">
+      <c r="G33" s="90"/>
     </row>
   </sheetData>
   <sortState ref="A40:G72">
     <sortCondition descending="1" ref="A40:A72"/>
   </sortState>
-  <mergeCells count="1">
-    <mergeCell ref="A10:C10"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2926,10 +2477,10 @@
   <dimension ref="A1:T60"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="P16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="O4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E31" sqref="E31"/>
+      <selection pane="bottomRight" activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.77734375" defaultRowHeight="13.8"/>
@@ -2950,26 +2501,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="E1" s="65"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="100" t="s">
-        <v>97</v>
-      </c>
-      <c r="K1" s="101"/>
-      <c r="L1" s="101"/>
-      <c r="M1" s="101"/>
-      <c r="N1" s="101"/>
-      <c r="O1" s="102"/>
-      <c r="P1" s="103" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q1" s="101"/>
-      <c r="R1" s="101"/>
-      <c r="S1" s="101"/>
-      <c r="T1" s="102"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="92" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="93"/>
+      <c r="N1" s="93"/>
+      <c r="O1" s="94"/>
+      <c r="P1" s="95" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q1" s="93"/>
+      <c r="R1" s="93"/>
+      <c r="S1" s="93"/>
+      <c r="T1" s="94"/>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="1" t="s">
@@ -2979,14 +2530,14 @@
       <c r="C2" s="1"/>
       <c r="D2" s="6"/>
       <c r="E2" s="24"/>
-      <c r="F2" s="107">
+      <c r="F2" s="99">
         <v>0</v>
       </c>
-      <c r="G2" s="108"/>
-      <c r="H2" s="107">
+      <c r="G2" s="100"/>
+      <c r="H2" s="99">
         <v>1</v>
       </c>
-      <c r="I2" s="108"/>
+      <c r="I2" s="100"/>
       <c r="J2" s="8">
         <v>2</v>
       </c>
@@ -2997,6 +2548,9 @@
         <v>4</v>
       </c>
       <c r="P2" s="2">
+        <v>1</v>
+      </c>
+      <c r="R2" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3008,18 +2562,18 @@
       <c r="C3" s="1"/>
       <c r="D3" s="6"/>
       <c r="E3" s="25"/>
-      <c r="F3" s="100" t="s">
+      <c r="F3" s="92" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="109"/>
-      <c r="H3" s="100" t="s">
+      <c r="G3" s="101"/>
+      <c r="H3" s="92" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="109"/>
-      <c r="J3" s="100" t="s">
+      <c r="I3" s="101"/>
+      <c r="J3" s="92" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="102"/>
+      <c r="K3" s="94"/>
       <c r="L3" s="2" t="s">
         <v>41</v>
       </c>
@@ -3027,7 +2581,7 @@
         <v>48</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -3053,7 +2607,7 @@
         <v>47</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -3125,26 +2679,26 @@
     <row r="8" spans="1:20">
       <c r="A8" s="46"/>
       <c r="B8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="N8" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="O8" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="104" t="s">
+      <c r="A9" s="96" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -3172,7 +2726,7 @@
       </c>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="105"/>
+      <c r="A10" s="97"/>
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
@@ -3198,7 +2752,7 @@
       </c>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11" s="105"/>
+      <c r="A11" s="97"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
         <v>15</v>
@@ -3221,7 +2775,7 @@
       </c>
     </row>
     <row r="12" spans="1:20">
-      <c r="A12" s="105"/>
+      <c r="A12" s="97"/>
       <c r="B12" s="1"/>
       <c r="C12" s="3"/>
       <c r="D12" s="11" t="s">
@@ -3233,7 +2787,7 @@
       </c>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="105"/>
+      <c r="A13" s="97"/>
       <c r="B13" s="1"/>
       <c r="C13" s="3"/>
       <c r="E13" s="19" t="s">
@@ -3248,7 +2802,7 @@
       </c>
     </row>
     <row r="14" spans="1:20">
-      <c r="A14" s="105"/>
+      <c r="A14" s="97"/>
       <c r="B14" s="1"/>
       <c r="C14" s="3"/>
       <c r="E14" s="19" t="s">
@@ -3262,7 +2816,7 @@
       </c>
     </row>
     <row r="15" spans="1:20">
-      <c r="A15" s="105"/>
+      <c r="A15" s="97"/>
       <c r="B15" s="1"/>
       <c r="C15" s="3"/>
       <c r="D15" s="19"/>
@@ -3270,7 +2824,7 @@
       <c r="H15" s="15"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="105"/>
+      <c r="A16" s="97"/>
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
         <v>16</v>
@@ -3293,14 +2847,14 @@
       </c>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="105"/>
+      <c r="A17" s="97"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="6"/>
       <c r="E17" s="25"/>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" s="105"/>
+      <c r="A18" s="97"/>
       <c r="B18" s="1" t="s">
         <v>10</v>
       </c>
@@ -3333,7 +2887,7 @@
       </c>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" s="105"/>
+      <c r="A19" s="97"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
         <v>17</v>
@@ -3359,7 +2913,7 @@
       </c>
     </row>
     <row r="20" spans="1:16">
-      <c r="A20" s="105"/>
+      <c r="A20" s="97"/>
       <c r="B20" s="1"/>
       <c r="C20" s="2" t="s">
         <v>39</v>
@@ -3370,7 +2924,7 @@
       </c>
     </row>
     <row r="21" spans="1:16">
-      <c r="A21" s="105"/>
+      <c r="A21" s="97"/>
       <c r="B21" s="1"/>
       <c r="C21" s="2" t="s">
         <v>40</v>
@@ -3381,7 +2935,7 @@
       </c>
     </row>
     <row r="22" spans="1:16">
-      <c r="A22" s="105"/>
+      <c r="A22" s="97"/>
       <c r="B22" s="1" t="s">
         <v>13</v>
       </c>
@@ -3411,7 +2965,7 @@
       </c>
     </row>
     <row r="23" spans="1:16">
-      <c r="A23" s="105"/>
+      <c r="A23" s="97"/>
       <c r="B23" s="1"/>
       <c r="C23" s="2" t="s">
         <v>18</v>
@@ -3432,7 +2986,7 @@
       </c>
     </row>
     <row r="24" spans="1:16">
-      <c r="A24" s="105"/>
+      <c r="A24" s="97"/>
       <c r="B24" s="1"/>
       <c r="D24" s="7" t="s">
         <v>43</v>
@@ -3447,7 +3001,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" ht="27.6">
-      <c r="A25" s="105"/>
+      <c r="A25" s="97"/>
       <c r="B25" s="1"/>
       <c r="E25" s="7" t="s">
         <v>42</v>
@@ -3462,7 +3016,7 @@
       </c>
     </row>
     <row r="26" spans="1:16">
-      <c r="A26" s="105"/>
+      <c r="A26" s="97"/>
       <c r="B26" s="1"/>
       <c r="C26" s="2" t="s">
         <v>19</v>
@@ -3479,7 +3033,7 @@
       </c>
     </row>
     <row r="27" spans="1:16">
-      <c r="A27" s="105"/>
+      <c r="A27" s="97"/>
       <c r="B27" s="1"/>
       <c r="C27" s="2" t="s">
         <v>20</v>
@@ -3493,7 +3047,7 @@
       </c>
     </row>
     <row r="28" spans="1:16">
-      <c r="A28" s="105"/>
+      <c r="A28" s="97"/>
       <c r="B28" s="1" t="s">
         <v>9</v>
       </c>
@@ -3523,7 +3077,7 @@
       </c>
     </row>
     <row r="29" spans="1:16">
-      <c r="A29" s="105"/>
+      <c r="A29" s="97"/>
       <c r="B29" s="1"/>
       <c r="C29" s="2" t="s">
         <v>21</v>
@@ -3543,7 +3097,7 @@
       </c>
     </row>
     <row r="30" spans="1:16">
-      <c r="A30" s="105"/>
+      <c r="A30" s="97"/>
       <c r="B30" s="1"/>
       <c r="C30" s="2" t="s">
         <v>22</v>
@@ -3556,7 +3110,7 @@
       </c>
     </row>
     <row r="31" spans="1:16">
-      <c r="A31" s="105"/>
+      <c r="A31" s="97"/>
       <c r="B31" s="1" t="s">
         <v>8</v>
       </c>
@@ -3583,7 +3137,7 @@
       </c>
     </row>
     <row r="32" spans="1:16">
-      <c r="A32" s="106"/>
+      <c r="A32" s="98"/>
       <c r="B32" s="1" t="s">
         <v>11</v>
       </c>
@@ -3686,7 +3240,7 @@
       </c>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="104" t="s">
+      <c r="A38" s="96" t="s">
         <v>24</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -3702,7 +3256,7 @@
       </c>
     </row>
     <row r="39" spans="1:14">
-      <c r="A39" s="105"/>
+      <c r="A39" s="97"/>
       <c r="B39" s="1" t="s">
         <v>12</v>
       </c>
@@ -3718,14 +3272,14 @@
       </c>
     </row>
     <row r="40" spans="1:14">
-      <c r="A40" s="105"/>
+      <c r="A40" s="97"/>
       <c r="B40" s="1"/>
       <c r="C40" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:14">
-      <c r="A41" s="105"/>
+      <c r="A41" s="97"/>
       <c r="B41" s="1"/>
       <c r="C41" s="3"/>
       <c r="D41" s="11" t="s">
@@ -3733,7 +3287,7 @@
       </c>
     </row>
     <row r="42" spans="1:14">
-      <c r="A42" s="105"/>
+      <c r="A42" s="97"/>
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
       <c r="E42" s="19" t="s">
@@ -3741,7 +3295,7 @@
       </c>
     </row>
     <row r="43" spans="1:14">
-      <c r="A43" s="105"/>
+      <c r="A43" s="97"/>
       <c r="B43" s="1"/>
       <c r="C43" s="3"/>
       <c r="E43" s="19" t="s">
@@ -3749,28 +3303,28 @@
       </c>
     </row>
     <row r="44" spans="1:14">
-      <c r="A44" s="105"/>
+      <c r="A44" s="97"/>
       <c r="B44" s="1"/>
       <c r="C44" s="3"/>
       <c r="D44" s="19"/>
       <c r="E44" s="27"/>
     </row>
     <row r="45" spans="1:14">
-      <c r="A45" s="105"/>
+      <c r="A45" s="97"/>
       <c r="B45" s="1"/>
       <c r="C45" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:14">
-      <c r="A46" s="105"/>
+      <c r="A46" s="97"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="6"/>
       <c r="E46" s="25"/>
     </row>
     <row r="47" spans="1:14">
-      <c r="A47" s="105"/>
+      <c r="A47" s="97"/>
       <c r="B47" s="1" t="s">
         <v>10</v>
       </c>
@@ -3786,7 +3340,7 @@
       </c>
     </row>
     <row r="48" spans="1:14">
-      <c r="A48" s="106"/>
+      <c r="A48" s="98"/>
       <c r="B48" s="1"/>
       <c r="C48" s="2" t="s">
         <v>17</v>
@@ -3918,8 +3472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3927,33 +3481,34 @@
     <col min="1" max="1" width="13.5546875" customWidth="1"/>
     <col min="2" max="4" width="11.21875" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
     <col min="8" max="8" width="12.21875" customWidth="1"/>
     <col min="11" max="11" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="B1" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="C1" t="s">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="D1" t="s">
         <v>116</v>
       </c>
       <c r="E1" t="s">
-        <v>82</v>
+        <v>117</v>
       </c>
       <c r="F1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="B2">
         <v>2048</v>
@@ -3968,14 +3523,14 @@
       <c r="E2">
         <v>6750</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="113">
         <f>(B2*C2)/E2</f>
         <v>0.3034074074074074</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B3">
         <v>32</v>
@@ -3990,14 +3545,14 @@
       <c r="E3">
         <v>2762</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="113">
         <f t="shared" ref="F3:F17" si="1">(B3*C3)/E3</f>
         <v>0.18537291817523532</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B4">
         <v>32</v>
@@ -4012,14 +3567,14 @@
       <c r="E4">
         <v>15180</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="113">
         <f t="shared" si="1"/>
         <v>0.26982872200263502</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B5">
         <v>64</v>
@@ -4034,14 +3589,14 @@
       <c r="E5">
         <v>15867</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="113">
         <f t="shared" si="1"/>
         <v>0.51629167454465241</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B6">
         <v>64</v>
@@ -4056,14 +3611,14 @@
       <c r="E6">
         <v>8451</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="113">
         <f t="shared" si="1"/>
         <v>0.48467636966039523</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B7">
         <v>128</v>
@@ -4078,14 +3633,14 @@
       <c r="E7">
         <v>9182</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="113">
         <f t="shared" si="1"/>
         <v>0.89218035286429975</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B8">
         <v>4096</v>
@@ -4100,14 +3655,14 @@
       <c r="E8">
         <v>118814</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="113">
         <f t="shared" si="1"/>
         <v>4.4126786405642431</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="14.4" thickBot="1">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B9">
         <v>1024</v>
@@ -4122,14 +3677,14 @@
       <c r="E9">
         <v>8301</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="113">
         <f t="shared" si="1"/>
         <v>3.947476207685821</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="14.4" thickBot="1">
       <c r="A10" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B10">
         <v>512</v>
@@ -4144,35 +3699,35 @@
       <c r="E10">
         <v>8726</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="113">
         <f t="shared" si="1"/>
         <v>3.7552143020857209</v>
       </c>
-      <c r="H10" s="54"/>
-      <c r="I10" s="111" t="s">
-        <v>90</v>
-      </c>
-      <c r="J10" s="112"/>
-      <c r="K10" s="113"/>
-      <c r="L10" s="114" t="s">
-        <v>92</v>
-      </c>
-      <c r="M10" s="115"/>
-      <c r="N10" s="116"/>
-      <c r="O10" s="114" t="s">
-        <v>91</v>
-      </c>
-      <c r="P10" s="115"/>
-      <c r="Q10" s="116"/>
-      <c r="R10" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="S10" s="57"/>
-      <c r="T10" s="58"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="103" t="s">
+        <v>82</v>
+      </c>
+      <c r="J10" s="104"/>
+      <c r="K10" s="105"/>
+      <c r="L10" s="106" t="s">
+        <v>84</v>
+      </c>
+      <c r="M10" s="107"/>
+      <c r="N10" s="108"/>
+      <c r="O10" s="106" t="s">
+        <v>83</v>
+      </c>
+      <c r="P10" s="107"/>
+      <c r="Q10" s="108"/>
+      <c r="R10" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="S10" s="56"/>
+      <c r="T10" s="57"/>
     </row>
     <row r="11" spans="1:20" ht="14.4" thickBot="1">
       <c r="A11" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B11">
         <v>1024</v>
@@ -4187,27 +3742,27 @@
       <c r="E11">
         <v>14726</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="113">
         <f t="shared" si="1"/>
         <v>4.45035990764634</v>
       </c>
-      <c r="H11" s="54"/>
-      <c r="I11" s="88"/>
-      <c r="J11" s="89"/>
-      <c r="K11" s="90"/>
-      <c r="L11" s="91"/>
-      <c r="M11" s="92"/>
-      <c r="N11" s="95"/>
-      <c r="O11" s="91"/>
-      <c r="P11" s="92"/>
-      <c r="Q11" s="95"/>
-      <c r="R11" s="56"/>
-      <c r="S11" s="57"/>
-      <c r="T11" s="94"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="83"/>
+      <c r="K11" s="84"/>
+      <c r="L11" s="85"/>
+      <c r="M11" s="86"/>
+      <c r="N11" s="89"/>
+      <c r="O11" s="85"/>
+      <c r="P11" s="86"/>
+      <c r="Q11" s="89"/>
+      <c r="R11" s="55"/>
+      <c r="S11" s="56"/>
+      <c r="T11" s="88"/>
     </row>
     <row r="12" spans="1:20" ht="14.4" thickBot="1">
       <c r="A12" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B12">
         <v>2048</v>
@@ -4222,27 +3777,27 @@
       <c r="E12">
         <v>27288</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="113">
         <f t="shared" si="1"/>
         <v>4.8032834945763705</v>
       </c>
-      <c r="H12" s="54"/>
-      <c r="I12" s="88"/>
-      <c r="J12" s="89"/>
-      <c r="K12" s="90"/>
-      <c r="L12" s="91"/>
-      <c r="M12" s="92"/>
-      <c r="N12" s="95"/>
-      <c r="O12" s="91"/>
-      <c r="P12" s="92"/>
-      <c r="Q12" s="95"/>
-      <c r="R12" s="56"/>
-      <c r="S12" s="57"/>
-      <c r="T12" s="94"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="82"/>
+      <c r="J12" s="83"/>
+      <c r="K12" s="84"/>
+      <c r="L12" s="85"/>
+      <c r="M12" s="86"/>
+      <c r="N12" s="89"/>
+      <c r="O12" s="85"/>
+      <c r="P12" s="86"/>
+      <c r="Q12" s="89"/>
+      <c r="R12" s="55"/>
+      <c r="S12" s="56"/>
+      <c r="T12" s="88"/>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B13">
         <v>256</v>
@@ -4257,51 +3812,51 @@
       <c r="E13">
         <v>10836</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="113">
         <f t="shared" si="1"/>
         <v>3.0239940937615355</v>
       </c>
-      <c r="H13" s="54"/>
-      <c r="I13" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="J13" s="57" t="s">
-        <v>104</v>
-      </c>
-      <c r="K13" s="58" t="s">
-        <v>95</v>
-      </c>
-      <c r="L13" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="M13" s="57" t="s">
-        <v>104</v>
-      </c>
-      <c r="N13" s="60" t="s">
-        <v>95</v>
-      </c>
-      <c r="O13" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="P13" s="57" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q13" s="60" t="s">
-        <v>95</v>
-      </c>
-      <c r="R13" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="S13" s="57" t="s">
-        <v>104</v>
-      </c>
-      <c r="T13" s="60" t="s">
-        <v>95</v>
+      <c r="H13" s="53"/>
+      <c r="I13" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="J13" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="K13" s="57" t="s">
+        <v>87</v>
+      </c>
+      <c r="L13" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="M13" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="N13" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="O13" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="P13" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q13" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="R13" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="S13" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="T13" s="59" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B14">
         <v>512</v>
@@ -4316,27 +3871,27 @@
       <c r="E14">
         <v>16342</v>
       </c>
-      <c r="F14" s="51">
+      <c r="F14" s="114">
         <f t="shared" si="1"/>
         <v>4.0102802594541673</v>
       </c>
-      <c r="H14" s="54"/>
-      <c r="I14" s="93"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="94"/>
-      <c r="L14" s="93"/>
-      <c r="M14" s="55"/>
-      <c r="N14" s="60"/>
-      <c r="O14" s="93"/>
-      <c r="P14" s="55"/>
-      <c r="Q14" s="60"/>
-      <c r="R14" s="93"/>
-      <c r="S14" s="55"/>
-      <c r="T14" s="60"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="87"/>
+      <c r="J14" s="54"/>
+      <c r="K14" s="88"/>
+      <c r="L14" s="87"/>
+      <c r="M14" s="54"/>
+      <c r="N14" s="59"/>
+      <c r="O14" s="87"/>
+      <c r="P14" s="54"/>
+      <c r="Q14" s="59"/>
+      <c r="R14" s="87"/>
+      <c r="S14" s="54"/>
+      <c r="T14" s="59"/>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B15">
         <v>1024</v>
@@ -4351,27 +3906,27 @@
       <c r="E15">
         <v>27577</v>
       </c>
-      <c r="F15" s="52">
+      <c r="F15" s="115">
         <f t="shared" si="1"/>
         <v>4.7529462958262316</v>
       </c>
-      <c r="H15" s="54"/>
-      <c r="I15" s="93"/>
-      <c r="J15" s="55"/>
-      <c r="K15" s="94"/>
-      <c r="L15" s="93"/>
-      <c r="M15" s="55"/>
-      <c r="N15" s="60"/>
-      <c r="O15" s="93"/>
-      <c r="P15" s="55"/>
-      <c r="Q15" s="60"/>
-      <c r="R15" s="93"/>
-      <c r="S15" s="55"/>
-      <c r="T15" s="60"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="87"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="88"/>
+      <c r="L15" s="87"/>
+      <c r="M15" s="54"/>
+      <c r="N15" s="59"/>
+      <c r="O15" s="87"/>
+      <c r="P15" s="54"/>
+      <c r="Q15" s="59"/>
+      <c r="R15" s="87"/>
+      <c r="S15" s="54"/>
+      <c r="T15" s="59"/>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B16">
         <v>2048</v>
@@ -4386,27 +3941,27 @@
       <c r="E16">
         <v>51313</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="113">
         <f t="shared" si="1"/>
         <v>5.1087248845321849</v>
       </c>
-      <c r="H16" s="54"/>
-      <c r="I16" s="93"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="94"/>
-      <c r="L16" s="93"/>
-      <c r="M16" s="55"/>
-      <c r="N16" s="60"/>
-      <c r="O16" s="93"/>
-      <c r="P16" s="55"/>
-      <c r="Q16" s="60"/>
-      <c r="R16" s="93"/>
-      <c r="S16" s="55"/>
-      <c r="T16" s="60"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="87"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="88"/>
+      <c r="L16" s="87"/>
+      <c r="M16" s="54"/>
+      <c r="N16" s="59"/>
+      <c r="O16" s="87"/>
+      <c r="P16" s="54"/>
+      <c r="Q16" s="59"/>
+      <c r="R16" s="87"/>
+      <c r="S16" s="54"/>
+      <c r="T16" s="59"/>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B17">
         <v>128</v>
@@ -4421,703 +3976,703 @@
       <c r="E17">
         <v>9919</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="113">
         <f t="shared" si="1"/>
         <v>3.3035588264946063</v>
       </c>
-      <c r="H17" s="54" t="s">
-        <v>87</v>
-      </c>
-      <c r="I17" s="59">
+      <c r="H17" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="I17" s="58">
         <v>1.5</v>
       </c>
-      <c r="J17" s="53">
+      <c r="J17" s="52">
         <v>2.2000000000000002</v>
       </c>
-      <c r="K17" s="60"/>
-      <c r="L17" s="59">
+      <c r="K17" s="59"/>
+      <c r="L17" s="58">
         <v>1.5</v>
       </c>
-      <c r="M17" s="53">
+      <c r="M17" s="52">
         <v>2.2000000000000002</v>
       </c>
-      <c r="N17" s="60"/>
-      <c r="O17" s="59">
+      <c r="N17" s="59"/>
+      <c r="O17" s="58">
         <v>1.5</v>
       </c>
-      <c r="P17" s="53">
+      <c r="P17" s="52">
         <v>2.2000000000000002</v>
       </c>
-      <c r="Q17" s="60"/>
-      <c r="R17" s="59">
+      <c r="Q17" s="59"/>
+      <c r="R17" s="58">
         <v>1.5</v>
       </c>
-      <c r="S17" s="53">
+      <c r="S17" s="52">
         <v>2.2000000000000002</v>
       </c>
-      <c r="T17" s="60"/>
+      <c r="T17" s="59"/>
     </row>
     <row r="18" spans="1:20">
       <c r="A18" t="s">
-        <v>114</v>
-      </c>
-      <c r="H18" s="54" t="s">
-        <v>102</v>
-      </c>
-      <c r="I18" s="59">
+        <v>103</v>
+      </c>
+      <c r="H18" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="I18" s="58">
         <v>0.11</v>
       </c>
-      <c r="J18" s="53"/>
-      <c r="K18" s="60">
+      <c r="J18" s="52"/>
+      <c r="K18" s="59">
         <v>83</v>
       </c>
-      <c r="L18" s="59">
+      <c r="L18" s="58">
         <v>0.17</v>
       </c>
-      <c r="M18" s="53"/>
-      <c r="N18" s="60">
+      <c r="M18" s="52"/>
+      <c r="N18" s="59">
         <f>K18*1.8</f>
         <v>149.4</v>
       </c>
-      <c r="O18" s="59">
+      <c r="O18" s="58">
         <v>0.25</v>
       </c>
-      <c r="P18" s="53"/>
-      <c r="Q18" s="60">
+      <c r="P18" s="52"/>
+      <c r="Q18" s="59">
         <f>K18*1.8</f>
         <v>149.4</v>
       </c>
-      <c r="R18" s="59">
+      <c r="R18" s="58">
         <v>0.35</v>
       </c>
-      <c r="S18" s="53"/>
-      <c r="T18" s="60">
+      <c r="S18" s="52"/>
+      <c r="T18" s="59">
         <f>K18*1.5*1.8</f>
         <v>224.1</v>
       </c>
     </row>
     <row r="19" spans="1:20">
       <c r="A19" t="s">
-        <v>114</v>
-      </c>
-      <c r="H19" s="54" t="s">
-        <v>88</v>
-      </c>
-      <c r="I19" s="59">
+        <v>103</v>
+      </c>
+      <c r="H19" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="I19" s="58">
         <f>I17-I18*2</f>
         <v>1.28</v>
       </c>
-      <c r="J19" s="53">
+      <c r="J19" s="52">
         <f>J17-I18*2</f>
         <v>1.9800000000000002</v>
       </c>
-      <c r="K19" s="60"/>
-      <c r="L19" s="59">
+      <c r="K19" s="59"/>
+      <c r="L19" s="58">
         <f>L17-L18*2</f>
         <v>1.1599999999999999</v>
       </c>
-      <c r="M19" s="53">
+      <c r="M19" s="52">
         <f>M17-L18*2</f>
         <v>1.86</v>
       </c>
-      <c r="N19" s="60"/>
-      <c r="O19" s="59">
+      <c r="N19" s="59"/>
+      <c r="O19" s="58">
         <f>O17-O18*2</f>
         <v>1</v>
       </c>
-      <c r="P19" s="53">
+      <c r="P19" s="52">
         <f>P17-O18*2</f>
         <v>1.7000000000000002</v>
       </c>
-      <c r="Q19" s="60"/>
-      <c r="R19" s="59">
+      <c r="Q19" s="59"/>
+      <c r="R19" s="58">
         <f>R17-R18*2</f>
         <v>0.8</v>
       </c>
-      <c r="S19" s="53">
+      <c r="S19" s="52">
         <f>S17-R18*2</f>
         <v>1.5000000000000002</v>
       </c>
-      <c r="T19" s="60"/>
+      <c r="T19" s="59"/>
     </row>
     <row r="20" spans="1:20" ht="14.4" thickBot="1">
       <c r="A20" t="s">
-        <v>114</v>
-      </c>
-      <c r="H20" s="54" t="s">
-        <v>94</v>
-      </c>
-      <c r="I20" s="61">
+        <v>103</v>
+      </c>
+      <c r="H20" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="I20" s="60">
         <f>I19*J19/I17/J17</f>
         <v>0.76800000000000002</v>
       </c>
-      <c r="J20" s="62"/>
-      <c r="K20" s="63"/>
-      <c r="L20" s="64">
+      <c r="J20" s="61"/>
+      <c r="K20" s="62"/>
+      <c r="L20" s="63">
         <f>L19*M19/L17/M17</f>
         <v>0.65381818181818174</v>
       </c>
-      <c r="M20" s="62"/>
-      <c r="N20" s="63"/>
-      <c r="O20" s="61">
+      <c r="M20" s="61"/>
+      <c r="N20" s="62"/>
+      <c r="O20" s="60">
         <f>O19*P19/O17/P17</f>
         <v>0.51515151515151525</v>
       </c>
-      <c r="P20" s="62"/>
-      <c r="Q20" s="63"/>
-      <c r="R20" s="61">
+      <c r="P20" s="61"/>
+      <c r="Q20" s="62"/>
+      <c r="R20" s="60">
         <f>R19*S19/R17/S17</f>
         <v>0.3636363636363637</v>
       </c>
-      <c r="S20" s="62"/>
-      <c r="T20" s="63"/>
+      <c r="S20" s="61"/>
+      <c r="T20" s="62"/>
     </row>
     <row r="21" spans="1:20">
       <c r="A21" t="s">
-        <v>114</v>
-      </c>
-      <c r="H21" s="53" t="s">
-        <v>96</v>
-      </c>
-      <c r="I21" s="55">
+        <v>103</v>
+      </c>
+      <c r="H21" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="I21" s="54">
         <f>K18/I19/J19</f>
         <v>32.749368686868685</v>
       </c>
-      <c r="J21" s="55"/>
-      <c r="K21" s="55"/>
-      <c r="L21" s="55">
+      <c r="J21" s="54"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="54">
         <f>N18/L19/M19</f>
         <v>69.243604004449395</v>
       </c>
-      <c r="M21" s="55"/>
-      <c r="N21" s="55"/>
-      <c r="O21" s="55">
+      <c r="M21" s="54"/>
+      <c r="N21" s="54"/>
+      <c r="O21" s="54">
         <f>Q18/O19/P19</f>
         <v>87.882352941176464</v>
       </c>
-      <c r="P21" s="55"/>
-      <c r="Q21" s="55"/>
-      <c r="R21" s="55">
+      <c r="P21" s="54"/>
+      <c r="Q21" s="54"/>
+      <c r="R21" s="54">
         <f>T18/R19/S19</f>
         <v>186.74999999999997</v>
       </c>
-      <c r="S21" s="55"/>
-      <c r="T21" s="55"/>
+      <c r="S21" s="54"/>
+      <c r="T21" s="54"/>
     </row>
     <row r="22" spans="1:20">
       <c r="A22" t="s">
-        <v>114</v>
-      </c>
-      <c r="H22" s="68" t="s">
-        <v>101</v>
-      </c>
-      <c r="I22" s="52"/>
-      <c r="J22" s="52"/>
-      <c r="K22" s="52">
+        <v>103</v>
+      </c>
+      <c r="H22" s="67" t="s">
+        <v>93</v>
+      </c>
+      <c r="I22" s="51"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="51">
         <f>K18/(I19+J19)/2</f>
         <v>12.730061349693251</v>
       </c>
-      <c r="L22" s="52"/>
-      <c r="M22" s="52"/>
-      <c r="N22" s="52">
+      <c r="L22" s="51"/>
+      <c r="M22" s="51"/>
+      <c r="N22" s="51">
         <f>N18/(L19+M19)/2</f>
         <v>24.735099337748345</v>
       </c>
     </row>
     <row r="23" spans="1:20">
-      <c r="H23" s="71" t="s">
-        <v>87</v>
-      </c>
-      <c r="I23" s="70">
+      <c r="H23" s="70" t="s">
+        <v>79</v>
+      </c>
+      <c r="I23" s="69">
         <f>I25+I24*2</f>
         <v>1.52</v>
       </c>
-      <c r="J23" s="70">
+      <c r="J23" s="69">
         <f>J25+I24*2</f>
         <v>1.52</v>
       </c>
-      <c r="K23" s="70">
+      <c r="K23" s="69">
         <f>I23*J23</f>
         <v>2.3104</v>
       </c>
-      <c r="L23" s="70">
+      <c r="L23" s="69">
         <f>L25+L24*2</f>
         <v>1.6400000000000001</v>
       </c>
-      <c r="M23" s="70">
+      <c r="M23" s="69">
         <f>M25+L24*2</f>
         <v>1.6400000000000001</v>
       </c>
-      <c r="N23" s="70">
+      <c r="N23" s="69">
         <f>L23*M23</f>
         <v>2.6896000000000004</v>
       </c>
     </row>
     <row r="24" spans="1:20">
-      <c r="H24" s="71" t="s">
-        <v>89</v>
-      </c>
-      <c r="I24" s="70">
+      <c r="H24" s="70" t="s">
+        <v>81</v>
+      </c>
+      <c r="I24" s="69">
         <v>0.11</v>
       </c>
-      <c r="J24" s="70"/>
-      <c r="K24" s="70">
+      <c r="J24" s="69"/>
+      <c r="K24" s="69">
         <f>K22*(I23+J23)*2</f>
         <v>77.398773006134974</v>
       </c>
-      <c r="L24" s="70">
+      <c r="L24" s="69">
         <v>0.17</v>
       </c>
-      <c r="M24" s="70"/>
-      <c r="N24" s="70">
+      <c r="M24" s="69"/>
+      <c r="N24" s="69">
         <f>N22*(L23+M23)*2</f>
         <v>162.26225165562914</v>
       </c>
     </row>
     <row r="25" spans="1:20">
-      <c r="H25" s="71" t="s">
-        <v>88</v>
-      </c>
-      <c r="I25" s="70">
+      <c r="H25" s="70" t="s">
+        <v>80</v>
+      </c>
+      <c r="I25" s="69">
         <v>1.3</v>
       </c>
-      <c r="J25" s="70">
+      <c r="J25" s="69">
         <v>1.3</v>
       </c>
-      <c r="K25" s="70">
+      <c r="K25" s="69">
         <f>I25*J25</f>
         <v>1.6900000000000002</v>
       </c>
-      <c r="L25" s="70">
+      <c r="L25" s="69">
         <v>1.3</v>
       </c>
-      <c r="M25" s="70">
+      <c r="M25" s="69">
         <v>1.3</v>
       </c>
-      <c r="N25" s="70"/>
+      <c r="N25" s="69"/>
     </row>
     <row r="26" spans="1:20">
-      <c r="H26" s="71" t="s">
-        <v>103</v>
-      </c>
-      <c r="I26" s="70"/>
-      <c r="J26" s="70"/>
-      <c r="K26" s="70">
+      <c r="H26" s="70" t="s">
+        <v>95</v>
+      </c>
+      <c r="I26" s="69"/>
+      <c r="J26" s="69"/>
+      <c r="K26" s="69">
         <f>I24*(I25+J25)*2</f>
         <v>0.57200000000000006</v>
       </c>
-      <c r="L26" s="70"/>
-      <c r="M26" s="70"/>
-      <c r="N26" s="70">
+      <c r="L26" s="69"/>
+      <c r="M26" s="69"/>
+      <c r="N26" s="69">
         <f>L24*(L25+M25)*2</f>
         <v>0.88400000000000012</v>
       </c>
     </row>
     <row r="27" spans="1:20" ht="14.4" thickBot="1">
-      <c r="H27" s="71" t="s">
-        <v>94</v>
-      </c>
-      <c r="I27" s="70"/>
-      <c r="J27" s="70"/>
-      <c r="K27" s="70"/>
-      <c r="L27" s="72">
+      <c r="H27" s="70" t="s">
+        <v>86</v>
+      </c>
+      <c r="I27" s="69"/>
+      <c r="J27" s="69"/>
+      <c r="K27" s="69"/>
+      <c r="L27" s="71">
         <f>L25*M25/L23/M23</f>
         <v>0.62834622248661509</v>
       </c>
-      <c r="M27" s="70"/>
-      <c r="N27" s="70"/>
+      <c r="M27" s="69"/>
+      <c r="N27" s="69"/>
     </row>
     <row r="28" spans="1:20">
-      <c r="H28" s="73" t="s">
-        <v>96</v>
-      </c>
-      <c r="I28" s="70"/>
-      <c r="J28" s="70"/>
-      <c r="K28" s="70"/>
-      <c r="L28" s="74">
+      <c r="H28" s="72" t="s">
+        <v>88</v>
+      </c>
+      <c r="I28" s="69"/>
+      <c r="J28" s="69"/>
+      <c r="K28" s="69"/>
+      <c r="L28" s="73">
         <f>N24/L25/M25</f>
         <v>96.013166660135582</v>
       </c>
-      <c r="M28" s="70"/>
-      <c r="N28" s="70"/>
+      <c r="M28" s="69"/>
+      <c r="N28" s="69"/>
     </row>
     <row r="29" spans="1:20" ht="14.4" thickBot="1">
-      <c r="H29" s="76"/>
-      <c r="I29" s="70"/>
-      <c r="J29" s="70"/>
-      <c r="K29" s="70"/>
-      <c r="L29" s="75"/>
-      <c r="M29" s="70"/>
-      <c r="N29" s="70"/>
+      <c r="H29" s="75"/>
+      <c r="I29" s="69"/>
+      <c r="J29" s="69"/>
+      <c r="K29" s="69"/>
+      <c r="L29" s="74"/>
+      <c r="M29" s="69"/>
+      <c r="N29" s="69"/>
     </row>
     <row r="30" spans="1:20">
-      <c r="H30" s="56"/>
-      <c r="I30" s="80" t="s">
-        <v>90</v>
-      </c>
-      <c r="J30" s="80"/>
-      <c r="K30" s="80"/>
-      <c r="L30" s="110" t="s">
-        <v>105</v>
-      </c>
-      <c r="M30" s="110"/>
-      <c r="N30" s="110"/>
-      <c r="O30" s="110" t="s">
-        <v>91</v>
-      </c>
-      <c r="P30" s="110"/>
-      <c r="Q30" s="110"/>
-      <c r="R30" s="57" t="s">
-        <v>93</v>
-      </c>
-      <c r="S30" s="57"/>
-      <c r="T30" s="58"/>
+      <c r="H30" s="55"/>
+      <c r="I30" s="79" t="s">
+        <v>82</v>
+      </c>
+      <c r="J30" s="79"/>
+      <c r="K30" s="79"/>
+      <c r="L30" s="102" t="s">
+        <v>97</v>
+      </c>
+      <c r="M30" s="102"/>
+      <c r="N30" s="102"/>
+      <c r="O30" s="102" t="s">
+        <v>83</v>
+      </c>
+      <c r="P30" s="102"/>
+      <c r="Q30" s="102"/>
+      <c r="R30" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="S30" s="56"/>
+      <c r="T30" s="57"/>
     </row>
     <row r="31" spans="1:20">
-      <c r="H31" s="59"/>
-      <c r="I31" s="53" t="s">
-        <v>86</v>
-      </c>
-      <c r="J31" s="53" t="s">
-        <v>104</v>
-      </c>
-      <c r="K31" s="53" t="s">
-        <v>106</v>
-      </c>
-      <c r="L31" s="53" t="s">
-        <v>86</v>
-      </c>
-      <c r="M31" s="53" t="s">
-        <v>104</v>
-      </c>
-      <c r="N31" s="53" t="s">
-        <v>95</v>
-      </c>
-      <c r="O31" s="53" t="s">
-        <v>86</v>
-      </c>
-      <c r="P31" s="53" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q31" s="53" t="s">
-        <v>95</v>
-      </c>
-      <c r="R31" s="53" t="s">
-        <v>86</v>
-      </c>
-      <c r="S31" s="53" t="s">
-        <v>104</v>
-      </c>
-      <c r="T31" s="60" t="s">
-        <v>95</v>
+      <c r="H31" s="58"/>
+      <c r="I31" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="J31" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="K31" s="52" t="s">
+        <v>98</v>
+      </c>
+      <c r="L31" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="M31" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="N31" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="O31" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="P31" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q31" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="R31" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="S31" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="T31" s="59" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:20">
-      <c r="H32" s="79" t="s">
-        <v>88</v>
-      </c>
-      <c r="I32" s="69">
+      <c r="H32" s="78" t="s">
+        <v>80</v>
+      </c>
+      <c r="I32" s="68">
         <v>1.7</v>
       </c>
-      <c r="J32" s="69">
+      <c r="J32" s="68">
         <v>1</v>
       </c>
-      <c r="K32" s="69">
+      <c r="K32" s="68">
         <v>0.11</v>
       </c>
-      <c r="L32" s="69">
+      <c r="L32" s="68">
         <v>1.7</v>
       </c>
-      <c r="M32" s="69">
+      <c r="M32" s="68">
         <v>1</v>
       </c>
-      <c r="N32" s="69">
+      <c r="N32" s="68">
         <v>1.7</v>
       </c>
-      <c r="O32" s="53"/>
-      <c r="P32" s="53"/>
-      <c r="Q32" s="53"/>
-      <c r="R32" s="53"/>
-      <c r="S32" s="53"/>
-      <c r="T32" s="60"/>
+      <c r="O32" s="52"/>
+      <c r="P32" s="52"/>
+      <c r="Q32" s="52"/>
+      <c r="R32" s="52"/>
+      <c r="S32" s="52"/>
+      <c r="T32" s="59"/>
     </row>
     <row r="33" spans="8:20">
-      <c r="H33" s="79" t="s">
-        <v>87</v>
-      </c>
-      <c r="I33" s="69">
+      <c r="H33" s="78" t="s">
+        <v>79</v>
+      </c>
+      <c r="I33" s="68">
         <f>I32+K32*2</f>
         <v>1.92</v>
       </c>
-      <c r="J33" s="69">
+      <c r="J33" s="68">
         <f>J32+K32*2</f>
         <v>1.22</v>
       </c>
-      <c r="K33" s="69">
+      <c r="K33" s="68">
         <f>I33*J33</f>
         <v>2.3424</v>
       </c>
-      <c r="L33" s="69">
+      <c r="L33" s="68">
         <f>L32+L34*2</f>
         <v>2.04</v>
       </c>
-      <c r="M33" s="69">
+      <c r="M33" s="68">
         <f>M32+L34*2</f>
         <v>1.34</v>
       </c>
-      <c r="N33" s="69">
+      <c r="N33" s="68">
         <f>L33*M33</f>
         <v>2.7336</v>
       </c>
-      <c r="O33" s="53"/>
-      <c r="P33" s="53"/>
-      <c r="Q33" s="53"/>
-      <c r="R33" s="53"/>
-      <c r="S33" s="53"/>
-      <c r="T33" s="60"/>
+      <c r="O33" s="52"/>
+      <c r="P33" s="52"/>
+      <c r="Q33" s="52"/>
+      <c r="R33" s="52"/>
+      <c r="S33" s="52"/>
+      <c r="T33" s="59"/>
     </row>
     <row r="34" spans="8:20">
-      <c r="H34" s="79" t="s">
-        <v>95</v>
-      </c>
-      <c r="J34" s="69"/>
-      <c r="K34" s="69">
+      <c r="H34" s="78" t="s">
+        <v>87</v>
+      </c>
+      <c r="J34" s="68"/>
+      <c r="K34" s="68">
         <f>K28*(I33+J33)*2</f>
         <v>0</v>
       </c>
-      <c r="L34" s="69">
+      <c r="L34" s="68">
         <v>0.17</v>
       </c>
-      <c r="M34" s="69"/>
-      <c r="N34" s="69">
+      <c r="M34" s="68"/>
+      <c r="N34" s="68">
         <f>N28*(L33+M33)*2</f>
         <v>0</v>
       </c>
-      <c r="O34" s="53"/>
-      <c r="P34" s="53"/>
-      <c r="Q34" s="53"/>
-      <c r="R34" s="53"/>
-      <c r="S34" s="53"/>
-      <c r="T34" s="60"/>
+      <c r="O34" s="52"/>
+      <c r="P34" s="52"/>
+      <c r="Q34" s="52"/>
+      <c r="R34" s="52"/>
+      <c r="S34" s="52"/>
+      <c r="T34" s="59"/>
     </row>
     <row r="35" spans="8:20">
-      <c r="H35" s="79" t="s">
-        <v>103</v>
-      </c>
-      <c r="I35" s="69"/>
-      <c r="J35" s="69"/>
-      <c r="K35" s="69" t="e">
+      <c r="H35" s="78" t="s">
+        <v>95</v>
+      </c>
+      <c r="I35" s="68"/>
+      <c r="J35" s="68"/>
+      <c r="K35" s="68" t="e">
         <f>K33-#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="L35" s="69"/>
-      <c r="M35" s="69"/>
-      <c r="N35" s="69">
+      <c r="L35" s="68"/>
+      <c r="M35" s="68"/>
+      <c r="N35" s="68">
         <f>N33-N32</f>
         <v>1.0336000000000001</v>
       </c>
-      <c r="O35" s="53"/>
-      <c r="P35" s="53"/>
-      <c r="Q35" s="53"/>
-      <c r="R35" s="53"/>
-      <c r="S35" s="53"/>
-      <c r="T35" s="60"/>
+      <c r="O35" s="52"/>
+      <c r="P35" s="52"/>
+      <c r="Q35" s="52"/>
+      <c r="R35" s="52"/>
+      <c r="S35" s="52"/>
+      <c r="T35" s="59"/>
     </row>
     <row r="36" spans="8:20">
-      <c r="H36" s="79" t="s">
-        <v>94</v>
-      </c>
-      <c r="I36" s="69"/>
-      <c r="J36" s="69"/>
-      <c r="K36" s="69"/>
-      <c r="L36" s="77">
+      <c r="H36" s="78" t="s">
+        <v>86</v>
+      </c>
+      <c r="I36" s="68"/>
+      <c r="J36" s="68"/>
+      <c r="K36" s="68"/>
+      <c r="L36" s="76">
         <f>L32*M32/L33/M33</f>
         <v>0.62189054726368154</v>
       </c>
-      <c r="M36" s="69"/>
-      <c r="N36" s="69"/>
-      <c r="O36" s="53"/>
-      <c r="P36" s="53"/>
-      <c r="Q36" s="53"/>
-      <c r="R36" s="53"/>
-      <c r="S36" s="53"/>
-      <c r="T36" s="60"/>
+      <c r="M36" s="68"/>
+      <c r="N36" s="68"/>
+      <c r="O36" s="52"/>
+      <c r="P36" s="52"/>
+      <c r="Q36" s="52"/>
+      <c r="R36" s="52"/>
+      <c r="S36" s="52"/>
+      <c r="T36" s="59"/>
     </row>
     <row r="37" spans="8:20">
-      <c r="H37" s="79" t="s">
-        <v>96</v>
-      </c>
-      <c r="I37" s="69"/>
-      <c r="J37" s="69"/>
-      <c r="K37" s="69"/>
-      <c r="L37" s="69">
+      <c r="H37" s="78" t="s">
+        <v>88</v>
+      </c>
+      <c r="I37" s="68"/>
+      <c r="J37" s="68"/>
+      <c r="K37" s="68"/>
+      <c r="L37" s="68">
         <f>N34/L32/M32</f>
         <v>0</v>
       </c>
-      <c r="M37" s="69"/>
-      <c r="N37" s="69"/>
-      <c r="O37" s="53"/>
-      <c r="P37" s="53"/>
-      <c r="Q37" s="53"/>
-      <c r="R37" s="53"/>
-      <c r="S37" s="53"/>
-      <c r="T37" s="60"/>
+      <c r="M37" s="68"/>
+      <c r="N37" s="68"/>
+      <c r="O37" s="52"/>
+      <c r="P37" s="52"/>
+      <c r="Q37" s="52"/>
+      <c r="R37" s="52"/>
+      <c r="S37" s="52"/>
+      <c r="T37" s="59"/>
     </row>
     <row r="38" spans="8:20">
-      <c r="H38" s="59" t="s">
-        <v>87</v>
-      </c>
-      <c r="I38" s="53">
+      <c r="H38" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="I38" s="52">
         <f>I40+I39*2</f>
         <v>1.07</v>
       </c>
-      <c r="J38" s="53">
+      <c r="J38" s="52">
         <f>J40+I39*2</f>
         <v>2.2200000000000002</v>
       </c>
-      <c r="K38" s="53">
+      <c r="K38" s="52">
         <f>I38*J38</f>
         <v>2.3754000000000004</v>
       </c>
-      <c r="L38" s="53">
+      <c r="L38" s="52">
         <f>L40+L39*2</f>
         <v>1.19</v>
       </c>
-      <c r="M38" s="53">
+      <c r="M38" s="52">
         <f>M40+L39*2</f>
         <v>2.34</v>
       </c>
-      <c r="N38" s="53">
+      <c r="N38" s="52">
         <f>L38*M38</f>
         <v>2.7845999999999997</v>
       </c>
-      <c r="O38" s="53"/>
-      <c r="P38" s="53"/>
-      <c r="Q38" s="53"/>
-      <c r="R38" s="53"/>
-      <c r="S38" s="53"/>
-      <c r="T38" s="60"/>
+      <c r="O38" s="52"/>
+      <c r="P38" s="52"/>
+      <c r="Q38" s="52"/>
+      <c r="R38" s="52"/>
+      <c r="S38" s="52"/>
+      <c r="T38" s="59"/>
     </row>
     <row r="39" spans="8:20">
-      <c r="H39" s="59" t="s">
-        <v>89</v>
-      </c>
-      <c r="I39" s="53">
+      <c r="H39" s="58" t="s">
+        <v>81</v>
+      </c>
+      <c r="I39" s="52">
         <v>0.11</v>
       </c>
-      <c r="J39" s="53"/>
-      <c r="K39" s="53">
+      <c r="J39" s="52"/>
+      <c r="K39" s="52">
         <f>K22*(I40+J40)*2</f>
         <v>72.561349693251529</v>
       </c>
-      <c r="L39" s="53">
+      <c r="L39" s="52">
         <v>0.17</v>
       </c>
-      <c r="M39" s="53"/>
-      <c r="N39" s="53">
+      <c r="M39" s="52"/>
+      <c r="N39" s="52">
         <f>N22*(L40+M40)*2</f>
         <v>140.99006622516558</v>
       </c>
-      <c r="O39" s="53"/>
-      <c r="P39" s="53"/>
-      <c r="Q39" s="53"/>
-      <c r="R39" s="53"/>
-      <c r="S39" s="53"/>
-      <c r="T39" s="60"/>
+      <c r="O39" s="52"/>
+      <c r="P39" s="52"/>
+      <c r="Q39" s="52"/>
+      <c r="R39" s="52"/>
+      <c r="S39" s="52"/>
+      <c r="T39" s="59"/>
     </row>
     <row r="40" spans="8:20">
-      <c r="H40" s="59" t="s">
-        <v>88</v>
-      </c>
-      <c r="I40" s="53">
+      <c r="H40" s="58" t="s">
+        <v>80</v>
+      </c>
+      <c r="I40" s="52">
         <f>K40/J40</f>
         <v>0.85</v>
       </c>
-      <c r="J40" s="53">
+      <c r="J40" s="52">
         <v>2</v>
       </c>
-      <c r="K40" s="53">
+      <c r="K40" s="52">
         <v>1.7</v>
       </c>
-      <c r="L40" s="53">
+      <c r="L40" s="52">
         <f>N40/M40</f>
         <v>0.85</v>
       </c>
-      <c r="M40" s="53">
+      <c r="M40" s="52">
         <v>2</v>
       </c>
-      <c r="N40" s="53">
+      <c r="N40" s="52">
         <v>1.7</v>
       </c>
-      <c r="O40" s="53"/>
-      <c r="P40" s="53"/>
-      <c r="Q40" s="53"/>
-      <c r="R40" s="53"/>
-      <c r="S40" s="53"/>
-      <c r="T40" s="60"/>
+      <c r="O40" s="52"/>
+      <c r="P40" s="52"/>
+      <c r="Q40" s="52"/>
+      <c r="R40" s="52"/>
+      <c r="S40" s="52"/>
+      <c r="T40" s="59"/>
     </row>
     <row r="41" spans="8:20">
-      <c r="H41" s="59" t="s">
-        <v>103</v>
-      </c>
-      <c r="I41" s="53"/>
-      <c r="J41" s="53"/>
-      <c r="K41" s="53">
+      <c r="H41" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="I41" s="52"/>
+      <c r="J41" s="52"/>
+      <c r="K41" s="52">
         <f>K38-K40</f>
         <v>0.67540000000000044</v>
       </c>
-      <c r="L41" s="53"/>
-      <c r="M41" s="53"/>
-      <c r="N41" s="53">
+      <c r="L41" s="52"/>
+      <c r="M41" s="52"/>
+      <c r="N41" s="52">
         <f>N38-N40</f>
         <v>1.0845999999999998</v>
       </c>
-      <c r="O41" s="53"/>
-      <c r="P41" s="53"/>
-      <c r="Q41" s="53"/>
-      <c r="R41" s="53"/>
-      <c r="S41" s="53"/>
-      <c r="T41" s="60"/>
+      <c r="O41" s="52"/>
+      <c r="P41" s="52"/>
+      <c r="Q41" s="52"/>
+      <c r="R41" s="52"/>
+      <c r="S41" s="52"/>
+      <c r="T41" s="59"/>
     </row>
     <row r="42" spans="8:20">
-      <c r="H42" s="59" t="s">
-        <v>94</v>
-      </c>
-      <c r="I42" s="53"/>
-      <c r="J42" s="53"/>
-      <c r="K42" s="53"/>
-      <c r="L42" s="78">
+      <c r="H42" s="58" t="s">
+        <v>86</v>
+      </c>
+      <c r="I42" s="52"/>
+      <c r="J42" s="52"/>
+      <c r="K42" s="52"/>
+      <c r="L42" s="77">
         <f>L40*M40/L38/M38</f>
         <v>0.61050061050061055</v>
       </c>
-      <c r="M42" s="53"/>
-      <c r="N42" s="53"/>
-      <c r="O42" s="53"/>
-      <c r="P42" s="53"/>
-      <c r="Q42" s="53"/>
-      <c r="R42" s="53"/>
-      <c r="S42" s="53"/>
-      <c r="T42" s="60"/>
+      <c r="M42" s="52"/>
+      <c r="N42" s="52"/>
+      <c r="O42" s="52"/>
+      <c r="P42" s="52"/>
+      <c r="Q42" s="52"/>
+      <c r="R42" s="52"/>
+      <c r="S42" s="52"/>
+      <c r="T42" s="59"/>
     </row>
     <row r="43" spans="8:20" ht="14.4" thickBot="1">
-      <c r="H43" s="61" t="s">
-        <v>96</v>
-      </c>
-      <c r="I43" s="62"/>
-      <c r="J43" s="62"/>
-      <c r="K43" s="62"/>
-      <c r="L43" s="62">
+      <c r="H43" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="I43" s="61"/>
+      <c r="J43" s="61"/>
+      <c r="K43" s="61"/>
+      <c r="L43" s="61">
         <f>N39/L40/M40</f>
         <v>82.935333073626808</v>
       </c>
-      <c r="M43" s="62"/>
-      <c r="N43" s="62"/>
-      <c r="O43" s="62"/>
-      <c r="P43" s="62"/>
-      <c r="Q43" s="62"/>
-      <c r="R43" s="62"/>
-      <c r="S43" s="62"/>
-      <c r="T43" s="63"/>
+      <c r="M43" s="61"/>
+      <c r="N43" s="61"/>
+      <c r="O43" s="61"/>
+      <c r="P43" s="61"/>
+      <c r="Q43" s="61"/>
+      <c r="R43" s="61"/>
+      <c r="S43" s="61"/>
+      <c r="T43" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
feat(HW Parameter): GLB area comparsion of Ports and Banks
</commit_message>
<xml_diff>
--- a/hardware/docs/01-top/点云硬件参数分析.xlsx
+++ b/hardware/docs/01-top/点云硬件参数分析.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="12960" windowHeight="4872" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="12960" windowHeight="4872" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="整体评估" sheetId="5" r:id="rId1"/>
@@ -468,7 +468,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="124">
   <si>
     <t>case</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -994,6 +994,22 @@
   </si>
   <si>
     <t>REG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date230329_Period1000_group_Track3vt_NoteGLB_area_16BANK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GLB (16bank, Bitwidth256, Word128, WR8, RD16, PAR2,)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date230329_Period1000_group_Track3vt_NoteGLB_area_2WRPAR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GLB (32bank, Bitwidth256, Word128, WR2, RD2, PAR2,)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1789,57 +1805,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1855,6 +1820,57 @@
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="180" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="180" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2290,7 +2306,7 @@
       <c r="A12" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="B12" s="110">
+      <c r="B12" s="93">
         <f>3.6/1024</f>
         <v>3.5156250000000001E-3</v>
       </c>
@@ -2334,7 +2350,7 @@
       <c r="A15" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="B15" s="111">
+      <c r="B15" s="94">
         <f>9*1024</f>
         <v>9216</v>
       </c>
@@ -2363,11 +2379,11 @@
       <c r="A17" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="B17" s="112">
+      <c r="B17" s="95">
         <f>B16/B14</f>
         <v>29.296874999999993</v>
       </c>
-      <c r="C17" s="109">
+      <c r="C17" s="92">
         <f>C16/C14</f>
         <v>1.9797333333333333</v>
       </c>
@@ -2476,11 +2492,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="O4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="5" ySplit="3" topLeftCell="P4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q10" sqref="Q10"/>
+      <selection pane="bottomRight" activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.77734375" defaultRowHeight="13.8"/>
@@ -2497,7 +2513,9 @@
     <col min="10" max="10" width="19.77734375" style="8" customWidth="1"/>
     <col min="11" max="12" width="19.77734375" style="2" customWidth="1"/>
     <col min="13" max="13" width="13.109375" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="19.77734375" style="2"/>
+    <col min="14" max="16" width="19.77734375" style="2"/>
+    <col min="17" max="17" width="33.33203125" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="19.77734375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -2506,21 +2524,21 @@
       <c r="G1" s="66"/>
       <c r="H1" s="65"/>
       <c r="I1" s="66"/>
-      <c r="J1" s="92" t="s">
+      <c r="J1" s="99" t="s">
         <v>89</v>
       </c>
-      <c r="K1" s="93"/>
-      <c r="L1" s="93"/>
-      <c r="M1" s="93"/>
-      <c r="N1" s="93"/>
-      <c r="O1" s="94"/>
-      <c r="P1" s="95" t="s">
+      <c r="K1" s="100"/>
+      <c r="L1" s="100"/>
+      <c r="M1" s="100"/>
+      <c r="N1" s="100"/>
+      <c r="O1" s="101"/>
+      <c r="P1" s="102" t="s">
         <v>90</v>
       </c>
-      <c r="Q1" s="93"/>
-      <c r="R1" s="93"/>
-      <c r="S1" s="93"/>
-      <c r="T1" s="94"/>
+      <c r="Q1" s="100"/>
+      <c r="R1" s="100"/>
+      <c r="S1" s="100"/>
+      <c r="T1" s="101"/>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="1" t="s">
@@ -2530,14 +2548,14 @@
       <c r="C2" s="1"/>
       <c r="D2" s="6"/>
       <c r="E2" s="24"/>
-      <c r="F2" s="99">
+      <c r="F2" s="106">
         <v>0</v>
       </c>
-      <c r="G2" s="100"/>
-      <c r="H2" s="99">
+      <c r="G2" s="107"/>
+      <c r="H2" s="106">
         <v>1</v>
       </c>
-      <c r="I2" s="100"/>
+      <c r="I2" s="107"/>
       <c r="J2" s="8">
         <v>2</v>
       </c>
@@ -2562,18 +2580,18 @@
       <c r="C3" s="1"/>
       <c r="D3" s="6"/>
       <c r="E3" s="25"/>
-      <c r="F3" s="92" t="s">
+      <c r="F3" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="101"/>
-      <c r="H3" s="92" t="s">
+      <c r="G3" s="108"/>
+      <c r="H3" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="101"/>
-      <c r="J3" s="92" t="s">
+      <c r="I3" s="108"/>
+      <c r="J3" s="99" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="94"/>
+      <c r="K3" s="101"/>
       <c r="L3" s="2" t="s">
         <v>41</v>
       </c>
@@ -2583,8 +2601,14 @@
       <c r="P3" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="4" spans="1:20">
+      <c r="Q3" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="41.4">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2609,6 +2633,12 @@
       <c r="P4" s="2" t="s">
         <v>91</v>
       </c>
+      <c r="Q4" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" s="1" t="s">
@@ -2698,7 +2728,7 @@
       </c>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="96" t="s">
+      <c r="A9" s="103" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2726,7 +2756,7 @@
       </c>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="97"/>
+      <c r="A10" s="104"/>
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
@@ -2752,7 +2782,7 @@
       </c>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11" s="97"/>
+      <c r="A11" s="104"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
         <v>15</v>
@@ -2775,7 +2805,7 @@
       </c>
     </row>
     <row r="12" spans="1:20">
-      <c r="A12" s="97"/>
+      <c r="A12" s="104"/>
       <c r="B12" s="1"/>
       <c r="C12" s="3"/>
       <c r="D12" s="11" t="s">
@@ -2787,7 +2817,7 @@
       </c>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="97"/>
+      <c r="A13" s="104"/>
       <c r="B13" s="1"/>
       <c r="C13" s="3"/>
       <c r="E13" s="19" t="s">
@@ -2802,7 +2832,7 @@
       </c>
     </row>
     <row r="14" spans="1:20">
-      <c r="A14" s="97"/>
+      <c r="A14" s="104"/>
       <c r="B14" s="1"/>
       <c r="C14" s="3"/>
       <c r="E14" s="19" t="s">
@@ -2816,7 +2846,7 @@
       </c>
     </row>
     <row r="15" spans="1:20">
-      <c r="A15" s="97"/>
+      <c r="A15" s="104"/>
       <c r="B15" s="1"/>
       <c r="C15" s="3"/>
       <c r="D15" s="19"/>
@@ -2824,7 +2854,7 @@
       <c r="H15" s="15"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="97"/>
+      <c r="A16" s="104"/>
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
         <v>16</v>
@@ -2846,15 +2876,15 @@
         <v>6041</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
-      <c r="A17" s="97"/>
+    <row r="17" spans="1:18">
+      <c r="A17" s="104"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="6"/>
       <c r="E17" s="25"/>
     </row>
-    <row r="18" spans="1:16">
-      <c r="A18" s="97"/>
+    <row r="18" spans="1:18">
+      <c r="A18" s="104"/>
       <c r="B18" s="1" t="s">
         <v>10</v>
       </c>
@@ -2885,9 +2915,15 @@
       <c r="P18" s="2">
         <v>540989</v>
       </c>
-    </row>
-    <row r="19" spans="1:16">
-      <c r="A19" s="97"/>
+      <c r="Q18" s="2">
+        <v>479411</v>
+      </c>
+      <c r="R18" s="2">
+        <v>443245</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" s="104"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
         <v>17</v>
@@ -2911,9 +2947,15 @@
       <c r="P19" s="2">
         <v>10023</v>
       </c>
-    </row>
-    <row r="20" spans="1:16">
-      <c r="A20" s="97"/>
+      <c r="Q19" s="2">
+        <v>10019</v>
+      </c>
+      <c r="R19" s="2">
+        <v>10021</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" s="104"/>
       <c r="B20" s="1"/>
       <c r="C20" s="2" t="s">
         <v>39</v>
@@ -2923,8 +2965,8 @@
         <v>0.193</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
-      <c r="A21" s="97"/>
+    <row r="21" spans="1:18">
+      <c r="A21" s="104"/>
       <c r="B21" s="1"/>
       <c r="C21" s="2" t="s">
         <v>40</v>
@@ -2934,8 +2976,8 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
-      <c r="A22" s="97"/>
+    <row r="22" spans="1:18">
+      <c r="A22" s="104"/>
       <c r="B22" s="1" t="s">
         <v>13</v>
       </c>
@@ -2964,8 +3006,8 @@
         <v>10849</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
-      <c r="A23" s="97"/>
+    <row r="23" spans="1:18">
+      <c r="A23" s="104"/>
       <c r="B23" s="1"/>
       <c r="C23" s="2" t="s">
         <v>18</v>
@@ -2985,8 +3027,8 @@
         <v>0.33747879510338818</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
-      <c r="A24" s="97"/>
+    <row r="24" spans="1:18">
+      <c r="A24" s="104"/>
       <c r="B24" s="1"/>
       <c r="D24" s="7" t="s">
         <v>43</v>
@@ -3000,8 +3042,8 @@
         <v>0.76429032367625582</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="27.6">
-      <c r="A25" s="97"/>
+    <row r="25" spans="1:18" ht="27.6">
+      <c r="A25" s="104"/>
       <c r="B25" s="1"/>
       <c r="E25" s="7" t="s">
         <v>42</v>
@@ -3015,8 +3057,8 @@
         <v>0.90067990934542064</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
-      <c r="A26" s="97"/>
+    <row r="26" spans="1:18">
+      <c r="A26" s="104"/>
       <c r="B26" s="1"/>
       <c r="C26" s="2" t="s">
         <v>19</v>
@@ -3032,8 +3074,8 @@
         <v>0.63920728072990696</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
-      <c r="A27" s="97"/>
+    <row r="27" spans="1:18">
+      <c r="A27" s="104"/>
       <c r="B27" s="1"/>
       <c r="C27" s="2" t="s">
         <v>20</v>
@@ -3046,8 +3088,8 @@
         <v>18589</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
-      <c r="A28" s="97"/>
+    <row r="28" spans="1:18">
+      <c r="A28" s="104"/>
       <c r="B28" s="1" t="s">
         <v>9</v>
       </c>
@@ -3076,8 +3118,8 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
-      <c r="A29" s="97"/>
+    <row r="29" spans="1:18">
+      <c r="A29" s="104"/>
       <c r="B29" s="1"/>
       <c r="C29" s="2" t="s">
         <v>21</v>
@@ -3096,8 +3138,8 @@
         <v>11719</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
-      <c r="A30" s="97"/>
+    <row r="30" spans="1:18">
+      <c r="A30" s="104"/>
       <c r="B30" s="1"/>
       <c r="C30" s="2" t="s">
         <v>22</v>
@@ -3109,8 +3151,8 @@
         <v>761</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
-      <c r="A31" s="97"/>
+    <row r="31" spans="1:18">
+      <c r="A31" s="104"/>
       <c r="B31" s="1" t="s">
         <v>8</v>
       </c>
@@ -3136,8 +3178,8 @@
         <v>0.24596312297574677</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
-      <c r="A32" s="98"/>
+    <row r="32" spans="1:18">
+      <c r="A32" s="105"/>
       <c r="B32" s="1" t="s">
         <v>11</v>
       </c>
@@ -3240,7 +3282,7 @@
       </c>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="96" t="s">
+      <c r="A38" s="103" t="s">
         <v>24</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -3256,7 +3298,7 @@
       </c>
     </row>
     <row r="39" spans="1:14">
-      <c r="A39" s="97"/>
+      <c r="A39" s="104"/>
       <c r="B39" s="1" t="s">
         <v>12</v>
       </c>
@@ -3272,14 +3314,14 @@
       </c>
     </row>
     <row r="40" spans="1:14">
-      <c r="A40" s="97"/>
+      <c r="A40" s="104"/>
       <c r="B40" s="1"/>
       <c r="C40" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:14">
-      <c r="A41" s="97"/>
+      <c r="A41" s="104"/>
       <c r="B41" s="1"/>
       <c r="C41" s="3"/>
       <c r="D41" s="11" t="s">
@@ -3287,7 +3329,7 @@
       </c>
     </row>
     <row r="42" spans="1:14">
-      <c r="A42" s="97"/>
+      <c r="A42" s="104"/>
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
       <c r="E42" s="19" t="s">
@@ -3295,7 +3337,7 @@
       </c>
     </row>
     <row r="43" spans="1:14">
-      <c r="A43" s="97"/>
+      <c r="A43" s="104"/>
       <c r="B43" s="1"/>
       <c r="C43" s="3"/>
       <c r="E43" s="19" t="s">
@@ -3303,28 +3345,28 @@
       </c>
     </row>
     <row r="44" spans="1:14">
-      <c r="A44" s="97"/>
+      <c r="A44" s="104"/>
       <c r="B44" s="1"/>
       <c r="C44" s="3"/>
       <c r="D44" s="19"/>
       <c r="E44" s="27"/>
     </row>
     <row r="45" spans="1:14">
-      <c r="A45" s="97"/>
+      <c r="A45" s="104"/>
       <c r="B45" s="1"/>
       <c r="C45" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:14">
-      <c r="A46" s="97"/>
+      <c r="A46" s="104"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="6"/>
       <c r="E46" s="25"/>
     </row>
     <row r="47" spans="1:14">
-      <c r="A47" s="97"/>
+      <c r="A47" s="104"/>
       <c r="B47" s="1" t="s">
         <v>10</v>
       </c>
@@ -3340,7 +3382,7 @@
       </c>
     </row>
     <row r="48" spans="1:14">
-      <c r="A48" s="98"/>
+      <c r="A48" s="105"/>
       <c r="B48" s="1"/>
       <c r="C48" s="2" t="s">
         <v>17</v>
@@ -3472,7 +3514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -3523,7 +3565,7 @@
       <c r="E2">
         <v>6750</v>
       </c>
-      <c r="F2" s="113">
+      <c r="F2" s="96">
         <f>(B2*C2)/E2</f>
         <v>0.3034074074074074</v>
       </c>
@@ -3545,7 +3587,7 @@
       <c r="E3">
         <v>2762</v>
       </c>
-      <c r="F3" s="113">
+      <c r="F3" s="96">
         <f t="shared" ref="F3:F17" si="1">(B3*C3)/E3</f>
         <v>0.18537291817523532</v>
       </c>
@@ -3567,7 +3609,7 @@
       <c r="E4">
         <v>15180</v>
       </c>
-      <c r="F4" s="113">
+      <c r="F4" s="96">
         <f t="shared" si="1"/>
         <v>0.26982872200263502</v>
       </c>
@@ -3589,7 +3631,7 @@
       <c r="E5">
         <v>15867</v>
       </c>
-      <c r="F5" s="113">
+      <c r="F5" s="96">
         <f t="shared" si="1"/>
         <v>0.51629167454465241</v>
       </c>
@@ -3611,7 +3653,7 @@
       <c r="E6">
         <v>8451</v>
       </c>
-      <c r="F6" s="113">
+      <c r="F6" s="96">
         <f t="shared" si="1"/>
         <v>0.48467636966039523</v>
       </c>
@@ -3633,7 +3675,7 @@
       <c r="E7">
         <v>9182</v>
       </c>
-      <c r="F7" s="113">
+      <c r="F7" s="96">
         <f t="shared" si="1"/>
         <v>0.89218035286429975</v>
       </c>
@@ -3655,7 +3697,7 @@
       <c r="E8">
         <v>118814</v>
       </c>
-      <c r="F8" s="113">
+      <c r="F8" s="96">
         <f t="shared" si="1"/>
         <v>4.4126786405642431</v>
       </c>
@@ -3677,7 +3719,7 @@
       <c r="E9">
         <v>8301</v>
       </c>
-      <c r="F9" s="113">
+      <c r="F9" s="96">
         <f t="shared" si="1"/>
         <v>3.947476207685821</v>
       </c>
@@ -3699,26 +3741,26 @@
       <c r="E10">
         <v>8726</v>
       </c>
-      <c r="F10" s="113">
+      <c r="F10" s="96">
         <f t="shared" si="1"/>
         <v>3.7552143020857209</v>
       </c>
       <c r="H10" s="53"/>
-      <c r="I10" s="103" t="s">
+      <c r="I10" s="110" t="s">
         <v>82</v>
       </c>
-      <c r="J10" s="104"/>
-      <c r="K10" s="105"/>
-      <c r="L10" s="106" t="s">
+      <c r="J10" s="111"/>
+      <c r="K10" s="112"/>
+      <c r="L10" s="113" t="s">
         <v>84</v>
       </c>
-      <c r="M10" s="107"/>
-      <c r="N10" s="108"/>
-      <c r="O10" s="106" t="s">
+      <c r="M10" s="114"/>
+      <c r="N10" s="115"/>
+      <c r="O10" s="113" t="s">
         <v>83</v>
       </c>
-      <c r="P10" s="107"/>
-      <c r="Q10" s="108"/>
+      <c r="P10" s="114"/>
+      <c r="Q10" s="115"/>
       <c r="R10" s="55" t="s">
         <v>85</v>
       </c>
@@ -3742,7 +3784,7 @@
       <c r="E11">
         <v>14726</v>
       </c>
-      <c r="F11" s="113">
+      <c r="F11" s="96">
         <f t="shared" si="1"/>
         <v>4.45035990764634</v>
       </c>
@@ -3777,7 +3819,7 @@
       <c r="E12">
         <v>27288</v>
       </c>
-      <c r="F12" s="113">
+      <c r="F12" s="96">
         <f t="shared" si="1"/>
         <v>4.8032834945763705</v>
       </c>
@@ -3812,7 +3854,7 @@
       <c r="E13">
         <v>10836</v>
       </c>
-      <c r="F13" s="113">
+      <c r="F13" s="96">
         <f t="shared" si="1"/>
         <v>3.0239940937615355</v>
       </c>
@@ -3871,7 +3913,7 @@
       <c r="E14">
         <v>16342</v>
       </c>
-      <c r="F14" s="114">
+      <c r="F14" s="97">
         <f t="shared" si="1"/>
         <v>4.0102802594541673</v>
       </c>
@@ -3906,7 +3948,7 @@
       <c r="E15">
         <v>27577</v>
       </c>
-      <c r="F15" s="115">
+      <c r="F15" s="98">
         <f t="shared" si="1"/>
         <v>4.7529462958262316</v>
       </c>
@@ -3941,7 +3983,7 @@
       <c r="E16">
         <v>51313</v>
       </c>
-      <c r="F16" s="113">
+      <c r="F16" s="96">
         <f t="shared" si="1"/>
         <v>5.1087248845321849</v>
       </c>
@@ -3976,7 +4018,7 @@
       <c r="E17">
         <v>9919</v>
       </c>
-      <c r="F17" s="113">
+      <c r="F17" s="96">
         <f t="shared" si="1"/>
         <v>3.3035588264946063</v>
       </c>
@@ -4312,16 +4354,16 @@
       </c>
       <c r="J30" s="79"/>
       <c r="K30" s="79"/>
-      <c r="L30" s="102" t="s">
+      <c r="L30" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="M30" s="102"/>
-      <c r="N30" s="102"/>
-      <c r="O30" s="102" t="s">
+      <c r="M30" s="109"/>
+      <c r="N30" s="109"/>
+      <c r="O30" s="109" t="s">
         <v>83</v>
       </c>
-      <c r="P30" s="102"/>
-      <c r="Q30" s="102"/>
+      <c r="P30" s="109"/>
+      <c r="Q30" s="109"/>
       <c r="R30" s="56" t="s">
         <v>85</v>
       </c>

</xml_diff>

<commit_message>
feat(HW Parameter.excel): Add Energy Consumption
</commit_message>
<xml_diff>
--- a/hardware/docs/01-top/点云硬件参数分析.xlsx
+++ b/hardware/docs/01-top/点云硬件参数分析.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="12960" windowHeight="4872" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="12960" windowHeight="4872"/>
   </bookViews>
   <sheets>
     <sheet name="整体评估" sheetId="5" r:id="rId1"/>
@@ -468,7 +468,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="125">
   <si>
     <t>case</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1010,6 +1010,10 @@
   </si>
   <si>
     <t>GLB (32bank, Bitwidth256, Word128, WR2, RD2, PAR2,)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Energy consumption (J/frame)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2153,8 +2157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
@@ -2389,7 +2393,13 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="35"/>
+      <c r="A18" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" s="92">
+        <f>B11*(B15*5*10^(-9))</f>
+        <v>6.9120000000000009E-6</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="14.4" thickBot="1">
       <c r="A21" s="32" t="s">
@@ -2492,8 +2502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="P4" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="5" ySplit="3" topLeftCell="P25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="Q4" sqref="Q4"/>

</xml_diff>

<commit_message>
feat(HW Parameter excel): Compare area, storage, and BW of 16-pair Dual Port SRAM and 32 SPSRAM
</commit_message>
<xml_diff>
--- a/hardware/docs/01-top/点云硬件参数分析.xlsx
+++ b/hardware/docs/01-top/点云硬件参数分析.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="12960" windowHeight="4872"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="12960" windowHeight="4872" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="整体评估" sheetId="5" r:id="rId1"/>
@@ -437,7 +437,115 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="0" shapeId="0">
+    <comment ref="H8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+与原先16块单口128wordx256bit容量相等，读写带宽因可同时而加倍，互联/块数一致；总之面积(0.55+0.16)/0.48=1.5倍，读写带宽2倍，划算
+与原始32块单口128wordx256bit相比，读写总带宽不变，减半，面积(0.55+0.16)/1.27=0.56</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+与原始32块单口128wordx256bit相比，读写总带宽不变，容量不变，面积(0.64+0.16)/1.27=0.63</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+作者:
+与原先16块单口128wordx256bit容量4倍，读写带宽因可同时而加倍，互联/块数一致；总之面积(0.82+0.16)/0.48=2倍，读写带宽2倍，容量4倍，划算
+与原始32块单口128wordx256bit相比，读写总带宽不变，容量倍，面积(0.82+0.16)/1.27=0.77
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+容量过于大了，256KB了</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -463,12 +571,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="F29" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+最合适的了，既带宽大，又密度高是双口的两倍</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="133">
   <si>
     <t>case</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -773,10 +907,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>宽</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Chip Size</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -789,30 +919,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Plan A: 单圈PAD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Plan B: 双圈PAD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Plan B: 交错圈PAD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Plan C: 双圈交错PAD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Core利用率</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PAD个数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PAD/Core</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -837,23 +943,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PAD单个长</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PAD SIZE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>高</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Plan B: 交错单圈PAD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PAD总长度</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1016,6 +1106,276 @@
     <t>Energy consumption (J/frame)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Plan A: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>单圈</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>PAD</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Plan B: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>交错圈</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>PAD</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Plan B: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>双圈</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>PAD</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Plan C: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>双圈交错</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>PAD</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>宽</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>高</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>PAD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>个数</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>PAD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>单个长</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Core</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>利用率</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Core</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>利用率</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Plan B: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>交错单圈</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>PAD</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>PAD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>总长度</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>PAD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>个数</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Core</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>利用率</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Density Increase </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Area of 32 banks (16 Pairs)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Area reduction rate Compared to SP128wordx256bitx32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Area increase rate Compared to SP128wordx256bitx32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total area including interconnnect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1028,7 +1388,7 @@
     <numFmt numFmtId="179" formatCode="0.0_ "/>
     <numFmt numFmtId="180" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1108,53 +1468,6 @@
       <family val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0" tint="-0.249977111117893"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0" tint="-0.249977111117893"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -1166,6 +1479,51 @@
       <color rgb="FFD4D4D4"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1590,7 +1948,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1742,19 +2100,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1764,117 +2109,136 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="180" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="180" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="180" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2157,11 +2521,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56.44140625" style="29" customWidth="1"/>
     <col min="2" max="2" width="25.33203125" style="29" customWidth="1"/>
@@ -2169,29 +2533,29 @@
     <col min="4" max="16384" width="8.88671875" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="39"/>
       <c r="B1" s="41" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C1" s="40" t="s">
         <v>65</v>
       </c>
       <c r="D1" s="30"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>64</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D2" s="30"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>63</v>
       </c>
@@ -2203,7 +2567,7 @@
       </c>
       <c r="D3" s="30"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>62</v>
       </c>
@@ -2215,20 +2579,20 @@
       </c>
       <c r="D4" s="30"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
         <v>60</v>
       </c>
       <c r="B5" s="45" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C5" s="44" t="s">
         <v>59</v>
       </c>
       <c r="D5" s="30"/>
-      <c r="G5" s="90"/>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="G5" s="56"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
         <v>75</v>
       </c>
@@ -2239,9 +2603,9 @@
         <v>74</v>
       </c>
       <c r="D6" s="30"/>
-      <c r="G6" s="90"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="G6" s="56"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
         <v>58</v>
       </c>
@@ -2252,9 +2616,9 @@
         <v>250</v>
       </c>
       <c r="D7" s="30"/>
-      <c r="G7" s="90"/>
-    </row>
-    <row r="8" spans="1:7" ht="14.4" thickBot="1">
+      <c r="G7" s="56"/>
+    </row>
+    <row r="8" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="35" t="s">
         <v>57</v>
       </c>
@@ -2265,9 +2629,9 @@
         <v>55</v>
       </c>
       <c r="D8" s="30"/>
-      <c r="G8" s="90"/>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="G8" s="56"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="39" t="s">
         <v>51</v>
       </c>
@@ -2278,9 +2642,9 @@
         <v>12288</v>
       </c>
       <c r="D9" s="30"/>
-      <c r="G9" s="90"/>
-    </row>
-    <row r="10" spans="1:7" ht="14.4" thickBot="1">
+      <c r="G9" s="56"/>
+    </row>
+    <row r="10" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="32" t="s">
         <v>54</v>
       </c>
@@ -2291,11 +2655,11 @@
         <v>53</v>
       </c>
       <c r="D10" s="30"/>
-      <c r="G10" s="90"/>
-    </row>
-    <row r="11" spans="1:7" ht="14.4" thickBot="1">
+      <c r="G10" s="56"/>
+    </row>
+    <row r="11" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="35" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B11" s="36">
         <v>0.15</v>
@@ -2304,23 +2668,23 @@
         <v>0.60899999999999999</v>
       </c>
       <c r="D11" s="30"/>
-      <c r="G11" s="90"/>
-    </row>
-    <row r="12" spans="1:7" ht="14.4" thickBot="1">
+      <c r="G11" s="56"/>
+    </row>
+    <row r="12" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="B12" s="93">
+        <v>97</v>
+      </c>
+      <c r="B12" s="59">
         <f>3.6/1024</f>
         <v>3.5156250000000001E-3</v>
       </c>
-      <c r="C12" s="91" t="s">
-        <v>112</v>
+      <c r="C12" s="57" t="s">
+        <v>101</v>
       </c>
       <c r="D12" s="30"/>
-      <c r="G12" s="90"/>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="G12" s="56"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="39" t="s">
         <v>72</v>
       </c>
@@ -2333,9 +2697,9 @@
         <v>5.859375</v>
       </c>
       <c r="D13" s="30"/>
-      <c r="G13" s="90"/>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="G13" s="56"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
         <v>73</v>
       </c>
@@ -2348,60 +2712,60 @@
         <v>9.6213054187192117</v>
       </c>
       <c r="D14" s="30"/>
-      <c r="G14" s="90"/>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="G14" s="56"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
-        <v>109</v>
-      </c>
-      <c r="B15" s="94">
+        <v>98</v>
+      </c>
+      <c r="B15" s="60">
         <f>9*1024</f>
         <v>9216</v>
       </c>
-      <c r="C15" s="80" t="s">
-        <v>112</v>
+      <c r="C15" s="54" t="s">
+        <v>101</v>
       </c>
       <c r="D15" s="30"/>
-      <c r="G15" s="90"/>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="G15" s="56"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="B16" s="81">
+        <v>99</v>
+      </c>
+      <c r="B16" s="55">
         <f>B12/(B15*5*10^(-9))</f>
         <v>76.293945312499986</v>
       </c>
-      <c r="C16" s="80">
+      <c r="C16" s="54">
         <f>C23/C11</f>
         <v>19.047619047619047</v>
       </c>
       <c r="D16" s="30"/>
-      <c r="G16" s="90"/>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="G16" s="56"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="35" t="s">
-        <v>111</v>
-      </c>
-      <c r="B17" s="95">
+        <v>100</v>
+      </c>
+      <c r="B17" s="61">
         <f>B16/B14</f>
         <v>29.296874999999993</v>
       </c>
-      <c r="C17" s="92">
+      <c r="C17" s="58">
         <f>C16/C14</f>
         <v>1.9797333333333333</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="35" t="s">
-        <v>124</v>
-      </c>
-      <c r="B18" s="92">
+        <v>113</v>
+      </c>
+      <c r="B18" s="58">
         <f>B11*(B15*5*10^(-9))</f>
         <v>6.9120000000000009E-6</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14.4" thickBot="1">
+    <row r="21" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="32" t="s">
         <v>76</v>
       </c>
@@ -2410,21 +2774,21 @@
         <f>C25/4*(1.1/0.9)^2</f>
         <v>7.1134626690182259</v>
       </c>
-      <c r="G21" s="90"/>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="G21" s="56"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B22" s="29">
         <f>B24/B13</f>
         <v>40</v>
       </c>
-      <c r="G22" s="90"/>
-    </row>
-    <row r="23" spans="1:7" ht="14.4">
+      <c r="G22" s="56"/>
+    </row>
+    <row r="23" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A23" s="35" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B23" s="34">
         <f>B13*10</f>
@@ -2434,11 +2798,11 @@
         <v>11.6</v>
       </c>
       <c r="D23" s="30"/>
-      <c r="G23" s="90"/>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="G23" s="56"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B24" s="34">
         <f>B23*4</f>
@@ -2446,9 +2810,9 @@
       </c>
       <c r="C24" s="49"/>
       <c r="D24" s="30"/>
-      <c r="G24" s="90"/>
-    </row>
-    <row r="25" spans="1:7" ht="14.4" thickBot="1">
+      <c r="G24" s="56"/>
+    </row>
+    <row r="25" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="32" t="s">
         <v>50</v>
       </c>
@@ -2461,31 +2825,31 @@
         <v>19.047619047619047</v>
       </c>
       <c r="D25" s="30"/>
-      <c r="G25" s="90"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="G26" s="90"/>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="G27" s="90"/>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="G28" s="90"/>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="G29" s="90"/>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="G30" s="90"/>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="G31" s="90"/>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="G32" s="90"/>
-    </row>
-    <row r="33" spans="7:7">
-      <c r="G33" s="90"/>
+      <c r="G25" s="56"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G26" s="56"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G27" s="56"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G28" s="56"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G29" s="56"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G30" s="56"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G31" s="56"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G32" s="56"/>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G33" s="56"/>
     </row>
   </sheetData>
   <sortState ref="A40:G72">
@@ -2503,13 +2867,13 @@
   <dimension ref="A1:T60"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="P25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="P4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q4" sqref="Q4"/>
+      <selection pane="bottomRight" activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="19.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.88671875" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.21875" style="2" customWidth="1"/>
@@ -2528,29 +2892,29 @@
     <col min="18" max="16384" width="19.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
-      <c r="E1" s="64"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="99" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="100"/>
-      <c r="L1" s="100"/>
-      <c r="M1" s="100"/>
-      <c r="N1" s="100"/>
-      <c r="O1" s="101"/>
-      <c r="P1" s="102" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q1" s="100"/>
-      <c r="R1" s="100"/>
-      <c r="S1" s="100"/>
-      <c r="T1" s="101"/>
-    </row>
-    <row r="2" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E1" s="51"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="62" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="65" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="64"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2558,14 +2922,14 @@
       <c r="C2" s="1"/>
       <c r="D2" s="6"/>
       <c r="E2" s="24"/>
-      <c r="F2" s="106">
+      <c r="F2" s="69">
         <v>0</v>
       </c>
-      <c r="G2" s="107"/>
-      <c r="H2" s="106">
+      <c r="G2" s="70"/>
+      <c r="H2" s="69">
         <v>1</v>
       </c>
-      <c r="I2" s="107"/>
+      <c r="I2" s="70"/>
       <c r="J2" s="8">
         <v>2</v>
       </c>
@@ -2582,7 +2946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="13.95" customHeight="1">
+    <row r="3" spans="1:20" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
@@ -2590,18 +2954,18 @@
       <c r="C3" s="1"/>
       <c r="D3" s="6"/>
       <c r="E3" s="25"/>
-      <c r="F3" s="99" t="s">
+      <c r="F3" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="108"/>
-      <c r="H3" s="99" t="s">
+      <c r="G3" s="71"/>
+      <c r="H3" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="108"/>
-      <c r="J3" s="99" t="s">
+      <c r="I3" s="71"/>
+      <c r="J3" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="101"/>
+      <c r="K3" s="64"/>
       <c r="L3" s="2" t="s">
         <v>41</v>
       </c>
@@ -2609,16 +2973,16 @@
         <v>48</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="41.4">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2641,16 +3005,16 @@
         <v>47</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2676,7 +3040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="56.4" customHeight="1">
+    <row r="6" spans="1:20" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2693,7 +3057,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2716,7 +3080,7 @@
         <v>1768</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="46"/>
       <c r="B8" s="1" t="s">
         <v>66</v>
@@ -2737,8 +3101,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
-      <c r="A9" s="103" t="s">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="66" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2765,8 +3129,8 @@
         <v>1101607</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
-      <c r="A10" s="104"/>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="67"/>
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
@@ -2791,8 +3155,8 @@
         <v>1.7485726911987398</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
-      <c r="A11" s="104"/>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="67"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
         <v>15</v>
@@ -2814,8 +3178,8 @@
         <v>745</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
-      <c r="A12" s="104"/>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="67"/>
       <c r="B12" s="1"/>
       <c r="C12" s="3"/>
       <c r="D12" s="11" t="s">
@@ -2826,8 +3190,8 @@
         <v>19250</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
-      <c r="A13" s="104"/>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="67"/>
       <c r="B13" s="1"/>
       <c r="C13" s="3"/>
       <c r="E13" s="19" t="s">
@@ -2841,8 +3205,8 @@
         <v>6660</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
-      <c r="A14" s="104"/>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="67"/>
       <c r="B14" s="1"/>
       <c r="C14" s="3"/>
       <c r="E14" s="19" t="s">
@@ -2855,16 +3219,16 @@
         <v>1419</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
-      <c r="A15" s="104"/>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="67"/>
       <c r="B15" s="1"/>
       <c r="C15" s="3"/>
       <c r="D15" s="19"/>
       <c r="E15" s="27"/>
       <c r="H15" s="15"/>
     </row>
-    <row r="16" spans="1:20">
-      <c r="A16" s="104"/>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="67"/>
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
         <v>16</v>
@@ -2886,15 +3250,15 @@
         <v>6041</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
-      <c r="A17" s="104"/>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="67"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="6"/>
       <c r="E17" s="25"/>
     </row>
-    <row r="18" spans="1:18">
-      <c r="A18" s="104"/>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="67"/>
       <c r="B18" s="1" t="s">
         <v>10</v>
       </c>
@@ -2932,8 +3296,8 @@
         <v>443245</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
-      <c r="A19" s="104"/>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="67"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
         <v>17</v>
@@ -2964,8 +3328,8 @@
         <v>10021</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
-      <c r="A20" s="104"/>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="67"/>
       <c r="B20" s="1"/>
       <c r="C20" s="2" t="s">
         <v>39</v>
@@ -2975,8 +3339,8 @@
         <v>0.193</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
-      <c r="A21" s="104"/>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="67"/>
       <c r="B21" s="1"/>
       <c r="C21" s="2" t="s">
         <v>40</v>
@@ -2986,8 +3350,8 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
-      <c r="A22" s="104"/>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="67"/>
       <c r="B22" s="1" t="s">
         <v>13</v>
       </c>
@@ -3016,8 +3380,8 @@
         <v>10849</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
-      <c r="A23" s="104"/>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="67"/>
       <c r="B23" s="1"/>
       <c r="C23" s="2" t="s">
         <v>18</v>
@@ -3037,8 +3401,8 @@
         <v>0.33747879510338818</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
-      <c r="A24" s="104"/>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="67"/>
       <c r="B24" s="1"/>
       <c r="D24" s="7" t="s">
         <v>43</v>
@@ -3052,8 +3416,8 @@
         <v>0.76429032367625582</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="27.6">
-      <c r="A25" s="104"/>
+    <row r="25" spans="1:18" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A25" s="67"/>
       <c r="B25" s="1"/>
       <c r="E25" s="7" t="s">
         <v>42</v>
@@ -3067,8 +3431,8 @@
         <v>0.90067990934542064</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
-      <c r="A26" s="104"/>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="67"/>
       <c r="B26" s="1"/>
       <c r="C26" s="2" t="s">
         <v>19</v>
@@ -3084,8 +3448,8 @@
         <v>0.63920728072990696</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
-      <c r="A27" s="104"/>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="67"/>
       <c r="B27" s="1"/>
       <c r="C27" s="2" t="s">
         <v>20</v>
@@ -3098,8 +3462,8 @@
         <v>18589</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
-      <c r="A28" s="104"/>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="67"/>
       <c r="B28" s="1" t="s">
         <v>9</v>
       </c>
@@ -3128,8 +3492,8 @@
         <v>3678</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
-      <c r="A29" s="104"/>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="67"/>
       <c r="B29" s="1"/>
       <c r="C29" s="2" t="s">
         <v>21</v>
@@ -3148,8 +3512,8 @@
         <v>11719</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
-      <c r="A30" s="104"/>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="67"/>
       <c r="B30" s="1"/>
       <c r="C30" s="2" t="s">
         <v>22</v>
@@ -3161,8 +3525,8 @@
         <v>761</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
-      <c r="A31" s="104"/>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="67"/>
       <c r="B31" s="1" t="s">
         <v>8</v>
       </c>
@@ -3188,8 +3552,8 @@
         <v>0.24596312297574677</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
-      <c r="A32" s="105"/>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="68"/>
       <c r="B32" s="1" t="s">
         <v>11</v>
       </c>
@@ -3221,7 +3585,7 @@
         <v>518399</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="1"/>
       <c r="C33" s="2" t="s">
@@ -3238,7 +3602,7 @@
         <v>44581</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="1"/>
       <c r="C34" s="2" t="s">
@@ -3255,7 +3619,7 @@
         <v>114849</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="13.95" customHeight="1">
+    <row r="35" spans="1:14" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="D35" s="7" t="s">
         <v>44</v>
@@ -3267,7 +3631,7 @@
         <v>7094</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="E36" s="26" t="s">
         <v>45</v>
@@ -3279,7 +3643,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="E37" s="25" t="s">
         <v>46</v>
@@ -3291,8 +3655,8 @@
         <v>689</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
-      <c r="A38" s="103" t="s">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="66" t="s">
         <v>24</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -3307,8 +3671,8 @@
         <v>74.7</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
-      <c r="A39" s="104"/>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="67"/>
       <c r="B39" s="1" t="s">
         <v>12</v>
       </c>
@@ -3323,60 +3687,60 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="40" spans="1:14">
-      <c r="A40" s="104"/>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="67"/>
       <c r="B40" s="1"/>
       <c r="C40" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
-      <c r="A41" s="104"/>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="67"/>
       <c r="B41" s="1"/>
       <c r="C41" s="3"/>
       <c r="D41" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:14">
-      <c r="A42" s="104"/>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="67"/>
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
       <c r="E42" s="19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
-      <c r="A43" s="104"/>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="67"/>
       <c r="B43" s="1"/>
       <c r="C43" s="3"/>
       <c r="E43" s="19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
-      <c r="A44" s="104"/>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="67"/>
       <c r="B44" s="1"/>
       <c r="C44" s="3"/>
       <c r="D44" s="19"/>
       <c r="E44" s="27"/>
     </row>
-    <row r="45" spans="1:14">
-      <c r="A45" s="104"/>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="67"/>
       <c r="B45" s="1"/>
       <c r="C45" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:14">
-      <c r="A46" s="104"/>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="67"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="6"/>
       <c r="E46" s="25"/>
     </row>
-    <row r="47" spans="1:14">
-      <c r="A47" s="104"/>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="67"/>
       <c r="B47" s="1" t="s">
         <v>10</v>
       </c>
@@ -3391,26 +3755,26 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
-      <c r="A48" s="105"/>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="68"/>
       <c r="B48" s="1"/>
       <c r="C48" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="2:15">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="C49" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="2:15">
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="C50" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="2:15">
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
         <v>13</v>
       </c>
@@ -3425,25 +3789,25 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="52" spans="2:15">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="2:15">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="C53" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="2:15">
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="C54" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="2:15">
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
         <v>9</v>
       </c>
@@ -3454,19 +3818,19 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="56" spans="2:15">
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="C56" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="2:15">
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
       <c r="C57" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="2:15">
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
         <v>8</v>
       </c>
@@ -3477,7 +3841,7 @@
         <v>6.7000000000000004E-2</v>
       </c>
     </row>
-    <row r="59" spans="2:15">
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
         <v>11</v>
       </c>
@@ -3496,7 +3860,7 @@
         <v>0.79250334672021416</v>
       </c>
     </row>
-    <row r="60" spans="2:15">
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O60" s="2" t="s">
         <v>49</v>
       </c>
@@ -3522,1217 +3886,1630 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T43"/>
+  <dimension ref="A1:AL71"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" customWidth="1"/>
-    <col min="2" max="4" width="11.21875" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.21875" customWidth="1"/>
-    <col min="11" max="11" width="12.77734375" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="76" customWidth="1"/>
+    <col min="2" max="4" width="11.21875" style="76" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="76" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="76" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="76"/>
+    <col min="8" max="9" width="12.21875" style="76" customWidth="1"/>
+    <col min="10" max="11" width="8.88671875" style="76"/>
+    <col min="12" max="12" width="12.77734375" style="76" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="76"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
-      <c r="A1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
-      <c r="A2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="72" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="72" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="72" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="72" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="72" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="72" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="76" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" s="76" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1" s="76" t="s">
+        <v>132</v>
+      </c>
+      <c r="J1" s="76" t="s">
+        <v>130</v>
+      </c>
+      <c r="K1" s="76" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="72" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="72">
         <v>2048</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="72">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="72">
         <f>B2*C2/8192</f>
         <v>0.25</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="72">
         <v>6750</v>
       </c>
-      <c r="F2" s="96">
+      <c r="F2" s="73">
         <f>(B2*C2)/E2</f>
         <v>0.3034074074074074</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
-      <c r="A3" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="72">
         <v>32</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="72">
         <v>16</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D17" si="0">B3*C3/8192</f>
+      <c r="D3" s="72">
+        <f t="shared" ref="D3:D29" si="0">B3*C3/8192</f>
         <v>6.25E-2</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="72">
         <v>2762</v>
       </c>
-      <c r="F3" s="96">
-        <f t="shared" ref="F3:F17" si="1">(B3*C3)/E3</f>
+      <c r="F3" s="73">
+        <f t="shared" ref="F3:F29" si="1">(B3*C3)/E3</f>
         <v>0.18537291817523532</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
-      <c r="A4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="74"/>
+      <c r="B4" s="72">
         <v>32</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="72">
         <v>128</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="72">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="72">
         <v>15180</v>
       </c>
-      <c r="F4" s="96">
+      <c r="F4" s="73">
         <f t="shared" si="1"/>
         <v>0.26982872200263502</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
-      <c r="A5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="74"/>
+      <c r="B5" s="72">
         <v>64</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="72">
         <v>128</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="72">
         <v>15867</v>
       </c>
-      <c r="F5" s="96">
+      <c r="F5" s="73">
         <f t="shared" si="1"/>
         <v>0.51629167454465241</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
-      <c r="A6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="74"/>
+      <c r="B6" s="72">
         <v>64</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="72">
         <v>64</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="72">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="72">
         <v>8451</v>
       </c>
-      <c r="F6" s="96">
+      <c r="F6" s="73">
         <f t="shared" si="1"/>
         <v>0.48467636966039523</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
-      <c r="A7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B7">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="74"/>
+      <c r="B7" s="72">
         <v>128</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="72">
         <v>64</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="72">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="72">
         <v>9182</v>
       </c>
-      <c r="F7" s="96">
+      <c r="F7" s="118">
         <f t="shared" si="1"/>
         <v>0.89218035286429975</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
-      <c r="A8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B8">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="74"/>
+      <c r="B8" s="72">
+        <v>128</v>
+      </c>
+      <c r="C8" s="72">
+        <v>128</v>
+      </c>
+      <c r="D8" s="72">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E8" s="72">
+        <v>17239</v>
+      </c>
+      <c r="F8" s="118">
+        <f t="shared" si="1"/>
+        <v>0.95040315563547773</v>
+      </c>
+      <c r="H8" s="76">
+        <f>E8*32/1000000</f>
+        <v>0.55164800000000003</v>
+      </c>
+      <c r="I8" s="76">
+        <f>H8+0.16</f>
+        <v>0.71164800000000006</v>
+      </c>
+      <c r="J8" s="76">
+        <f>(1.27-(H8+0.16))/1.27</f>
+        <v>0.43964724409448813</v>
+      </c>
+      <c r="K8" s="76">
+        <f>(D8-4)/4</f>
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="74"/>
+      <c r="B9" s="115">
+        <v>256</v>
+      </c>
+      <c r="C9" s="115">
+        <v>128</v>
+      </c>
+      <c r="D9" s="115">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E9" s="115">
+        <v>19964</v>
+      </c>
+      <c r="F9" s="118">
+        <f t="shared" si="1"/>
+        <v>1.6413544379883791</v>
+      </c>
+      <c r="G9" s="119">
+        <f>(F9-F8)/F8</f>
+        <v>0.72700861550791418</v>
+      </c>
+      <c r="H9" s="119">
+        <f t="shared" ref="H9:H13" si="2">E9*32/1000000</f>
+        <v>0.63884799999999997</v>
+      </c>
+      <c r="I9" s="119">
+        <f t="shared" ref="I9:I13" si="3">H9+0.16</f>
+        <v>0.798848</v>
+      </c>
+      <c r="J9" s="119">
+        <f t="shared" ref="J9:J10" si="4">(1.27-(H9+0.16))/1.27</f>
+        <v>0.37098582677165354</v>
+      </c>
+      <c r="K9" s="119">
+        <f t="shared" ref="K9:K10" si="5">(D9-4)/4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="74"/>
+      <c r="B10" s="114">
+        <v>512</v>
+      </c>
+      <c r="C10" s="114">
+        <v>128</v>
+      </c>
+      <c r="D10" s="114">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E10" s="114">
+        <v>25586</v>
+      </c>
+      <c r="F10" s="75">
+        <f t="shared" si="1"/>
+        <v>2.5614007660439304</v>
+      </c>
+      <c r="G10" s="103">
+        <f t="shared" ref="G10:G13" si="6">(F10-F9)/F9</f>
+        <v>0.56054092081607132</v>
+      </c>
+      <c r="H10" s="103">
+        <f t="shared" si="2"/>
+        <v>0.81875200000000004</v>
+      </c>
+      <c r="I10" s="76">
+        <f t="shared" si="3"/>
+        <v>0.97875200000000007</v>
+      </c>
+      <c r="J10" s="76">
+        <f t="shared" si="4"/>
+        <v>0.22932913385826767</v>
+      </c>
+      <c r="K10" s="76">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="74"/>
+      <c r="B11" s="72">
+        <v>1024</v>
+      </c>
+      <c r="C11" s="72">
+        <v>128</v>
+      </c>
+      <c r="D11" s="72">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E11" s="72">
+        <v>36545</v>
+      </c>
+      <c r="F11" s="73">
+        <f t="shared" si="1"/>
+        <v>3.5865918730332469</v>
+      </c>
+      <c r="G11" s="76">
+        <f t="shared" si="6"/>
+        <v>0.40024627171979754</v>
+      </c>
+      <c r="H11" s="76">
+        <f t="shared" si="2"/>
+        <v>1.16944</v>
+      </c>
+      <c r="I11" s="76">
+        <f t="shared" si="3"/>
+        <v>1.32944</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="74"/>
+      <c r="B12" s="72">
+        <v>2048</v>
+      </c>
+      <c r="C12" s="72">
+        <v>128</v>
+      </c>
+      <c r="D12" s="72">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="E12" s="72">
+        <v>63968</v>
+      </c>
+      <c r="F12" s="73">
+        <f t="shared" si="1"/>
+        <v>4.0980490245122558</v>
+      </c>
+      <c r="G12" s="76">
+        <f t="shared" si="6"/>
+        <v>0.14260255127563767</v>
+      </c>
+      <c r="H12" s="76">
+        <f t="shared" si="2"/>
+        <v>2.0469759999999999</v>
+      </c>
+      <c r="I12" s="76">
+        <f t="shared" si="3"/>
+        <v>2.206976</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="74"/>
+      <c r="B13" s="72">
         <v>4096</v>
       </c>
-      <c r="C8">
+      <c r="C13" s="72">
         <v>128</v>
       </c>
-      <c r="D8">
+      <c r="D13" s="72">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="E8">
+      <c r="E13" s="72">
         <v>118814</v>
       </c>
-      <c r="F8" s="96">
+      <c r="F13" s="73">
         <f t="shared" si="1"/>
         <v>4.4126786405642431</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" ht="14.4" thickBot="1">
-      <c r="A9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B9">
+      <c r="G13" s="76">
+        <f t="shared" si="6"/>
+        <v>7.6775464170888985E-2</v>
+      </c>
+      <c r="H13" s="76">
+        <f t="shared" si="2"/>
+        <v>3.8020480000000001</v>
+      </c>
+      <c r="I13" s="76">
+        <f t="shared" si="3"/>
+        <v>3.9620480000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="72"/>
+      <c r="B14" s="72"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="73"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="74" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="72">
         <v>1024</v>
       </c>
-      <c r="C9">
+      <c r="C15" s="72">
         <v>32</v>
       </c>
-      <c r="D9">
+      <c r="D15" s="72">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E9">
+      <c r="E15" s="72">
         <v>8301</v>
       </c>
-      <c r="F9" s="96">
+      <c r="F15" s="73">
         <f t="shared" si="1"/>
         <v>3.947476207685821</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="14.4" thickBot="1">
-      <c r="A10" t="s">
-        <v>103</v>
-      </c>
-      <c r="B10">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="74"/>
+      <c r="B16" s="72">
+        <v>128</v>
+      </c>
+      <c r="C16" s="72">
+        <v>64</v>
+      </c>
+      <c r="D16" s="72">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E16" s="72">
+        <v>4316</v>
+      </c>
+      <c r="F16" s="73">
+        <f t="shared" si="1"/>
+        <v>1.8980537534754403</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="74"/>
+      <c r="B17" s="72">
+        <v>256</v>
+      </c>
+      <c r="C17" s="72">
+        <v>64</v>
+      </c>
+      <c r="D17" s="72">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E17" s="72">
+        <v>5786</v>
+      </c>
+      <c r="F17" s="73">
+        <f t="shared" si="1"/>
+        <v>2.8316626339440027</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="74"/>
+      <c r="B18" s="72">
         <v>512</v>
       </c>
-      <c r="C10">
+      <c r="C18" s="72">
         <v>64</v>
       </c>
-      <c r="D10">
+      <c r="D18" s="72">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E10">
+      <c r="E18" s="72">
         <v>8726</v>
       </c>
-      <c r="F10" s="96">
+      <c r="F18" s="73">
         <f t="shared" si="1"/>
         <v>3.7552143020857209</v>
       </c>
-      <c r="H10" s="53"/>
-      <c r="I10" s="110" t="s">
-        <v>82</v>
-      </c>
-      <c r="J10" s="111"/>
-      <c r="K10" s="112"/>
-      <c r="L10" s="113" t="s">
-        <v>84</v>
-      </c>
-      <c r="M10" s="114"/>
-      <c r="N10" s="115"/>
-      <c r="O10" s="113" t="s">
-        <v>83</v>
-      </c>
-      <c r="P10" s="114"/>
-      <c r="Q10" s="115"/>
-      <c r="R10" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="S10" s="56"/>
-      <c r="T10" s="57"/>
-    </row>
-    <row r="11" spans="1:20" ht="14.4" thickBot="1">
-      <c r="A11" t="s">
-        <v>103</v>
-      </c>
-      <c r="B11">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="74"/>
+      <c r="B19" s="72">
         <v>1024</v>
       </c>
-      <c r="C11">
+      <c r="C19" s="72">
         <v>64</v>
       </c>
-      <c r="D11">
+      <c r="D19" s="72">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E11">
+      <c r="E19" s="72">
         <v>14726</v>
       </c>
-      <c r="F11" s="96">
+      <c r="F19" s="73">
         <f t="shared" si="1"/>
         <v>4.45035990764634</v>
       </c>
-      <c r="H11" s="53"/>
-      <c r="I11" s="82"/>
-      <c r="J11" s="83"/>
-      <c r="K11" s="84"/>
-      <c r="L11" s="85"/>
-      <c r="M11" s="86"/>
-      <c r="N11" s="89"/>
-      <c r="O11" s="85"/>
-      <c r="P11" s="86"/>
-      <c r="Q11" s="89"/>
-      <c r="R11" s="55"/>
-      <c r="S11" s="56"/>
-      <c r="T11" s="88"/>
-    </row>
-    <row r="12" spans="1:20" ht="14.4" thickBot="1">
-      <c r="A12" t="s">
-        <v>103</v>
-      </c>
-      <c r="B12">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="74"/>
+      <c r="B20" s="72">
         <v>2048</v>
       </c>
-      <c r="C12">
+      <c r="C20" s="72">
         <v>64</v>
       </c>
-      <c r="D12">
+      <c r="D20" s="72">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="E12">
+      <c r="E20" s="72">
         <v>27288</v>
       </c>
-      <c r="F12" s="96">
+      <c r="F20" s="73">
         <f t="shared" si="1"/>
         <v>4.8032834945763705</v>
       </c>
-      <c r="H12" s="53"/>
-      <c r="I12" s="82"/>
-      <c r="J12" s="83"/>
-      <c r="K12" s="84"/>
-      <c r="L12" s="85"/>
-      <c r="M12" s="86"/>
-      <c r="N12" s="89"/>
-      <c r="O12" s="85"/>
-      <c r="P12" s="86"/>
-      <c r="Q12" s="89"/>
-      <c r="R12" s="55"/>
-      <c r="S12" s="56"/>
-      <c r="T12" s="88"/>
-    </row>
-    <row r="13" spans="1:20">
-      <c r="A13" t="s">
-        <v>103</v>
-      </c>
-      <c r="B13">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="74"/>
+      <c r="B21" s="72">
+        <v>32</v>
+      </c>
+      <c r="C21" s="72">
+        <v>128</v>
+      </c>
+      <c r="D21" s="72">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="E21" s="72">
+        <v>3102</v>
+      </c>
+      <c r="F21" s="73">
+        <f t="shared" si="1"/>
+        <v>1.3204384268214056</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="74"/>
+      <c r="B22" s="72">
+        <v>64</v>
+      </c>
+      <c r="C22" s="72">
+        <v>128</v>
+      </c>
+      <c r="D22" s="72">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E22" s="72">
+        <v>3879</v>
+      </c>
+      <c r="F22" s="73">
+        <f t="shared" si="1"/>
+        <v>2.1118845063160609</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="74"/>
+      <c r="B23" s="72">
+        <v>128</v>
+      </c>
+      <c r="C23" s="72">
+        <v>128</v>
+      </c>
+      <c r="D23" s="72">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E23" s="72">
+        <v>8083</v>
+      </c>
+      <c r="F23" s="73">
+        <f t="shared" si="1"/>
+        <v>2.0269701843374985</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="74"/>
+      <c r="B24" s="72">
         <v>256</v>
       </c>
-      <c r="C13">
+      <c r="C24" s="72">
         <v>128</v>
       </c>
-      <c r="D13">
+      <c r="D24" s="72">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E13">
+      <c r="E24" s="72">
         <v>10836</v>
       </c>
-      <c r="F13" s="96">
+      <c r="F24" s="75">
         <f t="shared" si="1"/>
         <v>3.0239940937615355</v>
       </c>
-      <c r="H13" s="53"/>
-      <c r="I13" s="55" t="s">
-        <v>78</v>
-      </c>
-      <c r="J13" s="56" t="s">
-        <v>96</v>
-      </c>
-      <c r="K13" s="57" t="s">
-        <v>87</v>
-      </c>
-      <c r="L13" s="55" t="s">
-        <v>78</v>
-      </c>
-      <c r="M13" s="56" t="s">
-        <v>96</v>
-      </c>
-      <c r="N13" s="59" t="s">
-        <v>87</v>
-      </c>
-      <c r="O13" s="55" t="s">
-        <v>78</v>
-      </c>
-      <c r="P13" s="56" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q13" s="59" t="s">
-        <v>87</v>
-      </c>
-      <c r="R13" s="55" t="s">
-        <v>78</v>
-      </c>
-      <c r="S13" s="56" t="s">
-        <v>96</v>
-      </c>
-      <c r="T13" s="59" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20">
-      <c r="A14" t="s">
-        <v>103</v>
-      </c>
-      <c r="B14">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="74"/>
+      <c r="B25" s="72">
         <v>512</v>
       </c>
-      <c r="C14">
+      <c r="C25" s="72">
         <v>128</v>
       </c>
-      <c r="D14">
+      <c r="D25" s="72">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E14">
+      <c r="E25" s="72">
         <v>16342</v>
       </c>
-      <c r="F14" s="97">
+      <c r="F25" s="75">
         <f t="shared" si="1"/>
         <v>4.0102802594541673</v>
       </c>
-      <c r="H14" s="53"/>
-      <c r="I14" s="87"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="88"/>
-      <c r="L14" s="87"/>
-      <c r="M14" s="54"/>
-      <c r="N14" s="59"/>
-      <c r="O14" s="87"/>
-      <c r="P14" s="54"/>
-      <c r="Q14" s="59"/>
-      <c r="R14" s="87"/>
-      <c r="S14" s="54"/>
-      <c r="T14" s="59"/>
-    </row>
-    <row r="15" spans="1:20">
-      <c r="A15" t="s">
-        <v>103</v>
-      </c>
-      <c r="B15">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="74"/>
+      <c r="B26" s="72">
         <v>1024</v>
       </c>
-      <c r="C15">
+      <c r="C26" s="72">
         <v>128</v>
       </c>
-      <c r="D15">
+      <c r="D26" s="72">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="E15">
+      <c r="E26" s="72">
         <v>27577</v>
       </c>
-      <c r="F15" s="98">
+      <c r="F26" s="75">
         <f t="shared" si="1"/>
         <v>4.7529462958262316</v>
       </c>
-      <c r="H15" s="53"/>
-      <c r="I15" s="87"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="88"/>
-      <c r="L15" s="87"/>
-      <c r="M15" s="54"/>
-      <c r="N15" s="59"/>
-      <c r="O15" s="87"/>
-      <c r="P15" s="54"/>
-      <c r="Q15" s="59"/>
-      <c r="R15" s="87"/>
-      <c r="S15" s="54"/>
-      <c r="T15" s="59"/>
-    </row>
-    <row r="16" spans="1:20">
-      <c r="A16" t="s">
-        <v>103</v>
-      </c>
-      <c r="B16">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="74"/>
+      <c r="B27" s="72">
         <v>2048</v>
       </c>
-      <c r="C16">
+      <c r="C27" s="72">
         <v>128</v>
       </c>
-      <c r="D16">
+      <c r="D27" s="72">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="E16">
+      <c r="E27" s="72">
         <v>51313</v>
       </c>
-      <c r="F16" s="96">
+      <c r="F27" s="73">
         <f t="shared" si="1"/>
         <v>5.1087248845321849</v>
       </c>
-      <c r="H16" s="53"/>
-      <c r="I16" s="87"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="88"/>
-      <c r="L16" s="87"/>
-      <c r="M16" s="54"/>
-      <c r="N16" s="59"/>
-      <c r="O16" s="87"/>
-      <c r="P16" s="54"/>
-      <c r="Q16" s="59"/>
-      <c r="R16" s="87"/>
-      <c r="S16" s="54"/>
-      <c r="T16" s="59"/>
-    </row>
-    <row r="17" spans="1:20">
-      <c r="A17" t="s">
-        <v>103</v>
-      </c>
-      <c r="B17">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="74"/>
+      <c r="B28" s="72">
+        <v>64</v>
+      </c>
+      <c r="C28" s="72">
+        <v>256</v>
+      </c>
+      <c r="D28" s="72">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E28" s="72">
+        <v>7083</v>
+      </c>
+      <c r="F28" s="73">
+        <f t="shared" si="1"/>
+        <v>2.3131441479599042</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="74"/>
+      <c r="B29" s="72">
         <v>128</v>
       </c>
-      <c r="C17">
+      <c r="C29" s="72">
         <v>256</v>
       </c>
-      <c r="D17">
+      <c r="D29" s="72">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E17">
+      <c r="E29" s="72">
         <v>9919</v>
       </c>
-      <c r="F17" s="96">
+      <c r="F29" s="117">
         <f t="shared" si="1"/>
         <v>3.3035588264946063</v>
       </c>
-      <c r="H17" s="53" t="s">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="74"/>
+      <c r="B30" s="72"/>
+      <c r="C30" s="72"/>
+      <c r="D30" s="72"/>
+      <c r="E30" s="72"/>
+      <c r="F30" s="72"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="74"/>
+      <c r="B31" s="72"/>
+      <c r="C31" s="72"/>
+      <c r="D31" s="72"/>
+      <c r="E31" s="72"/>
+      <c r="F31" s="72"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="74"/>
+      <c r="B32" s="72"/>
+      <c r="C32" s="72"/>
+      <c r="D32" s="72"/>
+      <c r="E32" s="72"/>
+      <c r="F32" s="72"/>
+    </row>
+    <row r="33" spans="1:38" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="74"/>
+      <c r="B33" s="72"/>
+      <c r="C33" s="72"/>
+      <c r="D33" s="72"/>
+      <c r="E33" s="72"/>
+      <c r="F33" s="72"/>
+    </row>
+    <row r="34" spans="1:38" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="74"/>
+      <c r="B34" s="72"/>
+      <c r="C34" s="72"/>
+      <c r="D34" s="72"/>
+      <c r="E34" s="72"/>
+      <c r="F34" s="72"/>
+      <c r="Z34" s="77"/>
+      <c r="AA34" s="78" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB34" s="79"/>
+      <c r="AC34" s="80"/>
+      <c r="AD34" s="81" t="s">
+        <v>115</v>
+      </c>
+      <c r="AE34" s="82"/>
+      <c r="AF34" s="83"/>
+      <c r="AG34" s="81" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH34" s="82"/>
+      <c r="AI34" s="83"/>
+      <c r="AJ34" s="84" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK34" s="85"/>
+      <c r="AL34" s="86"/>
+    </row>
+    <row r="35" spans="1:38" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z35" s="77"/>
+      <c r="AA35" s="87"/>
+      <c r="AB35" s="88"/>
+      <c r="AC35" s="89"/>
+      <c r="AD35" s="90"/>
+      <c r="AE35" s="91"/>
+      <c r="AF35" s="92"/>
+      <c r="AG35" s="90"/>
+      <c r="AH35" s="91"/>
+      <c r="AI35" s="92"/>
+      <c r="AJ35" s="84"/>
+      <c r="AK35" s="85"/>
+      <c r="AL35" s="93"/>
+    </row>
+    <row r="36" spans="1:38" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z36" s="77"/>
+      <c r="AA36" s="87"/>
+      <c r="AB36" s="88"/>
+      <c r="AC36" s="89"/>
+      <c r="AD36" s="90"/>
+      <c r="AE36" s="91"/>
+      <c r="AF36" s="92"/>
+      <c r="AG36" s="90"/>
+      <c r="AH36" s="91"/>
+      <c r="AI36" s="92"/>
+      <c r="AJ36" s="84"/>
+      <c r="AK36" s="85"/>
+      <c r="AL36" s="93"/>
+    </row>
+    <row r="37" spans="1:38" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z37" s="77"/>
+      <c r="AA37" s="87"/>
+      <c r="AB37" s="88"/>
+      <c r="AC37" s="89"/>
+      <c r="AD37" s="90"/>
+      <c r="AE37" s="91"/>
+      <c r="AF37" s="92"/>
+      <c r="AG37" s="90"/>
+      <c r="AH37" s="91"/>
+      <c r="AI37" s="92"/>
+      <c r="AJ37" s="84"/>
+      <c r="AK37" s="85"/>
+      <c r="AL37" s="93"/>
+    </row>
+    <row r="38" spans="1:38" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z38" s="77"/>
+      <c r="AA38" s="87"/>
+      <c r="AB38" s="88"/>
+      <c r="AC38" s="89"/>
+      <c r="AD38" s="90"/>
+      <c r="AE38" s="91"/>
+      <c r="AF38" s="92"/>
+      <c r="AG38" s="90"/>
+      <c r="AH38" s="91"/>
+      <c r="AI38" s="92"/>
+      <c r="AJ38" s="84"/>
+      <c r="AK38" s="85"/>
+      <c r="AL38" s="93"/>
+    </row>
+    <row r="39" spans="1:38" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z39" s="77"/>
+      <c r="AA39" s="87"/>
+      <c r="AB39" s="88"/>
+      <c r="AC39" s="89"/>
+      <c r="AD39" s="90"/>
+      <c r="AE39" s="91"/>
+      <c r="AF39" s="92"/>
+      <c r="AG39" s="90"/>
+      <c r="AH39" s="91"/>
+      <c r="AI39" s="92"/>
+      <c r="AJ39" s="84"/>
+      <c r="AK39" s="85"/>
+      <c r="AL39" s="93"/>
+    </row>
+    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="Z40" s="77"/>
+      <c r="AA40" s="84" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB40" s="85" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC40" s="86" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD40" s="84" t="s">
+        <v>118</v>
+      </c>
+      <c r="AE40" s="85" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF40" s="94" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG40" s="84" t="s">
+        <v>118</v>
+      </c>
+      <c r="AH40" s="85" t="s">
+        <v>119</v>
+      </c>
+      <c r="AI40" s="94" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ40" s="84" t="s">
+        <v>118</v>
+      </c>
+      <c r="AK40" s="85" t="s">
+        <v>119</v>
+      </c>
+      <c r="AL40" s="94" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="Z41" s="77"/>
+      <c r="AA41" s="95"/>
+      <c r="AB41" s="96"/>
+      <c r="AC41" s="93"/>
+      <c r="AD41" s="95"/>
+      <c r="AE41" s="96"/>
+      <c r="AF41" s="94"/>
+      <c r="AG41" s="95"/>
+      <c r="AH41" s="96"/>
+      <c r="AI41" s="94"/>
+      <c r="AJ41" s="95"/>
+      <c r="AK41" s="96"/>
+      <c r="AL41" s="94"/>
+    </row>
+    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="Z42" s="77"/>
+      <c r="AA42" s="95"/>
+      <c r="AB42" s="96"/>
+      <c r="AC42" s="93"/>
+      <c r="AD42" s="95"/>
+      <c r="AE42" s="96"/>
+      <c r="AF42" s="94"/>
+      <c r="AG42" s="95"/>
+      <c r="AH42" s="96"/>
+      <c r="AI42" s="94"/>
+      <c r="AJ42" s="95"/>
+      <c r="AK42" s="96"/>
+      <c r="AL42" s="94"/>
+    </row>
+    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="Z43" s="77"/>
+      <c r="AA43" s="95"/>
+      <c r="AB43" s="96"/>
+      <c r="AC43" s="93"/>
+      <c r="AD43" s="95"/>
+      <c r="AE43" s="96"/>
+      <c r="AF43" s="94"/>
+      <c r="AG43" s="95"/>
+      <c r="AH43" s="96"/>
+      <c r="AI43" s="94"/>
+      <c r="AJ43" s="95"/>
+      <c r="AK43" s="96"/>
+      <c r="AL43" s="94"/>
+    </row>
+    <row r="44" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="Z44" s="77"/>
+      <c r="AA44" s="95"/>
+      <c r="AB44" s="96"/>
+      <c r="AC44" s="93"/>
+      <c r="AD44" s="95"/>
+      <c r="AE44" s="96"/>
+      <c r="AF44" s="94"/>
+      <c r="AG44" s="95"/>
+      <c r="AH44" s="96"/>
+      <c r="AI44" s="94"/>
+      <c r="AJ44" s="95"/>
+      <c r="AK44" s="96"/>
+      <c r="AL44" s="94"/>
+    </row>
+    <row r="45" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="Z45" s="77" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA45" s="97">
+        <v>1.5</v>
+      </c>
+      <c r="AB45" s="72">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AC45" s="94"/>
+      <c r="AD45" s="97">
+        <v>1.5</v>
+      </c>
+      <c r="AE45" s="72">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AF45" s="94"/>
+      <c r="AG45" s="97">
+        <v>1.5</v>
+      </c>
+      <c r="AH45" s="72">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AI45" s="94"/>
+      <c r="AJ45" s="97">
+        <v>1.5</v>
+      </c>
+      <c r="AK45" s="72">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AL45" s="94"/>
+    </row>
+    <row r="46" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="Z46" s="77" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA46" s="97">
+        <v>0.11</v>
+      </c>
+      <c r="AB46" s="72"/>
+      <c r="AC46" s="94">
+        <v>83</v>
+      </c>
+      <c r="AD46" s="97">
+        <v>0.17</v>
+      </c>
+      <c r="AE46" s="72"/>
+      <c r="AF46" s="94">
+        <f>AC46*1.8</f>
+        <v>149.4</v>
+      </c>
+      <c r="AG46" s="97">
+        <v>0.25</v>
+      </c>
+      <c r="AH46" s="72"/>
+      <c r="AI46" s="94">
+        <f>AC46*1.8</f>
+        <v>149.4</v>
+      </c>
+      <c r="AJ46" s="97">
+        <v>0.35</v>
+      </c>
+      <c r="AK46" s="72"/>
+      <c r="AL46" s="94">
+        <f>AC46*1.5*1.8</f>
+        <v>224.1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="Z47" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="I17" s="58">
-        <v>1.5</v>
-      </c>
-      <c r="J17" s="52">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="K17" s="59"/>
-      <c r="L17" s="58">
-        <v>1.5</v>
-      </c>
-      <c r="M17" s="52">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="N17" s="59"/>
-      <c r="O17" s="58">
-        <v>1.5</v>
-      </c>
-      <c r="P17" s="52">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="Q17" s="59"/>
-      <c r="R17" s="58">
-        <v>1.5</v>
-      </c>
-      <c r="S17" s="52">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="T17" s="59"/>
-    </row>
-    <row r="18" spans="1:20">
-      <c r="A18" t="s">
-        <v>103</v>
-      </c>
-      <c r="H18" s="53" t="s">
-        <v>94</v>
-      </c>
-      <c r="I18" s="58">
+      <c r="AA47" s="97">
+        <f>AA45-AA46*2</f>
+        <v>1.28</v>
+      </c>
+      <c r="AB47" s="72">
+        <f>AB45-AA46*2</f>
+        <v>1.9800000000000002</v>
+      </c>
+      <c r="AC47" s="94"/>
+      <c r="AD47" s="97">
+        <f>AD45-AD46*2</f>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="AE47" s="72">
+        <f>AE45-AD46*2</f>
+        <v>1.86</v>
+      </c>
+      <c r="AF47" s="94"/>
+      <c r="AG47" s="97">
+        <f>AG45-AG46*2</f>
+        <v>1</v>
+      </c>
+      <c r="AH47" s="72">
+        <f>AH45-AG46*2</f>
+        <v>1.7000000000000002</v>
+      </c>
+      <c r="AI47" s="94"/>
+      <c r="AJ47" s="97">
+        <f>AJ45-AJ46*2</f>
+        <v>0.8</v>
+      </c>
+      <c r="AK47" s="72">
+        <f>AK45-AJ46*2</f>
+        <v>1.5000000000000002</v>
+      </c>
+      <c r="AL47" s="94"/>
+    </row>
+    <row r="48" spans="1:38" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z48" s="77" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA48" s="98">
+        <f>AA47*AB47/AA45/AB45</f>
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="AB48" s="99"/>
+      <c r="AC48" s="100"/>
+      <c r="AD48" s="101">
+        <f>AD47*AE47/AD45/AE45</f>
+        <v>0.65381818181818174</v>
+      </c>
+      <c r="AE48" s="99"/>
+      <c r="AF48" s="100"/>
+      <c r="AG48" s="98">
+        <f>AG47*AH47/AG45/AH45</f>
+        <v>0.51515151515151525</v>
+      </c>
+      <c r="AH48" s="99"/>
+      <c r="AI48" s="100"/>
+      <c r="AJ48" s="98">
+        <f>AJ47*AK47/AJ45/AK45</f>
+        <v>0.3636363636363637</v>
+      </c>
+      <c r="AK48" s="99"/>
+      <c r="AL48" s="100"/>
+    </row>
+    <row r="49" spans="26:38" x14ac:dyDescent="0.25">
+      <c r="Z49" s="72" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA49" s="96">
+        <f>AC46/AA47/AB47</f>
+        <v>32.749368686868685</v>
+      </c>
+      <c r="AB49" s="96"/>
+      <c r="AC49" s="96"/>
+      <c r="AD49" s="96">
+        <f>AF46/AD47/AE47</f>
+        <v>69.243604004449395</v>
+      </c>
+      <c r="AE49" s="96"/>
+      <c r="AF49" s="96"/>
+      <c r="AG49" s="96">
+        <f>AI46/AG47/AH47</f>
+        <v>87.882352941176464</v>
+      </c>
+      <c r="AH49" s="96"/>
+      <c r="AI49" s="96"/>
+      <c r="AJ49" s="96">
+        <f>AL46/AJ47/AK47</f>
+        <v>186.74999999999997</v>
+      </c>
+      <c r="AK49" s="96"/>
+      <c r="AL49" s="96"/>
+    </row>
+    <row r="50" spans="26:38" x14ac:dyDescent="0.25">
+      <c r="Z50" s="102" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA50" s="103"/>
+      <c r="AB50" s="103"/>
+      <c r="AC50" s="103">
+        <f>AC46/(AA47+AB47)/2</f>
+        <v>12.730061349693251</v>
+      </c>
+      <c r="AD50" s="103"/>
+      <c r="AE50" s="103"/>
+      <c r="AF50" s="103">
+        <f>AF46/(AD47+AE47)/2</f>
+        <v>24.735099337748345</v>
+      </c>
+    </row>
+    <row r="51" spans="26:38" x14ac:dyDescent="0.25">
+      <c r="Z51" s="104" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA51" s="105">
+        <f>AA53+AA52*2</f>
+        <v>1.52</v>
+      </c>
+      <c r="AB51" s="105">
+        <f>AB53+AA52*2</f>
+        <v>1.52</v>
+      </c>
+      <c r="AC51" s="105">
+        <f>AA51*AB51</f>
+        <v>2.3104</v>
+      </c>
+      <c r="AD51" s="105">
+        <f>AD53+AD52*2</f>
+        <v>1.6400000000000001</v>
+      </c>
+      <c r="AE51" s="105">
+        <f>AE53+AD52*2</f>
+        <v>1.6400000000000001</v>
+      </c>
+      <c r="AF51" s="105">
+        <f>AD51*AE51</f>
+        <v>2.6896000000000004</v>
+      </c>
+    </row>
+    <row r="52" spans="26:38" x14ac:dyDescent="0.25">
+      <c r="Z52" s="104" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA52" s="105">
         <v>0.11</v>
       </c>
-      <c r="J18" s="52"/>
-      <c r="K18" s="59">
-        <v>83</v>
-      </c>
-      <c r="L18" s="58">
+      <c r="AB52" s="105"/>
+      <c r="AC52" s="105">
+        <f>AC50*(AA51+AB51)*2</f>
+        <v>77.398773006134974</v>
+      </c>
+      <c r="AD52" s="105">
         <v>0.17</v>
       </c>
-      <c r="M18" s="52"/>
-      <c r="N18" s="59">
-        <f>K18*1.8</f>
-        <v>149.4</v>
-      </c>
-      <c r="O18" s="58">
-        <v>0.25</v>
-      </c>
-      <c r="P18" s="52"/>
-      <c r="Q18" s="59">
-        <f>K18*1.8</f>
-        <v>149.4</v>
-      </c>
-      <c r="R18" s="58">
-        <v>0.35</v>
-      </c>
-      <c r="S18" s="52"/>
-      <c r="T18" s="59">
-        <f>K18*1.5*1.8</f>
-        <v>224.1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20">
-      <c r="A19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H19" s="53" t="s">
+      <c r="AE52" s="105"/>
+      <c r="AF52" s="105">
+        <f>AF50*(AD51+AE51)*2</f>
+        <v>162.26225165562914</v>
+      </c>
+    </row>
+    <row r="53" spans="26:38" x14ac:dyDescent="0.25">
+      <c r="Z53" s="104" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA53" s="105">
+        <v>1.3</v>
+      </c>
+      <c r="AB53" s="105">
+        <v>1.3</v>
+      </c>
+      <c r="AC53" s="105">
+        <f>AA53*AB53</f>
+        <v>1.6900000000000002</v>
+      </c>
+      <c r="AD53" s="105">
+        <v>1.3</v>
+      </c>
+      <c r="AE53" s="105">
+        <v>1.3</v>
+      </c>
+      <c r="AF53" s="105"/>
+    </row>
+    <row r="54" spans="26:38" x14ac:dyDescent="0.25">
+      <c r="Z54" s="104" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA54" s="105"/>
+      <c r="AB54" s="105"/>
+      <c r="AC54" s="105">
+        <f>AA52*(AA53+AB53)*2</f>
+        <v>0.57200000000000006</v>
+      </c>
+      <c r="AD54" s="105"/>
+      <c r="AE54" s="105"/>
+      <c r="AF54" s="105">
+        <f>AD52*(AD53+AE53)*2</f>
+        <v>0.88400000000000012</v>
+      </c>
+    </row>
+    <row r="55" spans="26:38" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z55" s="104" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA55" s="105"/>
+      <c r="AB55" s="105"/>
+      <c r="AC55" s="105"/>
+      <c r="AD55" s="106">
+        <f>AD53*AE53/AD51/AE51</f>
+        <v>0.62834622248661509</v>
+      </c>
+      <c r="AE55" s="105"/>
+      <c r="AF55" s="105"/>
+    </row>
+    <row r="56" spans="26:38" x14ac:dyDescent="0.25">
+      <c r="Z56" s="107" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA56" s="105"/>
+      <c r="AB56" s="105"/>
+      <c r="AC56" s="105"/>
+      <c r="AD56" s="108">
+        <f>AF52/AD53/AE53</f>
+        <v>96.013166660135582</v>
+      </c>
+      <c r="AE56" s="105"/>
+      <c r="AF56" s="105"/>
+    </row>
+    <row r="57" spans="26:38" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z57" s="109"/>
+      <c r="AA57" s="105"/>
+      <c r="AB57" s="105"/>
+      <c r="AC57" s="105"/>
+      <c r="AD57" s="110"/>
+      <c r="AE57" s="105"/>
+      <c r="AF57" s="105"/>
+    </row>
+    <row r="58" spans="26:38" x14ac:dyDescent="0.25">
+      <c r="Z58" s="84"/>
+      <c r="AA58" s="111" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB58" s="111"/>
+      <c r="AC58" s="111"/>
+      <c r="AD58" s="112" t="s">
+        <v>124</v>
+      </c>
+      <c r="AE58" s="112"/>
+      <c r="AF58" s="112"/>
+      <c r="AG58" s="112" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH58" s="112"/>
+      <c r="AI58" s="112"/>
+      <c r="AJ58" s="85" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK58" s="85"/>
+      <c r="AL58" s="86"/>
+    </row>
+    <row r="59" spans="26:38" x14ac:dyDescent="0.25">
+      <c r="Z59" s="97"/>
+      <c r="AA59" s="72" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB59" s="72" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC59" s="72" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD59" s="72" t="s">
+        <v>118</v>
+      </c>
+      <c r="AE59" s="72" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF59" s="72" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG59" s="72" t="s">
+        <v>118</v>
+      </c>
+      <c r="AH59" s="72" t="s">
+        <v>119</v>
+      </c>
+      <c r="AI59" s="72" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ59" s="72" t="s">
+        <v>118</v>
+      </c>
+      <c r="AK59" s="72" t="s">
+        <v>119</v>
+      </c>
+      <c r="AL59" s="94" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="60" spans="26:38" x14ac:dyDescent="0.25">
+      <c r="Z60" s="113" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA60" s="114">
+        <v>1.7</v>
+      </c>
+      <c r="AB60" s="114">
+        <v>1</v>
+      </c>
+      <c r="AC60" s="114">
+        <v>0.11</v>
+      </c>
+      <c r="AD60" s="114">
+        <v>1.7</v>
+      </c>
+      <c r="AE60" s="114">
+        <v>1</v>
+      </c>
+      <c r="AF60" s="114">
+        <v>1.7</v>
+      </c>
+      <c r="AG60" s="72"/>
+      <c r="AH60" s="72"/>
+      <c r="AI60" s="72"/>
+      <c r="AJ60" s="72"/>
+      <c r="AK60" s="72"/>
+      <c r="AL60" s="94"/>
+    </row>
+    <row r="61" spans="26:38" x14ac:dyDescent="0.25">
+      <c r="Z61" s="113" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA61" s="114">
+        <f>AA60+AC60*2</f>
+        <v>1.92</v>
+      </c>
+      <c r="AB61" s="114">
+        <f>AB60+AC60*2</f>
+        <v>1.22</v>
+      </c>
+      <c r="AC61" s="114">
+        <f>AA61*AB61</f>
+        <v>2.3424</v>
+      </c>
+      <c r="AD61" s="114">
+        <f>AD60+AD62*2</f>
+        <v>2.04</v>
+      </c>
+      <c r="AE61" s="114">
+        <f>AE60+AD62*2</f>
+        <v>1.34</v>
+      </c>
+      <c r="AF61" s="114">
+        <f>AD61*AE61</f>
+        <v>2.7336</v>
+      </c>
+      <c r="AG61" s="72"/>
+      <c r="AH61" s="72"/>
+      <c r="AI61" s="72"/>
+      <c r="AJ61" s="72"/>
+      <c r="AK61" s="72"/>
+      <c r="AL61" s="94"/>
+    </row>
+    <row r="62" spans="26:38" x14ac:dyDescent="0.25">
+      <c r="Z62" s="113" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB62" s="114"/>
+      <c r="AC62" s="114">
+        <f>AC56*(AA61+AB61)*2</f>
+        <v>0</v>
+      </c>
+      <c r="AD62" s="114">
+        <v>0.17</v>
+      </c>
+      <c r="AE62" s="114"/>
+      <c r="AF62" s="114">
+        <f>AF56*(AD61+AE61)*2</f>
+        <v>0</v>
+      </c>
+      <c r="AG62" s="72"/>
+      <c r="AH62" s="72"/>
+      <c r="AI62" s="72"/>
+      <c r="AJ62" s="72"/>
+      <c r="AK62" s="72"/>
+      <c r="AL62" s="94"/>
+    </row>
+    <row r="63" spans="26:38" x14ac:dyDescent="0.25">
+      <c r="Z63" s="113" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA63" s="114"/>
+      <c r="AB63" s="114"/>
+      <c r="AC63" s="114" t="e">
+        <f>AC61-#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AD63" s="114"/>
+      <c r="AE63" s="114"/>
+      <c r="AF63" s="114">
+        <f>AF61-AF60</f>
+        <v>1.0336000000000001</v>
+      </c>
+      <c r="AG63" s="72"/>
+      <c r="AH63" s="72"/>
+      <c r="AI63" s="72"/>
+      <c r="AJ63" s="72"/>
+      <c r="AK63" s="72"/>
+      <c r="AL63" s="94"/>
+    </row>
+    <row r="64" spans="26:38" x14ac:dyDescent="0.25">
+      <c r="Z64" s="113" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA64" s="114"/>
+      <c r="AB64" s="114"/>
+      <c r="AC64" s="114"/>
+      <c r="AD64" s="115">
+        <f>AD60*AE60/AD61/AE61</f>
+        <v>0.62189054726368154</v>
+      </c>
+      <c r="AE64" s="114"/>
+      <c r="AF64" s="114"/>
+      <c r="AG64" s="72"/>
+      <c r="AH64" s="72"/>
+      <c r="AI64" s="72"/>
+      <c r="AJ64" s="72"/>
+      <c r="AK64" s="72"/>
+      <c r="AL64" s="94"/>
+    </row>
+    <row r="65" spans="26:38" x14ac:dyDescent="0.25">
+      <c r="Z65" s="113" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA65" s="114"/>
+      <c r="AB65" s="114"/>
+      <c r="AC65" s="114"/>
+      <c r="AD65" s="114">
+        <f>AF62/AD60/AE60</f>
+        <v>0</v>
+      </c>
+      <c r="AE65" s="114"/>
+      <c r="AF65" s="114"/>
+      <c r="AG65" s="72"/>
+      <c r="AH65" s="72"/>
+      <c r="AI65" s="72"/>
+      <c r="AJ65" s="72"/>
+      <c r="AK65" s="72"/>
+      <c r="AL65" s="94"/>
+    </row>
+    <row r="66" spans="26:38" x14ac:dyDescent="0.25">
+      <c r="Z66" s="97" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA66" s="72">
+        <f>AA68+AA67*2</f>
+        <v>1.07</v>
+      </c>
+      <c r="AB66" s="72">
+        <f>AB68+AA67*2</f>
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="AC66" s="72">
+        <f>AA66*AB66</f>
+        <v>2.3754000000000004</v>
+      </c>
+      <c r="AD66" s="72">
+        <f>AD68+AD67*2</f>
+        <v>1.19</v>
+      </c>
+      <c r="AE66" s="72">
+        <f>AE68+AD67*2</f>
+        <v>2.34</v>
+      </c>
+      <c r="AF66" s="72">
+        <f>AD66*AE66</f>
+        <v>2.7845999999999997</v>
+      </c>
+      <c r="AG66" s="72"/>
+      <c r="AH66" s="72"/>
+      <c r="AI66" s="72"/>
+      <c r="AJ66" s="72"/>
+      <c r="AK66" s="72"/>
+      <c r="AL66" s="94"/>
+    </row>
+    <row r="67" spans="26:38" x14ac:dyDescent="0.25">
+      <c r="Z67" s="97" t="s">
         <v>80</v>
       </c>
-      <c r="I19" s="58">
-        <f>I17-I18*2</f>
-        <v>1.28</v>
-      </c>
-      <c r="J19" s="52">
-        <f>J17-I18*2</f>
-        <v>1.9800000000000002</v>
-      </c>
-      <c r="K19" s="59"/>
-      <c r="L19" s="58">
-        <f>L17-L18*2</f>
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="M19" s="52">
-        <f>M17-L18*2</f>
-        <v>1.86</v>
-      </c>
-      <c r="N19" s="59"/>
-      <c r="O19" s="58">
-        <f>O17-O18*2</f>
-        <v>1</v>
-      </c>
-      <c r="P19" s="52">
-        <f>P17-O18*2</f>
-        <v>1.7000000000000002</v>
-      </c>
-      <c r="Q19" s="59"/>
-      <c r="R19" s="58">
-        <f>R17-R18*2</f>
-        <v>0.8</v>
-      </c>
-      <c r="S19" s="52">
-        <f>S17-R18*2</f>
-        <v>1.5000000000000002</v>
-      </c>
-      <c r="T19" s="59"/>
-    </row>
-    <row r="20" spans="1:20" ht="14.4" thickBot="1">
-      <c r="A20" t="s">
-        <v>103</v>
-      </c>
-      <c r="H20" s="53" t="s">
-        <v>86</v>
-      </c>
-      <c r="I20" s="60">
-        <f>I19*J19/I17/J17</f>
-        <v>0.76800000000000002</v>
-      </c>
-      <c r="J20" s="61"/>
-      <c r="K20" s="62"/>
-      <c r="L20" s="63">
-        <f>L19*M19/L17/M17</f>
-        <v>0.65381818181818174</v>
-      </c>
-      <c r="M20" s="61"/>
-      <c r="N20" s="62"/>
-      <c r="O20" s="60">
-        <f>O19*P19/O17/P17</f>
-        <v>0.51515151515151525</v>
-      </c>
-      <c r="P20" s="61"/>
-      <c r="Q20" s="62"/>
-      <c r="R20" s="60">
-        <f>R19*S19/R17/S17</f>
-        <v>0.3636363636363637</v>
-      </c>
-      <c r="S20" s="61"/>
-      <c r="T20" s="62"/>
-    </row>
-    <row r="21" spans="1:20">
-      <c r="A21" t="s">
-        <v>103</v>
-      </c>
-      <c r="H21" s="52" t="s">
-        <v>88</v>
-      </c>
-      <c r="I21" s="54">
-        <f>K18/I19/J19</f>
-        <v>32.749368686868685</v>
-      </c>
-      <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="54">
-        <f>N18/L19/M19</f>
-        <v>69.243604004449395</v>
-      </c>
-      <c r="M21" s="54"/>
-      <c r="N21" s="54"/>
-      <c r="O21" s="54">
-        <f>Q18/O19/P19</f>
-        <v>87.882352941176464</v>
-      </c>
-      <c r="P21" s="54"/>
-      <c r="Q21" s="54"/>
-      <c r="R21" s="54">
-        <f>T18/R19/S19</f>
-        <v>186.74999999999997</v>
-      </c>
-      <c r="S21" s="54"/>
-      <c r="T21" s="54"/>
-    </row>
-    <row r="22" spans="1:20">
-      <c r="A22" t="s">
-        <v>103</v>
-      </c>
-      <c r="H22" s="67" t="s">
-        <v>93</v>
-      </c>
-      <c r="I22" s="51"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="51">
-        <f>K18/(I19+J19)/2</f>
-        <v>12.730061349693251</v>
-      </c>
-      <c r="L22" s="51"/>
-      <c r="M22" s="51"/>
-      <c r="N22" s="51">
-        <f>N18/(L19+M19)/2</f>
-        <v>24.735099337748345</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20">
-      <c r="H23" s="70" t="s">
+      <c r="AA67" s="72">
+        <v>0.11</v>
+      </c>
+      <c r="AB67" s="72"/>
+      <c r="AC67" s="72">
+        <f>AC50*(AA68+AB68)*2</f>
+        <v>72.561349693251529</v>
+      </c>
+      <c r="AD67" s="72">
+        <v>0.17</v>
+      </c>
+      <c r="AE67" s="72"/>
+      <c r="AF67" s="72">
+        <f>AF50*(AD68+AE68)*2</f>
+        <v>140.99006622516558</v>
+      </c>
+      <c r="AG67" s="72"/>
+      <c r="AH67" s="72"/>
+      <c r="AI67" s="72"/>
+      <c r="AJ67" s="72"/>
+      <c r="AK67" s="72"/>
+      <c r="AL67" s="94"/>
+    </row>
+    <row r="68" spans="26:38" x14ac:dyDescent="0.25">
+      <c r="Z68" s="97" t="s">
         <v>79</v>
       </c>
-      <c r="I23" s="69">
-        <f>I25+I24*2</f>
-        <v>1.52</v>
-      </c>
-      <c r="J23" s="69">
-        <f>J25+I24*2</f>
-        <v>1.52</v>
-      </c>
-      <c r="K23" s="69">
-        <f>I23*J23</f>
-        <v>2.3104</v>
-      </c>
-      <c r="L23" s="69">
-        <f>L25+L24*2</f>
-        <v>1.6400000000000001</v>
-      </c>
-      <c r="M23" s="69">
-        <f>M25+L24*2</f>
-        <v>1.6400000000000001</v>
-      </c>
-      <c r="N23" s="69">
-        <f>L23*M23</f>
-        <v>2.6896000000000004</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20">
-      <c r="H24" s="70" t="s">
+      <c r="AA68" s="72">
+        <f>AC68/AB68</f>
+        <v>0.85</v>
+      </c>
+      <c r="AB68" s="72">
+        <v>2</v>
+      </c>
+      <c r="AC68" s="72">
+        <v>1.7</v>
+      </c>
+      <c r="AD68" s="72">
+        <f>AF68/AE68</f>
+        <v>0.85</v>
+      </c>
+      <c r="AE68" s="72">
+        <v>2</v>
+      </c>
+      <c r="AF68" s="72">
+        <v>1.7</v>
+      </c>
+      <c r="AG68" s="72"/>
+      <c r="AH68" s="72"/>
+      <c r="AI68" s="72"/>
+      <c r="AJ68" s="72"/>
+      <c r="AK68" s="72"/>
+      <c r="AL68" s="94"/>
+    </row>
+    <row r="69" spans="26:38" x14ac:dyDescent="0.25">
+      <c r="Z69" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA69" s="72"/>
+      <c r="AB69" s="72"/>
+      <c r="AC69" s="72">
+        <f>AC66-AC68</f>
+        <v>0.67540000000000044</v>
+      </c>
+      <c r="AD69" s="72"/>
+      <c r="AE69" s="72"/>
+      <c r="AF69" s="72">
+        <f>AF66-AF68</f>
+        <v>1.0845999999999998</v>
+      </c>
+      <c r="AG69" s="72"/>
+      <c r="AH69" s="72"/>
+      <c r="AI69" s="72"/>
+      <c r="AJ69" s="72"/>
+      <c r="AK69" s="72"/>
+      <c r="AL69" s="94"/>
+    </row>
+    <row r="70" spans="26:38" x14ac:dyDescent="0.25">
+      <c r="Z70" s="97" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA70" s="72"/>
+      <c r="AB70" s="72"/>
+      <c r="AC70" s="72"/>
+      <c r="AD70" s="116">
+        <f>AD68*AE68/AD66/AE66</f>
+        <v>0.61050061050061055</v>
+      </c>
+      <c r="AE70" s="72"/>
+      <c r="AF70" s="72"/>
+      <c r="AG70" s="72"/>
+      <c r="AH70" s="72"/>
+      <c r="AI70" s="72"/>
+      <c r="AJ70" s="72"/>
+      <c r="AK70" s="72"/>
+      <c r="AL70" s="94"/>
+    </row>
+    <row r="71" spans="26:38" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z71" s="98" t="s">
         <v>81</v>
       </c>
-      <c r="I24" s="69">
-        <v>0.11</v>
-      </c>
-      <c r="J24" s="69"/>
-      <c r="K24" s="69">
-        <f>K22*(I23+J23)*2</f>
-        <v>77.398773006134974</v>
-      </c>
-      <c r="L24" s="69">
-        <v>0.17</v>
-      </c>
-      <c r="M24" s="69"/>
-      <c r="N24" s="69">
-        <f>N22*(L23+M23)*2</f>
-        <v>162.26225165562914</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20">
-      <c r="H25" s="70" t="s">
-        <v>80</v>
-      </c>
-      <c r="I25" s="69">
-        <v>1.3</v>
-      </c>
-      <c r="J25" s="69">
-        <v>1.3</v>
-      </c>
-      <c r="K25" s="69">
-        <f>I25*J25</f>
-        <v>1.6900000000000002</v>
-      </c>
-      <c r="L25" s="69">
-        <v>1.3</v>
-      </c>
-      <c r="M25" s="69">
-        <v>1.3</v>
-      </c>
-      <c r="N25" s="69"/>
-    </row>
-    <row r="26" spans="1:20">
-      <c r="H26" s="70" t="s">
-        <v>95</v>
-      </c>
-      <c r="I26" s="69"/>
-      <c r="J26" s="69"/>
-      <c r="K26" s="69">
-        <f>I24*(I25+J25)*2</f>
-        <v>0.57200000000000006</v>
-      </c>
-      <c r="L26" s="69"/>
-      <c r="M26" s="69"/>
-      <c r="N26" s="69">
-        <f>L24*(L25+M25)*2</f>
-        <v>0.88400000000000012</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" ht="14.4" thickBot="1">
-      <c r="H27" s="70" t="s">
-        <v>86</v>
-      </c>
-      <c r="I27" s="69"/>
-      <c r="J27" s="69"/>
-      <c r="K27" s="69"/>
-      <c r="L27" s="71">
-        <f>L25*M25/L23/M23</f>
-        <v>0.62834622248661509</v>
-      </c>
-      <c r="M27" s="69"/>
-      <c r="N27" s="69"/>
-    </row>
-    <row r="28" spans="1:20">
-      <c r="H28" s="72" t="s">
-        <v>88</v>
-      </c>
-      <c r="I28" s="69"/>
-      <c r="J28" s="69"/>
-      <c r="K28" s="69"/>
-      <c r="L28" s="73">
-        <f>N24/L25/M25</f>
-        <v>96.013166660135582</v>
-      </c>
-      <c r="M28" s="69"/>
-      <c r="N28" s="69"/>
-    </row>
-    <row r="29" spans="1:20" ht="14.4" thickBot="1">
-      <c r="H29" s="75"/>
-      <c r="I29" s="69"/>
-      <c r="J29" s="69"/>
-      <c r="K29" s="69"/>
-      <c r="L29" s="74"/>
-      <c r="M29" s="69"/>
-      <c r="N29" s="69"/>
-    </row>
-    <row r="30" spans="1:20">
-      <c r="H30" s="55"/>
-      <c r="I30" s="79" t="s">
-        <v>82</v>
-      </c>
-      <c r="J30" s="79"/>
-      <c r="K30" s="79"/>
-      <c r="L30" s="109" t="s">
-        <v>97</v>
-      </c>
-      <c r="M30" s="109"/>
-      <c r="N30" s="109"/>
-      <c r="O30" s="109" t="s">
-        <v>83</v>
-      </c>
-      <c r="P30" s="109"/>
-      <c r="Q30" s="109"/>
-      <c r="R30" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="S30" s="56"/>
-      <c r="T30" s="57"/>
-    </row>
-    <row r="31" spans="1:20">
-      <c r="H31" s="58"/>
-      <c r="I31" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="J31" s="52" t="s">
-        <v>96</v>
-      </c>
-      <c r="K31" s="52" t="s">
-        <v>98</v>
-      </c>
-      <c r="L31" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="M31" s="52" t="s">
-        <v>96</v>
-      </c>
-      <c r="N31" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="O31" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="P31" s="52" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q31" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="R31" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="S31" s="52" t="s">
-        <v>96</v>
-      </c>
-      <c r="T31" s="59" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20">
-      <c r="H32" s="78" t="s">
-        <v>80</v>
-      </c>
-      <c r="I32" s="68">
-        <v>1.7</v>
-      </c>
-      <c r="J32" s="68">
-        <v>1</v>
-      </c>
-      <c r="K32" s="68">
-        <v>0.11</v>
-      </c>
-      <c r="L32" s="68">
-        <v>1.7</v>
-      </c>
-      <c r="M32" s="68">
-        <v>1</v>
-      </c>
-      <c r="N32" s="68">
-        <v>1.7</v>
-      </c>
-      <c r="O32" s="52"/>
-      <c r="P32" s="52"/>
-      <c r="Q32" s="52"/>
-      <c r="R32" s="52"/>
-      <c r="S32" s="52"/>
-      <c r="T32" s="59"/>
-    </row>
-    <row r="33" spans="8:20">
-      <c r="H33" s="78" t="s">
-        <v>79</v>
-      </c>
-      <c r="I33" s="68">
-        <f>I32+K32*2</f>
-        <v>1.92</v>
-      </c>
-      <c r="J33" s="68">
-        <f>J32+K32*2</f>
-        <v>1.22</v>
-      </c>
-      <c r="K33" s="68">
-        <f>I33*J33</f>
-        <v>2.3424</v>
-      </c>
-      <c r="L33" s="68">
-        <f>L32+L34*2</f>
-        <v>2.04</v>
-      </c>
-      <c r="M33" s="68">
-        <f>M32+L34*2</f>
-        <v>1.34</v>
-      </c>
-      <c r="N33" s="68">
-        <f>L33*M33</f>
-        <v>2.7336</v>
-      </c>
-      <c r="O33" s="52"/>
-      <c r="P33" s="52"/>
-      <c r="Q33" s="52"/>
-      <c r="R33" s="52"/>
-      <c r="S33" s="52"/>
-      <c r="T33" s="59"/>
-    </row>
-    <row r="34" spans="8:20">
-      <c r="H34" s="78" t="s">
-        <v>87</v>
-      </c>
-      <c r="J34" s="68"/>
-      <c r="K34" s="68">
-        <f>K28*(I33+J33)*2</f>
-        <v>0</v>
-      </c>
-      <c r="L34" s="68">
-        <v>0.17</v>
-      </c>
-      <c r="M34" s="68"/>
-      <c r="N34" s="68">
-        <f>N28*(L33+M33)*2</f>
-        <v>0</v>
-      </c>
-      <c r="O34" s="52"/>
-      <c r="P34" s="52"/>
-      <c r="Q34" s="52"/>
-      <c r="R34" s="52"/>
-      <c r="S34" s="52"/>
-      <c r="T34" s="59"/>
-    </row>
-    <row r="35" spans="8:20">
-      <c r="H35" s="78" t="s">
-        <v>95</v>
-      </c>
-      <c r="I35" s="68"/>
-      <c r="J35" s="68"/>
-      <c r="K35" s="68" t="e">
-        <f>K33-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L35" s="68"/>
-      <c r="M35" s="68"/>
-      <c r="N35" s="68">
-        <f>N33-N32</f>
-        <v>1.0336000000000001</v>
-      </c>
-      <c r="O35" s="52"/>
-      <c r="P35" s="52"/>
-      <c r="Q35" s="52"/>
-      <c r="R35" s="52"/>
-      <c r="S35" s="52"/>
-      <c r="T35" s="59"/>
-    </row>
-    <row r="36" spans="8:20">
-      <c r="H36" s="78" t="s">
-        <v>86</v>
-      </c>
-      <c r="I36" s="68"/>
-      <c r="J36" s="68"/>
-      <c r="K36" s="68"/>
-      <c r="L36" s="76">
-        <f>L32*M32/L33/M33</f>
-        <v>0.62189054726368154</v>
-      </c>
-      <c r="M36" s="68"/>
-      <c r="N36" s="68"/>
-      <c r="O36" s="52"/>
-      <c r="P36" s="52"/>
-      <c r="Q36" s="52"/>
-      <c r="R36" s="52"/>
-      <c r="S36" s="52"/>
-      <c r="T36" s="59"/>
-    </row>
-    <row r="37" spans="8:20">
-      <c r="H37" s="78" t="s">
-        <v>88</v>
-      </c>
-      <c r="I37" s="68"/>
-      <c r="J37" s="68"/>
-      <c r="K37" s="68"/>
-      <c r="L37" s="68">
-        <f>N34/L32/M32</f>
-        <v>0</v>
-      </c>
-      <c r="M37" s="68"/>
-      <c r="N37" s="68"/>
-      <c r="O37" s="52"/>
-      <c r="P37" s="52"/>
-      <c r="Q37" s="52"/>
-      <c r="R37" s="52"/>
-      <c r="S37" s="52"/>
-      <c r="T37" s="59"/>
-    </row>
-    <row r="38" spans="8:20">
-      <c r="H38" s="58" t="s">
-        <v>79</v>
-      </c>
-      <c r="I38" s="52">
-        <f>I40+I39*2</f>
-        <v>1.07</v>
-      </c>
-      <c r="J38" s="52">
-        <f>J40+I39*2</f>
-        <v>2.2200000000000002</v>
-      </c>
-      <c r="K38" s="52">
-        <f>I38*J38</f>
-        <v>2.3754000000000004</v>
-      </c>
-      <c r="L38" s="52">
-        <f>L40+L39*2</f>
-        <v>1.19</v>
-      </c>
-      <c r="M38" s="52">
-        <f>M40+L39*2</f>
-        <v>2.34</v>
-      </c>
-      <c r="N38" s="52">
-        <f>L38*M38</f>
-        <v>2.7845999999999997</v>
-      </c>
-      <c r="O38" s="52"/>
-      <c r="P38" s="52"/>
-      <c r="Q38" s="52"/>
-      <c r="R38" s="52"/>
-      <c r="S38" s="52"/>
-      <c r="T38" s="59"/>
-    </row>
-    <row r="39" spans="8:20">
-      <c r="H39" s="58" t="s">
-        <v>81</v>
-      </c>
-      <c r="I39" s="52">
-        <v>0.11</v>
-      </c>
-      <c r="J39" s="52"/>
-      <c r="K39" s="52">
-        <f>K22*(I40+J40)*2</f>
-        <v>72.561349693251529</v>
-      </c>
-      <c r="L39" s="52">
-        <v>0.17</v>
-      </c>
-      <c r="M39" s="52"/>
-      <c r="N39" s="52">
-        <f>N22*(L40+M40)*2</f>
-        <v>140.99006622516558</v>
-      </c>
-      <c r="O39" s="52"/>
-      <c r="P39" s="52"/>
-      <c r="Q39" s="52"/>
-      <c r="R39" s="52"/>
-      <c r="S39" s="52"/>
-      <c r="T39" s="59"/>
-    </row>
-    <row r="40" spans="8:20">
-      <c r="H40" s="58" t="s">
-        <v>80</v>
-      </c>
-      <c r="I40" s="52">
-        <f>K40/J40</f>
-        <v>0.85</v>
-      </c>
-      <c r="J40" s="52">
-        <v>2</v>
-      </c>
-      <c r="K40" s="52">
-        <v>1.7</v>
-      </c>
-      <c r="L40" s="52">
-        <f>N40/M40</f>
-        <v>0.85</v>
-      </c>
-      <c r="M40" s="52">
-        <v>2</v>
-      </c>
-      <c r="N40" s="52">
-        <v>1.7</v>
-      </c>
-      <c r="O40" s="52"/>
-      <c r="P40" s="52"/>
-      <c r="Q40" s="52"/>
-      <c r="R40" s="52"/>
-      <c r="S40" s="52"/>
-      <c r="T40" s="59"/>
-    </row>
-    <row r="41" spans="8:20">
-      <c r="H41" s="58" t="s">
-        <v>95</v>
-      </c>
-      <c r="I41" s="52"/>
-      <c r="J41" s="52"/>
-      <c r="K41" s="52">
-        <f>K38-K40</f>
-        <v>0.67540000000000044</v>
-      </c>
-      <c r="L41" s="52"/>
-      <c r="M41" s="52"/>
-      <c r="N41" s="52">
-        <f>N38-N40</f>
-        <v>1.0845999999999998</v>
-      </c>
-      <c r="O41" s="52"/>
-      <c r="P41" s="52"/>
-      <c r="Q41" s="52"/>
-      <c r="R41" s="52"/>
-      <c r="S41" s="52"/>
-      <c r="T41" s="59"/>
-    </row>
-    <row r="42" spans="8:20">
-      <c r="H42" s="58" t="s">
-        <v>86</v>
-      </c>
-      <c r="I42" s="52"/>
-      <c r="J42" s="52"/>
-      <c r="K42" s="52"/>
-      <c r="L42" s="77">
-        <f>L40*M40/L38/M38</f>
-        <v>0.61050061050061055</v>
-      </c>
-      <c r="M42" s="52"/>
-      <c r="N42" s="52"/>
-      <c r="O42" s="52"/>
-      <c r="P42" s="52"/>
-      <c r="Q42" s="52"/>
-      <c r="R42" s="52"/>
-      <c r="S42" s="52"/>
-      <c r="T42" s="59"/>
-    </row>
-    <row r="43" spans="8:20" ht="14.4" thickBot="1">
-      <c r="H43" s="60" t="s">
-        <v>88</v>
-      </c>
-      <c r="I43" s="61"/>
-      <c r="J43" s="61"/>
-      <c r="K43" s="61"/>
-      <c r="L43" s="61">
-        <f>N39/L40/M40</f>
+      <c r="AA71" s="99"/>
+      <c r="AB71" s="99"/>
+      <c r="AC71" s="99"/>
+      <c r="AD71" s="99">
+        <f>AF67/AD68/AE68</f>
         <v>82.935333073626808</v>
       </c>
-      <c r="M43" s="61"/>
-      <c r="N43" s="61"/>
-      <c r="O43" s="61"/>
-      <c r="P43" s="61"/>
-      <c r="Q43" s="61"/>
-      <c r="R43" s="61"/>
-      <c r="S43" s="61"/>
-      <c r="T43" s="62"/>
+      <c r="AE71" s="99"/>
+      <c r="AF71" s="99"/>
+      <c r="AG71" s="99"/>
+      <c r="AH71" s="99"/>
+      <c r="AI71" s="99"/>
+      <c r="AJ71" s="99"/>
+      <c r="AK71" s="99"/>
+      <c r="AL71" s="100"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="O30:Q30"/>
-    <mergeCell ref="L30:N30"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="O10:Q10"/>
+  <mergeCells count="7">
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="A15:A34"/>
+    <mergeCell ref="AG58:AI58"/>
+    <mergeCell ref="AD58:AF58"/>
+    <mergeCell ref="AA34:AC34"/>
+    <mergeCell ref="AD34:AF34"/>
+    <mergeCell ref="AG34:AI34"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat(HW.vsdx, parameter, network): Add info
</commit_message>
<xml_diff>
--- a/hardware/docs/01-top/点云硬件参数分析.xlsx
+++ b/hardware/docs/01-top/点云硬件参数分析.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="12960" windowHeight="4872" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="12960" windowHeight="4872"/>
   </bookViews>
   <sheets>
     <sheet name="整体评估" sheetId="5" r:id="rId1"/>
     <sheet name="历次综合结果" sheetId="3" r:id="rId2"/>
     <sheet name="T28工艺库单元特性-面积" sheetId="6" r:id="rId3"/>
+    <sheet name="技术提升" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
     <author>作者</author>
   </authors>
   <commentList>
-    <comment ref="C9" authorId="0" shapeId="0">
+    <comment ref="D9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -74,11 +75,11 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-师姐100MHz综合前后90-50mW，我100MHz综合功耗63mW，后仿保守估计不变，200MHz120mW</t>
+总计算量为PointNeXt-S论文的TOPS</t>
         </r>
       </text>
     </comment>
-    <comment ref="A12" authorId="0" shapeId="0">
+    <comment ref="C12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -100,11 +101,63 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-总计算量为PointNeXt-S论文的TOPS</t>
+师姐100MHz综合前后90-50mW，我100MHz综合功耗63mW，后仿保守估计不变，200MHz120mW</t>
         </r>
       </text>
     </comment>
-    <comment ref="C13" authorId="0" shapeId="0">
+    <comment ref="B13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+PointNeXt-S总周期为FPS 3k的3倍9k</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+总时间计算的有效算力</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -130,59 +183,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A15" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">
-PointNeXt-S总周期为FPS 3k的3倍9k</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A16" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">
-总时间计算的有效算力</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C23" authorId="0" shapeId="0">
+    <comment ref="D33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -208,7 +209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B25" authorId="0" shapeId="0">
+    <comment ref="C35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -602,7 +603,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="142">
   <si>
     <t>case</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1374,6 +1375,42 @@
   </si>
   <si>
     <t>Total area including interconnnect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Real TOP (PointNeXt-S)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>??</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>All Tech.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Only Block-wise Delay-Aggregation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Block-wise Delay-Aggreation + MLP Fusion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Block-wise Delay-Aggreation + MLP Fusion + FPS Skipping</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Block-wise Delay-Aggreation + MLP Fusion + Filter Pruning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Baseline</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1534,7 +1571,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -1944,11 +1981,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -2061,9 +2142,6 @@
     <xf numFmtId="176" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2133,62 +2211,11 @@
     <xf numFmtId="179" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="180" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="180" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2229,9 +2256,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2239,6 +2263,96 @@
     <xf numFmtId="180" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="180" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2519,342 +2633,459 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.44140625" style="29" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" style="29" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" style="29" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="29"/>
+    <col min="1" max="1" width="47.77734375" style="29" customWidth="1"/>
+    <col min="2" max="2" width="56.44140625" style="29" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" style="29" customWidth="1"/>
+    <col min="4" max="4" width="25.44140625" style="29" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="39"/>
-      <c r="B1" s="41" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="125"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="D1" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="30"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="E1" s="30"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="30"/>
+      <c r="B2" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="C2" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="D2" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="30"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="E2" s="30"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="30"/>
+      <c r="B3" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="45">
+      <c r="C3" s="44">
         <v>3</v>
       </c>
-      <c r="C3" s="44">
+      <c r="D3" s="43">
         <v>12.96</v>
       </c>
-      <c r="D3" s="30"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+      <c r="E3" s="30"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="30"/>
+      <c r="B4" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="45">
+      <c r="C4" s="44">
         <v>140</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="D4" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="30"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="E4" s="30"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="30"/>
+      <c r="B5" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="C5" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="D5" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="G5" s="56"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="E5" s="30"/>
+      <c r="H5" s="55"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="30"/>
+      <c r="B6" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="45">
+      <c r="C6" s="44">
         <v>0.9</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="D6" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="G6" s="56"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
+      <c r="E6" s="30"/>
+      <c r="H6" s="55"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="45">
+      <c r="C7" s="44">
         <v>200</v>
       </c>
-      <c r="C7" s="44">
+      <c r="D7" s="43">
         <v>250</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="G7" s="56"/>
-    </row>
-    <row r="8" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="35" t="s">
+      <c r="E7" s="30"/>
+      <c r="H7" s="55"/>
+    </row>
+    <row r="8" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="30"/>
+      <c r="B8" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="C8" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="D8" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="G8" s="56"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="39" t="s">
+      <c r="E8" s="30"/>
+      <c r="H8" s="55"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="125"/>
+      <c r="B9" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="41">
+      <c r="C9" s="40">
         <v>1024</v>
       </c>
-      <c r="C9" s="50">
+      <c r="D9" s="49">
         <v>12288</v>
       </c>
-      <c r="D9" s="30"/>
-      <c r="G9" s="56"/>
-    </row>
-    <row r="10" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="32" t="s">
+      <c r="E9" s="30"/>
+      <c r="H9" s="55"/>
+    </row>
+    <row r="10" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="126"/>
+      <c r="B10" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="C10" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="D10" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="30"/>
-      <c r="G10" s="56"/>
-    </row>
-    <row r="11" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" s="36">
-        <v>0.15</v>
-      </c>
-      <c r="C11" s="33">
-        <v>0.60899999999999999</v>
-      </c>
-      <c r="D11" s="30"/>
-      <c r="G11" s="56"/>
-    </row>
-    <row r="12" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="39" t="s">
+      <c r="E10" s="30"/>
+      <c r="H10" s="55"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="125"/>
+      <c r="B11" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="B12" s="59">
+      <c r="C11" s="58">
         <f>3.6/1024</f>
         <v>3.5156250000000001E-3</v>
       </c>
-      <c r="C12" s="57" t="s">
+      <c r="D11" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="D12" s="30"/>
-      <c r="G12" s="56"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="39" t="s">
+      <c r="E11" s="30"/>
+      <c r="H11" s="55"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="127" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="36">
+        <v>0.15</v>
+      </c>
+      <c r="D12" s="33">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="E12" s="30"/>
+      <c r="H12" s="55"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="128"/>
+      <c r="B13" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="59">
+        <f>5.715*1024</f>
+        <v>5852.16</v>
+      </c>
+      <c r="D13" s="53" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" s="30"/>
+      <c r="H13" s="55"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="128"/>
+      <c r="B14" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="54">
+        <f>C11/(C13*5*10^(-9))</f>
+        <v>120.14794537401575</v>
+      </c>
+      <c r="D14" s="53">
+        <f>D33/D12</f>
+        <v>19.047619047619047</v>
+      </c>
+      <c r="E14" s="30"/>
+      <c r="H14" s="55"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="128"/>
+      <c r="B15" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="60">
+        <f>C14/C19</f>
+        <v>46.136811023622045</v>
+      </c>
+      <c r="D15" s="57">
+        <f>D14/D19</f>
+        <v>1.9797333333333333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="128"/>
+      <c r="B16" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="57">
+        <f>C12*(C13*5*10^(-9))</f>
+        <v>4.3891199999999997E-6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="128"/>
+      <c r="B17" s="119" t="s">
+        <v>133</v>
+      </c>
+      <c r="C17" s="123" t="s">
+        <v>134</v>
+      </c>
+      <c r="D17" s="121" t="s">
+        <v>135</v>
+      </c>
+      <c r="E17" s="30"/>
+      <c r="H17" s="122"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="128"/>
+      <c r="B18" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="38">
-        <f>B9*B7*2/1024/1024</f>
+      <c r="C18" s="124">
+        <f>C9*C7*2/1024/1024</f>
         <v>0.390625</v>
       </c>
-      <c r="C13" s="37">
-        <f>C9*C7*2/1024/1024</f>
+      <c r="D18" s="37">
+        <f>D9*D7*2/1024/1024</f>
         <v>5.859375</v>
       </c>
-      <c r="D13" s="30"/>
-      <c r="G13" s="56"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="35" t="s">
+      <c r="E18" s="30"/>
+      <c r="H18" s="55"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="129"/>
+      <c r="B19" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="34">
-        <f>B13/B11</f>
+      <c r="C19" s="34">
+        <f>C18/C12</f>
         <v>2.604166666666667</v>
       </c>
-      <c r="C14" s="49">
-        <f>C13/C11</f>
+      <c r="D19" s="48">
+        <f>D18/D12</f>
         <v>9.6213054187192117</v>
       </c>
-      <c r="D14" s="30"/>
-      <c r="G14" s="56"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="B15" s="60">
-        <f>9*1024</f>
-        <v>9216</v>
-      </c>
-      <c r="C15" s="54" t="s">
-        <v>101</v>
-      </c>
-      <c r="D15" s="30"/>
-      <c r="G15" s="56"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="B16" s="55">
-        <f>B12/(B15*5*10^(-9))</f>
-        <v>76.293945312499986</v>
-      </c>
-      <c r="C16" s="54">
-        <f>C23/C11</f>
+      <c r="E19" s="30"/>
+      <c r="H19" s="55"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="35"/>
+      <c r="B20" s="119"/>
+      <c r="C20" s="120"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="30"/>
+      <c r="H20" s="122"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="B21" s="119"/>
+      <c r="C21" s="120"/>
+      <c r="D21" s="121"/>
+      <c r="E21" s="30"/>
+      <c r="H21" s="122"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="35"/>
+      <c r="B22" s="130"/>
+      <c r="C22" s="120"/>
+      <c r="D22" s="121"/>
+      <c r="E22" s="30"/>
+      <c r="H22" s="122"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="35" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="35"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="35"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="B26" s="126"/>
+      <c r="C26" s="126"/>
+      <c r="D26" s="126"/>
+      <c r="H26" s="122"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="35"/>
+      <c r="B27" s="126"/>
+      <c r="C27" s="126"/>
+      <c r="D27" s="126"/>
+      <c r="H27" s="122"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="B28" s="126"/>
+      <c r="C28" s="126"/>
+      <c r="D28" s="126"/>
+      <c r="H28" s="122"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="126"/>
+      <c r="C29" s="126"/>
+      <c r="D29" s="126"/>
+      <c r="H29" s="122"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="B30" s="126"/>
+      <c r="C30" s="126"/>
+      <c r="D30" s="126"/>
+      <c r="H30" s="122"/>
+    </row>
+    <row r="31" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32">
+        <f>D35/4*(1.1/0.9)^2</f>
+        <v>7.1134626690182259</v>
+      </c>
+      <c r="H31" s="55"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="29">
+        <f>C34/C18</f>
+        <v>40</v>
+      </c>
+      <c r="H32" s="55"/>
+    </row>
+    <row r="33" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A33" s="30"/>
+      <c r="B33" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="34">
+        <f>C18*10</f>
+        <v>3.90625</v>
+      </c>
+      <c r="D33" s="48">
+        <v>11.6</v>
+      </c>
+      <c r="E33" s="30"/>
+      <c r="H33" s="55"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="34">
+        <f>C33*4</f>
+        <v>15.625</v>
+      </c>
+      <c r="D34" s="48"/>
+      <c r="E34" s="30"/>
+      <c r="H34" s="55"/>
+    </row>
+    <row r="35" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="126"/>
+      <c r="B35" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="47">
+        <f>C34/C12</f>
+        <v>104.16666666666667</v>
+      </c>
+      <c r="D35" s="31">
+        <f>D33/D12</f>
         <v>19.047619047619047</v>
       </c>
-      <c r="D16" s="30"/>
-      <c r="G16" s="56"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="B17" s="61">
-        <f>B16/B14</f>
-        <v>29.296874999999993</v>
-      </c>
-      <c r="C17" s="58">
-        <f>C16/C14</f>
-        <v>1.9797333333333333</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="B18" s="58">
-        <f>B11*(B15*5*10^(-9))</f>
-        <v>6.9120000000000009E-6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32">
-        <f>C25/4*(1.1/0.9)^2</f>
-        <v>7.1134626690182259</v>
-      </c>
-      <c r="G21" s="56"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="B22" s="29">
-        <f>B24/B13</f>
-        <v>40</v>
-      </c>
-      <c r="G22" s="56"/>
-    </row>
-    <row r="23" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="B23" s="34">
-        <f>B13*10</f>
-        <v>3.90625</v>
-      </c>
-      <c r="C23" s="49">
-        <v>11.6</v>
-      </c>
-      <c r="D23" s="30"/>
-      <c r="G23" s="56"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="B24" s="34">
-        <f>B23*4</f>
-        <v>15.625</v>
-      </c>
-      <c r="C24" s="49"/>
-      <c r="D24" s="30"/>
-      <c r="G24" s="56"/>
-    </row>
-    <row r="25" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="48">
-        <f>B24/B11</f>
-        <v>104.16666666666667</v>
-      </c>
-      <c r="C25" s="31">
-        <f>C23/C11</f>
-        <v>19.047619047619047</v>
-      </c>
-      <c r="D25" s="30"/>
-      <c r="G25" s="56"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G26" s="56"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G27" s="56"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G28" s="56"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G29" s="56"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G30" s="56"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G31" s="56"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G32" s="56"/>
-    </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G33" s="56"/>
+      <c r="E35" s="30"/>
+      <c r="H35" s="55"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H36" s="55"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H37" s="55"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H38" s="55"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H39" s="55"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H40" s="55"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H41" s="55"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H42" s="55"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H43" s="55"/>
     </row>
   </sheetData>
-  <sortState ref="A40:G72">
-    <sortCondition descending="1" ref="A40:A72"/>
+  <sortState ref="B40:H72">
+    <sortCondition descending="1" ref="B40:B72"/>
   </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="A12:A19"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2893,26 +3124,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="E1" s="51"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="62" t="s">
+      <c r="E1" s="50"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="101" t="s">
         <v>82</v>
       </c>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
-      <c r="O1" s="64"/>
-      <c r="P1" s="65" t="s">
+      <c r="K1" s="102"/>
+      <c r="L1" s="102"/>
+      <c r="M1" s="102"/>
+      <c r="N1" s="102"/>
+      <c r="O1" s="103"/>
+      <c r="P1" s="104" t="s">
         <v>83</v>
       </c>
-      <c r="Q1" s="63"/>
-      <c r="R1" s="63"/>
-      <c r="S1" s="63"/>
-      <c r="T1" s="64"/>
+      <c r="Q1" s="102"/>
+      <c r="R1" s="102"/>
+      <c r="S1" s="102"/>
+      <c r="T1" s="103"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2922,14 +3153,14 @@
       <c r="C2" s="1"/>
       <c r="D2" s="6"/>
       <c r="E2" s="24"/>
-      <c r="F2" s="69">
+      <c r="F2" s="108">
         <v>0</v>
       </c>
-      <c r="G2" s="70"/>
-      <c r="H2" s="69">
+      <c r="G2" s="109"/>
+      <c r="H2" s="108">
         <v>1</v>
       </c>
-      <c r="I2" s="70"/>
+      <c r="I2" s="109"/>
       <c r="J2" s="8">
         <v>2</v>
       </c>
@@ -2954,18 +3185,18 @@
       <c r="C3" s="1"/>
       <c r="D3" s="6"/>
       <c r="E3" s="25"/>
-      <c r="F3" s="62" t="s">
+      <c r="F3" s="101" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="71"/>
-      <c r="H3" s="62" t="s">
+      <c r="G3" s="110"/>
+      <c r="H3" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="71"/>
-      <c r="J3" s="62" t="s">
+      <c r="I3" s="110"/>
+      <c r="J3" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="64"/>
+      <c r="K3" s="103"/>
       <c r="L3" s="2" t="s">
         <v>41</v>
       </c>
@@ -3081,7 +3312,7 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
+      <c r="A8" s="45"/>
       <c r="B8" s="1" t="s">
         <v>66</v>
       </c>
@@ -3102,7 +3333,7 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="105" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -3130,7 +3361,7 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="67"/>
+      <c r="A10" s="106"/>
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
@@ -3156,7 +3387,7 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="67"/>
+      <c r="A11" s="106"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
         <v>15</v>
@@ -3179,7 +3410,7 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="67"/>
+      <c r="A12" s="106"/>
       <c r="B12" s="1"/>
       <c r="C12" s="3"/>
       <c r="D12" s="11" t="s">
@@ -3191,7 +3422,7 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="67"/>
+      <c r="A13" s="106"/>
       <c r="B13" s="1"/>
       <c r="C13" s="3"/>
       <c r="E13" s="19" t="s">
@@ -3206,7 +3437,7 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="67"/>
+      <c r="A14" s="106"/>
       <c r="B14" s="1"/>
       <c r="C14" s="3"/>
       <c r="E14" s="19" t="s">
@@ -3220,7 +3451,7 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="67"/>
+      <c r="A15" s="106"/>
       <c r="B15" s="1"/>
       <c r="C15" s="3"/>
       <c r="D15" s="19"/>
@@ -3228,7 +3459,7 @@
       <c r="H15" s="15"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="67"/>
+      <c r="A16" s="106"/>
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
         <v>16</v>
@@ -3251,14 +3482,14 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="67"/>
+      <c r="A17" s="106"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="6"/>
       <c r="E17" s="25"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="67"/>
+      <c r="A18" s="106"/>
       <c r="B18" s="1" t="s">
         <v>10</v>
       </c>
@@ -3282,7 +3513,7 @@
       <c r="N18" s="2">
         <v>477691</v>
       </c>
-      <c r="O18" s="47">
+      <c r="O18" s="46">
         <f>N18/N9*100</f>
         <v>39.680638357787046</v>
       </c>
@@ -3297,7 +3528,7 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="67"/>
+      <c r="A19" s="106"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
         <v>17</v>
@@ -3329,7 +3560,7 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="67"/>
+      <c r="A20" s="106"/>
       <c r="B20" s="1"/>
       <c r="C20" s="2" t="s">
         <v>39</v>
@@ -3340,7 +3571,7 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="67"/>
+      <c r="A21" s="106"/>
       <c r="B21" s="1"/>
       <c r="C21" s="2" t="s">
         <v>40</v>
@@ -3351,7 +3582,7 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="67"/>
+      <c r="A22" s="106"/>
       <c r="B22" s="1" t="s">
         <v>13</v>
       </c>
@@ -3381,7 +3612,7 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="67"/>
+      <c r="A23" s="106"/>
       <c r="B23" s="1"/>
       <c r="C23" s="2" t="s">
         <v>18</v>
@@ -3402,7 +3633,7 @@
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="67"/>
+      <c r="A24" s="106"/>
       <c r="B24" s="1"/>
       <c r="D24" s="7" t="s">
         <v>43</v>
@@ -3417,7 +3648,7 @@
       </c>
     </row>
     <row r="25" spans="1:18" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A25" s="67"/>
+      <c r="A25" s="106"/>
       <c r="B25" s="1"/>
       <c r="E25" s="7" t="s">
         <v>42</v>
@@ -3432,7 +3663,7 @@
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="67"/>
+      <c r="A26" s="106"/>
       <c r="B26" s="1"/>
       <c r="C26" s="2" t="s">
         <v>19</v>
@@ -3449,7 +3680,7 @@
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="67"/>
+      <c r="A27" s="106"/>
       <c r="B27" s="1"/>
       <c r="C27" s="2" t="s">
         <v>20</v>
@@ -3463,7 +3694,7 @@
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="67"/>
+      <c r="A28" s="106"/>
       <c r="B28" s="1" t="s">
         <v>9</v>
       </c>
@@ -3493,7 +3724,7 @@
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="67"/>
+      <c r="A29" s="106"/>
       <c r="B29" s="1"/>
       <c r="C29" s="2" t="s">
         <v>21</v>
@@ -3513,7 +3744,7 @@
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="67"/>
+      <c r="A30" s="106"/>
       <c r="B30" s="1"/>
       <c r="C30" s="2" t="s">
         <v>22</v>
@@ -3526,7 +3757,7 @@
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="67"/>
+      <c r="A31" s="106"/>
       <c r="B31" s="1" t="s">
         <v>8</v>
       </c>
@@ -3553,7 +3784,7 @@
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="68"/>
+      <c r="A32" s="107"/>
       <c r="B32" s="1" t="s">
         <v>11</v>
       </c>
@@ -3577,7 +3808,7 @@
       <c r="N32" s="2">
         <v>507456</v>
       </c>
-      <c r="O32" s="47">
+      <c r="O32" s="46">
         <f>N32/N9*100</f>
         <v>42.153145063417945</v>
       </c>
@@ -3656,7 +3887,7 @@
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="66" t="s">
+      <c r="A38" s="105" t="s">
         <v>24</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -3672,7 +3903,7 @@
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="67"/>
+      <c r="A39" s="106"/>
       <c r="B39" s="1" t="s">
         <v>12</v>
       </c>
@@ -3688,14 +3919,14 @@
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="67"/>
+      <c r="A40" s="106"/>
       <c r="B40" s="1"/>
       <c r="C40" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="67"/>
+      <c r="A41" s="106"/>
       <c r="B41" s="1"/>
       <c r="C41" s="3"/>
       <c r="D41" s="11" t="s">
@@ -3703,7 +3934,7 @@
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="67"/>
+      <c r="A42" s="106"/>
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
       <c r="E42" s="19" t="s">
@@ -3711,7 +3942,7 @@
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="67"/>
+      <c r="A43" s="106"/>
       <c r="B43" s="1"/>
       <c r="C43" s="3"/>
       <c r="E43" s="19" t="s">
@@ -3719,28 +3950,28 @@
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="67"/>
+      <c r="A44" s="106"/>
       <c r="B44" s="1"/>
       <c r="C44" s="3"/>
       <c r="D44" s="19"/>
       <c r="E44" s="27"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="67"/>
+      <c r="A45" s="106"/>
       <c r="B45" s="1"/>
       <c r="C45" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="67"/>
+      <c r="A46" s="106"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="6"/>
       <c r="E46" s="25"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="67"/>
+      <c r="A47" s="106"/>
       <c r="B47" s="1" t="s">
         <v>10</v>
       </c>
@@ -3756,7 +3987,7 @@
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="68"/>
+      <c r="A48" s="107"/>
       <c r="B48" s="1"/>
       <c r="C48" s="2" t="s">
         <v>17</v>
@@ -3888,1257 +4119,1257 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="76" customWidth="1"/>
-    <col min="2" max="4" width="11.21875" style="76" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="76" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" style="76" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="76"/>
-    <col min="8" max="9" width="12.21875" style="76" customWidth="1"/>
-    <col min="10" max="11" width="8.88671875" style="76"/>
-    <col min="12" max="12" width="12.77734375" style="76" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="76"/>
+    <col min="1" max="1" width="13.5546875" style="64" customWidth="1"/>
+    <col min="2" max="4" width="11.21875" style="64" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="64" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="64" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="64"/>
+    <col min="8" max="9" width="12.21875" style="64" customWidth="1"/>
+    <col min="10" max="11" width="8.88671875" style="64"/>
+    <col min="12" max="12" width="12.77734375" style="64" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="64"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="61" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="61" t="s">
         <v>104</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="61" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="72" t="s">
+      <c r="E1" s="61" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="72" t="s">
+      <c r="F1" s="61" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="76" t="s">
+      <c r="G1" s="64" t="s">
         <v>128</v>
       </c>
-      <c r="H1" s="76" t="s">
+      <c r="H1" s="64" t="s">
         <v>129</v>
       </c>
-      <c r="I1" s="76" t="s">
+      <c r="I1" s="64" t="s">
         <v>132</v>
       </c>
-      <c r="J1" s="76" t="s">
+      <c r="J1" s="64" t="s">
         <v>130</v>
       </c>
-      <c r="K1" s="76" t="s">
+      <c r="K1" s="64" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="72">
+      <c r="B2" s="61">
         <v>2048</v>
       </c>
-      <c r="C2" s="72">
+      <c r="C2" s="61">
         <v>1</v>
       </c>
-      <c r="D2" s="72">
+      <c r="D2" s="61">
         <f>B2*C2/8192</f>
         <v>0.25</v>
       </c>
-      <c r="E2" s="72">
+      <c r="E2" s="61">
         <v>6750</v>
       </c>
-      <c r="F2" s="73">
+      <c r="F2" s="62">
         <f>(B2*C2)/E2</f>
         <v>0.3034074074074074</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="111" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="72">
+      <c r="B3" s="61">
         <v>32</v>
       </c>
-      <c r="C3" s="72">
+      <c r="C3" s="61">
         <v>16</v>
       </c>
-      <c r="D3" s="72">
+      <c r="D3" s="61">
         <f t="shared" ref="D3:D29" si="0">B3*C3/8192</f>
         <v>6.25E-2</v>
       </c>
-      <c r="E3" s="72">
+      <c r="E3" s="61">
         <v>2762</v>
       </c>
-      <c r="F3" s="73">
+      <c r="F3" s="62">
         <f t="shared" ref="F3:F29" si="1">(B3*C3)/E3</f>
         <v>0.18537291817523532</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="74"/>
-      <c r="B4" s="72">
+      <c r="A4" s="111"/>
+      <c r="B4" s="61">
         <v>32</v>
       </c>
-      <c r="C4" s="72">
+      <c r="C4" s="61">
         <v>128</v>
       </c>
-      <c r="D4" s="72">
+      <c r="D4" s="61">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="E4" s="72">
+      <c r="E4" s="61">
         <v>15180</v>
       </c>
-      <c r="F4" s="73">
+      <c r="F4" s="62">
         <f t="shared" si="1"/>
         <v>0.26982872200263502</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="74"/>
-      <c r="B5" s="72">
+      <c r="A5" s="111"/>
+      <c r="B5" s="61">
         <v>64</v>
       </c>
-      <c r="C5" s="72">
+      <c r="C5" s="61">
         <v>128</v>
       </c>
-      <c r="D5" s="72">
+      <c r="D5" s="61">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E5" s="72">
+      <c r="E5" s="61">
         <v>15867</v>
       </c>
-      <c r="F5" s="73">
+      <c r="F5" s="62">
         <f t="shared" si="1"/>
         <v>0.51629167454465241</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="74"/>
-      <c r="B6" s="72">
+      <c r="A6" s="111"/>
+      <c r="B6" s="61">
         <v>64</v>
       </c>
-      <c r="C6" s="72">
+      <c r="C6" s="61">
         <v>64</v>
       </c>
-      <c r="D6" s="72">
+      <c r="D6" s="61">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="E6" s="72">
+      <c r="E6" s="61">
         <v>8451</v>
       </c>
-      <c r="F6" s="73">
+      <c r="F6" s="62">
         <f t="shared" si="1"/>
         <v>0.48467636966039523</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="74"/>
-      <c r="B7" s="72">
+      <c r="A7" s="111"/>
+      <c r="B7" s="61">
         <v>128</v>
       </c>
-      <c r="C7" s="72">
+      <c r="C7" s="61">
         <v>64</v>
       </c>
-      <c r="D7" s="72">
+      <c r="D7" s="61">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E7" s="72">
+      <c r="E7" s="61">
         <v>9182</v>
       </c>
-      <c r="F7" s="118">
+      <c r="F7" s="99">
         <f t="shared" si="1"/>
         <v>0.89218035286429975</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="74"/>
-      <c r="B8" s="72">
+      <c r="A8" s="111"/>
+      <c r="B8" s="61">
         <v>128</v>
       </c>
-      <c r="C8" s="72">
+      <c r="C8" s="61">
         <v>128</v>
       </c>
-      <c r="D8" s="72">
+      <c r="D8" s="61">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E8" s="72">
+      <c r="E8" s="61">
         <v>17239</v>
       </c>
-      <c r="F8" s="118">
+      <c r="F8" s="99">
         <f t="shared" si="1"/>
         <v>0.95040315563547773</v>
       </c>
-      <c r="H8" s="76">
+      <c r="H8" s="64">
         <f>E8*32/1000000</f>
         <v>0.55164800000000003</v>
       </c>
-      <c r="I8" s="76">
+      <c r="I8" s="64">
         <f>H8+0.16</f>
         <v>0.71164800000000006</v>
       </c>
-      <c r="J8" s="76">
+      <c r="J8" s="64">
         <f>(1.27-(H8+0.16))/1.27</f>
         <v>0.43964724409448813</v>
       </c>
-      <c r="K8" s="76">
+      <c r="K8" s="64">
         <f>(D8-4)/4</f>
         <v>-0.5</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="74"/>
-      <c r="B9" s="115">
+      <c r="A9" s="111"/>
+      <c r="B9" s="96">
         <v>256</v>
       </c>
-      <c r="C9" s="115">
+      <c r="C9" s="96">
         <v>128</v>
       </c>
-      <c r="D9" s="115">
+      <c r="D9" s="96">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E9" s="115">
+      <c r="E9" s="96">
         <v>19964</v>
       </c>
-      <c r="F9" s="118">
+      <c r="F9" s="99">
         <f t="shared" si="1"/>
         <v>1.6413544379883791</v>
       </c>
-      <c r="G9" s="119">
+      <c r="G9" s="100">
         <f>(F9-F8)/F8</f>
         <v>0.72700861550791418</v>
       </c>
-      <c r="H9" s="119">
+      <c r="H9" s="100">
         <f t="shared" ref="H9:H13" si="2">E9*32/1000000</f>
         <v>0.63884799999999997</v>
       </c>
-      <c r="I9" s="119">
+      <c r="I9" s="100">
         <f t="shared" ref="I9:I13" si="3">H9+0.16</f>
         <v>0.798848</v>
       </c>
-      <c r="J9" s="119">
+      <c r="J9" s="100">
         <f t="shared" ref="J9:J10" si="4">(1.27-(H9+0.16))/1.27</f>
         <v>0.37098582677165354</v>
       </c>
-      <c r="K9" s="119">
+      <c r="K9" s="100">
         <f t="shared" ref="K9:K10" si="5">(D9-4)/4</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="74"/>
-      <c r="B10" s="114">
+      <c r="A10" s="111"/>
+      <c r="B10" s="95">
         <v>512</v>
       </c>
-      <c r="C10" s="114">
+      <c r="C10" s="95">
         <v>128</v>
       </c>
-      <c r="D10" s="114">
+      <c r="D10" s="95">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E10" s="114">
+      <c r="E10" s="95">
         <v>25586</v>
       </c>
-      <c r="F10" s="75">
+      <c r="F10" s="63">
         <f t="shared" si="1"/>
         <v>2.5614007660439304</v>
       </c>
-      <c r="G10" s="103">
+      <c r="G10" s="85">
         <f t="shared" ref="G10:G13" si="6">(F10-F9)/F9</f>
         <v>0.56054092081607132</v>
       </c>
-      <c r="H10" s="103">
+      <c r="H10" s="85">
         <f t="shared" si="2"/>
         <v>0.81875200000000004</v>
       </c>
-      <c r="I10" s="76">
+      <c r="I10" s="64">
         <f t="shared" si="3"/>
         <v>0.97875200000000007</v>
       </c>
-      <c r="J10" s="76">
+      <c r="J10" s="64">
         <f t="shared" si="4"/>
         <v>0.22932913385826767</v>
       </c>
-      <c r="K10" s="76">
+      <c r="K10" s="64">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="74"/>
-      <c r="B11" s="72">
+      <c r="A11" s="111"/>
+      <c r="B11" s="61">
         <v>1024</v>
       </c>
-      <c r="C11" s="72">
+      <c r="C11" s="61">
         <v>128</v>
       </c>
-      <c r="D11" s="72">
+      <c r="D11" s="61">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="E11" s="72">
+      <c r="E11" s="61">
         <v>36545</v>
       </c>
-      <c r="F11" s="73">
+      <c r="F11" s="62">
         <f t="shared" si="1"/>
         <v>3.5865918730332469</v>
       </c>
-      <c r="G11" s="76">
+      <c r="G11" s="64">
         <f t="shared" si="6"/>
         <v>0.40024627171979754</v>
       </c>
-      <c r="H11" s="76">
+      <c r="H11" s="64">
         <f t="shared" si="2"/>
         <v>1.16944</v>
       </c>
-      <c r="I11" s="76">
+      <c r="I11" s="64">
         <f t="shared" si="3"/>
         <v>1.32944</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="74"/>
-      <c r="B12" s="72">
+      <c r="A12" s="111"/>
+      <c r="B12" s="61">
         <v>2048</v>
       </c>
-      <c r="C12" s="72">
+      <c r="C12" s="61">
         <v>128</v>
       </c>
-      <c r="D12" s="72">
+      <c r="D12" s="61">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="E12" s="72">
+      <c r="E12" s="61">
         <v>63968</v>
       </c>
-      <c r="F12" s="73">
+      <c r="F12" s="62">
         <f t="shared" si="1"/>
         <v>4.0980490245122558</v>
       </c>
-      <c r="G12" s="76">
+      <c r="G12" s="64">
         <f t="shared" si="6"/>
         <v>0.14260255127563767</v>
       </c>
-      <c r="H12" s="76">
+      <c r="H12" s="64">
         <f t="shared" si="2"/>
         <v>2.0469759999999999</v>
       </c>
-      <c r="I12" s="76">
+      <c r="I12" s="64">
         <f t="shared" si="3"/>
         <v>2.206976</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="74"/>
-      <c r="B13" s="72">
+      <c r="A13" s="111"/>
+      <c r="B13" s="61">
         <v>4096</v>
       </c>
-      <c r="C13" s="72">
+      <c r="C13" s="61">
         <v>128</v>
       </c>
-      <c r="D13" s="72">
+      <c r="D13" s="61">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="E13" s="72">
+      <c r="E13" s="61">
         <v>118814</v>
       </c>
-      <c r="F13" s="73">
+      <c r="F13" s="62">
         <f t="shared" si="1"/>
         <v>4.4126786405642431</v>
       </c>
-      <c r="G13" s="76">
+      <c r="G13" s="64">
         <f t="shared" si="6"/>
         <v>7.6775464170888985E-2</v>
       </c>
-      <c r="H13" s="76">
+      <c r="H13" s="64">
         <f t="shared" si="2"/>
         <v>3.8020480000000001</v>
       </c>
-      <c r="I13" s="76">
+      <c r="I13" s="64">
         <f t="shared" si="3"/>
         <v>3.9620480000000002</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="72"/>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="73"/>
+      <c r="A14" s="61"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="62"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="74" t="s">
+      <c r="A15" s="111" t="s">
         <v>92</v>
       </c>
-      <c r="B15" s="72">
+      <c r="B15" s="61">
         <v>1024</v>
       </c>
-      <c r="C15" s="72">
+      <c r="C15" s="61">
         <v>32</v>
       </c>
-      <c r="D15" s="72">
+      <c r="D15" s="61">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E15" s="72">
+      <c r="E15" s="61">
         <v>8301</v>
       </c>
-      <c r="F15" s="73">
+      <c r="F15" s="62">
         <f t="shared" si="1"/>
         <v>3.947476207685821</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="74"/>
-      <c r="B16" s="72">
+      <c r="A16" s="111"/>
+      <c r="B16" s="61">
         <v>128</v>
       </c>
-      <c r="C16" s="72">
+      <c r="C16" s="61">
         <v>64</v>
       </c>
-      <c r="D16" s="72">
+      <c r="D16" s="61">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E16" s="72">
+      <c r="E16" s="61">
         <v>4316</v>
       </c>
-      <c r="F16" s="73">
+      <c r="F16" s="62">
         <f t="shared" si="1"/>
         <v>1.8980537534754403</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="74"/>
-      <c r="B17" s="72">
+      <c r="A17" s="111"/>
+      <c r="B17" s="61">
         <v>256</v>
       </c>
-      <c r="C17" s="72">
+      <c r="C17" s="61">
         <v>64</v>
       </c>
-      <c r="D17" s="72">
+      <c r="D17" s="61">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E17" s="72">
+      <c r="E17" s="61">
         <v>5786</v>
       </c>
-      <c r="F17" s="73">
+      <c r="F17" s="62">
         <f t="shared" si="1"/>
         <v>2.8316626339440027</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="74"/>
-      <c r="B18" s="72">
+      <c r="A18" s="111"/>
+      <c r="B18" s="61">
         <v>512</v>
       </c>
-      <c r="C18" s="72">
+      <c r="C18" s="61">
         <v>64</v>
       </c>
-      <c r="D18" s="72">
+      <c r="D18" s="61">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E18" s="72">
+      <c r="E18" s="61">
         <v>8726</v>
       </c>
-      <c r="F18" s="73">
+      <c r="F18" s="62">
         <f t="shared" si="1"/>
         <v>3.7552143020857209</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="74"/>
-      <c r="B19" s="72">
+      <c r="A19" s="111"/>
+      <c r="B19" s="61">
         <v>1024</v>
       </c>
-      <c r="C19" s="72">
+      <c r="C19" s="61">
         <v>64</v>
       </c>
-      <c r="D19" s="72">
+      <c r="D19" s="61">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E19" s="72">
+      <c r="E19" s="61">
         <v>14726</v>
       </c>
-      <c r="F19" s="73">
+      <c r="F19" s="62">
         <f t="shared" si="1"/>
         <v>4.45035990764634</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="74"/>
-      <c r="B20" s="72">
+      <c r="A20" s="111"/>
+      <c r="B20" s="61">
         <v>2048</v>
       </c>
-      <c r="C20" s="72">
+      <c r="C20" s="61">
         <v>64</v>
       </c>
-      <c r="D20" s="72">
+      <c r="D20" s="61">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="E20" s="72">
+      <c r="E20" s="61">
         <v>27288</v>
       </c>
-      <c r="F20" s="73">
+      <c r="F20" s="62">
         <f t="shared" si="1"/>
         <v>4.8032834945763705</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="74"/>
-      <c r="B21" s="72">
+      <c r="A21" s="111"/>
+      <c r="B21" s="61">
         <v>32</v>
       </c>
-      <c r="C21" s="72">
+      <c r="C21" s="61">
         <v>128</v>
       </c>
-      <c r="D21" s="72">
+      <c r="D21" s="61">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="E21" s="72">
+      <c r="E21" s="61">
         <v>3102</v>
       </c>
-      <c r="F21" s="73">
+      <c r="F21" s="62">
         <f t="shared" si="1"/>
         <v>1.3204384268214056</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="74"/>
-      <c r="B22" s="72">
+      <c r="A22" s="111"/>
+      <c r="B22" s="61">
         <v>64</v>
       </c>
-      <c r="C22" s="72">
+      <c r="C22" s="61">
         <v>128</v>
       </c>
-      <c r="D22" s="72">
+      <c r="D22" s="61">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E22" s="72">
+      <c r="E22" s="61">
         <v>3879</v>
       </c>
-      <c r="F22" s="73">
+      <c r="F22" s="62">
         <f t="shared" si="1"/>
         <v>2.1118845063160609</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="74"/>
-      <c r="B23" s="72">
+      <c r="A23" s="111"/>
+      <c r="B23" s="61">
         <v>128</v>
       </c>
-      <c r="C23" s="72">
+      <c r="C23" s="61">
         <v>128</v>
       </c>
-      <c r="D23" s="72">
+      <c r="D23" s="61">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E23" s="72">
+      <c r="E23" s="61">
         <v>8083</v>
       </c>
-      <c r="F23" s="73">
+      <c r="F23" s="62">
         <f t="shared" si="1"/>
         <v>2.0269701843374985</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="74"/>
-      <c r="B24" s="72">
+      <c r="A24" s="111"/>
+      <c r="B24" s="61">
         <v>256</v>
       </c>
-      <c r="C24" s="72">
+      <c r="C24" s="61">
         <v>128</v>
       </c>
-      <c r="D24" s="72">
+      <c r="D24" s="61">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E24" s="72">
+      <c r="E24" s="61">
         <v>10836</v>
       </c>
-      <c r="F24" s="75">
+      <c r="F24" s="63">
         <f t="shared" si="1"/>
         <v>3.0239940937615355</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="74"/>
-      <c r="B25" s="72">
+      <c r="A25" s="111"/>
+      <c r="B25" s="61">
         <v>512</v>
       </c>
-      <c r="C25" s="72">
+      <c r="C25" s="61">
         <v>128</v>
       </c>
-      <c r="D25" s="72">
+      <c r="D25" s="61">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E25" s="72">
+      <c r="E25" s="61">
         <v>16342</v>
       </c>
-      <c r="F25" s="75">
+      <c r="F25" s="63">
         <f t="shared" si="1"/>
         <v>4.0102802594541673</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="74"/>
-      <c r="B26" s="72">
+      <c r="A26" s="111"/>
+      <c r="B26" s="61">
         <v>1024</v>
       </c>
-      <c r="C26" s="72">
+      <c r="C26" s="61">
         <v>128</v>
       </c>
-      <c r="D26" s="72">
+      <c r="D26" s="61">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="E26" s="72">
+      <c r="E26" s="61">
         <v>27577</v>
       </c>
-      <c r="F26" s="75">
+      <c r="F26" s="63">
         <f t="shared" si="1"/>
         <v>4.7529462958262316</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="74"/>
-      <c r="B27" s="72">
+      <c r="A27" s="111"/>
+      <c r="B27" s="61">
         <v>2048</v>
       </c>
-      <c r="C27" s="72">
+      <c r="C27" s="61">
         <v>128</v>
       </c>
-      <c r="D27" s="72">
+      <c r="D27" s="61">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="E27" s="72">
+      <c r="E27" s="61">
         <v>51313</v>
       </c>
-      <c r="F27" s="73">
+      <c r="F27" s="62">
         <f t="shared" si="1"/>
         <v>5.1087248845321849</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="74"/>
-      <c r="B28" s="72">
+      <c r="A28" s="111"/>
+      <c r="B28" s="61">
         <v>64</v>
       </c>
-      <c r="C28" s="72">
+      <c r="C28" s="61">
         <v>256</v>
       </c>
-      <c r="D28" s="72">
+      <c r="D28" s="61">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E28" s="72">
+      <c r="E28" s="61">
         <v>7083</v>
       </c>
-      <c r="F28" s="73">
+      <c r="F28" s="62">
         <f t="shared" si="1"/>
         <v>2.3131441479599042</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="74"/>
-      <c r="B29" s="72">
+      <c r="A29" s="111"/>
+      <c r="B29" s="61">
         <v>128</v>
       </c>
-      <c r="C29" s="72">
+      <c r="C29" s="61">
         <v>256</v>
       </c>
-      <c r="D29" s="72">
+      <c r="D29" s="61">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E29" s="72">
+      <c r="E29" s="61">
         <v>9919</v>
       </c>
-      <c r="F29" s="117">
+      <c r="F29" s="98">
         <f t="shared" si="1"/>
         <v>3.3035588264946063</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="74"/>
-      <c r="B30" s="72"/>
-      <c r="C30" s="72"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="72"/>
-      <c r="F30" s="72"/>
+      <c r="A30" s="111"/>
+      <c r="B30" s="61"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="61"/>
+      <c r="E30" s="61"/>
+      <c r="F30" s="61"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="74"/>
-      <c r="B31" s="72"/>
-      <c r="C31" s="72"/>
-      <c r="D31" s="72"/>
-      <c r="E31" s="72"/>
-      <c r="F31" s="72"/>
+      <c r="A31" s="111"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="61"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="74"/>
-      <c r="B32" s="72"/>
-      <c r="C32" s="72"/>
-      <c r="D32" s="72"/>
-      <c r="E32" s="72"/>
-      <c r="F32" s="72"/>
+      <c r="A32" s="111"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="61"/>
     </row>
     <row r="33" spans="1:38" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="74"/>
-      <c r="B33" s="72"/>
-      <c r="C33" s="72"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="72"/>
-      <c r="F33" s="72"/>
+      <c r="A33" s="111"/>
+      <c r="B33" s="61"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="61"/>
     </row>
     <row r="34" spans="1:38" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="74"/>
-      <c r="B34" s="72"/>
-      <c r="C34" s="72"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="72"/>
-      <c r="F34" s="72"/>
-      <c r="Z34" s="77"/>
-      <c r="AA34" s="78" t="s">
+      <c r="A34" s="111"/>
+      <c r="B34" s="61"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="61"/>
+      <c r="Z34" s="65"/>
+      <c r="AA34" s="113" t="s">
         <v>114</v>
       </c>
-      <c r="AB34" s="79"/>
-      <c r="AC34" s="80"/>
-      <c r="AD34" s="81" t="s">
+      <c r="AB34" s="114"/>
+      <c r="AC34" s="115"/>
+      <c r="AD34" s="116" t="s">
         <v>115</v>
       </c>
-      <c r="AE34" s="82"/>
-      <c r="AF34" s="83"/>
-      <c r="AG34" s="81" t="s">
+      <c r="AE34" s="117"/>
+      <c r="AF34" s="118"/>
+      <c r="AG34" s="116" t="s">
         <v>116</v>
       </c>
-      <c r="AH34" s="82"/>
-      <c r="AI34" s="83"/>
-      <c r="AJ34" s="84" t="s">
+      <c r="AH34" s="117"/>
+      <c r="AI34" s="118"/>
+      <c r="AJ34" s="66" t="s">
         <v>117</v>
       </c>
-      <c r="AK34" s="85"/>
-      <c r="AL34" s="86"/>
+      <c r="AK34" s="67"/>
+      <c r="AL34" s="68"/>
     </row>
     <row r="35" spans="1:38" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Z35" s="77"/>
-      <c r="AA35" s="87"/>
-      <c r="AB35" s="88"/>
-      <c r="AC35" s="89"/>
-      <c r="AD35" s="90"/>
-      <c r="AE35" s="91"/>
-      <c r="AF35" s="92"/>
-      <c r="AG35" s="90"/>
-      <c r="AH35" s="91"/>
-      <c r="AI35" s="92"/>
-      <c r="AJ35" s="84"/>
-      <c r="AK35" s="85"/>
-      <c r="AL35" s="93"/>
+      <c r="Z35" s="65"/>
+      <c r="AA35" s="69"/>
+      <c r="AB35" s="70"/>
+      <c r="AC35" s="71"/>
+      <c r="AD35" s="72"/>
+      <c r="AE35" s="73"/>
+      <c r="AF35" s="74"/>
+      <c r="AG35" s="72"/>
+      <c r="AH35" s="73"/>
+      <c r="AI35" s="74"/>
+      <c r="AJ35" s="66"/>
+      <c r="AK35" s="67"/>
+      <c r="AL35" s="75"/>
     </row>
     <row r="36" spans="1:38" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Z36" s="77"/>
-      <c r="AA36" s="87"/>
-      <c r="AB36" s="88"/>
-      <c r="AC36" s="89"/>
-      <c r="AD36" s="90"/>
-      <c r="AE36" s="91"/>
-      <c r="AF36" s="92"/>
-      <c r="AG36" s="90"/>
-      <c r="AH36" s="91"/>
-      <c r="AI36" s="92"/>
-      <c r="AJ36" s="84"/>
-      <c r="AK36" s="85"/>
-      <c r="AL36" s="93"/>
+      <c r="Z36" s="65"/>
+      <c r="AA36" s="69"/>
+      <c r="AB36" s="70"/>
+      <c r="AC36" s="71"/>
+      <c r="AD36" s="72"/>
+      <c r="AE36" s="73"/>
+      <c r="AF36" s="74"/>
+      <c r="AG36" s="72"/>
+      <c r="AH36" s="73"/>
+      <c r="AI36" s="74"/>
+      <c r="AJ36" s="66"/>
+      <c r="AK36" s="67"/>
+      <c r="AL36" s="75"/>
     </row>
     <row r="37" spans="1:38" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Z37" s="77"/>
-      <c r="AA37" s="87"/>
-      <c r="AB37" s="88"/>
-      <c r="AC37" s="89"/>
-      <c r="AD37" s="90"/>
-      <c r="AE37" s="91"/>
-      <c r="AF37" s="92"/>
-      <c r="AG37" s="90"/>
-      <c r="AH37" s="91"/>
-      <c r="AI37" s="92"/>
-      <c r="AJ37" s="84"/>
-      <c r="AK37" s="85"/>
-      <c r="AL37" s="93"/>
+      <c r="Z37" s="65"/>
+      <c r="AA37" s="69"/>
+      <c r="AB37" s="70"/>
+      <c r="AC37" s="71"/>
+      <c r="AD37" s="72"/>
+      <c r="AE37" s="73"/>
+      <c r="AF37" s="74"/>
+      <c r="AG37" s="72"/>
+      <c r="AH37" s="73"/>
+      <c r="AI37" s="74"/>
+      <c r="AJ37" s="66"/>
+      <c r="AK37" s="67"/>
+      <c r="AL37" s="75"/>
     </row>
     <row r="38" spans="1:38" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Z38" s="77"/>
-      <c r="AA38" s="87"/>
-      <c r="AB38" s="88"/>
-      <c r="AC38" s="89"/>
-      <c r="AD38" s="90"/>
-      <c r="AE38" s="91"/>
-      <c r="AF38" s="92"/>
-      <c r="AG38" s="90"/>
-      <c r="AH38" s="91"/>
-      <c r="AI38" s="92"/>
-      <c r="AJ38" s="84"/>
-      <c r="AK38" s="85"/>
-      <c r="AL38" s="93"/>
+      <c r="Z38" s="65"/>
+      <c r="AA38" s="69"/>
+      <c r="AB38" s="70"/>
+      <c r="AC38" s="71"/>
+      <c r="AD38" s="72"/>
+      <c r="AE38" s="73"/>
+      <c r="AF38" s="74"/>
+      <c r="AG38" s="72"/>
+      <c r="AH38" s="73"/>
+      <c r="AI38" s="74"/>
+      <c r="AJ38" s="66"/>
+      <c r="AK38" s="67"/>
+      <c r="AL38" s="75"/>
     </row>
     <row r="39" spans="1:38" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Z39" s="77"/>
-      <c r="AA39" s="87"/>
-      <c r="AB39" s="88"/>
-      <c r="AC39" s="89"/>
-      <c r="AD39" s="90"/>
-      <c r="AE39" s="91"/>
-      <c r="AF39" s="92"/>
-      <c r="AG39" s="90"/>
-      <c r="AH39" s="91"/>
-      <c r="AI39" s="92"/>
-      <c r="AJ39" s="84"/>
-      <c r="AK39" s="85"/>
-      <c r="AL39" s="93"/>
+      <c r="Z39" s="65"/>
+      <c r="AA39" s="69"/>
+      <c r="AB39" s="70"/>
+      <c r="AC39" s="71"/>
+      <c r="AD39" s="72"/>
+      <c r="AE39" s="73"/>
+      <c r="AF39" s="74"/>
+      <c r="AG39" s="72"/>
+      <c r="AH39" s="73"/>
+      <c r="AI39" s="74"/>
+      <c r="AJ39" s="66"/>
+      <c r="AK39" s="67"/>
+      <c r="AL39" s="75"/>
     </row>
     <row r="40" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="Z40" s="77"/>
-      <c r="AA40" s="84" t="s">
+      <c r="Z40" s="65"/>
+      <c r="AA40" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="AB40" s="85" t="s">
+      <c r="AB40" s="67" t="s">
         <v>119</v>
       </c>
-      <c r="AC40" s="86" t="s">
+      <c r="AC40" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="AD40" s="84" t="s">
+      <c r="AD40" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="AE40" s="85" t="s">
+      <c r="AE40" s="67" t="s">
         <v>119</v>
       </c>
-      <c r="AF40" s="94" t="s">
+      <c r="AF40" s="76" t="s">
         <v>120</v>
       </c>
-      <c r="AG40" s="84" t="s">
+      <c r="AG40" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="AH40" s="85" t="s">
+      <c r="AH40" s="67" t="s">
         <v>119</v>
       </c>
-      <c r="AI40" s="94" t="s">
+      <c r="AI40" s="76" t="s">
         <v>120</v>
       </c>
-      <c r="AJ40" s="84" t="s">
+      <c r="AJ40" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="AK40" s="85" t="s">
+      <c r="AK40" s="67" t="s">
         <v>119</v>
       </c>
-      <c r="AL40" s="94" t="s">
+      <c r="AL40" s="76" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="Z41" s="77"/>
-      <c r="AA41" s="95"/>
-      <c r="AB41" s="96"/>
-      <c r="AC41" s="93"/>
-      <c r="AD41" s="95"/>
-      <c r="AE41" s="96"/>
-      <c r="AF41" s="94"/>
-      <c r="AG41" s="95"/>
-      <c r="AH41" s="96"/>
-      <c r="AI41" s="94"/>
-      <c r="AJ41" s="95"/>
-      <c r="AK41" s="96"/>
-      <c r="AL41" s="94"/>
+      <c r="Z41" s="65"/>
+      <c r="AA41" s="77"/>
+      <c r="AB41" s="78"/>
+      <c r="AC41" s="75"/>
+      <c r="AD41" s="77"/>
+      <c r="AE41" s="78"/>
+      <c r="AF41" s="76"/>
+      <c r="AG41" s="77"/>
+      <c r="AH41" s="78"/>
+      <c r="AI41" s="76"/>
+      <c r="AJ41" s="77"/>
+      <c r="AK41" s="78"/>
+      <c r="AL41" s="76"/>
     </row>
     <row r="42" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="Z42" s="77"/>
-      <c r="AA42" s="95"/>
-      <c r="AB42" s="96"/>
-      <c r="AC42" s="93"/>
-      <c r="AD42" s="95"/>
-      <c r="AE42" s="96"/>
-      <c r="AF42" s="94"/>
-      <c r="AG42" s="95"/>
-      <c r="AH42" s="96"/>
-      <c r="AI42" s="94"/>
-      <c r="AJ42" s="95"/>
-      <c r="AK42" s="96"/>
-      <c r="AL42" s="94"/>
+      <c r="Z42" s="65"/>
+      <c r="AA42" s="77"/>
+      <c r="AB42" s="78"/>
+      <c r="AC42" s="75"/>
+      <c r="AD42" s="77"/>
+      <c r="AE42" s="78"/>
+      <c r="AF42" s="76"/>
+      <c r="AG42" s="77"/>
+      <c r="AH42" s="78"/>
+      <c r="AI42" s="76"/>
+      <c r="AJ42" s="77"/>
+      <c r="AK42" s="78"/>
+      <c r="AL42" s="76"/>
     </row>
     <row r="43" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="Z43" s="77"/>
-      <c r="AA43" s="95"/>
-      <c r="AB43" s="96"/>
-      <c r="AC43" s="93"/>
-      <c r="AD43" s="95"/>
-      <c r="AE43" s="96"/>
-      <c r="AF43" s="94"/>
-      <c r="AG43" s="95"/>
-      <c r="AH43" s="96"/>
-      <c r="AI43" s="94"/>
-      <c r="AJ43" s="95"/>
-      <c r="AK43" s="96"/>
-      <c r="AL43" s="94"/>
+      <c r="Z43" s="65"/>
+      <c r="AA43" s="77"/>
+      <c r="AB43" s="78"/>
+      <c r="AC43" s="75"/>
+      <c r="AD43" s="77"/>
+      <c r="AE43" s="78"/>
+      <c r="AF43" s="76"/>
+      <c r="AG43" s="77"/>
+      <c r="AH43" s="78"/>
+      <c r="AI43" s="76"/>
+      <c r="AJ43" s="77"/>
+      <c r="AK43" s="78"/>
+      <c r="AL43" s="76"/>
     </row>
     <row r="44" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="Z44" s="77"/>
-      <c r="AA44" s="95"/>
-      <c r="AB44" s="96"/>
-      <c r="AC44" s="93"/>
-      <c r="AD44" s="95"/>
-      <c r="AE44" s="96"/>
-      <c r="AF44" s="94"/>
-      <c r="AG44" s="95"/>
-      <c r="AH44" s="96"/>
-      <c r="AI44" s="94"/>
-      <c r="AJ44" s="95"/>
-      <c r="AK44" s="96"/>
-      <c r="AL44" s="94"/>
+      <c r="Z44" s="65"/>
+      <c r="AA44" s="77"/>
+      <c r="AB44" s="78"/>
+      <c r="AC44" s="75"/>
+      <c r="AD44" s="77"/>
+      <c r="AE44" s="78"/>
+      <c r="AF44" s="76"/>
+      <c r="AG44" s="77"/>
+      <c r="AH44" s="78"/>
+      <c r="AI44" s="76"/>
+      <c r="AJ44" s="77"/>
+      <c r="AK44" s="78"/>
+      <c r="AL44" s="76"/>
     </row>
     <row r="45" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="Z45" s="77" t="s">
+      <c r="Z45" s="65" t="s">
         <v>78</v>
       </c>
-      <c r="AA45" s="97">
+      <c r="AA45" s="79">
         <v>1.5</v>
       </c>
-      <c r="AB45" s="72">
+      <c r="AB45" s="61">
         <v>2.2000000000000002</v>
       </c>
-      <c r="AC45" s="94"/>
-      <c r="AD45" s="97">
+      <c r="AC45" s="76"/>
+      <c r="AD45" s="79">
         <v>1.5</v>
       </c>
-      <c r="AE45" s="72">
+      <c r="AE45" s="61">
         <v>2.2000000000000002</v>
       </c>
-      <c r="AF45" s="94"/>
-      <c r="AG45" s="97">
+      <c r="AF45" s="76"/>
+      <c r="AG45" s="79">
         <v>1.5</v>
       </c>
-      <c r="AH45" s="72">
+      <c r="AH45" s="61">
         <v>2.2000000000000002</v>
       </c>
-      <c r="AI45" s="94"/>
-      <c r="AJ45" s="97">
+      <c r="AI45" s="76"/>
+      <c r="AJ45" s="79">
         <v>1.5</v>
       </c>
-      <c r="AK45" s="72">
+      <c r="AK45" s="61">
         <v>2.2000000000000002</v>
       </c>
-      <c r="AL45" s="94"/>
+      <c r="AL45" s="76"/>
     </row>
     <row r="46" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="Z46" s="77" t="s">
+      <c r="Z46" s="65" t="s">
         <v>121</v>
       </c>
-      <c r="AA46" s="97">
+      <c r="AA46" s="79">
         <v>0.11</v>
       </c>
-      <c r="AB46" s="72"/>
-      <c r="AC46" s="94">
+      <c r="AB46" s="61"/>
+      <c r="AC46" s="76">
         <v>83</v>
       </c>
-      <c r="AD46" s="97">
+      <c r="AD46" s="79">
         <v>0.17</v>
       </c>
-      <c r="AE46" s="72"/>
-      <c r="AF46" s="94">
+      <c r="AE46" s="61"/>
+      <c r="AF46" s="76">
         <f>AC46*1.8</f>
         <v>149.4</v>
       </c>
-      <c r="AG46" s="97">
+      <c r="AG46" s="79">
         <v>0.25</v>
       </c>
-      <c r="AH46" s="72"/>
-      <c r="AI46" s="94">
+      <c r="AH46" s="61"/>
+      <c r="AI46" s="76">
         <f>AC46*1.8</f>
         <v>149.4</v>
       </c>
-      <c r="AJ46" s="97">
+      <c r="AJ46" s="79">
         <v>0.35</v>
       </c>
-      <c r="AK46" s="72"/>
-      <c r="AL46" s="94">
+      <c r="AK46" s="61"/>
+      <c r="AL46" s="76">
         <f>AC46*1.5*1.8</f>
         <v>224.1</v>
       </c>
     </row>
     <row r="47" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="Z47" s="77" t="s">
+      <c r="Z47" s="65" t="s">
         <v>79</v>
       </c>
-      <c r="AA47" s="97">
+      <c r="AA47" s="79">
         <f>AA45-AA46*2</f>
         <v>1.28</v>
       </c>
-      <c r="AB47" s="72">
+      <c r="AB47" s="61">
         <f>AB45-AA46*2</f>
         <v>1.9800000000000002</v>
       </c>
-      <c r="AC47" s="94"/>
-      <c r="AD47" s="97">
+      <c r="AC47" s="76"/>
+      <c r="AD47" s="79">
         <f>AD45-AD46*2</f>
         <v>1.1599999999999999</v>
       </c>
-      <c r="AE47" s="72">
+      <c r="AE47" s="61">
         <f>AE45-AD46*2</f>
         <v>1.86</v>
       </c>
-      <c r="AF47" s="94"/>
-      <c r="AG47" s="97">
+      <c r="AF47" s="76"/>
+      <c r="AG47" s="79">
         <f>AG45-AG46*2</f>
         <v>1</v>
       </c>
-      <c r="AH47" s="72">
+      <c r="AH47" s="61">
         <f>AH45-AG46*2</f>
         <v>1.7000000000000002</v>
       </c>
-      <c r="AI47" s="94"/>
-      <c r="AJ47" s="97">
+      <c r="AI47" s="76"/>
+      <c r="AJ47" s="79">
         <f>AJ45-AJ46*2</f>
         <v>0.8</v>
       </c>
-      <c r="AK47" s="72">
+      <c r="AK47" s="61">
         <f>AK45-AJ46*2</f>
         <v>1.5000000000000002</v>
       </c>
-      <c r="AL47" s="94"/>
+      <c r="AL47" s="76"/>
     </row>
     <row r="48" spans="1:38" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Z48" s="77" t="s">
+      <c r="Z48" s="65" t="s">
         <v>122</v>
       </c>
-      <c r="AA48" s="98">
+      <c r="AA48" s="80">
         <f>AA47*AB47/AA45/AB45</f>
         <v>0.76800000000000002</v>
       </c>
-      <c r="AB48" s="99"/>
-      <c r="AC48" s="100"/>
-      <c r="AD48" s="101">
+      <c r="AB48" s="81"/>
+      <c r="AC48" s="82"/>
+      <c r="AD48" s="83">
         <f>AD47*AE47/AD45/AE45</f>
         <v>0.65381818181818174</v>
       </c>
-      <c r="AE48" s="99"/>
-      <c r="AF48" s="100"/>
-      <c r="AG48" s="98">
+      <c r="AE48" s="81"/>
+      <c r="AF48" s="82"/>
+      <c r="AG48" s="80">
         <f>AG47*AH47/AG45/AH45</f>
         <v>0.51515151515151525</v>
       </c>
-      <c r="AH48" s="99"/>
-      <c r="AI48" s="100"/>
-      <c r="AJ48" s="98">
+      <c r="AH48" s="81"/>
+      <c r="AI48" s="82"/>
+      <c r="AJ48" s="80">
         <f>AJ47*AK47/AJ45/AK45</f>
         <v>0.3636363636363637</v>
       </c>
-      <c r="AK48" s="99"/>
-      <c r="AL48" s="100"/>
+      <c r="AK48" s="81"/>
+      <c r="AL48" s="82"/>
     </row>
     <row r="49" spans="26:38" x14ac:dyDescent="0.25">
-      <c r="Z49" s="72" t="s">
+      <c r="Z49" s="61" t="s">
         <v>81</v>
       </c>
-      <c r="AA49" s="96">
+      <c r="AA49" s="78">
         <f>AC46/AA47/AB47</f>
         <v>32.749368686868685</v>
       </c>
-      <c r="AB49" s="96"/>
-      <c r="AC49" s="96"/>
-      <c r="AD49" s="96">
+      <c r="AB49" s="78"/>
+      <c r="AC49" s="78"/>
+      <c r="AD49" s="78">
         <f>AF46/AD47/AE47</f>
         <v>69.243604004449395</v>
       </c>
-      <c r="AE49" s="96"/>
-      <c r="AF49" s="96"/>
-      <c r="AG49" s="96">
+      <c r="AE49" s="78"/>
+      <c r="AF49" s="78"/>
+      <c r="AG49" s="78">
         <f>AI46/AG47/AH47</f>
         <v>87.882352941176464</v>
       </c>
-      <c r="AH49" s="96"/>
-      <c r="AI49" s="96"/>
-      <c r="AJ49" s="96">
+      <c r="AH49" s="78"/>
+      <c r="AI49" s="78"/>
+      <c r="AJ49" s="78">
         <f>AL46/AJ47/AK47</f>
         <v>186.74999999999997</v>
       </c>
-      <c r="AK49" s="96"/>
-      <c r="AL49" s="96"/>
+      <c r="AK49" s="78"/>
+      <c r="AL49" s="78"/>
     </row>
     <row r="50" spans="26:38" x14ac:dyDescent="0.25">
-      <c r="Z50" s="102" t="s">
+      <c r="Z50" s="84" t="s">
         <v>86</v>
       </c>
-      <c r="AA50" s="103"/>
-      <c r="AB50" s="103"/>
-      <c r="AC50" s="103">
+      <c r="AA50" s="85"/>
+      <c r="AB50" s="85"/>
+      <c r="AC50" s="85">
         <f>AC46/(AA47+AB47)/2</f>
         <v>12.730061349693251</v>
       </c>
-      <c r="AD50" s="103"/>
-      <c r="AE50" s="103"/>
-      <c r="AF50" s="103">
+      <c r="AD50" s="85"/>
+      <c r="AE50" s="85"/>
+      <c r="AF50" s="85">
         <f>AF46/(AD47+AE47)/2</f>
         <v>24.735099337748345</v>
       </c>
     </row>
     <row r="51" spans="26:38" x14ac:dyDescent="0.25">
-      <c r="Z51" s="104" t="s">
+      <c r="Z51" s="86" t="s">
         <v>78</v>
       </c>
-      <c r="AA51" s="105">
+      <c r="AA51" s="87">
         <f>AA53+AA52*2</f>
         <v>1.52</v>
       </c>
-      <c r="AB51" s="105">
+      <c r="AB51" s="87">
         <f>AB53+AA52*2</f>
         <v>1.52</v>
       </c>
-      <c r="AC51" s="105">
+      <c r="AC51" s="87">
         <f>AA51*AB51</f>
         <v>2.3104</v>
       </c>
-      <c r="AD51" s="105">
+      <c r="AD51" s="87">
         <f>AD53+AD52*2</f>
         <v>1.6400000000000001</v>
       </c>
-      <c r="AE51" s="105">
+      <c r="AE51" s="87">
         <f>AE53+AD52*2</f>
         <v>1.6400000000000001</v>
       </c>
-      <c r="AF51" s="105">
+      <c r="AF51" s="87">
         <f>AD51*AE51</f>
         <v>2.6896000000000004</v>
       </c>
     </row>
     <row r="52" spans="26:38" x14ac:dyDescent="0.25">
-      <c r="Z52" s="104" t="s">
+      <c r="Z52" s="86" t="s">
         <v>80</v>
       </c>
-      <c r="AA52" s="105">
+      <c r="AA52" s="87">
         <v>0.11</v>
       </c>
-      <c r="AB52" s="105"/>
-      <c r="AC52" s="105">
+      <c r="AB52" s="87"/>
+      <c r="AC52" s="87">
         <f>AC50*(AA51+AB51)*2</f>
         <v>77.398773006134974</v>
       </c>
-      <c r="AD52" s="105">
+      <c r="AD52" s="87">
         <v>0.17</v>
       </c>
-      <c r="AE52" s="105"/>
-      <c r="AF52" s="105">
+      <c r="AE52" s="87"/>
+      <c r="AF52" s="87">
         <f>AF50*(AD51+AE51)*2</f>
         <v>162.26225165562914</v>
       </c>
     </row>
     <row r="53" spans="26:38" x14ac:dyDescent="0.25">
-      <c r="Z53" s="104" t="s">
+      <c r="Z53" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="AA53" s="105">
+      <c r="AA53" s="87">
         <v>1.3</v>
       </c>
-      <c r="AB53" s="105">
+      <c r="AB53" s="87">
         <v>1.3</v>
       </c>
-      <c r="AC53" s="105">
+      <c r="AC53" s="87">
         <f>AA53*AB53</f>
         <v>1.6900000000000002</v>
       </c>
-      <c r="AD53" s="105">
+      <c r="AD53" s="87">
         <v>1.3</v>
       </c>
-      <c r="AE53" s="105">
+      <c r="AE53" s="87">
         <v>1.3</v>
       </c>
-      <c r="AF53" s="105"/>
+      <c r="AF53" s="87"/>
     </row>
     <row r="54" spans="26:38" x14ac:dyDescent="0.25">
-      <c r="Z54" s="104" t="s">
+      <c r="Z54" s="86" t="s">
         <v>87</v>
       </c>
-      <c r="AA54" s="105"/>
-      <c r="AB54" s="105"/>
-      <c r="AC54" s="105">
+      <c r="AA54" s="87"/>
+      <c r="AB54" s="87"/>
+      <c r="AC54" s="87">
         <f>AA52*(AA53+AB53)*2</f>
         <v>0.57200000000000006</v>
       </c>
-      <c r="AD54" s="105"/>
-      <c r="AE54" s="105"/>
-      <c r="AF54" s="105">
+      <c r="AD54" s="87"/>
+      <c r="AE54" s="87"/>
+      <c r="AF54" s="87">
         <f>AD52*(AD53+AE53)*2</f>
         <v>0.88400000000000012</v>
       </c>
     </row>
     <row r="55" spans="26:38" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Z55" s="104" t="s">
+      <c r="Z55" s="86" t="s">
         <v>123</v>
       </c>
-      <c r="AA55" s="105"/>
-      <c r="AB55" s="105"/>
-      <c r="AC55" s="105"/>
-      <c r="AD55" s="106">
+      <c r="AA55" s="87"/>
+      <c r="AB55" s="87"/>
+      <c r="AC55" s="87"/>
+      <c r="AD55" s="88">
         <f>AD53*AE53/AD51/AE51</f>
         <v>0.62834622248661509</v>
       </c>
-      <c r="AE55" s="105"/>
-      <c r="AF55" s="105"/>
+      <c r="AE55" s="87"/>
+      <c r="AF55" s="87"/>
     </row>
     <row r="56" spans="26:38" x14ac:dyDescent="0.25">
-      <c r="Z56" s="107" t="s">
+      <c r="Z56" s="89" t="s">
         <v>81</v>
       </c>
-      <c r="AA56" s="105"/>
-      <c r="AB56" s="105"/>
-      <c r="AC56" s="105"/>
-      <c r="AD56" s="108">
+      <c r="AA56" s="87"/>
+      <c r="AB56" s="87"/>
+      <c r="AC56" s="87"/>
+      <c r="AD56" s="90">
         <f>AF52/AD53/AE53</f>
         <v>96.013166660135582</v>
       </c>
-      <c r="AE56" s="105"/>
-      <c r="AF56" s="105"/>
+      <c r="AE56" s="87"/>
+      <c r="AF56" s="87"/>
     </row>
     <row r="57" spans="26:38" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Z57" s="109"/>
-      <c r="AA57" s="105"/>
-      <c r="AB57" s="105"/>
-      <c r="AC57" s="105"/>
-      <c r="AD57" s="110"/>
-      <c r="AE57" s="105"/>
-      <c r="AF57" s="105"/>
+      <c r="Z57" s="91"/>
+      <c r="AA57" s="87"/>
+      <c r="AB57" s="87"/>
+      <c r="AC57" s="87"/>
+      <c r="AD57" s="92"/>
+      <c r="AE57" s="87"/>
+      <c r="AF57" s="87"/>
     </row>
     <row r="58" spans="26:38" x14ac:dyDescent="0.25">
-      <c r="Z58" s="84"/>
-      <c r="AA58" s="111" t="s">
+      <c r="Z58" s="66"/>
+      <c r="AA58" s="93" t="s">
         <v>114</v>
       </c>
-      <c r="AB58" s="111"/>
-      <c r="AC58" s="111"/>
+      <c r="AB58" s="93"/>
+      <c r="AC58" s="93"/>
       <c r="AD58" s="112" t="s">
         <v>124</v>
       </c>
@@ -5149,357 +5380,357 @@
       </c>
       <c r="AH58" s="112"/>
       <c r="AI58" s="112"/>
-      <c r="AJ58" s="85" t="s">
+      <c r="AJ58" s="67" t="s">
         <v>117</v>
       </c>
-      <c r="AK58" s="85"/>
-      <c r="AL58" s="86"/>
+      <c r="AK58" s="67"/>
+      <c r="AL58" s="68"/>
     </row>
     <row r="59" spans="26:38" x14ac:dyDescent="0.25">
-      <c r="Z59" s="97"/>
-      <c r="AA59" s="72" t="s">
+      <c r="Z59" s="79"/>
+      <c r="AA59" s="61" t="s">
         <v>118</v>
       </c>
-      <c r="AB59" s="72" t="s">
+      <c r="AB59" s="61" t="s">
         <v>119</v>
       </c>
-      <c r="AC59" s="72" t="s">
+      <c r="AC59" s="61" t="s">
         <v>125</v>
       </c>
-      <c r="AD59" s="72" t="s">
+      <c r="AD59" s="61" t="s">
         <v>118</v>
       </c>
-      <c r="AE59" s="72" t="s">
+      <c r="AE59" s="61" t="s">
         <v>119</v>
       </c>
-      <c r="AF59" s="72" t="s">
+      <c r="AF59" s="61" t="s">
         <v>120</v>
       </c>
-      <c r="AG59" s="72" t="s">
+      <c r="AG59" s="61" t="s">
         <v>118</v>
       </c>
-      <c r="AH59" s="72" t="s">
+      <c r="AH59" s="61" t="s">
         <v>119</v>
       </c>
-      <c r="AI59" s="72" t="s">
+      <c r="AI59" s="61" t="s">
         <v>120</v>
       </c>
-      <c r="AJ59" s="72" t="s">
+      <c r="AJ59" s="61" t="s">
         <v>118</v>
       </c>
-      <c r="AK59" s="72" t="s">
+      <c r="AK59" s="61" t="s">
         <v>119</v>
       </c>
-      <c r="AL59" s="94" t="s">
+      <c r="AL59" s="76" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="60" spans="26:38" x14ac:dyDescent="0.25">
-      <c r="Z60" s="113" t="s">
+      <c r="Z60" s="94" t="s">
         <v>79</v>
       </c>
-      <c r="AA60" s="114">
+      <c r="AA60" s="95">
         <v>1.7</v>
       </c>
-      <c r="AB60" s="114">
+      <c r="AB60" s="95">
         <v>1</v>
       </c>
-      <c r="AC60" s="114">
+      <c r="AC60" s="95">
         <v>0.11</v>
       </c>
-      <c r="AD60" s="114">
+      <c r="AD60" s="95">
         <v>1.7</v>
       </c>
-      <c r="AE60" s="114">
+      <c r="AE60" s="95">
         <v>1</v>
       </c>
-      <c r="AF60" s="114">
+      <c r="AF60" s="95">
         <v>1.7</v>
       </c>
-      <c r="AG60" s="72"/>
-      <c r="AH60" s="72"/>
-      <c r="AI60" s="72"/>
-      <c r="AJ60" s="72"/>
-      <c r="AK60" s="72"/>
-      <c r="AL60" s="94"/>
+      <c r="AG60" s="61"/>
+      <c r="AH60" s="61"/>
+      <c r="AI60" s="61"/>
+      <c r="AJ60" s="61"/>
+      <c r="AK60" s="61"/>
+      <c r="AL60" s="76"/>
     </row>
     <row r="61" spans="26:38" x14ac:dyDescent="0.25">
-      <c r="Z61" s="113" t="s">
+      <c r="Z61" s="94" t="s">
         <v>78</v>
       </c>
-      <c r="AA61" s="114">
+      <c r="AA61" s="95">
         <f>AA60+AC60*2</f>
         <v>1.92</v>
       </c>
-      <c r="AB61" s="114">
+      <c r="AB61" s="95">
         <f>AB60+AC60*2</f>
         <v>1.22</v>
       </c>
-      <c r="AC61" s="114">
+      <c r="AC61" s="95">
         <f>AA61*AB61</f>
         <v>2.3424</v>
       </c>
-      <c r="AD61" s="114">
+      <c r="AD61" s="95">
         <f>AD60+AD62*2</f>
         <v>2.04</v>
       </c>
-      <c r="AE61" s="114">
+      <c r="AE61" s="95">
         <f>AE60+AD62*2</f>
         <v>1.34</v>
       </c>
-      <c r="AF61" s="114">
+      <c r="AF61" s="95">
         <f>AD61*AE61</f>
         <v>2.7336</v>
       </c>
-      <c r="AG61" s="72"/>
-      <c r="AH61" s="72"/>
-      <c r="AI61" s="72"/>
-      <c r="AJ61" s="72"/>
-      <c r="AK61" s="72"/>
-      <c r="AL61" s="94"/>
+      <c r="AG61" s="61"/>
+      <c r="AH61" s="61"/>
+      <c r="AI61" s="61"/>
+      <c r="AJ61" s="61"/>
+      <c r="AK61" s="61"/>
+      <c r="AL61" s="76"/>
     </row>
     <row r="62" spans="26:38" x14ac:dyDescent="0.25">
-      <c r="Z62" s="113" t="s">
+      <c r="Z62" s="94" t="s">
         <v>126</v>
       </c>
-      <c r="AB62" s="114"/>
-      <c r="AC62" s="114">
+      <c r="AB62" s="95"/>
+      <c r="AC62" s="95">
         <f>AC56*(AA61+AB61)*2</f>
         <v>0</v>
       </c>
-      <c r="AD62" s="114">
+      <c r="AD62" s="95">
         <v>0.17</v>
       </c>
-      <c r="AE62" s="114"/>
-      <c r="AF62" s="114">
+      <c r="AE62" s="95"/>
+      <c r="AF62" s="95">
         <f>AF56*(AD61+AE61)*2</f>
         <v>0</v>
       </c>
-      <c r="AG62" s="72"/>
-      <c r="AH62" s="72"/>
-      <c r="AI62" s="72"/>
-      <c r="AJ62" s="72"/>
-      <c r="AK62" s="72"/>
-      <c r="AL62" s="94"/>
+      <c r="AG62" s="61"/>
+      <c r="AH62" s="61"/>
+      <c r="AI62" s="61"/>
+      <c r="AJ62" s="61"/>
+      <c r="AK62" s="61"/>
+      <c r="AL62" s="76"/>
     </row>
     <row r="63" spans="26:38" x14ac:dyDescent="0.25">
-      <c r="Z63" s="113" t="s">
+      <c r="Z63" s="94" t="s">
         <v>87</v>
       </c>
-      <c r="AA63" s="114"/>
-      <c r="AB63" s="114"/>
-      <c r="AC63" s="114" t="e">
+      <c r="AA63" s="95"/>
+      <c r="AB63" s="95"/>
+      <c r="AC63" s="95" t="e">
         <f>AC61-#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="AD63" s="114"/>
-      <c r="AE63" s="114"/>
-      <c r="AF63" s="114">
+      <c r="AD63" s="95"/>
+      <c r="AE63" s="95"/>
+      <c r="AF63" s="95">
         <f>AF61-AF60</f>
         <v>1.0336000000000001</v>
       </c>
-      <c r="AG63" s="72"/>
-      <c r="AH63" s="72"/>
-      <c r="AI63" s="72"/>
-      <c r="AJ63" s="72"/>
-      <c r="AK63" s="72"/>
-      <c r="AL63" s="94"/>
+      <c r="AG63" s="61"/>
+      <c r="AH63" s="61"/>
+      <c r="AI63" s="61"/>
+      <c r="AJ63" s="61"/>
+      <c r="AK63" s="61"/>
+      <c r="AL63" s="76"/>
     </row>
     <row r="64" spans="26:38" x14ac:dyDescent="0.25">
-      <c r="Z64" s="113" t="s">
+      <c r="Z64" s="94" t="s">
         <v>127</v>
       </c>
-      <c r="AA64" s="114"/>
-      <c r="AB64" s="114"/>
-      <c r="AC64" s="114"/>
-      <c r="AD64" s="115">
+      <c r="AA64" s="95"/>
+      <c r="AB64" s="95"/>
+      <c r="AC64" s="95"/>
+      <c r="AD64" s="96">
         <f>AD60*AE60/AD61/AE61</f>
         <v>0.62189054726368154</v>
       </c>
-      <c r="AE64" s="114"/>
-      <c r="AF64" s="114"/>
-      <c r="AG64" s="72"/>
-      <c r="AH64" s="72"/>
-      <c r="AI64" s="72"/>
-      <c r="AJ64" s="72"/>
-      <c r="AK64" s="72"/>
-      <c r="AL64" s="94"/>
+      <c r="AE64" s="95"/>
+      <c r="AF64" s="95"/>
+      <c r="AG64" s="61"/>
+      <c r="AH64" s="61"/>
+      <c r="AI64" s="61"/>
+      <c r="AJ64" s="61"/>
+      <c r="AK64" s="61"/>
+      <c r="AL64" s="76"/>
     </row>
     <row r="65" spans="26:38" x14ac:dyDescent="0.25">
-      <c r="Z65" s="113" t="s">
+      <c r="Z65" s="94" t="s">
         <v>81</v>
       </c>
-      <c r="AA65" s="114"/>
-      <c r="AB65" s="114"/>
-      <c r="AC65" s="114"/>
-      <c r="AD65" s="114">
+      <c r="AA65" s="95"/>
+      <c r="AB65" s="95"/>
+      <c r="AC65" s="95"/>
+      <c r="AD65" s="95">
         <f>AF62/AD60/AE60</f>
         <v>0</v>
       </c>
-      <c r="AE65" s="114"/>
-      <c r="AF65" s="114"/>
-      <c r="AG65" s="72"/>
-      <c r="AH65" s="72"/>
-      <c r="AI65" s="72"/>
-      <c r="AJ65" s="72"/>
-      <c r="AK65" s="72"/>
-      <c r="AL65" s="94"/>
+      <c r="AE65" s="95"/>
+      <c r="AF65" s="95"/>
+      <c r="AG65" s="61"/>
+      <c r="AH65" s="61"/>
+      <c r="AI65" s="61"/>
+      <c r="AJ65" s="61"/>
+      <c r="AK65" s="61"/>
+      <c r="AL65" s="76"/>
     </row>
     <row r="66" spans="26:38" x14ac:dyDescent="0.25">
-      <c r="Z66" s="97" t="s">
+      <c r="Z66" s="79" t="s">
         <v>78</v>
       </c>
-      <c r="AA66" s="72">
+      <c r="AA66" s="61">
         <f>AA68+AA67*2</f>
         <v>1.07</v>
       </c>
-      <c r="AB66" s="72">
+      <c r="AB66" s="61">
         <f>AB68+AA67*2</f>
         <v>2.2200000000000002</v>
       </c>
-      <c r="AC66" s="72">
+      <c r="AC66" s="61">
         <f>AA66*AB66</f>
         <v>2.3754000000000004</v>
       </c>
-      <c r="AD66" s="72">
+      <c r="AD66" s="61">
         <f>AD68+AD67*2</f>
         <v>1.19</v>
       </c>
-      <c r="AE66" s="72">
+      <c r="AE66" s="61">
         <f>AE68+AD67*2</f>
         <v>2.34</v>
       </c>
-      <c r="AF66" s="72">
+      <c r="AF66" s="61">
         <f>AD66*AE66</f>
         <v>2.7845999999999997</v>
       </c>
-      <c r="AG66" s="72"/>
-      <c r="AH66" s="72"/>
-      <c r="AI66" s="72"/>
-      <c r="AJ66" s="72"/>
-      <c r="AK66" s="72"/>
-      <c r="AL66" s="94"/>
+      <c r="AG66" s="61"/>
+      <c r="AH66" s="61"/>
+      <c r="AI66" s="61"/>
+      <c r="AJ66" s="61"/>
+      <c r="AK66" s="61"/>
+      <c r="AL66" s="76"/>
     </row>
     <row r="67" spans="26:38" x14ac:dyDescent="0.25">
-      <c r="Z67" s="97" t="s">
+      <c r="Z67" s="79" t="s">
         <v>80</v>
       </c>
-      <c r="AA67" s="72">
+      <c r="AA67" s="61">
         <v>0.11</v>
       </c>
-      <c r="AB67" s="72"/>
-      <c r="AC67" s="72">
+      <c r="AB67" s="61"/>
+      <c r="AC67" s="61">
         <f>AC50*(AA68+AB68)*2</f>
         <v>72.561349693251529</v>
       </c>
-      <c r="AD67" s="72">
+      <c r="AD67" s="61">
         <v>0.17</v>
       </c>
-      <c r="AE67" s="72"/>
-      <c r="AF67" s="72">
+      <c r="AE67" s="61"/>
+      <c r="AF67" s="61">
         <f>AF50*(AD68+AE68)*2</f>
         <v>140.99006622516558</v>
       </c>
-      <c r="AG67" s="72"/>
-      <c r="AH67" s="72"/>
-      <c r="AI67" s="72"/>
-      <c r="AJ67" s="72"/>
-      <c r="AK67" s="72"/>
-      <c r="AL67" s="94"/>
+      <c r="AG67" s="61"/>
+      <c r="AH67" s="61"/>
+      <c r="AI67" s="61"/>
+      <c r="AJ67" s="61"/>
+      <c r="AK67" s="61"/>
+      <c r="AL67" s="76"/>
     </row>
     <row r="68" spans="26:38" x14ac:dyDescent="0.25">
-      <c r="Z68" s="97" t="s">
+      <c r="Z68" s="79" t="s">
         <v>79</v>
       </c>
-      <c r="AA68" s="72">
+      <c r="AA68" s="61">
         <f>AC68/AB68</f>
         <v>0.85</v>
       </c>
-      <c r="AB68" s="72">
+      <c r="AB68" s="61">
         <v>2</v>
       </c>
-      <c r="AC68" s="72">
+      <c r="AC68" s="61">
         <v>1.7</v>
       </c>
-      <c r="AD68" s="72">
+      <c r="AD68" s="61">
         <f>AF68/AE68</f>
         <v>0.85</v>
       </c>
-      <c r="AE68" s="72">
+      <c r="AE68" s="61">
         <v>2</v>
       </c>
-      <c r="AF68" s="72">
+      <c r="AF68" s="61">
         <v>1.7</v>
       </c>
-      <c r="AG68" s="72"/>
-      <c r="AH68" s="72"/>
-      <c r="AI68" s="72"/>
-      <c r="AJ68" s="72"/>
-      <c r="AK68" s="72"/>
-      <c r="AL68" s="94"/>
+      <c r="AG68" s="61"/>
+      <c r="AH68" s="61"/>
+      <c r="AI68" s="61"/>
+      <c r="AJ68" s="61"/>
+      <c r="AK68" s="61"/>
+      <c r="AL68" s="76"/>
     </row>
     <row r="69" spans="26:38" x14ac:dyDescent="0.25">
-      <c r="Z69" s="97" t="s">
+      <c r="Z69" s="79" t="s">
         <v>87</v>
       </c>
-      <c r="AA69" s="72"/>
-      <c r="AB69" s="72"/>
-      <c r="AC69" s="72">
+      <c r="AA69" s="61"/>
+      <c r="AB69" s="61"/>
+      <c r="AC69" s="61">
         <f>AC66-AC68</f>
         <v>0.67540000000000044</v>
       </c>
-      <c r="AD69" s="72"/>
-      <c r="AE69" s="72"/>
-      <c r="AF69" s="72">
+      <c r="AD69" s="61"/>
+      <c r="AE69" s="61"/>
+      <c r="AF69" s="61">
         <f>AF66-AF68</f>
         <v>1.0845999999999998</v>
       </c>
-      <c r="AG69" s="72"/>
-      <c r="AH69" s="72"/>
-      <c r="AI69" s="72"/>
-      <c r="AJ69" s="72"/>
-      <c r="AK69" s="72"/>
-      <c r="AL69" s="94"/>
+      <c r="AG69" s="61"/>
+      <c r="AH69" s="61"/>
+      <c r="AI69" s="61"/>
+      <c r="AJ69" s="61"/>
+      <c r="AK69" s="61"/>
+      <c r="AL69" s="76"/>
     </row>
     <row r="70" spans="26:38" x14ac:dyDescent="0.25">
-      <c r="Z70" s="97" t="s">
+      <c r="Z70" s="79" t="s">
         <v>122</v>
       </c>
-      <c r="AA70" s="72"/>
-      <c r="AB70" s="72"/>
-      <c r="AC70" s="72"/>
-      <c r="AD70" s="116">
+      <c r="AA70" s="61"/>
+      <c r="AB70" s="61"/>
+      <c r="AC70" s="61"/>
+      <c r="AD70" s="97">
         <f>AD68*AE68/AD66/AE66</f>
         <v>0.61050061050061055</v>
       </c>
-      <c r="AE70" s="72"/>
-      <c r="AF70" s="72"/>
-      <c r="AG70" s="72"/>
-      <c r="AH70" s="72"/>
-      <c r="AI70" s="72"/>
-      <c r="AJ70" s="72"/>
-      <c r="AK70" s="72"/>
-      <c r="AL70" s="94"/>
+      <c r="AE70" s="61"/>
+      <c r="AF70" s="61"/>
+      <c r="AG70" s="61"/>
+      <c r="AH70" s="61"/>
+      <c r="AI70" s="61"/>
+      <c r="AJ70" s="61"/>
+      <c r="AK70" s="61"/>
+      <c r="AL70" s="76"/>
     </row>
     <row r="71" spans="26:38" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Z71" s="98" t="s">
+      <c r="Z71" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="AA71" s="99"/>
-      <c r="AB71" s="99"/>
-      <c r="AC71" s="99"/>
-      <c r="AD71" s="99">
+      <c r="AA71" s="81"/>
+      <c r="AB71" s="81"/>
+      <c r="AC71" s="81"/>
+      <c r="AD71" s="81">
         <f>AF67/AD68/AE68</f>
         <v>82.935333073626808</v>
       </c>
-      <c r="AE71" s="99"/>
-      <c r="AF71" s="99"/>
-      <c r="AG71" s="99"/>
-      <c r="AH71" s="99"/>
-      <c r="AI71" s="99"/>
-      <c r="AJ71" s="99"/>
-      <c r="AK71" s="99"/>
-      <c r="AL71" s="100"/>
+      <c r="AE71" s="81"/>
+      <c r="AF71" s="81"/>
+      <c r="AG71" s="81"/>
+      <c r="AH71" s="81"/>
+      <c r="AI71" s="81"/>
+      <c r="AJ71" s="81"/>
+      <c r="AK71" s="81"/>
+      <c r="AL71" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -5516,4 +5747,18 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>